<commit_message>
Added "FSM deadband" to the Settings sheet
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/prw_energinet_dk/Documents/Dokumenter/GitHub/MTB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="11_65313A6E4C5506009E52DA9B1CE17435CB52B360" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{869C8DB8-AC28-4D07-8F5B-80774FA0CC3C}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="11_65313A6E4C5506009E52DA9B1CE17435CB52B360" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADAE1870-AFBD-4A5B-B92E-E02D13B5CF6A}"/>
   <bookViews>
     <workbookView xWindow="-16700" yWindow="-21710" windowWidth="51420" windowHeight="21100" tabRatio="822" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -290,7 +290,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2846" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2847" uniqueCount="681">
   <si>
     <t>Range</t>
   </si>
@@ -2520,6 +2520,9 @@
   </si>
   <si>
     <t>Initial Settings</t>
+  </si>
+  <si>
+    <t>If any</t>
   </si>
 </sst>
 </file>
@@ -3268,7 +3271,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="283">
+  <cellXfs count="284">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -3930,6 +3933,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3945,13 +3958,25 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3972,10 +3997,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3987,28 +4012,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -4573,7 +4577,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4590,19 +4594,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A1" s="275" t="s">
+      <c r="A1" s="256" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="276" t="s">
+      <c r="B1" s="257" t="s">
         <v>228</v>
       </c>
-      <c r="C1" s="276" t="s">
+      <c r="C1" s="257" t="s">
         <v>218</v>
       </c>
-      <c r="D1" s="276" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="275" t="s">
+      <c r="D1" s="257" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="256" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4696,16 +4700,16 @@
         <v>435</v>
       </c>
       <c r="H7" s="144"/>
-      <c r="I7" s="256" t="s">
+      <c r="I7" s="260" t="s">
         <v>466</v>
       </c>
-      <c r="J7" s="256"/>
-      <c r="K7" s="256"/>
-      <c r="L7" s="256" t="s">
+      <c r="J7" s="260"/>
+      <c r="K7" s="260"/>
+      <c r="L7" s="260" t="s">
         <v>467</v>
       </c>
-      <c r="M7" s="256"/>
-      <c r="N7" s="257"/>
+      <c r="M7" s="260"/>
+      <c r="N7" s="261"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" s="27" t="s">
@@ -4742,13 +4746,15 @@
       <c r="A9" s="247" t="s">
         <v>677</v>
       </c>
-      <c r="B9" s="277">
+      <c r="B9" s="258">
         <v>0</v>
       </c>
       <c r="C9" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="E9" s="162"/>
+      <c r="E9" s="283" t="s">
+        <v>680</v>
+      </c>
       <c r="H9" s="145"/>
       <c r="I9" s="143"/>
       <c r="J9" s="143"/>
@@ -5128,7 +5134,7 @@
       <c r="B2" s="237" t="s">
         <v>378</v>
       </c>
-      <c r="C2" s="269" t="s">
+      <c r="C2" s="277" t="s">
         <v>514</v>
       </c>
       <c r="D2" s="186" t="s">
@@ -5142,7 +5148,7 @@
       <c r="B3" s="239" t="s">
         <v>379</v>
       </c>
-      <c r="C3" s="271"/>
+      <c r="C3" s="278"/>
       <c r="D3" s="177" t="s">
         <v>11</v>
       </c>
@@ -5154,7 +5160,7 @@
       <c r="B4" s="239" t="s">
         <v>380</v>
       </c>
-      <c r="C4" s="271"/>
+      <c r="C4" s="278"/>
       <c r="D4" s="177" t="s">
         <v>11</v>
       </c>
@@ -5166,7 +5172,7 @@
       <c r="B5" s="239" t="s">
         <v>381</v>
       </c>
-      <c r="C5" s="271"/>
+      <c r="C5" s="278"/>
       <c r="D5" s="177" t="s">
         <v>11</v>
       </c>
@@ -5178,7 +5184,7 @@
       <c r="B6" s="239" t="s">
         <v>382</v>
       </c>
-      <c r="C6" s="271"/>
+      <c r="C6" s="278"/>
       <c r="D6" s="177" t="s">
         <v>11</v>
       </c>
@@ -5190,7 +5196,7 @@
       <c r="B7" s="241" t="s">
         <v>383</v>
       </c>
-      <c r="C7" s="270"/>
+      <c r="C7" s="279"/>
       <c r="D7" s="182" t="s">
         <v>11</v>
       </c>
@@ -5216,7 +5222,7 @@
       <c r="B9" s="173" t="s">
         <v>385</v>
       </c>
-      <c r="C9" s="272" t="s">
+      <c r="C9" s="280" t="s">
         <v>637</v>
       </c>
       <c r="D9" s="186" t="s">
@@ -5230,7 +5236,7 @@
       <c r="B10" s="230" t="s">
         <v>386</v>
       </c>
-      <c r="C10" s="273"/>
+      <c r="C10" s="281"/>
       <c r="D10" s="182" t="s">
         <v>639</v>
       </c>
@@ -5242,7 +5248,7 @@
       <c r="B11" s="227" t="s">
         <v>387</v>
       </c>
-      <c r="C11" s="269" t="s">
+      <c r="C11" s="277" t="s">
         <v>640</v>
       </c>
       <c r="D11" s="186" t="s">
@@ -5256,7 +5262,7 @@
       <c r="B12" s="228" t="s">
         <v>388</v>
       </c>
-      <c r="C12" s="271"/>
+      <c r="C12" s="278"/>
       <c r="D12" s="177" t="s">
         <v>642</v>
       </c>
@@ -5268,7 +5274,7 @@
       <c r="B13" s="229" t="s">
         <v>389</v>
       </c>
-      <c r="C13" s="270"/>
+      <c r="C13" s="279"/>
       <c r="D13" s="182" t="s">
         <v>643</v>
       </c>
@@ -5280,7 +5286,7 @@
       <c r="B14" s="197" t="s">
         <v>390</v>
       </c>
-      <c r="C14" s="272" t="s">
+      <c r="C14" s="280" t="s">
         <v>561</v>
       </c>
       <c r="D14" s="186" t="s">
@@ -5294,7 +5300,7 @@
       <c r="B15" s="199" t="s">
         <v>391</v>
       </c>
-      <c r="C15" s="274"/>
+      <c r="C15" s="282"/>
       <c r="D15" s="177" t="s">
         <v>11</v>
       </c>
@@ -5306,7 +5312,7 @@
       <c r="B16" s="199" t="s">
         <v>392</v>
       </c>
-      <c r="C16" s="274"/>
+      <c r="C16" s="282"/>
       <c r="D16" s="177" t="s">
         <v>11</v>
       </c>
@@ -5318,7 +5324,7 @@
       <c r="B17" s="199" t="s">
         <v>393</v>
       </c>
-      <c r="C17" s="274"/>
+      <c r="C17" s="282"/>
       <c r="D17" s="177" t="s">
         <v>11</v>
       </c>
@@ -5330,7 +5336,7 @@
       <c r="B18" s="199" t="s">
         <v>394</v>
       </c>
-      <c r="C18" s="274"/>
+      <c r="C18" s="282"/>
       <c r="D18" s="177" t="s">
         <v>11</v>
       </c>
@@ -5342,7 +5348,7 @@
       <c r="B19" s="199" t="s">
         <v>395</v>
       </c>
-      <c r="C19" s="274"/>
+      <c r="C19" s="282"/>
       <c r="D19" s="177" t="s">
         <v>11</v>
       </c>
@@ -5354,7 +5360,7 @@
       <c r="B20" s="199" t="s">
         <v>396</v>
       </c>
-      <c r="C20" s="274"/>
+      <c r="C20" s="282"/>
       <c r="D20" s="177" t="s">
         <v>11</v>
       </c>
@@ -5366,7 +5372,7 @@
       <c r="B21" s="199" t="s">
         <v>397</v>
       </c>
-      <c r="C21" s="274"/>
+      <c r="C21" s="282"/>
       <c r="D21" s="177" t="s">
         <v>11</v>
       </c>
@@ -5378,7 +5384,7 @@
       <c r="B22" s="199" t="s">
         <v>398</v>
       </c>
-      <c r="C22" s="274"/>
+      <c r="C22" s="282"/>
       <c r="D22" s="177" t="s">
         <v>11</v>
       </c>
@@ -5390,7 +5396,7 @@
       <c r="B23" s="199" t="s">
         <v>399</v>
       </c>
-      <c r="C23" s="274"/>
+      <c r="C23" s="282"/>
       <c r="D23" s="177" t="s">
         <v>11</v>
       </c>
@@ -5402,7 +5408,7 @@
       <c r="B24" s="199" t="s">
         <v>400</v>
       </c>
-      <c r="C24" s="274"/>
+      <c r="C24" s="282"/>
       <c r="D24" s="177" t="s">
         <v>11</v>
       </c>
@@ -5414,7 +5420,7 @@
       <c r="B25" s="199" t="s">
         <v>401</v>
       </c>
-      <c r="C25" s="274"/>
+      <c r="C25" s="282"/>
       <c r="D25" s="177" t="s">
         <v>11</v>
       </c>
@@ -5426,7 +5432,7 @@
       <c r="B26" s="199" t="s">
         <v>402</v>
       </c>
-      <c r="C26" s="274"/>
+      <c r="C26" s="282"/>
       <c r="D26" s="177" t="s">
         <v>564</v>
       </c>
@@ -5438,7 +5444,7 @@
       <c r="B27" s="199" t="s">
         <v>403</v>
       </c>
-      <c r="C27" s="274"/>
+      <c r="C27" s="282"/>
       <c r="D27" s="177" t="s">
         <v>565</v>
       </c>
@@ -5450,7 +5456,7 @@
       <c r="B28" s="199" t="s">
         <v>404</v>
       </c>
-      <c r="C28" s="274"/>
+      <c r="C28" s="282"/>
       <c r="D28" s="177" t="s">
         <v>566</v>
       </c>
@@ -5462,7 +5468,7 @@
       <c r="B29" s="199" t="s">
         <v>405</v>
       </c>
-      <c r="C29" s="274"/>
+      <c r="C29" s="282"/>
       <c r="D29" s="177" t="s">
         <v>567</v>
       </c>
@@ -5474,7 +5480,7 @@
       <c r="B30" s="199" t="s">
         <v>406</v>
       </c>
-      <c r="C30" s="274"/>
+      <c r="C30" s="282"/>
       <c r="D30" s="183" t="s">
         <v>645</v>
       </c>
@@ -5486,7 +5492,7 @@
       <c r="B31" s="199" t="s">
         <v>407</v>
       </c>
-      <c r="C31" s="274"/>
+      <c r="C31" s="282"/>
       <c r="D31" s="183" t="s">
         <v>645</v>
       </c>
@@ -5498,7 +5504,7 @@
       <c r="B32" s="199" t="s">
         <v>408</v>
       </c>
-      <c r="C32" s="274"/>
+      <c r="C32" s="282"/>
       <c r="D32" s="177" t="s">
         <v>595</v>
       </c>
@@ -5510,7 +5516,7 @@
       <c r="B33" s="199" t="s">
         <v>409</v>
       </c>
-      <c r="C33" s="274"/>
+      <c r="C33" s="282"/>
       <c r="D33" s="177" t="s">
         <v>595</v>
       </c>
@@ -5522,7 +5528,7 @@
       <c r="B34" s="199" t="s">
         <v>410</v>
       </c>
-      <c r="C34" s="274"/>
+      <c r="C34" s="282"/>
       <c r="D34" s="177" t="s">
         <v>568</v>
       </c>
@@ -5534,7 +5540,7 @@
       <c r="B35" s="199" t="s">
         <v>411</v>
       </c>
-      <c r="C35" s="274"/>
+      <c r="C35" s="282"/>
       <c r="D35" s="177" t="s">
         <v>569</v>
       </c>
@@ -5546,7 +5552,7 @@
       <c r="B36" s="199" t="s">
         <v>412</v>
       </c>
-      <c r="C36" s="274"/>
+      <c r="C36" s="282"/>
       <c r="D36" s="177" t="s">
         <v>646</v>
       </c>
@@ -5558,7 +5564,7 @@
       <c r="B37" s="226" t="s">
         <v>487</v>
       </c>
-      <c r="C37" s="273"/>
+      <c r="C37" s="281"/>
       <c r="D37" s="177" t="s">
         <v>647</v>
       </c>
@@ -5570,7 +5576,7 @@
       <c r="B38" s="227" t="s">
         <v>413</v>
       </c>
-      <c r="C38" s="269" t="s">
+      <c r="C38" s="277" t="s">
         <v>640</v>
       </c>
       <c r="D38" s="186" t="s">
@@ -5584,7 +5590,7 @@
       <c r="B39" s="228" t="s">
         <v>414</v>
       </c>
-      <c r="C39" s="271"/>
+      <c r="C39" s="278"/>
       <c r="D39" s="177" t="s">
         <v>554</v>
       </c>
@@ -5596,7 +5602,7 @@
       <c r="B40" s="228" t="s">
         <v>415</v>
       </c>
-      <c r="C40" s="271"/>
+      <c r="C40" s="278"/>
       <c r="D40" s="177" t="s">
         <v>557</v>
       </c>
@@ -5608,7 +5614,7 @@
       <c r="B41" s="229" t="s">
         <v>416</v>
       </c>
-      <c r="C41" s="270"/>
+      <c r="C41" s="279"/>
       <c r="D41" s="182" t="s">
         <v>558</v>
       </c>
@@ -5620,7 +5626,7 @@
       <c r="B42" s="232" t="s">
         <v>461</v>
       </c>
-      <c r="C42" s="269" t="s">
+      <c r="C42" s="277" t="s">
         <v>648</v>
       </c>
       <c r="D42" s="186" t="s">
@@ -5634,7 +5640,7 @@
       <c r="B43" s="220" t="s">
         <v>462</v>
       </c>
-      <c r="C43" s="271"/>
+      <c r="C43" s="278"/>
       <c r="D43" s="177" t="s">
         <v>650</v>
       </c>
@@ -5646,7 +5652,7 @@
       <c r="B44" s="220" t="s">
         <v>417</v>
       </c>
-      <c r="C44" s="271"/>
+      <c r="C44" s="278"/>
       <c r="D44" s="177" t="s">
         <v>651</v>
       </c>
@@ -5658,7 +5664,7 @@
       <c r="B45" s="220" t="s">
         <v>418</v>
       </c>
-      <c r="C45" s="271"/>
+      <c r="C45" s="278"/>
       <c r="D45" s="177" t="s">
         <v>11</v>
       </c>
@@ -5670,7 +5676,7 @@
       <c r="B46" s="220" t="s">
         <v>419</v>
       </c>
-      <c r="C46" s="271"/>
+      <c r="C46" s="278"/>
       <c r="D46" s="177" t="s">
         <v>11</v>
       </c>
@@ -5682,7 +5688,7 @@
       <c r="B47" s="220" t="s">
         <v>420</v>
       </c>
-      <c r="C47" s="271"/>
+      <c r="C47" s="278"/>
       <c r="D47" s="177" t="s">
         <v>11</v>
       </c>
@@ -5694,7 +5700,7 @@
       <c r="B48" s="220" t="s">
         <v>452</v>
       </c>
-      <c r="C48" s="271"/>
+      <c r="C48" s="278"/>
       <c r="D48" s="177" t="s">
         <v>609</v>
       </c>
@@ -5706,7 +5712,7 @@
       <c r="B49" s="220" t="s">
         <v>453</v>
       </c>
-      <c r="C49" s="271"/>
+      <c r="C49" s="278"/>
       <c r="D49" s="177" t="s">
         <v>610</v>
       </c>
@@ -5718,7 +5724,7 @@
       <c r="B50" s="220" t="s">
         <v>485</v>
       </c>
-      <c r="C50" s="271"/>
+      <c r="C50" s="278"/>
       <c r="D50" s="177" t="s">
         <v>633</v>
       </c>
@@ -5730,7 +5736,7 @@
       <c r="B51" s="220" t="s">
         <v>486</v>
       </c>
-      <c r="C51" s="271"/>
+      <c r="C51" s="278"/>
       <c r="D51" s="177" t="s">
         <v>634</v>
       </c>
@@ -5742,7 +5748,7 @@
       <c r="B52" s="220" t="s">
         <v>460</v>
       </c>
-      <c r="C52" s="271"/>
+      <c r="C52" s="278"/>
       <c r="D52" s="177" t="s">
         <v>611</v>
       </c>
@@ -5754,7 +5760,7 @@
       <c r="B53" s="220" t="s">
         <v>456</v>
       </c>
-      <c r="C53" s="271"/>
+      <c r="C53" s="278"/>
       <c r="D53" s="177" t="s">
         <v>11</v>
       </c>
@@ -5766,7 +5772,7 @@
       <c r="B54" s="220" t="s">
         <v>457</v>
       </c>
-      <c r="C54" s="271"/>
+      <c r="C54" s="278"/>
       <c r="D54" s="177" t="s">
         <v>11</v>
       </c>
@@ -5778,7 +5784,7 @@
       <c r="B55" s="220" t="s">
         <v>459</v>
       </c>
-      <c r="C55" s="271"/>
+      <c r="C55" s="278"/>
       <c r="D55" s="177" t="s">
         <v>11</v>
       </c>
@@ -5790,7 +5796,7 @@
       <c r="B56" s="220" t="s">
         <v>458</v>
       </c>
-      <c r="C56" s="271"/>
+      <c r="C56" s="278"/>
       <c r="D56" s="177" t="s">
         <v>11</v>
       </c>
@@ -5802,7 +5808,7 @@
       <c r="B57" s="220" t="s">
         <v>421</v>
       </c>
-      <c r="C57" s="271"/>
+      <c r="C57" s="278"/>
       <c r="D57" s="177" t="s">
         <v>612</v>
       </c>
@@ -5814,7 +5820,7 @@
       <c r="B58" s="220" t="s">
         <v>422</v>
       </c>
-      <c r="C58" s="271"/>
+      <c r="C58" s="278"/>
       <c r="D58" s="177" t="s">
         <v>613</v>
       </c>
@@ -5826,7 +5832,7 @@
       <c r="B59" s="220" t="s">
         <v>423</v>
       </c>
-      <c r="C59" s="271"/>
+      <c r="C59" s="278"/>
       <c r="D59" s="177" t="s">
         <v>614</v>
       </c>
@@ -5838,7 +5844,7 @@
       <c r="B60" s="235" t="s">
         <v>424</v>
       </c>
-      <c r="C60" s="270"/>
+      <c r="C60" s="279"/>
       <c r="D60" s="182" t="s">
         <v>615</v>
       </c>
@@ -6009,16 +6015,16 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="48"/>
-      <c r="B1" s="258" t="s">
+      <c r="B1" s="262" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="259"/>
-      <c r="D1" s="260"/>
-      <c r="E1" s="258" t="s">
+      <c r="C1" s="263"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="262" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="259"/>
-      <c r="G1" s="259"/>
+      <c r="F1" s="263"/>
+      <c r="G1" s="263"/>
       <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
@@ -7060,94 +7066,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.4">
-      <c r="A1" s="278" t="s">
+      <c r="A1" s="265" t="s">
         <v>678</v>
       </c>
-      <c r="B1" s="278"/>
-      <c r="C1" s="278"/>
-      <c r="D1" s="278"/>
-      <c r="E1" s="280" t="s">
+      <c r="B1" s="265"/>
+      <c r="C1" s="265"/>
+      <c r="D1" s="265"/>
+      <c r="E1" s="266" t="s">
         <v>679</v>
       </c>
-      <c r="F1" s="281"/>
-      <c r="G1" s="281"/>
-      <c r="H1" s="281"/>
-      <c r="I1" s="281"/>
-      <c r="J1" s="281"/>
-      <c r="K1" s="281"/>
-      <c r="L1" s="282"/>
-      <c r="M1" s="262" t="s">
+      <c r="F1" s="267"/>
+      <c r="G1" s="267"/>
+      <c r="H1" s="267"/>
+      <c r="I1" s="267"/>
+      <c r="J1" s="267"/>
+      <c r="K1" s="267"/>
+      <c r="L1" s="268"/>
+      <c r="M1" s="269" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="262"/>
-      <c r="O1" s="262"/>
-      <c r="P1" s="262"/>
-      <c r="Q1" s="278" t="s">
+      <c r="N1" s="269"/>
+      <c r="O1" s="269"/>
+      <c r="P1" s="269"/>
+      <c r="Q1" s="265" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="278"/>
-      <c r="S1" s="278"/>
-      <c r="T1" s="278"/>
-      <c r="U1" s="262" t="s">
+      <c r="R1" s="265"/>
+      <c r="S1" s="265"/>
+      <c r="T1" s="265"/>
+      <c r="U1" s="269" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="262"/>
-      <c r="W1" s="262"/>
-      <c r="X1" s="262"/>
-      <c r="Y1" s="278" t="s">
+      <c r="V1" s="269"/>
+      <c r="W1" s="269"/>
+      <c r="X1" s="269"/>
+      <c r="Y1" s="265" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" s="278"/>
-      <c r="AA1" s="278"/>
-      <c r="AB1" s="278"/>
-      <c r="AC1" s="262" t="s">
+      <c r="Z1" s="265"/>
+      <c r="AA1" s="265"/>
+      <c r="AB1" s="265"/>
+      <c r="AC1" s="269" t="s">
         <v>83</v>
       </c>
-      <c r="AD1" s="262"/>
-      <c r="AE1" s="262"/>
-      <c r="AF1" s="262"/>
-      <c r="AG1" s="278" t="s">
+      <c r="AD1" s="269"/>
+      <c r="AE1" s="269"/>
+      <c r="AF1" s="269"/>
+      <c r="AG1" s="265" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="278"/>
-      <c r="AI1" s="278"/>
-      <c r="AJ1" s="278"/>
-      <c r="AK1" s="262" t="s">
+      <c r="AH1" s="265"/>
+      <c r="AI1" s="265"/>
+      <c r="AJ1" s="265"/>
+      <c r="AK1" s="269" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="262"/>
-      <c r="AM1" s="262"/>
-      <c r="AN1" s="262"/>
-      <c r="AO1" s="278" t="s">
+      <c r="AL1" s="269"/>
+      <c r="AM1" s="269"/>
+      <c r="AN1" s="269"/>
+      <c r="AO1" s="265" t="s">
         <v>86</v>
       </c>
-      <c r="AP1" s="278"/>
-      <c r="AQ1" s="278"/>
-      <c r="AR1" s="278"/>
-      <c r="AS1" s="262" t="s">
+      <c r="AP1" s="265"/>
+      <c r="AQ1" s="265"/>
+      <c r="AR1" s="265"/>
+      <c r="AS1" s="269" t="s">
         <v>87</v>
       </c>
-      <c r="AT1" s="262"/>
-      <c r="AU1" s="262"/>
-      <c r="AV1" s="262"/>
-      <c r="AW1" s="278" t="s">
+      <c r="AT1" s="269"/>
+      <c r="AU1" s="269"/>
+      <c r="AV1" s="269"/>
+      <c r="AW1" s="265" t="s">
         <v>88</v>
       </c>
-      <c r="AX1" s="278"/>
-      <c r="AY1" s="278"/>
-      <c r="AZ1" s="278"/>
-      <c r="BA1" s="262" t="s">
+      <c r="AX1" s="265"/>
+      <c r="AY1" s="265"/>
+      <c r="AZ1" s="265"/>
+      <c r="BA1" s="269" t="s">
         <v>89</v>
       </c>
-      <c r="BB1" s="262"/>
-      <c r="BC1" s="262"/>
-      <c r="BD1" s="262"/>
-      <c r="BE1" s="278" t="s">
+      <c r="BB1" s="269"/>
+      <c r="BC1" s="269"/>
+      <c r="BD1" s="269"/>
+      <c r="BE1" s="265" t="s">
         <v>90</v>
       </c>
-      <c r="BF1" s="278"/>
-      <c r="BG1" s="278"/>
-      <c r="BH1" s="278"/>
+      <c r="BF1" s="265"/>
+      <c r="BG1" s="265"/>
+      <c r="BH1" s="265"/>
     </row>
     <row r="2" spans="1:60" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -9059,7 +9065,7 @@
       <c r="BE20" s="96"/>
       <c r="BF20" s="96"/>
       <c r="BG20" s="96"/>
-      <c r="BH20" s="279"/>
+      <c r="BH20" s="259"/>
     </row>
     <row r="21" spans="1:60" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
@@ -10377,7 +10383,7 @@
       <c r="BE31" s="96"/>
       <c r="BF31" s="96"/>
       <c r="BG31" s="96"/>
-      <c r="BH31" s="279"/>
+      <c r="BH31" s="259"/>
     </row>
     <row r="32" spans="1:60" x14ac:dyDescent="0.4">
       <c r="A32" s="1">
@@ -10830,7 +10836,7 @@
       <c r="BE35" s="96"/>
       <c r="BF35" s="96"/>
       <c r="BG35" s="96"/>
-      <c r="BH35" s="279"/>
+      <c r="BH35" s="259"/>
     </row>
     <row r="36" spans="1:92" x14ac:dyDescent="0.4">
       <c r="A36" s="1">
@@ -11021,7 +11027,7 @@
       <c r="BE37" s="96"/>
       <c r="BF37" s="96"/>
       <c r="BG37" s="96"/>
-      <c r="BH37" s="279"/>
+      <c r="BH37" s="259"/>
     </row>
     <row r="38" spans="1:92" x14ac:dyDescent="0.4">
       <c r="A38" s="1">
@@ -11210,7 +11216,7 @@
       <c r="BE39" s="96"/>
       <c r="BF39" s="96"/>
       <c r="BG39" s="96"/>
-      <c r="BH39" s="279"/>
+      <c r="BH39" s="259"/>
     </row>
     <row r="40" spans="1:92" x14ac:dyDescent="0.4">
       <c r="A40" s="1">
@@ -11548,7 +11554,7 @@
       <c r="BG41" s="96">
         <v>0</v>
       </c>
-      <c r="BH41" s="279"/>
+      <c r="BH41" s="259"/>
     </row>
     <row r="42" spans="1:92" x14ac:dyDescent="0.4">
       <c r="A42" s="1">
@@ -11875,7 +11881,7 @@
       <c r="BE43" s="96"/>
       <c r="BF43" s="96"/>
       <c r="BG43" s="96"/>
-      <c r="BH43" s="279"/>
+      <c r="BH43" s="259"/>
     </row>
     <row r="44" spans="1:92" x14ac:dyDescent="0.4">
       <c r="A44" s="1">
@@ -12092,7 +12098,7 @@
       <c r="BE45" s="96"/>
       <c r="BF45" s="96"/>
       <c r="BG45" s="96"/>
-      <c r="BH45" s="279"/>
+      <c r="BH45" s="259"/>
     </row>
     <row r="46" spans="1:92" x14ac:dyDescent="0.4">
       <c r="A46" s="1">
@@ -12284,7 +12290,7 @@
       <c r="BE47" s="96"/>
       <c r="BF47" s="96"/>
       <c r="BG47" s="96"/>
-      <c r="BH47" s="279"/>
+      <c r="BH47" s="259"/>
     </row>
     <row r="48" spans="1:92" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="1">
@@ -12380,7 +12386,7 @@
       <c r="BE48" s="96"/>
       <c r="BF48" s="96"/>
       <c r="BG48" s="96"/>
-      <c r="BH48" s="279"/>
+      <c r="BH48" s="259"/>
     </row>
     <row r="49" spans="1:61" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A49" s="1">
@@ -12476,7 +12482,7 @@
       <c r="BE49" s="96"/>
       <c r="BF49" s="96"/>
       <c r="BG49" s="96"/>
-      <c r="BH49" s="279"/>
+      <c r="BH49" s="259"/>
     </row>
     <row r="50" spans="1:61" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="1">
@@ -12573,7 +12579,7 @@
       <c r="BE50" s="96"/>
       <c r="BF50" s="96"/>
       <c r="BG50" s="96"/>
-      <c r="BH50" s="279"/>
+      <c r="BH50" s="259"/>
     </row>
     <row r="51" spans="1:61" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A51" s="1">
@@ -12670,7 +12676,7 @@
       <c r="BE51" s="96"/>
       <c r="BF51" s="96"/>
       <c r="BG51" s="96"/>
-      <c r="BH51" s="279"/>
+      <c r="BH51" s="259"/>
     </row>
     <row r="52" spans="1:61" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A52" s="1">
@@ -12767,7 +12773,7 @@
       <c r="BE52" s="96"/>
       <c r="BF52" s="96"/>
       <c r="BG52" s="96"/>
-      <c r="BH52" s="279"/>
+      <c r="BH52" s="259"/>
     </row>
     <row r="53" spans="1:61" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="1">
@@ -12864,7 +12870,7 @@
       <c r="BE53" s="96"/>
       <c r="BF53" s="96"/>
       <c r="BG53" s="96"/>
-      <c r="BH53" s="279"/>
+      <c r="BH53" s="259"/>
     </row>
     <row r="54" spans="1:61" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A54" s="1">
@@ -12961,7 +12967,7 @@
       <c r="BE54" s="96"/>
       <c r="BF54" s="96"/>
       <c r="BG54" s="96"/>
-      <c r="BH54" s="279"/>
+      <c r="BH54" s="259"/>
     </row>
     <row r="55" spans="1:61" x14ac:dyDescent="0.4">
       <c r="A55" s="1">
@@ -13535,7 +13541,7 @@
       <c r="BE59" s="96"/>
       <c r="BF59" s="96"/>
       <c r="BG59" s="96"/>
-      <c r="BH59" s="279"/>
+      <c r="BH59" s="259"/>
       <c r="BI59" s="94"/>
     </row>
     <row r="60" spans="1:61" x14ac:dyDescent="0.4">
@@ -13661,7 +13667,7 @@
       <c r="BE60" s="96"/>
       <c r="BF60" s="96"/>
       <c r="BG60" s="96"/>
-      <c r="BH60" s="279"/>
+      <c r="BH60" s="259"/>
       <c r="BI60" s="94"/>
     </row>
     <row r="61" spans="1:61" x14ac:dyDescent="0.4">
@@ -14719,7 +14725,7 @@
       <c r="BE68" s="96"/>
       <c r="BF68" s="96"/>
       <c r="BG68" s="96"/>
-      <c r="BH68" s="279"/>
+      <c r="BH68" s="259"/>
     </row>
     <row r="69" spans="1:92" x14ac:dyDescent="0.4">
       <c r="A69" s="1">
@@ -16544,7 +16550,7 @@
       <c r="BE85" s="96"/>
       <c r="BF85" s="96"/>
       <c r="BG85" s="96"/>
-      <c r="BH85" s="279"/>
+      <c r="BH85" s="259"/>
     </row>
     <row r="86" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A86" s="1">
@@ -16653,7 +16659,7 @@
       <c r="BE86" s="96"/>
       <c r="BF86" s="96"/>
       <c r="BG86" s="96"/>
-      <c r="BH86" s="279"/>
+      <c r="BH86" s="259"/>
     </row>
     <row r="87" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A87" s="1">
@@ -16762,7 +16768,7 @@
       <c r="BE87" s="96"/>
       <c r="BF87" s="96"/>
       <c r="BG87" s="96"/>
-      <c r="BH87" s="279"/>
+      <c r="BH87" s="259"/>
     </row>
     <row r="88" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A88" s="1">
@@ -16873,7 +16879,7 @@
       <c r="BE88" s="96"/>
       <c r="BF88" s="96"/>
       <c r="BG88" s="96"/>
-      <c r="BH88" s="279"/>
+      <c r="BH88" s="259"/>
     </row>
     <row r="89" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A89" s="1">
@@ -16984,7 +16990,7 @@
       <c r="BE89" s="96"/>
       <c r="BF89" s="96"/>
       <c r="BG89" s="96"/>
-      <c r="BH89" s="279"/>
+      <c r="BH89" s="259"/>
     </row>
     <row r="90" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A90" s="1">
@@ -17126,7 +17132,7 @@
       <c r="BD90" s="104"/>
       <c r="BF90" s="96"/>
       <c r="BG90" s="96"/>
-      <c r="BH90" s="279"/>
+      <c r="BH90" s="259"/>
     </row>
     <row r="91" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A91" s="1">
@@ -17240,7 +17246,7 @@
       <c r="BD91" s="104"/>
       <c r="BF91" s="96"/>
       <c r="BG91" s="96"/>
-      <c r="BH91" s="279"/>
+      <c r="BH91" s="259"/>
     </row>
     <row r="92" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A92" s="1">
@@ -17339,7 +17345,7 @@
       <c r="BD92" s="104"/>
       <c r="BF92" s="96"/>
       <c r="BG92" s="96"/>
-      <c r="BH92" s="279"/>
+      <c r="BH92" s="259"/>
     </row>
     <row r="93" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="1">
@@ -17460,7 +17466,7 @@
       <c r="BD93" s="104"/>
       <c r="BF93" s="96"/>
       <c r="BG93" s="96"/>
-      <c r="BH93" s="279"/>
+      <c r="BH93" s="259"/>
     </row>
     <row r="94" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A94" s="1">
@@ -17571,7 +17577,7 @@
       <c r="BD94" s="104"/>
       <c r="BF94" s="96"/>
       <c r="BG94" s="96"/>
-      <c r="BH94" s="279"/>
+      <c r="BH94" s="259"/>
     </row>
     <row r="95" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="1">
@@ -17701,7 +17707,7 @@
       <c r="BD95" s="104"/>
       <c r="BF95" s="96"/>
       <c r="BG95" s="96"/>
-      <c r="BH95" s="279"/>
+      <c r="BH95" s="259"/>
     </row>
     <row r="96" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A96" s="1">
@@ -17809,7 +17815,7 @@
       <c r="BD96" s="104"/>
       <c r="BF96" s="96"/>
       <c r="BG96" s="96"/>
-      <c r="BH96" s="279"/>
+      <c r="BH96" s="259"/>
     </row>
     <row r="97" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" s="1">
@@ -17921,7 +17927,7 @@
       <c r="BD97" s="104"/>
       <c r="BF97" s="96"/>
       <c r="BG97" s="96"/>
-      <c r="BH97" s="279"/>
+      <c r="BH97" s="259"/>
     </row>
     <row r="98" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A98" s="1">
@@ -18032,7 +18038,7 @@
       <c r="BD98" s="104"/>
       <c r="BF98" s="96"/>
       <c r="BG98" s="96"/>
-      <c r="BH98" s="279"/>
+      <c r="BH98" s="259"/>
     </row>
     <row r="99" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A99" s="1">
@@ -18140,7 +18146,7 @@
       <c r="BD99" s="104"/>
       <c r="BF99" s="96"/>
       <c r="BG99" s="96"/>
-      <c r="BH99" s="279"/>
+      <c r="BH99" s="259"/>
     </row>
     <row r="100" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="1">
@@ -18254,7 +18260,7 @@
       <c r="BD100" s="104"/>
       <c r="BF100" s="96"/>
       <c r="BG100" s="96"/>
-      <c r="BH100" s="279"/>
+      <c r="BH100" s="259"/>
     </row>
     <row r="101" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="1">
@@ -18366,7 +18372,7 @@
       <c r="BD101" s="104"/>
       <c r="BF101" s="96"/>
       <c r="BG101" s="96"/>
-      <c r="BH101" s="279"/>
+      <c r="BH101" s="259"/>
     </row>
     <row r="102" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A102" s="1">
@@ -18491,7 +18497,7 @@
       <c r="BD102" s="104"/>
       <c r="BF102" s="96"/>
       <c r="BG102" s="96"/>
-      <c r="BH102" s="279"/>
+      <c r="BH102" s="259"/>
     </row>
     <row r="103" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A103" s="1">
@@ -18616,7 +18622,7 @@
       <c r="BD103" s="104"/>
       <c r="BF103" s="96"/>
       <c r="BG103" s="96"/>
-      <c r="BH103" s="279"/>
+      <c r="BH103" s="259"/>
     </row>
     <row r="104" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="1">
@@ -18775,7 +18781,7 @@
       </c>
       <c r="BF104" s="96"/>
       <c r="BG104" s="96"/>
-      <c r="BH104" s="279"/>
+      <c r="BH104" s="259"/>
     </row>
     <row r="105" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="1">
@@ -18934,7 +18940,7 @@
       </c>
       <c r="BF105" s="96"/>
       <c r="BG105" s="96"/>
-      <c r="BH105" s="279"/>
+      <c r="BH105" s="259"/>
     </row>
     <row r="106" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="1">
@@ -19035,7 +19041,7 @@
       <c r="BD106" s="104"/>
       <c r="BF106" s="96"/>
       <c r="BG106" s="96"/>
-      <c r="BH106" s="279"/>
+      <c r="BH106" s="259"/>
     </row>
     <row r="107" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A107" s="1">
@@ -19130,7 +19136,7 @@
       <c r="BD107" s="104"/>
       <c r="BF107" s="96"/>
       <c r="BG107" s="96"/>
-      <c r="BH107" s="279"/>
+      <c r="BH107" s="259"/>
     </row>
     <row r="108" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="1">
@@ -19225,7 +19231,7 @@
       <c r="BD108" s="104"/>
       <c r="BF108" s="96"/>
       <c r="BG108" s="96"/>
-      <c r="BH108" s="279"/>
+      <c r="BH108" s="259"/>
     </row>
     <row r="109" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="1">
@@ -19320,7 +19326,7 @@
       <c r="BD109" s="104"/>
       <c r="BF109" s="96"/>
       <c r="BG109" s="96"/>
-      <c r="BH109" s="279"/>
+      <c r="BH109" s="259"/>
     </row>
     <row r="110" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="1">
@@ -19416,7 +19422,7 @@
       <c r="BD110" s="104"/>
       <c r="BF110" s="96"/>
       <c r="BG110" s="96"/>
-      <c r="BH110" s="279"/>
+      <c r="BH110" s="259"/>
     </row>
     <row r="111" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A111" s="1">
@@ -19511,7 +19517,7 @@
       <c r="BD111" s="104"/>
       <c r="BF111" s="96"/>
       <c r="BG111" s="96"/>
-      <c r="BH111" s="279"/>
+      <c r="BH111" s="259"/>
     </row>
     <row r="112" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A112" s="1">
@@ -19606,7 +19612,7 @@
       <c r="BD112" s="104"/>
       <c r="BF112" s="96"/>
       <c r="BG112" s="96"/>
-      <c r="BH112" s="279"/>
+      <c r="BH112" s="259"/>
     </row>
     <row r="113" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A113" s="1">
@@ -19701,7 +19707,7 @@
       <c r="BD113" s="104"/>
       <c r="BF113" s="96"/>
       <c r="BG113" s="96"/>
-      <c r="BH113" s="279"/>
+      <c r="BH113" s="259"/>
     </row>
     <row r="114" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A114" s="1">
@@ -19796,7 +19802,7 @@
       <c r="BD114" s="104"/>
       <c r="BF114" s="96"/>
       <c r="BG114" s="96"/>
-      <c r="BH114" s="279"/>
+      <c r="BH114" s="259"/>
     </row>
     <row r="115" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" s="1">
@@ -19891,7 +19897,7 @@
       <c r="BD115" s="104"/>
       <c r="BF115" s="96"/>
       <c r="BG115" s="96"/>
-      <c r="BH115" s="279"/>
+      <c r="BH115" s="259"/>
     </row>
     <row r="116" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A116" s="1">
@@ -19986,7 +19992,7 @@
       <c r="BD116" s="104"/>
       <c r="BF116" s="96"/>
       <c r="BG116" s="96"/>
-      <c r="BH116" s="279"/>
+      <c r="BH116" s="259"/>
     </row>
     <row r="117" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A117" s="1">
@@ -20093,7 +20099,7 @@
       <c r="BD117" s="104"/>
       <c r="BF117" s="96"/>
       <c r="BG117" s="96"/>
-      <c r="BH117" s="279"/>
+      <c r="BH117" s="259"/>
     </row>
     <row r="118" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A118" s="1">
@@ -20200,7 +20206,7 @@
       <c r="BD118" s="104"/>
       <c r="BF118" s="96"/>
       <c r="BG118" s="96"/>
-      <c r="BH118" s="279"/>
+      <c r="BH118" s="259"/>
     </row>
     <row r="119" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A119" s="1">
@@ -20297,7 +20303,7 @@
       <c r="BD119" s="104"/>
       <c r="BF119" s="96"/>
       <c r="BG119" s="96"/>
-      <c r="BH119" s="279"/>
+      <c r="BH119" s="259"/>
     </row>
     <row r="120" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A120" s="1">
@@ -20393,7 +20399,7 @@
       <c r="BD120" s="104"/>
       <c r="BF120" s="96"/>
       <c r="BG120" s="96"/>
-      <c r="BH120" s="279"/>
+      <c r="BH120" s="259"/>
     </row>
     <row r="121" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A121" s="1">
@@ -20489,7 +20495,7 @@
       <c r="BD121" s="104"/>
       <c r="BF121" s="96"/>
       <c r="BG121" s="96"/>
-      <c r="BH121" s="279"/>
+      <c r="BH121" s="259"/>
     </row>
     <row r="122" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A122" s="1">
@@ -20594,7 +20600,7 @@
       <c r="BD122" s="104"/>
       <c r="BF122" s="96"/>
       <c r="BG122" s="96"/>
-      <c r="BH122" s="279"/>
+      <c r="BH122" s="259"/>
     </row>
     <row r="123" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A123" s="1">
@@ -20709,7 +20715,7 @@
       <c r="BD123" s="104"/>
       <c r="BF123" s="96"/>
       <c r="BG123" s="96"/>
-      <c r="BH123" s="279"/>
+      <c r="BH123" s="259"/>
     </row>
     <row r="124" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A124" s="1">
@@ -20801,7 +20807,7 @@
       <c r="BD124" s="104"/>
       <c r="BF124" s="96"/>
       <c r="BG124" s="96"/>
-      <c r="BH124" s="279"/>
+      <c r="BH124" s="259"/>
     </row>
     <row r="125" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A125" s="1">
@@ -20893,7 +20899,7 @@
       <c r="BD125" s="104"/>
       <c r="BF125" s="96"/>
       <c r="BG125" s="96"/>
-      <c r="BH125" s="279"/>
+      <c r="BH125" s="259"/>
     </row>
     <row r="126" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A126" s="1">
@@ -21039,7 +21045,7 @@
       <c r="BD126" s="104"/>
       <c r="BF126" s="96"/>
       <c r="BG126" s="96"/>
-      <c r="BH126" s="279"/>
+      <c r="BH126" s="259"/>
     </row>
     <row r="127" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A127" s="1">
@@ -21185,7 +21191,7 @@
       <c r="BD127" s="104"/>
       <c r="BF127" s="96"/>
       <c r="BG127" s="96"/>
-      <c r="BH127" s="279"/>
+      <c r="BH127" s="259"/>
     </row>
     <row r="128" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A128" s="1">
@@ -21305,7 +21311,7 @@
       <c r="BD128" s="104"/>
       <c r="BF128" s="96"/>
       <c r="BG128" s="96"/>
-      <c r="BH128" s="279"/>
+      <c r="BH128" s="259"/>
     </row>
     <row r="129" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A129" s="1">
@@ -21425,7 +21431,7 @@
       <c r="BD129" s="104"/>
       <c r="BF129" s="96"/>
       <c r="BG129" s="96"/>
-      <c r="BH129" s="279"/>
+      <c r="BH129" s="259"/>
     </row>
     <row r="130" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A130" s="1">
@@ -21532,7 +21538,7 @@
       <c r="BD130" s="104"/>
       <c r="BF130" s="96"/>
       <c r="BG130" s="96"/>
-      <c r="BH130" s="279"/>
+      <c r="BH130" s="259"/>
     </row>
     <row r="131" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A131" s="1">
@@ -21640,7 +21646,7 @@
       <c r="BD131" s="104"/>
       <c r="BF131" s="96"/>
       <c r="BG131" s="96"/>
-      <c r="BH131" s="279"/>
+      <c r="BH131" s="259"/>
     </row>
     <row r="132" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A132" s="1">
@@ -21728,7 +21734,7 @@
       <c r="BD132" s="104"/>
       <c r="BF132" s="96"/>
       <c r="BG132" s="96"/>
-      <c r="BH132" s="279"/>
+      <c r="BH132" s="259"/>
     </row>
     <row r="133" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A133" s="1">
@@ -21817,7 +21823,7 @@
       <c r="BD133" s="104"/>
       <c r="BF133" s="96"/>
       <c r="BG133" s="96"/>
-      <c r="BH133" s="279"/>
+      <c r="BH133" s="259"/>
     </row>
     <row r="134" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A134" s="1">
@@ -21907,7 +21913,7 @@
       <c r="BD134" s="104"/>
       <c r="BF134" s="96"/>
       <c r="BG134" s="96"/>
-      <c r="BH134" s="279"/>
+      <c r="BH134" s="259"/>
     </row>
     <row r="135" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A135" s="1">
@@ -21998,7 +22004,7 @@
       <c r="BD135" s="104"/>
       <c r="BF135" s="96"/>
       <c r="BG135" s="96"/>
-      <c r="BH135" s="279"/>
+      <c r="BH135" s="259"/>
     </row>
     <row r="136" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A136" s="1">
@@ -22086,7 +22092,7 @@
       <c r="BD136" s="104"/>
       <c r="BF136" s="96"/>
       <c r="BG136" s="96"/>
-      <c r="BH136" s="279"/>
+      <c r="BH136" s="259"/>
     </row>
     <row r="137" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A137" s="1">
@@ -22176,7 +22182,7 @@
       <c r="BD137" s="104"/>
       <c r="BF137" s="96"/>
       <c r="BG137" s="96"/>
-      <c r="BH137" s="279"/>
+      <c r="BH137" s="259"/>
     </row>
     <row r="138" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A138" s="1">
@@ -22264,7 +22270,7 @@
       <c r="BD138" s="104"/>
       <c r="BF138" s="96"/>
       <c r="BG138" s="96"/>
-      <c r="BH138" s="279"/>
+      <c r="BH138" s="259"/>
     </row>
     <row r="139" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A139" s="1">
@@ -22354,7 +22360,7 @@
       <c r="BD139" s="104"/>
       <c r="BF139" s="96"/>
       <c r="BG139" s="96"/>
-      <c r="BH139" s="279"/>
+      <c r="BH139" s="259"/>
     </row>
     <row r="140" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A140" s="1">
@@ -22448,7 +22454,7 @@
       <c r="BD140" s="131"/>
       <c r="BF140" s="96"/>
       <c r="BG140" s="96"/>
-      <c r="BH140" s="279"/>
+      <c r="BH140" s="259"/>
     </row>
     <row r="141" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A141" s="1">
@@ -22542,7 +22548,7 @@
       <c r="BD141" s="131"/>
       <c r="BF141" s="96"/>
       <c r="BG141" s="96"/>
-      <c r="BH141" s="279"/>
+      <c r="BH141" s="259"/>
     </row>
     <row r="142" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A142" s="1">
@@ -22635,7 +22641,7 @@
       <c r="BD142" s="131"/>
       <c r="BF142" s="96"/>
       <c r="BG142" s="96"/>
-      <c r="BH142" s="279"/>
+      <c r="BH142" s="259"/>
     </row>
     <row r="143" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A143" s="1">
@@ -22728,7 +22734,7 @@
       <c r="BD143" s="131"/>
       <c r="BF143" s="96"/>
       <c r="BG143" s="96"/>
-      <c r="BH143" s="279"/>
+      <c r="BH143" s="259"/>
     </row>
     <row r="144" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A144" s="1">
@@ -22893,7 +22899,7 @@
       <c r="BG144" s="96">
         <v>1</v>
       </c>
-      <c r="BH144" s="279"/>
+      <c r="BH144" s="259"/>
     </row>
     <row r="145" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A145" s="1">
@@ -23058,7 +23064,7 @@
       <c r="BG145" s="96">
         <v>1</v>
       </c>
-      <c r="BH145" s="279"/>
+      <c r="BH145" s="259"/>
     </row>
     <row r="146" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A146" s="1">
@@ -23152,7 +23158,7 @@
       <c r="BD146" s="131"/>
       <c r="BF146" s="96"/>
       <c r="BG146" s="96"/>
-      <c r="BH146" s="279"/>
+      <c r="BH146" s="259"/>
     </row>
     <row r="147" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A147" s="1">
@@ -23246,7 +23252,7 @@
       <c r="BD147" s="131"/>
       <c r="BF147" s="96"/>
       <c r="BG147" s="96"/>
-      <c r="BH147" s="279"/>
+      <c r="BH147" s="259"/>
     </row>
     <row r="148" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A148" s="1">
@@ -23340,7 +23346,7 @@
       <c r="BD148" s="131"/>
       <c r="BF148" s="96"/>
       <c r="BG148" s="96"/>
-      <c r="BH148" s="279"/>
+      <c r="BH148" s="259"/>
     </row>
     <row r="149" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A149" s="1">
@@ -23434,7 +23440,7 @@
       <c r="BD149" s="131"/>
       <c r="BF149" s="96"/>
       <c r="BG149" s="96"/>
-      <c r="BH149" s="279"/>
+      <c r="BH149" s="259"/>
     </row>
     <row r="150" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A150" s="1">
@@ -23526,7 +23532,7 @@
       <c r="BD150" s="131"/>
       <c r="BF150" s="96"/>
       <c r="BG150" s="96"/>
-      <c r="BH150" s="279"/>
+      <c r="BH150" s="259"/>
     </row>
     <row r="151" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A151" s="1">
@@ -23618,7 +23624,7 @@
       <c r="BD151" s="131"/>
       <c r="BF151" s="96"/>
       <c r="BG151" s="96"/>
-      <c r="BH151" s="279"/>
+      <c r="BH151" s="259"/>
     </row>
     <row r="152" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A152" s="1">
@@ -23743,7 +23749,7 @@
       <c r="BD152" s="131"/>
       <c r="BF152" s="96"/>
       <c r="BG152" s="96"/>
-      <c r="BH152" s="279"/>
+      <c r="BH152" s="259"/>
     </row>
     <row r="153" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A153" s="1">
@@ -23867,7 +23873,7 @@
       <c r="BD153" s="131"/>
       <c r="BF153" s="96"/>
       <c r="BG153" s="96"/>
-      <c r="BH153" s="279"/>
+      <c r="BH153" s="259"/>
     </row>
     <row r="154" spans="1:60" s="94" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A154" s="1">
@@ -23955,7 +23961,7 @@
       <c r="BC154" s="131"/>
       <c r="BD154" s="131"/>
       <c r="BG154" s="96"/>
-      <c r="BH154" s="279"/>
+      <c r="BH154" s="259"/>
     </row>
     <row r="155" spans="1:60" x14ac:dyDescent="0.4">
       <c r="L155" s="6"/>
@@ -24382,94 +24388,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:92" x14ac:dyDescent="0.4">
-      <c r="A1" s="278" t="s">
+      <c r="A1" s="265" t="s">
         <v>678</v>
       </c>
-      <c r="B1" s="278"/>
-      <c r="C1" s="278"/>
-      <c r="D1" s="278"/>
-      <c r="E1" s="280" t="s">
+      <c r="B1" s="265"/>
+      <c r="C1" s="265"/>
+      <c r="D1" s="265"/>
+      <c r="E1" s="266" t="s">
         <v>679</v>
       </c>
-      <c r="F1" s="281"/>
-      <c r="G1" s="281"/>
-      <c r="H1" s="281"/>
-      <c r="I1" s="281"/>
-      <c r="J1" s="281"/>
-      <c r="K1" s="281"/>
-      <c r="L1" s="282"/>
-      <c r="M1" s="265" t="s">
+      <c r="F1" s="267"/>
+      <c r="G1" s="267"/>
+      <c r="H1" s="267"/>
+      <c r="I1" s="267"/>
+      <c r="J1" s="267"/>
+      <c r="K1" s="267"/>
+      <c r="L1" s="268"/>
+      <c r="M1" s="273" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="266"/>
-      <c r="O1" s="266"/>
-      <c r="P1" s="267"/>
-      <c r="Q1" s="280" t="s">
+      <c r="N1" s="274"/>
+      <c r="O1" s="274"/>
+      <c r="P1" s="275"/>
+      <c r="Q1" s="266" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="281"/>
-      <c r="S1" s="281"/>
-      <c r="T1" s="281"/>
-      <c r="U1" s="265" t="s">
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="267"/>
+      <c r="U1" s="273" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="266"/>
-      <c r="W1" s="266"/>
-      <c r="X1" s="267"/>
-      <c r="Y1" s="263" t="s">
+      <c r="V1" s="274"/>
+      <c r="W1" s="274"/>
+      <c r="X1" s="275"/>
+      <c r="Y1" s="270" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" s="261"/>
-      <c r="AA1" s="261"/>
-      <c r="AB1" s="264"/>
-      <c r="AC1" s="265" t="s">
+      <c r="Z1" s="271"/>
+      <c r="AA1" s="271"/>
+      <c r="AB1" s="272"/>
+      <c r="AC1" s="273" t="s">
         <v>83</v>
       </c>
-      <c r="AD1" s="266"/>
-      <c r="AE1" s="266"/>
-      <c r="AF1" s="267"/>
-      <c r="AG1" s="263" t="s">
+      <c r="AD1" s="274"/>
+      <c r="AE1" s="274"/>
+      <c r="AF1" s="275"/>
+      <c r="AG1" s="270" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="261"/>
-      <c r="AI1" s="261"/>
-      <c r="AJ1" s="264"/>
-      <c r="AK1" s="265" t="s">
+      <c r="AH1" s="271"/>
+      <c r="AI1" s="271"/>
+      <c r="AJ1" s="272"/>
+      <c r="AK1" s="273" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="266"/>
-      <c r="AM1" s="266"/>
-      <c r="AN1" s="267"/>
-      <c r="AO1" s="263" t="s">
+      <c r="AL1" s="274"/>
+      <c r="AM1" s="274"/>
+      <c r="AN1" s="275"/>
+      <c r="AO1" s="270" t="s">
         <v>86</v>
       </c>
-      <c r="AP1" s="261"/>
-      <c r="AQ1" s="261"/>
-      <c r="AR1" s="264"/>
-      <c r="AS1" s="265" t="s">
+      <c r="AP1" s="271"/>
+      <c r="AQ1" s="271"/>
+      <c r="AR1" s="272"/>
+      <c r="AS1" s="273" t="s">
         <v>87</v>
       </c>
-      <c r="AT1" s="266"/>
-      <c r="AU1" s="266"/>
-      <c r="AV1" s="267"/>
-      <c r="AW1" s="263" t="s">
+      <c r="AT1" s="274"/>
+      <c r="AU1" s="274"/>
+      <c r="AV1" s="275"/>
+      <c r="AW1" s="270" t="s">
         <v>88</v>
       </c>
-      <c r="AX1" s="261"/>
-      <c r="AY1" s="261"/>
-      <c r="AZ1" s="264"/>
-      <c r="BA1" s="265" t="s">
+      <c r="AX1" s="271"/>
+      <c r="AY1" s="271"/>
+      <c r="AZ1" s="272"/>
+      <c r="BA1" s="273" t="s">
         <v>89</v>
       </c>
-      <c r="BB1" s="266"/>
-      <c r="BC1" s="266"/>
-      <c r="BD1" s="267"/>
-      <c r="BE1" s="263" t="s">
+      <c r="BB1" s="274"/>
+      <c r="BC1" s="274"/>
+      <c r="BD1" s="275"/>
+      <c r="BE1" s="270" t="s">
         <v>90</v>
       </c>
-      <c r="BF1" s="261"/>
-      <c r="BG1" s="261"/>
-      <c r="BH1" s="264"/>
+      <c r="BF1" s="271"/>
+      <c r="BG1" s="271"/>
+      <c r="BH1" s="272"/>
     </row>
     <row r="2" spans="1:92" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -29671,94 +29677,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.4">
-      <c r="A1" s="278" t="s">
+      <c r="A1" s="265" t="s">
         <v>678</v>
       </c>
-      <c r="B1" s="278"/>
-      <c r="C1" s="278"/>
-      <c r="D1" s="278"/>
-      <c r="E1" s="280" t="s">
+      <c r="B1" s="265"/>
+      <c r="C1" s="265"/>
+      <c r="D1" s="265"/>
+      <c r="E1" s="266" t="s">
         <v>679</v>
       </c>
-      <c r="F1" s="281"/>
-      <c r="G1" s="281"/>
-      <c r="H1" s="281"/>
-      <c r="I1" s="281"/>
-      <c r="J1" s="281"/>
-      <c r="K1" s="281"/>
-      <c r="L1" s="282"/>
-      <c r="M1" s="268" t="s">
+      <c r="F1" s="267"/>
+      <c r="G1" s="267"/>
+      <c r="H1" s="267"/>
+      <c r="I1" s="267"/>
+      <c r="J1" s="267"/>
+      <c r="K1" s="267"/>
+      <c r="L1" s="268"/>
+      <c r="M1" s="276" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="268"/>
-      <c r="O1" s="268"/>
-      <c r="P1" s="268"/>
-      <c r="Q1" s="278" t="s">
+      <c r="N1" s="276"/>
+      <c r="O1" s="276"/>
+      <c r="P1" s="276"/>
+      <c r="Q1" s="265" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="278"/>
-      <c r="S1" s="278"/>
-      <c r="T1" s="278"/>
-      <c r="U1" s="268" t="s">
+      <c r="R1" s="265"/>
+      <c r="S1" s="265"/>
+      <c r="T1" s="265"/>
+      <c r="U1" s="276" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="268"/>
-      <c r="W1" s="268"/>
-      <c r="X1" s="268"/>
-      <c r="Y1" s="278" t="s">
+      <c r="V1" s="276"/>
+      <c r="W1" s="276"/>
+      <c r="X1" s="276"/>
+      <c r="Y1" s="265" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" s="278"/>
-      <c r="AA1" s="278"/>
-      <c r="AB1" s="278"/>
-      <c r="AC1" s="268" t="s">
+      <c r="Z1" s="265"/>
+      <c r="AA1" s="265"/>
+      <c r="AB1" s="265"/>
+      <c r="AC1" s="276" t="s">
         <v>83</v>
       </c>
-      <c r="AD1" s="268"/>
-      <c r="AE1" s="268"/>
-      <c r="AF1" s="268"/>
-      <c r="AG1" s="278" t="s">
+      <c r="AD1" s="276"/>
+      <c r="AE1" s="276"/>
+      <c r="AF1" s="276"/>
+      <c r="AG1" s="265" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="278"/>
-      <c r="AI1" s="278"/>
-      <c r="AJ1" s="278"/>
-      <c r="AK1" s="268" t="s">
+      <c r="AH1" s="265"/>
+      <c r="AI1" s="265"/>
+      <c r="AJ1" s="265"/>
+      <c r="AK1" s="276" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="268"/>
-      <c r="AM1" s="268"/>
-      <c r="AN1" s="268"/>
-      <c r="AO1" s="278" t="s">
+      <c r="AL1" s="276"/>
+      <c r="AM1" s="276"/>
+      <c r="AN1" s="276"/>
+      <c r="AO1" s="265" t="s">
         <v>86</v>
       </c>
-      <c r="AP1" s="278"/>
-      <c r="AQ1" s="278"/>
-      <c r="AR1" s="278"/>
-      <c r="AS1" s="268" t="s">
+      <c r="AP1" s="265"/>
+      <c r="AQ1" s="265"/>
+      <c r="AR1" s="265"/>
+      <c r="AS1" s="276" t="s">
         <v>87</v>
       </c>
-      <c r="AT1" s="268"/>
-      <c r="AU1" s="268"/>
-      <c r="AV1" s="268"/>
-      <c r="AW1" s="278" t="s">
+      <c r="AT1" s="276"/>
+      <c r="AU1" s="276"/>
+      <c r="AV1" s="276"/>
+      <c r="AW1" s="265" t="s">
         <v>88</v>
       </c>
-      <c r="AX1" s="278"/>
-      <c r="AY1" s="278"/>
-      <c r="AZ1" s="278"/>
-      <c r="BA1" s="268" t="s">
+      <c r="AX1" s="265"/>
+      <c r="AY1" s="265"/>
+      <c r="AZ1" s="265"/>
+      <c r="BA1" s="276" t="s">
         <v>89</v>
       </c>
-      <c r="BB1" s="268"/>
-      <c r="BC1" s="268"/>
-      <c r="BD1" s="268"/>
-      <c r="BE1" s="278" t="s">
+      <c r="BB1" s="276"/>
+      <c r="BC1" s="276"/>
+      <c r="BD1" s="276"/>
+      <c r="BE1" s="265" t="s">
         <v>90</v>
       </c>
-      <c r="BF1" s="278"/>
-      <c r="BG1" s="278"/>
-      <c r="BH1" s="278"/>
+      <c r="BF1" s="265"/>
+      <c r="BG1" s="265"/>
+      <c r="BH1" s="265"/>
     </row>
     <row r="2" spans="1:60" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -36353,94 +36359,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.4">
-      <c r="A1" s="278" t="s">
+      <c r="A1" s="265" t="s">
         <v>678</v>
       </c>
-      <c r="B1" s="278"/>
-      <c r="C1" s="278"/>
-      <c r="D1" s="278"/>
-      <c r="E1" s="280" t="s">
+      <c r="B1" s="265"/>
+      <c r="C1" s="265"/>
+      <c r="D1" s="265"/>
+      <c r="E1" s="266" t="s">
         <v>679</v>
       </c>
-      <c r="F1" s="281"/>
-      <c r="G1" s="281"/>
-      <c r="H1" s="281"/>
-      <c r="I1" s="281"/>
-      <c r="J1" s="281"/>
-      <c r="K1" s="281"/>
-      <c r="L1" s="282"/>
-      <c r="M1" s="268" t="s">
+      <c r="F1" s="267"/>
+      <c r="G1" s="267"/>
+      <c r="H1" s="267"/>
+      <c r="I1" s="267"/>
+      <c r="J1" s="267"/>
+      <c r="K1" s="267"/>
+      <c r="L1" s="268"/>
+      <c r="M1" s="276" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="268"/>
-      <c r="O1" s="268"/>
-      <c r="P1" s="268"/>
-      <c r="Q1" s="280" t="s">
+      <c r="N1" s="276"/>
+      <c r="O1" s="276"/>
+      <c r="P1" s="276"/>
+      <c r="Q1" s="266" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="281"/>
-      <c r="S1" s="281"/>
-      <c r="T1" s="281"/>
-      <c r="U1" s="268" t="s">
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="267"/>
+      <c r="U1" s="276" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="268"/>
-      <c r="W1" s="268"/>
-      <c r="X1" s="268"/>
-      <c r="Y1" s="280" t="s">
+      <c r="V1" s="276"/>
+      <c r="W1" s="276"/>
+      <c r="X1" s="276"/>
+      <c r="Y1" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" s="281"/>
-      <c r="AA1" s="281"/>
-      <c r="AB1" s="281"/>
-      <c r="AC1" s="268" t="s">
+      <c r="Z1" s="267"/>
+      <c r="AA1" s="267"/>
+      <c r="AB1" s="267"/>
+      <c r="AC1" s="276" t="s">
         <v>83</v>
       </c>
-      <c r="AD1" s="268"/>
-      <c r="AE1" s="268"/>
-      <c r="AF1" s="268"/>
-      <c r="AG1" s="280" t="s">
+      <c r="AD1" s="276"/>
+      <c r="AE1" s="276"/>
+      <c r="AF1" s="276"/>
+      <c r="AG1" s="266" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="281"/>
-      <c r="AI1" s="281"/>
-      <c r="AJ1" s="281"/>
-      <c r="AK1" s="268" t="s">
+      <c r="AH1" s="267"/>
+      <c r="AI1" s="267"/>
+      <c r="AJ1" s="267"/>
+      <c r="AK1" s="276" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="268"/>
-      <c r="AM1" s="268"/>
-      <c r="AN1" s="268"/>
-      <c r="AO1" s="280" t="s">
+      <c r="AL1" s="276"/>
+      <c r="AM1" s="276"/>
+      <c r="AN1" s="276"/>
+      <c r="AO1" s="266" t="s">
         <v>86</v>
       </c>
-      <c r="AP1" s="281"/>
-      <c r="AQ1" s="281"/>
-      <c r="AR1" s="281"/>
-      <c r="AS1" s="268" t="s">
+      <c r="AP1" s="267"/>
+      <c r="AQ1" s="267"/>
+      <c r="AR1" s="267"/>
+      <c r="AS1" s="276" t="s">
         <v>87</v>
       </c>
-      <c r="AT1" s="268"/>
-      <c r="AU1" s="268"/>
-      <c r="AV1" s="268"/>
-      <c r="AW1" s="280" t="s">
+      <c r="AT1" s="276"/>
+      <c r="AU1" s="276"/>
+      <c r="AV1" s="276"/>
+      <c r="AW1" s="266" t="s">
         <v>88</v>
       </c>
-      <c r="AX1" s="281"/>
-      <c r="AY1" s="281"/>
-      <c r="AZ1" s="281"/>
-      <c r="BA1" s="268" t="s">
+      <c r="AX1" s="267"/>
+      <c r="AY1" s="267"/>
+      <c r="AZ1" s="267"/>
+      <c r="BA1" s="276" t="s">
         <v>89</v>
       </c>
-      <c r="BB1" s="268"/>
-      <c r="BC1" s="268"/>
-      <c r="BD1" s="268"/>
-      <c r="BE1" s="280" t="s">
+      <c r="BB1" s="276"/>
+      <c r="BC1" s="276"/>
+      <c r="BD1" s="276"/>
+      <c r="BE1" s="266" t="s">
         <v>90</v>
       </c>
-      <c r="BF1" s="281"/>
-      <c r="BG1" s="281"/>
-      <c r="BH1" s="281"/>
+      <c r="BF1" s="267"/>
+      <c r="BG1" s="267"/>
+      <c r="BH1" s="267"/>
     </row>
     <row r="2" spans="1:60" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -38321,7 +38327,7 @@
       <c r="B2" s="158" t="s">
         <v>493</v>
       </c>
-      <c r="C2" s="269" t="s">
+      <c r="C2" s="277" t="s">
         <v>514</v>
       </c>
       <c r="D2" s="159" t="s">
@@ -38335,7 +38341,7 @@
       <c r="B3" s="161" t="s">
         <v>494</v>
       </c>
-      <c r="C3" s="271"/>
+      <c r="C3" s="278"/>
       <c r="D3" s="162" t="s">
         <v>516</v>
       </c>
@@ -38347,7 +38353,7 @@
       <c r="B4" s="161" t="s">
         <v>495</v>
       </c>
-      <c r="C4" s="271"/>
+      <c r="C4" s="278"/>
       <c r="D4" s="162" t="s">
         <v>11</v>
       </c>
@@ -38359,7 +38365,7 @@
       <c r="B5" s="161" t="s">
         <v>496</v>
       </c>
-      <c r="C5" s="271"/>
+      <c r="C5" s="278"/>
       <c r="D5" s="162" t="s">
         <v>11</v>
       </c>
@@ -38371,7 +38377,7 @@
       <c r="B6" s="161" t="s">
         <v>497</v>
       </c>
-      <c r="C6" s="271"/>
+      <c r="C6" s="278"/>
       <c r="D6" s="162" t="s">
         <v>11</v>
       </c>
@@ -38383,7 +38389,7 @@
       <c r="B7" s="161" t="s">
         <v>498</v>
       </c>
-      <c r="C7" s="271"/>
+      <c r="C7" s="278"/>
       <c r="D7" s="162" t="s">
         <v>11</v>
       </c>
@@ -38395,7 +38401,7 @@
       <c r="B8" s="161" t="s">
         <v>499</v>
       </c>
-      <c r="C8" s="271"/>
+      <c r="C8" s="278"/>
       <c r="D8" s="162" t="s">
         <v>11</v>
       </c>
@@ -38407,7 +38413,7 @@
       <c r="B9" s="161" t="s">
         <v>500</v>
       </c>
-      <c r="C9" s="271"/>
+      <c r="C9" s="278"/>
       <c r="D9" s="162" t="s">
         <v>11</v>
       </c>
@@ -38419,7 +38425,7 @@
       <c r="B10" s="161" t="s">
         <v>501</v>
       </c>
-      <c r="C10" s="271"/>
+      <c r="C10" s="278"/>
       <c r="D10" s="162" t="s">
         <v>11</v>
       </c>
@@ -38431,7 +38437,7 @@
       <c r="B11" s="164" t="s">
         <v>511</v>
       </c>
-      <c r="C11" s="270"/>
+      <c r="C11" s="279"/>
       <c r="D11" s="165" t="s">
         <v>11</v>
       </c>
@@ -38443,7 +38449,7 @@
       <c r="B12" s="166" t="s">
         <v>240</v>
       </c>
-      <c r="C12" s="269" t="s">
+      <c r="C12" s="277" t="s">
         <v>517</v>
       </c>
       <c r="D12" s="159" t="s">
@@ -38457,7 +38463,7 @@
       <c r="B13" s="167" t="s">
         <v>241</v>
       </c>
-      <c r="C13" s="271"/>
+      <c r="C13" s="278"/>
       <c r="D13" s="162" t="s">
         <v>519</v>
       </c>
@@ -38469,7 +38475,7 @@
       <c r="B14" s="167" t="s">
         <v>242</v>
       </c>
-      <c r="C14" s="271"/>
+      <c r="C14" s="278"/>
       <c r="D14" s="162" t="s">
         <v>11</v>
       </c>
@@ -38481,7 +38487,7 @@
       <c r="B15" s="167" t="s">
         <v>243</v>
       </c>
-      <c r="C15" s="271"/>
+      <c r="C15" s="278"/>
       <c r="D15" s="162" t="s">
         <v>11</v>
       </c>
@@ -38493,7 +38499,7 @@
       <c r="B16" s="167" t="s">
         <v>244</v>
       </c>
-      <c r="C16" s="271"/>
+      <c r="C16" s="278"/>
       <c r="D16" s="162" t="s">
         <v>11</v>
       </c>
@@ -38505,7 +38511,7 @@
       <c r="B17" s="168" t="s">
         <v>245</v>
       </c>
-      <c r="C17" s="270"/>
+      <c r="C17" s="279"/>
       <c r="D17" s="165" t="s">
         <v>11</v>
       </c>
@@ -38517,7 +38523,7 @@
       <c r="B18" s="169" t="s">
         <v>246</v>
       </c>
-      <c r="C18" s="269" t="s">
+      <c r="C18" s="277" t="s">
         <v>109</v>
       </c>
       <c r="D18" s="159" t="s">
@@ -38531,7 +38537,7 @@
       <c r="B19" s="171" t="s">
         <v>247</v>
       </c>
-      <c r="C19" s="271"/>
+      <c r="C19" s="278"/>
       <c r="D19" s="162" t="s">
         <v>521</v>
       </c>
@@ -38543,7 +38549,7 @@
       <c r="B20" s="170" t="s">
         <v>248</v>
       </c>
-      <c r="C20" s="271"/>
+      <c r="C20" s="278"/>
       <c r="D20" s="162" t="s">
         <v>522</v>
       </c>
@@ -38555,7 +38561,7 @@
       <c r="B21" s="170" t="s">
         <v>249</v>
       </c>
-      <c r="C21" s="271"/>
+      <c r="C21" s="278"/>
       <c r="D21" s="162" t="s">
         <v>523</v>
       </c>
@@ -38567,7 +38573,7 @@
       <c r="B22" s="170" t="s">
         <v>250</v>
       </c>
-      <c r="C22" s="271"/>
+      <c r="C22" s="278"/>
       <c r="D22" s="162" t="s">
         <v>524</v>
       </c>
@@ -38579,7 +38585,7 @@
       <c r="B23" s="170" t="s">
         <v>251</v>
       </c>
-      <c r="C23" s="271"/>
+      <c r="C23" s="278"/>
       <c r="D23" s="162" t="s">
         <v>525</v>
       </c>
@@ -38591,7 +38597,7 @@
       <c r="B24" s="170" t="s">
         <v>491</v>
       </c>
-      <c r="C24" s="271"/>
+      <c r="C24" s="278"/>
       <c r="D24" s="162" t="s">
         <v>11</v>
       </c>
@@ -38603,7 +38609,7 @@
       <c r="B25" s="170" t="s">
         <v>492</v>
       </c>
-      <c r="C25" s="271"/>
+      <c r="C25" s="278"/>
       <c r="D25" s="162" t="s">
         <v>526</v>
       </c>
@@ -38615,7 +38621,7 @@
       <c r="B26" s="170" t="s">
         <v>252</v>
       </c>
-      <c r="C26" s="271"/>
+      <c r="C26" s="278"/>
       <c r="D26" s="162" t="s">
         <v>11</v>
       </c>
@@ -38627,7 +38633,7 @@
       <c r="B27" s="171" t="s">
         <v>502</v>
       </c>
-      <c r="C27" s="271"/>
+      <c r="C27" s="278"/>
       <c r="D27" s="162" t="s">
         <v>527</v>
       </c>
@@ -38639,7 +38645,7 @@
       <c r="B28" s="171" t="s">
         <v>503</v>
       </c>
-      <c r="C28" s="270"/>
+      <c r="C28" s="279"/>
       <c r="D28" s="162" t="s">
         <v>528</v>
       </c>
@@ -38651,7 +38657,7 @@
       <c r="B29" s="173" t="s">
         <v>253</v>
       </c>
-      <c r="C29" s="269" t="s">
+      <c r="C29" s="277" t="s">
         <v>529</v>
       </c>
       <c r="D29" s="159" t="s">
@@ -38665,7 +38671,7 @@
       <c r="B30" s="175" t="s">
         <v>254</v>
       </c>
-      <c r="C30" s="271"/>
+      <c r="C30" s="278"/>
       <c r="D30" s="177" t="s">
         <v>675</v>
       </c>
@@ -38677,7 +38683,7 @@
       <c r="B31" s="176" t="s">
         <v>255</v>
       </c>
-      <c r="C31" s="271"/>
+      <c r="C31" s="278"/>
       <c r="D31" s="162" t="s">
         <v>531</v>
       </c>
@@ -38689,7 +38695,7 @@
       <c r="B32" s="176" t="s">
         <v>256</v>
       </c>
-      <c r="C32" s="271"/>
+      <c r="C32" s="278"/>
       <c r="D32" s="162" t="s">
         <v>532</v>
       </c>
@@ -38701,7 +38707,7 @@
       <c r="B33" s="176" t="s">
         <v>257</v>
       </c>
-      <c r="C33" s="271"/>
+      <c r="C33" s="278"/>
       <c r="D33" s="177" t="s">
         <v>533</v>
       </c>
@@ -38713,7 +38719,7 @@
       <c r="B34" s="175" t="s">
         <v>258</v>
       </c>
-      <c r="C34" s="271"/>
+      <c r="C34" s="278"/>
       <c r="D34" s="162" t="s">
         <v>534</v>
       </c>
@@ -38725,7 +38731,7 @@
       <c r="B35" s="176" t="s">
         <v>259</v>
       </c>
-      <c r="C35" s="271"/>
+      <c r="C35" s="278"/>
       <c r="D35" s="162" t="s">
         <v>535</v>
       </c>
@@ -38737,7 +38743,7 @@
       <c r="B36" s="175" t="s">
         <v>260</v>
       </c>
-      <c r="C36" s="271"/>
+      <c r="C36" s="278"/>
       <c r="D36" s="162" t="s">
         <v>535</v>
       </c>
@@ -38749,7 +38755,7 @@
       <c r="B37" s="176" t="s">
         <v>261</v>
       </c>
-      <c r="C37" s="271"/>
+      <c r="C37" s="278"/>
       <c r="D37" s="162" t="s">
         <v>536</v>
       </c>
@@ -38761,7 +38767,7 @@
       <c r="B38" s="175" t="s">
         <v>262</v>
       </c>
-      <c r="C38" s="271"/>
+      <c r="C38" s="278"/>
       <c r="D38" s="162" t="s">
         <v>536</v>
       </c>
@@ -38773,7 +38779,7 @@
       <c r="B39" s="176" t="s">
         <v>263</v>
       </c>
-      <c r="C39" s="271"/>
+      <c r="C39" s="278"/>
       <c r="D39" s="177" t="s">
         <v>670</v>
       </c>
@@ -38785,7 +38791,7 @@
       <c r="B40" s="175" t="s">
         <v>264</v>
       </c>
-      <c r="C40" s="271"/>
+      <c r="C40" s="278"/>
       <c r="D40" s="162" t="s">
         <v>537</v>
       </c>
@@ -38797,7 +38803,7 @@
       <c r="B41" s="176" t="s">
         <v>265</v>
       </c>
-      <c r="C41" s="271"/>
+      <c r="C41" s="278"/>
       <c r="D41" s="162" t="s">
         <v>538</v>
       </c>
@@ -38834,7 +38840,7 @@
       <c r="B44" s="185" t="s">
         <v>266</v>
       </c>
-      <c r="C44" s="269" t="s">
+      <c r="C44" s="277" t="s">
         <v>541</v>
       </c>
       <c r="D44" s="186" t="s">
@@ -38848,7 +38854,7 @@
       <c r="B45" s="188" t="s">
         <v>267</v>
       </c>
-      <c r="C45" s="271"/>
+      <c r="C45" s="278"/>
       <c r="D45" s="162" t="s">
         <v>11</v>
       </c>
@@ -38860,7 +38866,7 @@
       <c r="B46" s="188" t="s">
         <v>268</v>
       </c>
-      <c r="C46" s="271"/>
+      <c r="C46" s="278"/>
       <c r="D46" s="162" t="s">
         <v>542</v>
       </c>
@@ -38872,7 +38878,7 @@
       <c r="B47" s="188" t="s">
         <v>269</v>
       </c>
-      <c r="C47" s="271"/>
+      <c r="C47" s="278"/>
       <c r="D47" s="177" t="s">
         <v>543</v>
       </c>
@@ -38884,7 +38890,7 @@
       <c r="B48" s="188" t="s">
         <v>270</v>
       </c>
-      <c r="C48" s="271"/>
+      <c r="C48" s="278"/>
       <c r="D48" s="162" t="s">
         <v>11</v>
       </c>
@@ -38896,7 +38902,7 @@
       <c r="B49" s="188" t="s">
         <v>271</v>
       </c>
-      <c r="C49" s="271"/>
+      <c r="C49" s="278"/>
       <c r="D49" s="162" t="s">
         <v>544</v>
       </c>
@@ -38908,7 +38914,7 @@
       <c r="B50" s="188" t="s">
         <v>272</v>
       </c>
-      <c r="C50" s="271"/>
+      <c r="C50" s="278"/>
       <c r="D50" s="162" t="s">
         <v>11</v>
       </c>
@@ -38920,7 +38926,7 @@
       <c r="B51" s="188" t="s">
         <v>273</v>
       </c>
-      <c r="C51" s="271"/>
+      <c r="C51" s="278"/>
       <c r="D51" s="177" t="s">
         <v>676</v>
       </c>
@@ -38932,7 +38938,7 @@
       <c r="B52" s="188" t="s">
         <v>274</v>
       </c>
-      <c r="C52" s="271"/>
+      <c r="C52" s="278"/>
       <c r="D52" s="177" t="s">
         <v>543</v>
       </c>
@@ -38944,7 +38950,7 @@
       <c r="B53" s="190" t="s">
         <v>275</v>
       </c>
-      <c r="C53" s="270"/>
+      <c r="C53" s="279"/>
       <c r="D53" s="165" t="s">
         <v>11</v>
       </c>
@@ -38956,7 +38962,7 @@
       <c r="B54" s="191" t="s">
         <v>276</v>
       </c>
-      <c r="C54" s="269" t="s">
+      <c r="C54" s="277" t="s">
         <v>545</v>
       </c>
       <c r="D54" s="177" t="s">
@@ -38970,7 +38976,7 @@
       <c r="B55" s="191" t="s">
         <v>277</v>
       </c>
-      <c r="C55" s="271"/>
+      <c r="C55" s="278"/>
       <c r="D55" s="162" t="s">
         <v>547</v>
       </c>
@@ -38982,7 +38988,7 @@
       <c r="B56" s="191" t="s">
         <v>278</v>
       </c>
-      <c r="C56" s="271"/>
+      <c r="C56" s="278"/>
       <c r="D56" s="162" t="s">
         <v>548</v>
       </c>
@@ -38994,7 +39000,7 @@
       <c r="B57" s="191" t="s">
         <v>279</v>
       </c>
-      <c r="C57" s="270"/>
+      <c r="C57" s="279"/>
       <c r="D57" s="162" t="s">
         <v>549</v>
       </c>
@@ -39006,7 +39012,7 @@
       <c r="B58" s="254" t="s">
         <v>280</v>
       </c>
-      <c r="C58" s="269" t="s">
+      <c r="C58" s="277" t="s">
         <v>550</v>
       </c>
       <c r="D58" s="159" t="s">
@@ -39020,7 +39026,7 @@
       <c r="B59" s="192" t="s">
         <v>671</v>
       </c>
-      <c r="C59" s="270"/>
+      <c r="C59" s="279"/>
       <c r="D59" s="182" t="s">
         <v>674</v>
       </c>
@@ -39032,7 +39038,7 @@
       <c r="B60" s="193" t="s">
         <v>281</v>
       </c>
-      <c r="C60" s="269" t="s">
+      <c r="C60" s="277" t="s">
         <v>552</v>
       </c>
       <c r="D60" s="162" t="s">
@@ -39046,7 +39052,7 @@
       <c r="B61" s="193" t="s">
         <v>282</v>
       </c>
-      <c r="C61" s="271"/>
+      <c r="C61" s="278"/>
       <c r="D61" s="162" t="s">
         <v>554</v>
       </c>
@@ -39058,7 +39064,7 @@
       <c r="B62" s="193" t="s">
         <v>283</v>
       </c>
-      <c r="C62" s="271"/>
+      <c r="C62" s="278"/>
       <c r="D62" s="162" t="s">
         <v>555</v>
       </c>
@@ -39070,7 +39076,7 @@
       <c r="B63" s="193" t="s">
         <v>284</v>
       </c>
-      <c r="C63" s="271"/>
+      <c r="C63" s="278"/>
       <c r="D63" s="162" t="s">
         <v>556</v>
       </c>
@@ -39082,7 +39088,7 @@
       <c r="B64" s="193" t="s">
         <v>285</v>
       </c>
-      <c r="C64" s="271"/>
+      <c r="C64" s="278"/>
       <c r="D64" s="162" t="s">
         <v>557</v>
       </c>
@@ -39094,7 +39100,7 @@
       <c r="B65" s="193" t="s">
         <v>286</v>
       </c>
-      <c r="C65" s="271"/>
+      <c r="C65" s="278"/>
       <c r="D65" s="162" t="s">
         <v>558</v>
       </c>
@@ -39106,7 +39112,7 @@
       <c r="B66" s="193" t="s">
         <v>287</v>
       </c>
-      <c r="C66" s="271"/>
+      <c r="C66" s="278"/>
       <c r="D66" s="162" t="s">
         <v>559</v>
       </c>
@@ -39118,7 +39124,7 @@
       <c r="B67" s="195" t="s">
         <v>288</v>
       </c>
-      <c r="C67" s="270"/>
+      <c r="C67" s="279"/>
       <c r="D67" s="165" t="s">
         <v>560</v>
       </c>
@@ -39130,7 +39136,7 @@
       <c r="B68" s="197" t="s">
         <v>289</v>
       </c>
-      <c r="C68" s="269" t="s">
+      <c r="C68" s="277" t="s">
         <v>561</v>
       </c>
       <c r="D68" s="159" t="s">
@@ -39144,7 +39150,7 @@
       <c r="B69" s="199" t="s">
         <v>290</v>
       </c>
-      <c r="C69" s="271"/>
+      <c r="C69" s="278"/>
       <c r="D69" s="162" t="s">
         <v>11</v>
       </c>
@@ -39156,7 +39162,7 @@
       <c r="B70" s="199" t="s">
         <v>291</v>
       </c>
-      <c r="C70" s="271"/>
+      <c r="C70" s="278"/>
       <c r="D70" s="162" t="s">
         <v>11</v>
       </c>
@@ -39168,7 +39174,7 @@
       <c r="B71" s="199" t="s">
         <v>292</v>
       </c>
-      <c r="C71" s="271"/>
+      <c r="C71" s="278"/>
       <c r="D71" s="162" t="s">
         <v>11</v>
       </c>
@@ -39180,7 +39186,7 @@
       <c r="B72" s="199" t="s">
         <v>293</v>
       </c>
-      <c r="C72" s="271"/>
+      <c r="C72" s="278"/>
       <c r="D72" s="162" t="s">
         <v>563</v>
       </c>
@@ -39192,7 +39198,7 @@
       <c r="B73" s="199" t="s">
         <v>294</v>
       </c>
-      <c r="C73" s="271"/>
+      <c r="C73" s="278"/>
       <c r="D73" s="162" t="s">
         <v>11</v>
       </c>
@@ -39204,7 +39210,7 @@
       <c r="B74" s="199" t="s">
         <v>295</v>
       </c>
-      <c r="C74" s="271"/>
+      <c r="C74" s="278"/>
       <c r="D74" s="162" t="s">
         <v>11</v>
       </c>
@@ -39216,7 +39222,7 @@
       <c r="B75" s="199" t="s">
         <v>296</v>
       </c>
-      <c r="C75" s="271"/>
+      <c r="C75" s="278"/>
       <c r="D75" s="162" t="s">
         <v>11</v>
       </c>
@@ -39228,7 +39234,7 @@
       <c r="B76" s="199" t="s">
         <v>297</v>
       </c>
-      <c r="C76" s="271"/>
+      <c r="C76" s="278"/>
       <c r="D76" s="162" t="s">
         <v>11</v>
       </c>
@@ -39240,7 +39246,7 @@
       <c r="B77" s="199" t="s">
         <v>298</v>
       </c>
-      <c r="C77" s="271"/>
+      <c r="C77" s="278"/>
       <c r="D77" s="162" t="s">
         <v>563</v>
       </c>
@@ -39252,7 +39258,7 @@
       <c r="B78" s="199" t="s">
         <v>299</v>
       </c>
-      <c r="C78" s="271"/>
+      <c r="C78" s="278"/>
       <c r="D78" s="162" t="s">
         <v>11</v>
       </c>
@@ -39264,7 +39270,7 @@
       <c r="B79" s="199" t="s">
         <v>300</v>
       </c>
-      <c r="C79" s="271"/>
+      <c r="C79" s="278"/>
       <c r="D79" s="162" t="s">
         <v>11</v>
       </c>
@@ -39276,7 +39282,7 @@
       <c r="B80" s="200" t="s">
         <v>301</v>
       </c>
-      <c r="C80" s="271"/>
+      <c r="C80" s="278"/>
       <c r="D80" s="162" t="s">
         <v>11</v>
       </c>
@@ -39288,7 +39294,7 @@
       <c r="B81" s="200" t="s">
         <v>302</v>
       </c>
-      <c r="C81" s="271"/>
+      <c r="C81" s="278"/>
       <c r="D81" s="162" t="s">
         <v>11</v>
       </c>
@@ -39300,7 +39306,7 @@
       <c r="B82" s="200" t="s">
         <v>303</v>
       </c>
-      <c r="C82" s="271"/>
+      <c r="C82" s="278"/>
       <c r="D82" s="162" t="s">
         <v>563</v>
       </c>
@@ -39312,7 +39318,7 @@
       <c r="B83" s="200" t="s">
         <v>304</v>
       </c>
-      <c r="C83" s="271"/>
+      <c r="C83" s="278"/>
       <c r="D83" s="162" t="s">
         <v>564</v>
       </c>
@@ -39324,7 +39330,7 @@
       <c r="B84" s="201" t="s">
         <v>305</v>
       </c>
-      <c r="C84" s="271"/>
+      <c r="C84" s="278"/>
       <c r="D84" s="162" t="s">
         <v>565</v>
       </c>
@@ -39336,7 +39342,7 @@
       <c r="B85" s="201" t="s">
         <v>306</v>
       </c>
-      <c r="C85" s="271"/>
+      <c r="C85" s="278"/>
       <c r="D85" s="162" t="s">
         <v>566</v>
       </c>
@@ -39348,7 +39354,7 @@
       <c r="B86" s="201" t="s">
         <v>307</v>
       </c>
-      <c r="C86" s="271"/>
+      <c r="C86" s="278"/>
       <c r="D86" s="162" t="s">
         <v>567</v>
       </c>
@@ -39360,7 +39366,7 @@
       <c r="B87" s="201" t="s">
         <v>308</v>
       </c>
-      <c r="C87" s="271"/>
+      <c r="C87" s="278"/>
       <c r="D87" s="162" t="s">
         <v>568</v>
       </c>
@@ -39372,7 +39378,7 @@
       <c r="B88" s="203" t="s">
         <v>309</v>
       </c>
-      <c r="C88" s="270"/>
+      <c r="C88" s="279"/>
       <c r="D88" s="165" t="s">
         <v>569</v>
       </c>
@@ -39384,7 +39390,7 @@
       <c r="B89" s="205" t="s">
         <v>310</v>
       </c>
-      <c r="C89" s="269" t="s">
+      <c r="C89" s="277" t="s">
         <v>570</v>
       </c>
       <c r="D89" s="162" t="s">
@@ -39398,7 +39404,7 @@
       <c r="B90" s="205" t="s">
         <v>438</v>
       </c>
-      <c r="C90" s="271"/>
+      <c r="C90" s="278"/>
       <c r="D90" s="206" t="s">
         <v>572</v>
       </c>
@@ -39410,7 +39416,7 @@
       <c r="B91" s="205" t="s">
         <v>311</v>
       </c>
-      <c r="C91" s="271"/>
+      <c r="C91" s="278"/>
       <c r="D91" s="207" t="s">
         <v>573</v>
       </c>
@@ -39422,7 +39428,7 @@
       <c r="B92" s="209" t="s">
         <v>312</v>
       </c>
-      <c r="C92" s="270"/>
+      <c r="C92" s="279"/>
       <c r="D92" s="182" t="s">
         <v>574</v>
       </c>
@@ -39434,7 +39440,7 @@
       <c r="B93" s="185" t="s">
         <v>313</v>
       </c>
-      <c r="C93" s="269" t="s">
+      <c r="C93" s="277" t="s">
         <v>575</v>
       </c>
       <c r="D93" s="186" t="s">
@@ -39448,7 +39454,7 @@
       <c r="B94" s="188" t="s">
         <v>319</v>
       </c>
-      <c r="C94" s="271"/>
+      <c r="C94" s="278"/>
       <c r="D94" s="177" t="s">
         <v>577</v>
       </c>
@@ -39460,7 +39466,7 @@
       <c r="B95" s="188" t="s">
         <v>488</v>
       </c>
-      <c r="C95" s="271"/>
+      <c r="C95" s="278"/>
       <c r="D95" s="162" t="s">
         <v>578</v>
       </c>
@@ -39472,7 +39478,7 @@
       <c r="B96" s="188" t="s">
         <v>489</v>
       </c>
-      <c r="C96" s="271"/>
+      <c r="C96" s="278"/>
       <c r="D96" s="162" t="s">
         <v>579</v>
       </c>
@@ -39484,7 +39490,7 @@
       <c r="B97" s="188" t="s">
         <v>490</v>
       </c>
-      <c r="C97" s="271"/>
+      <c r="C97" s="278"/>
       <c r="D97" s="162" t="s">
         <v>580</v>
       </c>
@@ -39496,7 +39502,7 @@
       <c r="B98" s="190" t="s">
         <v>657</v>
       </c>
-      <c r="C98" s="270"/>
+      <c r="C98" s="279"/>
       <c r="D98" s="182" t="s">
         <v>658</v>
       </c>
@@ -39508,7 +39514,7 @@
       <c r="B99" s="211" t="s">
         <v>454</v>
       </c>
-      <c r="C99" s="269" t="s">
+      <c r="C99" s="277" t="s">
         <v>581</v>
       </c>
       <c r="D99" s="159" t="s">
@@ -39522,7 +39528,7 @@
       <c r="B100" s="213" t="s">
         <v>314</v>
       </c>
-      <c r="C100" s="271"/>
+      <c r="C100" s="278"/>
       <c r="D100" s="162" t="s">
         <v>583</v>
       </c>
@@ -39534,7 +39540,7 @@
       <c r="B101" s="213" t="s">
         <v>315</v>
       </c>
-      <c r="C101" s="271"/>
+      <c r="C101" s="278"/>
       <c r="D101" s="162" t="s">
         <v>584</v>
       </c>
@@ -39546,7 +39552,7 @@
       <c r="B102" s="213" t="s">
         <v>316</v>
       </c>
-      <c r="C102" s="271"/>
+      <c r="C102" s="278"/>
       <c r="D102" s="162" t="s">
         <v>584</v>
       </c>
@@ -39558,7 +39564,7 @@
       <c r="B103" s="213" t="s">
         <v>317</v>
       </c>
-      <c r="C103" s="271"/>
+      <c r="C103" s="278"/>
       <c r="D103" s="162" t="s">
         <v>585</v>
       </c>
@@ -39570,7 +39576,7 @@
       <c r="B104" s="215" t="s">
         <v>318</v>
       </c>
-      <c r="C104" s="270"/>
+      <c r="C104" s="279"/>
       <c r="D104" s="165" t="s">
         <v>585</v>
       </c>
@@ -39582,7 +39588,7 @@
       <c r="B105" s="216" t="s">
         <v>439</v>
       </c>
-      <c r="C105" s="269" t="s">
+      <c r="C105" s="277" t="s">
         <v>586</v>
       </c>
       <c r="D105" s="186" t="s">
@@ -39596,7 +39602,7 @@
       <c r="B106" s="217" t="s">
         <v>440</v>
       </c>
-      <c r="C106" s="271"/>
+      <c r="C106" s="278"/>
       <c r="D106" s="162" t="s">
         <v>11</v>
       </c>
@@ -39608,7 +39614,7 @@
       <c r="B107" s="217" t="s">
         <v>441</v>
       </c>
-      <c r="C107" s="271"/>
+      <c r="C107" s="278"/>
       <c r="D107" s="162" t="s">
         <v>11</v>
       </c>
@@ -39620,7 +39626,7 @@
       <c r="B108" s="217" t="s">
         <v>442</v>
       </c>
-      <c r="C108" s="271"/>
+      <c r="C108" s="278"/>
       <c r="D108" s="162" t="s">
         <v>11</v>
       </c>
@@ -39632,7 +39638,7 @@
       <c r="B109" s="217" t="s">
         <v>443</v>
       </c>
-      <c r="C109" s="271"/>
+      <c r="C109" s="278"/>
       <c r="D109" s="162" t="s">
         <v>563</v>
       </c>
@@ -39644,7 +39650,7 @@
       <c r="B110" s="217" t="s">
         <v>444</v>
       </c>
-      <c r="C110" s="271"/>
+      <c r="C110" s="278"/>
       <c r="D110" s="162" t="s">
         <v>11</v>
       </c>
@@ -39656,7 +39662,7 @@
       <c r="B111" s="217" t="s">
         <v>445</v>
       </c>
-      <c r="C111" s="271"/>
+      <c r="C111" s="278"/>
       <c r="D111" s="162" t="s">
         <v>11</v>
       </c>
@@ -39668,7 +39674,7 @@
       <c r="B112" s="217" t="s">
         <v>506</v>
       </c>
-      <c r="C112" s="271"/>
+      <c r="C112" s="278"/>
       <c r="D112" s="162" t="s">
         <v>11</v>
       </c>
@@ -39680,7 +39686,7 @@
       <c r="B113" s="217" t="s">
         <v>507</v>
       </c>
-      <c r="C113" s="271"/>
+      <c r="C113" s="278"/>
       <c r="D113" s="162" t="s">
         <v>11</v>
       </c>
@@ -39692,7 +39698,7 @@
       <c r="B114" s="217" t="s">
         <v>508</v>
       </c>
-      <c r="C114" s="271"/>
+      <c r="C114" s="278"/>
       <c r="D114" s="162" t="s">
         <v>11</v>
       </c>
@@ -39704,7 +39710,7 @@
       <c r="B115" s="217" t="s">
         <v>509</v>
       </c>
-      <c r="C115" s="271"/>
+      <c r="C115" s="278"/>
       <c r="D115" s="162" t="s">
         <v>11</v>
       </c>
@@ -39716,7 +39722,7 @@
       <c r="B116" s="217" t="s">
         <v>446</v>
       </c>
-      <c r="C116" s="271"/>
+      <c r="C116" s="278"/>
       <c r="D116" s="162" t="s">
         <v>588</v>
       </c>
@@ -39728,7 +39734,7 @@
       <c r="B117" s="217" t="s">
         <v>447</v>
       </c>
-      <c r="C117" s="271"/>
+      <c r="C117" s="278"/>
       <c r="D117" s="162" t="s">
         <v>589</v>
       </c>
@@ -39740,7 +39746,7 @@
       <c r="B118" s="217" t="s">
         <v>477</v>
       </c>
-      <c r="C118" s="271"/>
+      <c r="C118" s="278"/>
       <c r="D118" s="162" t="s">
         <v>590</v>
       </c>
@@ -39752,7 +39758,7 @@
       <c r="B119" s="217" t="s">
         <v>478</v>
       </c>
-      <c r="C119" s="271"/>
+      <c r="C119" s="278"/>
       <c r="D119" s="162" t="s">
         <v>591</v>
       </c>
@@ -39764,7 +39770,7 @@
       <c r="B120" s="217" t="s">
         <v>510</v>
       </c>
-      <c r="C120" s="271"/>
+      <c r="C120" s="278"/>
       <c r="D120" s="162" t="s">
         <v>592</v>
       </c>
@@ -39776,7 +39782,7 @@
       <c r="B121" s="217" t="s">
         <v>513</v>
       </c>
-      <c r="C121" s="271"/>
+      <c r="C121" s="278"/>
       <c r="D121" s="162" t="s">
         <v>593</v>
       </c>
@@ -39788,7 +39794,7 @@
       <c r="B122" s="217" t="s">
         <v>512</v>
       </c>
-      <c r="C122" s="271"/>
+      <c r="C122" s="278"/>
       <c r="D122" s="177" t="s">
         <v>594</v>
       </c>
@@ -39800,7 +39806,7 @@
       <c r="B123" s="217" t="s">
         <v>320</v>
       </c>
-      <c r="C123" s="271"/>
+      <c r="C123" s="278"/>
       <c r="D123" s="162" t="s">
         <v>595</v>
       </c>
@@ -39812,7 +39818,7 @@
       <c r="B124" s="217" t="s">
         <v>321</v>
       </c>
-      <c r="C124" s="271"/>
+      <c r="C124" s="278"/>
       <c r="D124" s="162" t="s">
         <v>595</v>
       </c>
@@ -39824,7 +39830,7 @@
       <c r="B125" s="217" t="s">
         <v>322</v>
       </c>
-      <c r="C125" s="271"/>
+      <c r="C125" s="278"/>
       <c r="D125" s="177" t="s">
         <v>672</v>
       </c>
@@ -39836,7 +39842,7 @@
       <c r="B126" s="217" t="s">
         <v>323</v>
       </c>
-      <c r="C126" s="271"/>
+      <c r="C126" s="278"/>
       <c r="D126" s="162" t="s">
         <v>596</v>
       </c>
@@ -39848,7 +39854,7 @@
       <c r="B127" s="217" t="s">
         <v>448</v>
       </c>
-      <c r="C127" s="271"/>
+      <c r="C127" s="278"/>
       <c r="D127" s="177" t="s">
         <v>673</v>
       </c>
@@ -39860,7 +39866,7 @@
       <c r="B128" s="217" t="s">
         <v>449</v>
       </c>
-      <c r="C128" s="271"/>
+      <c r="C128" s="278"/>
       <c r="D128" s="177" t="s">
         <v>669</v>
       </c>
@@ -39872,7 +39878,7 @@
       <c r="B129" s="217" t="s">
         <v>324</v>
       </c>
-      <c r="C129" s="271"/>
+      <c r="C129" s="278"/>
       <c r="D129" s="177" t="s">
         <v>597</v>
       </c>
@@ -39884,7 +39890,7 @@
       <c r="B130" s="217" t="s">
         <v>480</v>
       </c>
-      <c r="C130" s="271"/>
+      <c r="C130" s="278"/>
       <c r="D130" s="177" t="s">
         <v>598</v>
       </c>
@@ -39896,7 +39902,7 @@
       <c r="B131" s="217" t="s">
         <v>325</v>
       </c>
-      <c r="C131" s="271"/>
+      <c r="C131" s="278"/>
       <c r="D131" s="162" t="s">
         <v>599</v>
       </c>
@@ -39908,7 +39914,7 @@
       <c r="B132" s="217" t="s">
         <v>326</v>
       </c>
-      <c r="C132" s="271"/>
+      <c r="C132" s="278"/>
       <c r="D132" s="162" t="s">
         <v>600</v>
       </c>
@@ -39920,7 +39926,7 @@
       <c r="B133" s="217" t="s">
         <v>327</v>
       </c>
-      <c r="C133" s="271"/>
+      <c r="C133" s="278"/>
       <c r="D133" s="218" t="s">
         <v>601</v>
       </c>
@@ -39932,7 +39938,7 @@
       <c r="B134" s="217" t="s">
         <v>328</v>
       </c>
-      <c r="C134" s="271"/>
+      <c r="C134" s="278"/>
       <c r="D134" s="218" t="s">
         <v>601</v>
       </c>
@@ -39944,7 +39950,7 @@
       <c r="B135" s="217" t="s">
         <v>329</v>
       </c>
-      <c r="C135" s="271"/>
+      <c r="C135" s="278"/>
       <c r="D135" s="162" t="s">
         <v>602</v>
       </c>
@@ -39956,7 +39962,7 @@
       <c r="B136" s="217" t="s">
         <v>330</v>
       </c>
-      <c r="C136" s="271"/>
+      <c r="C136" s="278"/>
       <c r="D136" s="162" t="s">
         <v>603</v>
       </c>
@@ -39968,7 +39974,7 @@
       <c r="B137" s="217" t="s">
         <v>463</v>
       </c>
-      <c r="C137" s="271"/>
+      <c r="C137" s="278"/>
       <c r="D137" s="162" t="s">
         <v>604</v>
       </c>
@@ -39980,7 +39986,7 @@
       <c r="B138" s="219" t="s">
         <v>464</v>
       </c>
-      <c r="C138" s="270"/>
+      <c r="C138" s="279"/>
       <c r="D138" s="165" t="s">
         <v>605</v>
       </c>
@@ -39992,7 +39998,7 @@
       <c r="B139" s="221" t="s">
         <v>331</v>
       </c>
-      <c r="C139" s="269" t="s">
+      <c r="C139" s="277" t="s">
         <v>606</v>
       </c>
       <c r="D139" s="162" t="s">
@@ -40006,7 +40012,7 @@
       <c r="B140" s="221" t="s">
         <v>332</v>
       </c>
-      <c r="C140" s="271"/>
+      <c r="C140" s="278"/>
       <c r="D140" s="177" t="s">
         <v>608</v>
       </c>
@@ -40018,7 +40024,7 @@
       <c r="B141" s="221" t="s">
         <v>333</v>
       </c>
-      <c r="C141" s="271"/>
+      <c r="C141" s="278"/>
       <c r="D141" s="162" t="s">
         <v>11</v>
       </c>
@@ -40030,7 +40036,7 @@
       <c r="B142" s="221" t="s">
         <v>334</v>
       </c>
-      <c r="C142" s="271"/>
+      <c r="C142" s="278"/>
       <c r="D142" s="162" t="s">
         <v>11</v>
       </c>
@@ -40042,7 +40048,7 @@
       <c r="B143" s="221" t="s">
         <v>450</v>
       </c>
-      <c r="C143" s="271"/>
+      <c r="C143" s="278"/>
       <c r="D143" s="177" t="s">
         <v>609</v>
       </c>
@@ -40054,7 +40060,7 @@
       <c r="B144" s="221" t="s">
         <v>451</v>
       </c>
-      <c r="C144" s="271"/>
+      <c r="C144" s="278"/>
       <c r="D144" s="177" t="s">
         <v>610</v>
       </c>
@@ -40066,7 +40072,7 @@
       <c r="B145" s="221" t="s">
         <v>335</v>
       </c>
-      <c r="C145" s="271"/>
+      <c r="C145" s="278"/>
       <c r="D145" s="162" t="s">
         <v>611</v>
       </c>
@@ -40078,7 +40084,7 @@
       <c r="B146" s="221" t="s">
         <v>336</v>
       </c>
-      <c r="C146" s="271"/>
+      <c r="C146" s="278"/>
       <c r="D146" s="162" t="s">
         <v>11</v>
       </c>
@@ -40090,7 +40096,7 @@
       <c r="B147" s="221" t="s">
         <v>337</v>
       </c>
-      <c r="C147" s="271"/>
+      <c r="C147" s="278"/>
       <c r="D147" s="162" t="s">
         <v>11</v>
       </c>
@@ -40102,7 +40108,7 @@
       <c r="B148" s="221" t="s">
         <v>338</v>
       </c>
-      <c r="C148" s="271"/>
+      <c r="C148" s="278"/>
       <c r="D148" s="162" t="s">
         <v>11</v>
       </c>
@@ -40114,7 +40120,7 @@
       <c r="B149" s="221" t="s">
         <v>339</v>
       </c>
-      <c r="C149" s="271"/>
+      <c r="C149" s="278"/>
       <c r="D149" s="162" t="s">
         <v>612</v>
       </c>
@@ -40126,7 +40132,7 @@
       <c r="B150" s="221" t="s">
         <v>340</v>
       </c>
-      <c r="C150" s="271"/>
+      <c r="C150" s="278"/>
       <c r="D150" s="162" t="s">
         <v>613</v>
       </c>
@@ -40138,7 +40144,7 @@
       <c r="B151" s="221" t="s">
         <v>341</v>
       </c>
-      <c r="C151" s="271"/>
+      <c r="C151" s="278"/>
       <c r="D151" s="162" t="s">
         <v>614</v>
       </c>
@@ -40150,7 +40156,7 @@
       <c r="B152" s="222" t="s">
         <v>342</v>
       </c>
-      <c r="C152" s="270"/>
+      <c r="C152" s="279"/>
       <c r="D152" s="165" t="s">
         <v>615</v>
       </c>
@@ -40172,6 +40178,13 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="C18:C28"/>
+    <mergeCell ref="C29:C41"/>
+    <mergeCell ref="C44:C53"/>
     <mergeCell ref="C139:C152"/>
     <mergeCell ref="C60:C67"/>
     <mergeCell ref="C68:C88"/>
@@ -40179,13 +40192,6 @@
     <mergeCell ref="C93:C98"/>
     <mergeCell ref="C99:C104"/>
     <mergeCell ref="C105:C138"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="C18:C28"/>
-    <mergeCell ref="C29:C41"/>
-    <mergeCell ref="C44:C53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -40231,7 +40237,7 @@
       <c r="B2" s="197" t="s">
         <v>344</v>
       </c>
-      <c r="C2" s="269" t="s">
+      <c r="C2" s="277" t="s">
         <v>561</v>
       </c>
       <c r="D2" s="159" t="s">
@@ -40245,7 +40251,7 @@
       <c r="B3" s="199" t="s">
         <v>345</v>
       </c>
-      <c r="C3" s="271"/>
+      <c r="C3" s="278"/>
       <c r="D3" s="162" t="s">
         <v>11</v>
       </c>
@@ -40257,7 +40263,7 @@
       <c r="B4" s="199" t="s">
         <v>346</v>
       </c>
-      <c r="C4" s="271"/>
+      <c r="C4" s="278"/>
       <c r="D4" s="162" t="s">
         <v>11</v>
       </c>
@@ -40269,7 +40275,7 @@
       <c r="B5" s="199" t="s">
         <v>347</v>
       </c>
-      <c r="C5" s="271"/>
+      <c r="C5" s="278"/>
       <c r="D5" s="162" t="s">
         <v>11</v>
       </c>
@@ -40281,7 +40287,7 @@
       <c r="B6" s="199" t="s">
         <v>348</v>
       </c>
-      <c r="C6" s="271"/>
+      <c r="C6" s="278"/>
       <c r="D6" s="162" t="s">
         <v>11</v>
       </c>
@@ -40293,7 +40299,7 @@
       <c r="B7" s="199" t="s">
         <v>349</v>
       </c>
-      <c r="C7" s="271"/>
+      <c r="C7" s="278"/>
       <c r="D7" s="162" t="s">
         <v>11</v>
       </c>
@@ -40305,7 +40311,7 @@
       <c r="B8" s="199" t="s">
         <v>350</v>
       </c>
-      <c r="C8" s="271"/>
+      <c r="C8" s="278"/>
       <c r="D8" s="162" t="s">
         <v>11</v>
       </c>
@@ -40317,7 +40323,7 @@
       <c r="B9" s="199" t="s">
         <v>351</v>
       </c>
-      <c r="C9" s="271"/>
+      <c r="C9" s="278"/>
       <c r="D9" s="162" t="s">
         <v>11</v>
       </c>
@@ -40329,7 +40335,7 @@
       <c r="B10" s="199" t="s">
         <v>352</v>
       </c>
-      <c r="C10" s="271"/>
+      <c r="C10" s="278"/>
       <c r="D10" s="162" t="s">
         <v>11</v>
       </c>
@@ -40341,7 +40347,7 @@
       <c r="B11" s="199" t="s">
         <v>353</v>
       </c>
-      <c r="C11" s="271"/>
+      <c r="C11" s="278"/>
       <c r="D11" s="162" t="s">
         <v>11</v>
       </c>
@@ -40353,7 +40359,7 @@
       <c r="B12" s="199" t="s">
         <v>354</v>
       </c>
-      <c r="C12" s="271"/>
+      <c r="C12" s="278"/>
       <c r="D12" s="162" t="s">
         <v>11</v>
       </c>
@@ -40365,7 +40371,7 @@
       <c r="B13" s="199" t="s">
         <v>355</v>
       </c>
-      <c r="C13" s="271"/>
+      <c r="C13" s="278"/>
       <c r="D13" s="162" t="s">
         <v>11</v>
       </c>
@@ -40377,7 +40383,7 @@
       <c r="B14" s="199" t="s">
         <v>356</v>
       </c>
-      <c r="C14" s="271"/>
+      <c r="C14" s="278"/>
       <c r="D14" s="162" t="s">
         <v>619</v>
       </c>
@@ -40389,7 +40395,7 @@
       <c r="B15" s="199" t="s">
         <v>357</v>
       </c>
-      <c r="C15" s="271"/>
+      <c r="C15" s="278"/>
       <c r="D15" s="162" t="s">
         <v>619</v>
       </c>
@@ -40401,7 +40407,7 @@
       <c r="B16" s="226" t="s">
         <v>479</v>
       </c>
-      <c r="C16" s="270"/>
+      <c r="C16" s="279"/>
       <c r="D16" s="165" t="s">
         <v>620</v>
       </c>
@@ -40413,7 +40419,7 @@
       <c r="B17" s="227" t="s">
         <v>358</v>
       </c>
-      <c r="C17" s="269" t="s">
+      <c r="C17" s="277" t="s">
         <v>621</v>
       </c>
       <c r="D17" s="159" t="s">
@@ -40427,7 +40433,7 @@
       <c r="B18" s="228" t="s">
         <v>359</v>
       </c>
-      <c r="C18" s="271"/>
+      <c r="C18" s="278"/>
       <c r="D18" s="162" t="s">
         <v>623</v>
       </c>
@@ -40439,7 +40445,7 @@
       <c r="B19" s="228" t="s">
         <v>360</v>
       </c>
-      <c r="C19" s="271"/>
+      <c r="C19" s="278"/>
       <c r="D19" s="162" t="s">
         <v>624</v>
       </c>
@@ -40451,7 +40457,7 @@
       <c r="B20" s="228" t="s">
         <v>361</v>
       </c>
-      <c r="C20" s="271"/>
+      <c r="C20" s="278"/>
       <c r="D20" s="162" t="s">
         <v>553</v>
       </c>
@@ -40463,7 +40469,7 @@
       <c r="B21" s="228" t="s">
         <v>362</v>
       </c>
-      <c r="C21" s="271"/>
+      <c r="C21" s="278"/>
       <c r="D21" s="162" t="s">
         <v>554</v>
       </c>
@@ -40475,7 +40481,7 @@
       <c r="B22" s="228" t="s">
         <v>363</v>
       </c>
-      <c r="C22" s="271"/>
+      <c r="C22" s="278"/>
       <c r="D22" s="162" t="s">
         <v>555</v>
       </c>
@@ -40487,7 +40493,7 @@
       <c r="B23" s="228" t="s">
         <v>364</v>
       </c>
-      <c r="C23" s="271"/>
+      <c r="C23" s="278"/>
       <c r="D23" s="162" t="s">
         <v>556</v>
       </c>
@@ -40499,7 +40505,7 @@
       <c r="B24" s="228" t="s">
         <v>365</v>
       </c>
-      <c r="C24" s="271"/>
+      <c r="C24" s="278"/>
       <c r="D24" s="162" t="s">
         <v>557</v>
       </c>
@@ -40511,7 +40517,7 @@
       <c r="B25" s="229" t="s">
         <v>366</v>
       </c>
-      <c r="C25" s="270"/>
+      <c r="C25" s="279"/>
       <c r="D25" s="165" t="s">
         <v>558</v>
       </c>
@@ -40523,7 +40529,7 @@
       <c r="B26" s="173" t="s">
         <v>367</v>
       </c>
-      <c r="C26" s="269" t="s">
+      <c r="C26" s="277" t="s">
         <v>625</v>
       </c>
       <c r="D26" s="159" t="s">
@@ -40537,7 +40543,7 @@
       <c r="B27" s="176" t="s">
         <v>368</v>
       </c>
-      <c r="C27" s="271"/>
+      <c r="C27" s="278"/>
       <c r="D27" s="162" t="s">
         <v>627</v>
       </c>
@@ -40549,7 +40555,7 @@
       <c r="B28" s="176" t="s">
         <v>369</v>
       </c>
-      <c r="C28" s="271"/>
+      <c r="C28" s="278"/>
       <c r="D28" s="162" t="s">
         <v>628</v>
       </c>
@@ -40561,7 +40567,7 @@
       <c r="B29" s="176" t="s">
         <v>370</v>
       </c>
-      <c r="C29" s="271"/>
+      <c r="C29" s="278"/>
       <c r="D29" s="162" t="s">
         <v>629</v>
       </c>
@@ -40573,7 +40579,7 @@
       <c r="B30" s="176" t="s">
         <v>371</v>
       </c>
-      <c r="C30" s="271"/>
+      <c r="C30" s="278"/>
       <c r="D30" s="162" t="s">
         <v>630</v>
       </c>
@@ -40585,7 +40591,7 @@
       <c r="B31" s="176" t="s">
         <v>372</v>
       </c>
-      <c r="C31" s="271"/>
+      <c r="C31" s="278"/>
       <c r="D31" s="162" t="s">
         <v>630</v>
       </c>
@@ -40597,7 +40603,7 @@
       <c r="B32" s="176" t="s">
         <v>373</v>
       </c>
-      <c r="C32" s="271"/>
+      <c r="C32" s="278"/>
       <c r="D32" s="162" t="s">
         <v>631</v>
       </c>
@@ -40609,7 +40615,7 @@
       <c r="B33" s="176" t="s">
         <v>374</v>
       </c>
-      <c r="C33" s="271"/>
+      <c r="C33" s="278"/>
       <c r="D33" s="162" t="s">
         <v>631</v>
       </c>
@@ -40621,7 +40627,7 @@
       <c r="B34" s="176" t="s">
         <v>375</v>
       </c>
-      <c r="C34" s="271"/>
+      <c r="C34" s="278"/>
       <c r="D34" s="162" t="s">
         <v>631</v>
       </c>
@@ -40633,7 +40639,7 @@
       <c r="B35" s="176" t="s">
         <v>376</v>
       </c>
-      <c r="C35" s="271"/>
+      <c r="C35" s="278"/>
       <c r="D35" s="162" t="s">
         <v>631</v>
       </c>
@@ -40645,7 +40651,7 @@
       <c r="B36" s="230" t="s">
         <v>377</v>
       </c>
-      <c r="C36" s="270"/>
+      <c r="C36" s="279"/>
       <c r="D36" s="162" t="s">
         <v>631</v>
       </c>
@@ -40657,7 +40663,7 @@
       <c r="B37" s="232" t="s">
         <v>481</v>
       </c>
-      <c r="C37" s="269" t="s">
+      <c r="C37" s="277" t="s">
         <v>632</v>
       </c>
       <c r="D37" s="186" t="s">
@@ -40671,7 +40677,7 @@
       <c r="B38" s="220" t="s">
         <v>482</v>
       </c>
-      <c r="C38" s="271"/>
+      <c r="C38" s="278"/>
       <c r="D38" s="177" t="s">
         <v>610</v>
       </c>
@@ -40683,7 +40689,7 @@
       <c r="B39" s="220" t="s">
         <v>483</v>
       </c>
-      <c r="C39" s="271"/>
+      <c r="C39" s="278"/>
       <c r="D39" s="177" t="s">
         <v>633</v>
       </c>
@@ -40695,7 +40701,7 @@
       <c r="B40" s="235" t="s">
         <v>484</v>
       </c>
-      <c r="C40" s="270"/>
+      <c r="C40" s="279"/>
       <c r="D40" s="182" t="s">
         <v>634</v>
       </c>
@@ -40713,15 +40719,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004FD8CECCB51EC843BF514AFE68379818" ma:contentTypeVersion="18" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="eda339f53f012ceb64677667a741b441">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="107e75b3-53cc-4838-92d2-ebc011bd4832" xmlns:ns3="888ccf44-0d39-41a2-ab17-f7efb2bf6977" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04a86f3db711706e561c315688f1c464" ns2:_="" ns3:_="">
     <xsd:import namespace="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
@@ -40970,6 +40967,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -40982,14 +40988,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F91B7B9-75FF-4624-B506-952B5B54766C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41004,6 +41002,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add posibility to include or exclude the generation of the Ideal signal in the results
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/prw_energinet_dk/Documents/Dokumenter/GitHub/MTB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="11_65313A6E4C5506009E52DA9B1CE17435CB52B360" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADAE1870-AFBD-4A5B-B92E-E02D13B5CF6A}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="11_65313A6E4C5506009E52DA9B1CE17435CB52B360" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C97A57C7-5E32-4B71-AAC0-EEDCD587FBCB}"/>
   <bookViews>
-    <workbookView xWindow="-16700" yWindow="-21710" windowWidth="51420" windowHeight="21100" tabRatio="822" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19335" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -3943,6 +3943,7 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3997,10 +3998,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4012,7 +4013,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -4576,8 +4576,8 @@
   </sheetPr>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4700,16 +4700,16 @@
         <v>435</v>
       </c>
       <c r="H7" s="144"/>
-      <c r="I7" s="260" t="s">
+      <c r="I7" s="261" t="s">
         <v>466</v>
       </c>
-      <c r="J7" s="260"/>
-      <c r="K7" s="260"/>
-      <c r="L7" s="260" t="s">
+      <c r="J7" s="261"/>
+      <c r="K7" s="261"/>
+      <c r="L7" s="261" t="s">
         <v>467</v>
       </c>
-      <c r="M7" s="260"/>
-      <c r="N7" s="261"/>
+      <c r="M7" s="261"/>
+      <c r="N7" s="262"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" s="27" t="s">
@@ -4752,7 +4752,7 @@
       <c r="C9" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="E9" s="283" t="s">
+      <c r="E9" s="260" t="s">
         <v>680</v>
       </c>
       <c r="H9" s="145"/>
@@ -5134,7 +5134,7 @@
       <c r="B2" s="237" t="s">
         <v>378</v>
       </c>
-      <c r="C2" s="277" t="s">
+      <c r="C2" s="278" t="s">
         <v>514</v>
       </c>
       <c r="D2" s="186" t="s">
@@ -5148,7 +5148,7 @@
       <c r="B3" s="239" t="s">
         <v>379</v>
       </c>
-      <c r="C3" s="278"/>
+      <c r="C3" s="280"/>
       <c r="D3" s="177" t="s">
         <v>11</v>
       </c>
@@ -5160,7 +5160,7 @@
       <c r="B4" s="239" t="s">
         <v>380</v>
       </c>
-      <c r="C4" s="278"/>
+      <c r="C4" s="280"/>
       <c r="D4" s="177" t="s">
         <v>11</v>
       </c>
@@ -5172,7 +5172,7 @@
       <c r="B5" s="239" t="s">
         <v>381</v>
       </c>
-      <c r="C5" s="278"/>
+      <c r="C5" s="280"/>
       <c r="D5" s="177" t="s">
         <v>11</v>
       </c>
@@ -5184,7 +5184,7 @@
       <c r="B6" s="239" t="s">
         <v>382</v>
       </c>
-      <c r="C6" s="278"/>
+      <c r="C6" s="280"/>
       <c r="D6" s="177" t="s">
         <v>11</v>
       </c>
@@ -5222,7 +5222,7 @@
       <c r="B9" s="173" t="s">
         <v>385</v>
       </c>
-      <c r="C9" s="280" t="s">
+      <c r="C9" s="281" t="s">
         <v>637</v>
       </c>
       <c r="D9" s="186" t="s">
@@ -5236,7 +5236,7 @@
       <c r="B10" s="230" t="s">
         <v>386</v>
       </c>
-      <c r="C10" s="281"/>
+      <c r="C10" s="282"/>
       <c r="D10" s="182" t="s">
         <v>639</v>
       </c>
@@ -5248,7 +5248,7 @@
       <c r="B11" s="227" t="s">
         <v>387</v>
       </c>
-      <c r="C11" s="277" t="s">
+      <c r="C11" s="278" t="s">
         <v>640</v>
       </c>
       <c r="D11" s="186" t="s">
@@ -5262,7 +5262,7 @@
       <c r="B12" s="228" t="s">
         <v>388</v>
       </c>
-      <c r="C12" s="278"/>
+      <c r="C12" s="280"/>
       <c r="D12" s="177" t="s">
         <v>642</v>
       </c>
@@ -5286,7 +5286,7 @@
       <c r="B14" s="197" t="s">
         <v>390</v>
       </c>
-      <c r="C14" s="280" t="s">
+      <c r="C14" s="281" t="s">
         <v>561</v>
       </c>
       <c r="D14" s="186" t="s">
@@ -5300,7 +5300,7 @@
       <c r="B15" s="199" t="s">
         <v>391</v>
       </c>
-      <c r="C15" s="282"/>
+      <c r="C15" s="283"/>
       <c r="D15" s="177" t="s">
         <v>11</v>
       </c>
@@ -5312,7 +5312,7 @@
       <c r="B16" s="199" t="s">
         <v>392</v>
       </c>
-      <c r="C16" s="282"/>
+      <c r="C16" s="283"/>
       <c r="D16" s="177" t="s">
         <v>11</v>
       </c>
@@ -5324,7 +5324,7 @@
       <c r="B17" s="199" t="s">
         <v>393</v>
       </c>
-      <c r="C17" s="282"/>
+      <c r="C17" s="283"/>
       <c r="D17" s="177" t="s">
         <v>11</v>
       </c>
@@ -5336,7 +5336,7 @@
       <c r="B18" s="199" t="s">
         <v>394</v>
       </c>
-      <c r="C18" s="282"/>
+      <c r="C18" s="283"/>
       <c r="D18" s="177" t="s">
         <v>11</v>
       </c>
@@ -5348,7 +5348,7 @@
       <c r="B19" s="199" t="s">
         <v>395</v>
       </c>
-      <c r="C19" s="282"/>
+      <c r="C19" s="283"/>
       <c r="D19" s="177" t="s">
         <v>11</v>
       </c>
@@ -5360,7 +5360,7 @@
       <c r="B20" s="199" t="s">
         <v>396</v>
       </c>
-      <c r="C20" s="282"/>
+      <c r="C20" s="283"/>
       <c r="D20" s="177" t="s">
         <v>11</v>
       </c>
@@ -5372,7 +5372,7 @@
       <c r="B21" s="199" t="s">
         <v>397</v>
       </c>
-      <c r="C21" s="282"/>
+      <c r="C21" s="283"/>
       <c r="D21" s="177" t="s">
         <v>11</v>
       </c>
@@ -5384,7 +5384,7 @@
       <c r="B22" s="199" t="s">
         <v>398</v>
       </c>
-      <c r="C22" s="282"/>
+      <c r="C22" s="283"/>
       <c r="D22" s="177" t="s">
         <v>11</v>
       </c>
@@ -5396,7 +5396,7 @@
       <c r="B23" s="199" t="s">
         <v>399</v>
       </c>
-      <c r="C23" s="282"/>
+      <c r="C23" s="283"/>
       <c r="D23" s="177" t="s">
         <v>11</v>
       </c>
@@ -5408,7 +5408,7 @@
       <c r="B24" s="199" t="s">
         <v>400</v>
       </c>
-      <c r="C24" s="282"/>
+      <c r="C24" s="283"/>
       <c r="D24" s="177" t="s">
         <v>11</v>
       </c>
@@ -5420,7 +5420,7 @@
       <c r="B25" s="199" t="s">
         <v>401</v>
       </c>
-      <c r="C25" s="282"/>
+      <c r="C25" s="283"/>
       <c r="D25" s="177" t="s">
         <v>11</v>
       </c>
@@ -5432,7 +5432,7 @@
       <c r="B26" s="199" t="s">
         <v>402</v>
       </c>
-      <c r="C26" s="282"/>
+      <c r="C26" s="283"/>
       <c r="D26" s="177" t="s">
         <v>564</v>
       </c>
@@ -5444,7 +5444,7 @@
       <c r="B27" s="199" t="s">
         <v>403</v>
       </c>
-      <c r="C27" s="282"/>
+      <c r="C27" s="283"/>
       <c r="D27" s="177" t="s">
         <v>565</v>
       </c>
@@ -5456,7 +5456,7 @@
       <c r="B28" s="199" t="s">
         <v>404</v>
       </c>
-      <c r="C28" s="282"/>
+      <c r="C28" s="283"/>
       <c r="D28" s="177" t="s">
         <v>566</v>
       </c>
@@ -5468,7 +5468,7 @@
       <c r="B29" s="199" t="s">
         <v>405</v>
       </c>
-      <c r="C29" s="282"/>
+      <c r="C29" s="283"/>
       <c r="D29" s="177" t="s">
         <v>567</v>
       </c>
@@ -5480,7 +5480,7 @@
       <c r="B30" s="199" t="s">
         <v>406</v>
       </c>
-      <c r="C30" s="282"/>
+      <c r="C30" s="283"/>
       <c r="D30" s="183" t="s">
         <v>645</v>
       </c>
@@ -5492,7 +5492,7 @@
       <c r="B31" s="199" t="s">
         <v>407</v>
       </c>
-      <c r="C31" s="282"/>
+      <c r="C31" s="283"/>
       <c r="D31" s="183" t="s">
         <v>645</v>
       </c>
@@ -5504,7 +5504,7 @@
       <c r="B32" s="199" t="s">
         <v>408</v>
       </c>
-      <c r="C32" s="282"/>
+      <c r="C32" s="283"/>
       <c r="D32" s="177" t="s">
         <v>595</v>
       </c>
@@ -5516,7 +5516,7 @@
       <c r="B33" s="199" t="s">
         <v>409</v>
       </c>
-      <c r="C33" s="282"/>
+      <c r="C33" s="283"/>
       <c r="D33" s="177" t="s">
         <v>595</v>
       </c>
@@ -5528,7 +5528,7 @@
       <c r="B34" s="199" t="s">
         <v>410</v>
       </c>
-      <c r="C34" s="282"/>
+      <c r="C34" s="283"/>
       <c r="D34" s="177" t="s">
         <v>568</v>
       </c>
@@ -5540,7 +5540,7 @@
       <c r="B35" s="199" t="s">
         <v>411</v>
       </c>
-      <c r="C35" s="282"/>
+      <c r="C35" s="283"/>
       <c r="D35" s="177" t="s">
         <v>569</v>
       </c>
@@ -5552,7 +5552,7 @@
       <c r="B36" s="199" t="s">
         <v>412</v>
       </c>
-      <c r="C36" s="282"/>
+      <c r="C36" s="283"/>
       <c r="D36" s="177" t="s">
         <v>646</v>
       </c>
@@ -5564,7 +5564,7 @@
       <c r="B37" s="226" t="s">
         <v>487</v>
       </c>
-      <c r="C37" s="281"/>
+      <c r="C37" s="282"/>
       <c r="D37" s="177" t="s">
         <v>647</v>
       </c>
@@ -5576,7 +5576,7 @@
       <c r="B38" s="227" t="s">
         <v>413</v>
       </c>
-      <c r="C38" s="277" t="s">
+      <c r="C38" s="278" t="s">
         <v>640</v>
       </c>
       <c r="D38" s="186" t="s">
@@ -5590,7 +5590,7 @@
       <c r="B39" s="228" t="s">
         <v>414</v>
       </c>
-      <c r="C39" s="278"/>
+      <c r="C39" s="280"/>
       <c r="D39" s="177" t="s">
         <v>554</v>
       </c>
@@ -5602,7 +5602,7 @@
       <c r="B40" s="228" t="s">
         <v>415</v>
       </c>
-      <c r="C40" s="278"/>
+      <c r="C40" s="280"/>
       <c r="D40" s="177" t="s">
         <v>557</v>
       </c>
@@ -5626,7 +5626,7 @@
       <c r="B42" s="232" t="s">
         <v>461</v>
       </c>
-      <c r="C42" s="277" t="s">
+      <c r="C42" s="278" t="s">
         <v>648</v>
       </c>
       <c r="D42" s="186" t="s">
@@ -5640,7 +5640,7 @@
       <c r="B43" s="220" t="s">
         <v>462</v>
       </c>
-      <c r="C43" s="278"/>
+      <c r="C43" s="280"/>
       <c r="D43" s="177" t="s">
         <v>650</v>
       </c>
@@ -5652,7 +5652,7 @@
       <c r="B44" s="220" t="s">
         <v>417</v>
       </c>
-      <c r="C44" s="278"/>
+      <c r="C44" s="280"/>
       <c r="D44" s="177" t="s">
         <v>651</v>
       </c>
@@ -5664,7 +5664,7 @@
       <c r="B45" s="220" t="s">
         <v>418</v>
       </c>
-      <c r="C45" s="278"/>
+      <c r="C45" s="280"/>
       <c r="D45" s="177" t="s">
         <v>11</v>
       </c>
@@ -5676,7 +5676,7 @@
       <c r="B46" s="220" t="s">
         <v>419</v>
       </c>
-      <c r="C46" s="278"/>
+      <c r="C46" s="280"/>
       <c r="D46" s="177" t="s">
         <v>11</v>
       </c>
@@ -5688,7 +5688,7 @@
       <c r="B47" s="220" t="s">
         <v>420</v>
       </c>
-      <c r="C47" s="278"/>
+      <c r="C47" s="280"/>
       <c r="D47" s="177" t="s">
         <v>11</v>
       </c>
@@ -5700,7 +5700,7 @@
       <c r="B48" s="220" t="s">
         <v>452</v>
       </c>
-      <c r="C48" s="278"/>
+      <c r="C48" s="280"/>
       <c r="D48" s="177" t="s">
         <v>609</v>
       </c>
@@ -5712,7 +5712,7 @@
       <c r="B49" s="220" t="s">
         <v>453</v>
       </c>
-      <c r="C49" s="278"/>
+      <c r="C49" s="280"/>
       <c r="D49" s="177" t="s">
         <v>610</v>
       </c>
@@ -5724,7 +5724,7 @@
       <c r="B50" s="220" t="s">
         <v>485</v>
       </c>
-      <c r="C50" s="278"/>
+      <c r="C50" s="280"/>
       <c r="D50" s="177" t="s">
         <v>633</v>
       </c>
@@ -5736,7 +5736,7 @@
       <c r="B51" s="220" t="s">
         <v>486</v>
       </c>
-      <c r="C51" s="278"/>
+      <c r="C51" s="280"/>
       <c r="D51" s="177" t="s">
         <v>634</v>
       </c>
@@ -5748,7 +5748,7 @@
       <c r="B52" s="220" t="s">
         <v>460</v>
       </c>
-      <c r="C52" s="278"/>
+      <c r="C52" s="280"/>
       <c r="D52" s="177" t="s">
         <v>611</v>
       </c>
@@ -5760,7 +5760,7 @@
       <c r="B53" s="220" t="s">
         <v>456</v>
       </c>
-      <c r="C53" s="278"/>
+      <c r="C53" s="280"/>
       <c r="D53" s="177" t="s">
         <v>11</v>
       </c>
@@ -5772,7 +5772,7 @@
       <c r="B54" s="220" t="s">
         <v>457</v>
       </c>
-      <c r="C54" s="278"/>
+      <c r="C54" s="280"/>
       <c r="D54" s="177" t="s">
         <v>11</v>
       </c>
@@ -5784,7 +5784,7 @@
       <c r="B55" s="220" t="s">
         <v>459</v>
       </c>
-      <c r="C55" s="278"/>
+      <c r="C55" s="280"/>
       <c r="D55" s="177" t="s">
         <v>11</v>
       </c>
@@ -5796,7 +5796,7 @@
       <c r="B56" s="220" t="s">
         <v>458</v>
       </c>
-      <c r="C56" s="278"/>
+      <c r="C56" s="280"/>
       <c r="D56" s="177" t="s">
         <v>11</v>
       </c>
@@ -5808,7 +5808,7 @@
       <c r="B57" s="220" t="s">
         <v>421</v>
       </c>
-      <c r="C57" s="278"/>
+      <c r="C57" s="280"/>
       <c r="D57" s="177" t="s">
         <v>612</v>
       </c>
@@ -5820,7 +5820,7 @@
       <c r="B58" s="220" t="s">
         <v>422</v>
       </c>
-      <c r="C58" s="278"/>
+      <c r="C58" s="280"/>
       <c r="D58" s="177" t="s">
         <v>613</v>
       </c>
@@ -5832,7 +5832,7 @@
       <c r="B59" s="220" t="s">
         <v>423</v>
       </c>
-      <c r="C59" s="278"/>
+      <c r="C59" s="280"/>
       <c r="D59" s="177" t="s">
         <v>614</v>
       </c>
@@ -6015,16 +6015,16 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="48"/>
-      <c r="B1" s="262" t="s">
+      <c r="B1" s="263" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="263"/>
-      <c r="D1" s="264"/>
-      <c r="E1" s="262" t="s">
+      <c r="C1" s="264"/>
+      <c r="D1" s="265"/>
+      <c r="E1" s="263" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="263"/>
-      <c r="G1" s="263"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
       <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
@@ -7001,15 +7001,15 @@
   </sheetPr>
   <dimension ref="A1:CN196"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:L1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="3" width="12.69140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.69140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.3828125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.69140625" style="1" customWidth="1"/>
     <col min="7" max="9" width="12.69140625" style="1" customWidth="1"/>
     <col min="10" max="11" width="10.69140625" style="1" customWidth="1"/>
@@ -7066,94 +7066,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.4">
-      <c r="A1" s="265" t="s">
+      <c r="A1" s="266" t="s">
         <v>678</v>
       </c>
-      <c r="B1" s="265"/>
-      <c r="C1" s="265"/>
-      <c r="D1" s="265"/>
-      <c r="E1" s="266" t="s">
+      <c r="B1" s="266"/>
+      <c r="C1" s="266"/>
+      <c r="D1" s="266"/>
+      <c r="E1" s="267" t="s">
         <v>679</v>
       </c>
-      <c r="F1" s="267"/>
-      <c r="G1" s="267"/>
-      <c r="H1" s="267"/>
-      <c r="I1" s="267"/>
-      <c r="J1" s="267"/>
-      <c r="K1" s="267"/>
-      <c r="L1" s="268"/>
-      <c r="M1" s="269" t="s">
+      <c r="F1" s="268"/>
+      <c r="G1" s="268"/>
+      <c r="H1" s="268"/>
+      <c r="I1" s="268"/>
+      <c r="J1" s="268"/>
+      <c r="K1" s="268"/>
+      <c r="L1" s="269"/>
+      <c r="M1" s="270" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="269"/>
-      <c r="O1" s="269"/>
-      <c r="P1" s="269"/>
-      <c r="Q1" s="265" t="s">
+      <c r="N1" s="270"/>
+      <c r="O1" s="270"/>
+      <c r="P1" s="270"/>
+      <c r="Q1" s="266" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="265"/>
-      <c r="S1" s="265"/>
-      <c r="T1" s="265"/>
-      <c r="U1" s="269" t="s">
+      <c r="R1" s="266"/>
+      <c r="S1" s="266"/>
+      <c r="T1" s="266"/>
+      <c r="U1" s="270" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="269"/>
-      <c r="W1" s="269"/>
-      <c r="X1" s="269"/>
-      <c r="Y1" s="265" t="s">
+      <c r="V1" s="270"/>
+      <c r="W1" s="270"/>
+      <c r="X1" s="270"/>
+      <c r="Y1" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" s="265"/>
-      <c r="AA1" s="265"/>
-      <c r="AB1" s="265"/>
-      <c r="AC1" s="269" t="s">
+      <c r="Z1" s="266"/>
+      <c r="AA1" s="266"/>
+      <c r="AB1" s="266"/>
+      <c r="AC1" s="270" t="s">
         <v>83</v>
       </c>
-      <c r="AD1" s="269"/>
-      <c r="AE1" s="269"/>
-      <c r="AF1" s="269"/>
-      <c r="AG1" s="265" t="s">
+      <c r="AD1" s="270"/>
+      <c r="AE1" s="270"/>
+      <c r="AF1" s="270"/>
+      <c r="AG1" s="266" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="265"/>
-      <c r="AI1" s="265"/>
-      <c r="AJ1" s="265"/>
-      <c r="AK1" s="269" t="s">
+      <c r="AH1" s="266"/>
+      <c r="AI1" s="266"/>
+      <c r="AJ1" s="266"/>
+      <c r="AK1" s="270" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="269"/>
-      <c r="AM1" s="269"/>
-      <c r="AN1" s="269"/>
-      <c r="AO1" s="265" t="s">
+      <c r="AL1" s="270"/>
+      <c r="AM1" s="270"/>
+      <c r="AN1" s="270"/>
+      <c r="AO1" s="266" t="s">
         <v>86</v>
       </c>
-      <c r="AP1" s="265"/>
-      <c r="AQ1" s="265"/>
-      <c r="AR1" s="265"/>
-      <c r="AS1" s="269" t="s">
+      <c r="AP1" s="266"/>
+      <c r="AQ1" s="266"/>
+      <c r="AR1" s="266"/>
+      <c r="AS1" s="270" t="s">
         <v>87</v>
       </c>
-      <c r="AT1" s="269"/>
-      <c r="AU1" s="269"/>
-      <c r="AV1" s="269"/>
-      <c r="AW1" s="265" t="s">
+      <c r="AT1" s="270"/>
+      <c r="AU1" s="270"/>
+      <c r="AV1" s="270"/>
+      <c r="AW1" s="266" t="s">
         <v>88</v>
       </c>
-      <c r="AX1" s="265"/>
-      <c r="AY1" s="265"/>
-      <c r="AZ1" s="265"/>
-      <c r="BA1" s="269" t="s">
+      <c r="AX1" s="266"/>
+      <c r="AY1" s="266"/>
+      <c r="AZ1" s="266"/>
+      <c r="BA1" s="270" t="s">
         <v>89</v>
       </c>
-      <c r="BB1" s="269"/>
-      <c r="BC1" s="269"/>
-      <c r="BD1" s="269"/>
-      <c r="BE1" s="265" t="s">
+      <c r="BB1" s="270"/>
+      <c r="BC1" s="270"/>
+      <c r="BD1" s="270"/>
+      <c r="BE1" s="266" t="s">
         <v>90</v>
       </c>
-      <c r="BF1" s="265"/>
-      <c r="BG1" s="265"/>
-      <c r="BH1" s="265"/>
+      <c r="BF1" s="266"/>
+      <c r="BG1" s="266"/>
+      <c r="BH1" s="266"/>
     </row>
     <row r="2" spans="1:60" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -24323,7 +24323,7 @@
   </sheetPr>
   <dimension ref="A1:CN171"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="BE1" sqref="BE1:BH1"/>
     </sheetView>
@@ -24388,94 +24388,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:92" x14ac:dyDescent="0.4">
-      <c r="A1" s="265" t="s">
+      <c r="A1" s="266" t="s">
         <v>678</v>
       </c>
-      <c r="B1" s="265"/>
-      <c r="C1" s="265"/>
-      <c r="D1" s="265"/>
-      <c r="E1" s="266" t="s">
+      <c r="B1" s="266"/>
+      <c r="C1" s="266"/>
+      <c r="D1" s="266"/>
+      <c r="E1" s="267" t="s">
         <v>679</v>
       </c>
-      <c r="F1" s="267"/>
-      <c r="G1" s="267"/>
-      <c r="H1" s="267"/>
-      <c r="I1" s="267"/>
-      <c r="J1" s="267"/>
-      <c r="K1" s="267"/>
-      <c r="L1" s="268"/>
-      <c r="M1" s="273" t="s">
+      <c r="F1" s="268"/>
+      <c r="G1" s="268"/>
+      <c r="H1" s="268"/>
+      <c r="I1" s="268"/>
+      <c r="J1" s="268"/>
+      <c r="K1" s="268"/>
+      <c r="L1" s="269"/>
+      <c r="M1" s="274" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="274"/>
-      <c r="O1" s="274"/>
-      <c r="P1" s="275"/>
-      <c r="Q1" s="266" t="s">
+      <c r="N1" s="275"/>
+      <c r="O1" s="275"/>
+      <c r="P1" s="276"/>
+      <c r="Q1" s="267" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="267"/>
-      <c r="S1" s="267"/>
-      <c r="T1" s="267"/>
-      <c r="U1" s="273" t="s">
+      <c r="R1" s="268"/>
+      <c r="S1" s="268"/>
+      <c r="T1" s="268"/>
+      <c r="U1" s="274" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="274"/>
-      <c r="W1" s="274"/>
-      <c r="X1" s="275"/>
-      <c r="Y1" s="270" t="s">
+      <c r="V1" s="275"/>
+      <c r="W1" s="275"/>
+      <c r="X1" s="276"/>
+      <c r="Y1" s="271" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" s="271"/>
-      <c r="AA1" s="271"/>
-      <c r="AB1" s="272"/>
-      <c r="AC1" s="273" t="s">
+      <c r="Z1" s="272"/>
+      <c r="AA1" s="272"/>
+      <c r="AB1" s="273"/>
+      <c r="AC1" s="274" t="s">
         <v>83</v>
       </c>
-      <c r="AD1" s="274"/>
-      <c r="AE1" s="274"/>
-      <c r="AF1" s="275"/>
-      <c r="AG1" s="270" t="s">
+      <c r="AD1" s="275"/>
+      <c r="AE1" s="275"/>
+      <c r="AF1" s="276"/>
+      <c r="AG1" s="271" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="271"/>
-      <c r="AI1" s="271"/>
-      <c r="AJ1" s="272"/>
-      <c r="AK1" s="273" t="s">
+      <c r="AH1" s="272"/>
+      <c r="AI1" s="272"/>
+      <c r="AJ1" s="273"/>
+      <c r="AK1" s="274" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="274"/>
-      <c r="AM1" s="274"/>
-      <c r="AN1" s="275"/>
-      <c r="AO1" s="270" t="s">
+      <c r="AL1" s="275"/>
+      <c r="AM1" s="275"/>
+      <c r="AN1" s="276"/>
+      <c r="AO1" s="271" t="s">
         <v>86</v>
       </c>
-      <c r="AP1" s="271"/>
-      <c r="AQ1" s="271"/>
-      <c r="AR1" s="272"/>
-      <c r="AS1" s="273" t="s">
+      <c r="AP1" s="272"/>
+      <c r="AQ1" s="272"/>
+      <c r="AR1" s="273"/>
+      <c r="AS1" s="274" t="s">
         <v>87</v>
       </c>
-      <c r="AT1" s="274"/>
-      <c r="AU1" s="274"/>
-      <c r="AV1" s="275"/>
-      <c r="AW1" s="270" t="s">
+      <c r="AT1" s="275"/>
+      <c r="AU1" s="275"/>
+      <c r="AV1" s="276"/>
+      <c r="AW1" s="271" t="s">
         <v>88</v>
       </c>
-      <c r="AX1" s="271"/>
-      <c r="AY1" s="271"/>
-      <c r="AZ1" s="272"/>
-      <c r="BA1" s="273" t="s">
+      <c r="AX1" s="272"/>
+      <c r="AY1" s="272"/>
+      <c r="AZ1" s="273"/>
+      <c r="BA1" s="274" t="s">
         <v>89</v>
       </c>
-      <c r="BB1" s="274"/>
-      <c r="BC1" s="274"/>
-      <c r="BD1" s="275"/>
-      <c r="BE1" s="270" t="s">
+      <c r="BB1" s="275"/>
+      <c r="BC1" s="275"/>
+      <c r="BD1" s="276"/>
+      <c r="BE1" s="271" t="s">
         <v>90</v>
       </c>
-      <c r="BF1" s="271"/>
-      <c r="BG1" s="271"/>
-      <c r="BH1" s="272"/>
+      <c r="BF1" s="272"/>
+      <c r="BG1" s="272"/>
+      <c r="BH1" s="273"/>
     </row>
     <row r="2" spans="1:92" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -29612,7 +29612,7 @@
   </sheetPr>
   <dimension ref="A1:BH62"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="BH2" sqref="BH1:BH1048576"/>
     </sheetView>
@@ -29677,94 +29677,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.4">
-      <c r="A1" s="265" t="s">
+      <c r="A1" s="266" t="s">
         <v>678</v>
       </c>
-      <c r="B1" s="265"/>
-      <c r="C1" s="265"/>
-      <c r="D1" s="265"/>
-      <c r="E1" s="266" t="s">
+      <c r="B1" s="266"/>
+      <c r="C1" s="266"/>
+      <c r="D1" s="266"/>
+      <c r="E1" s="267" t="s">
         <v>679</v>
       </c>
-      <c r="F1" s="267"/>
-      <c r="G1" s="267"/>
-      <c r="H1" s="267"/>
-      <c r="I1" s="267"/>
-      <c r="J1" s="267"/>
-      <c r="K1" s="267"/>
-      <c r="L1" s="268"/>
-      <c r="M1" s="276" t="s">
+      <c r="F1" s="268"/>
+      <c r="G1" s="268"/>
+      <c r="H1" s="268"/>
+      <c r="I1" s="268"/>
+      <c r="J1" s="268"/>
+      <c r="K1" s="268"/>
+      <c r="L1" s="269"/>
+      <c r="M1" s="277" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="276"/>
-      <c r="O1" s="276"/>
-      <c r="P1" s="276"/>
-      <c r="Q1" s="265" t="s">
+      <c r="N1" s="277"/>
+      <c r="O1" s="277"/>
+      <c r="P1" s="277"/>
+      <c r="Q1" s="266" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="265"/>
-      <c r="S1" s="265"/>
-      <c r="T1" s="265"/>
-      <c r="U1" s="276" t="s">
+      <c r="R1" s="266"/>
+      <c r="S1" s="266"/>
+      <c r="T1" s="266"/>
+      <c r="U1" s="277" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="276"/>
-      <c r="W1" s="276"/>
-      <c r="X1" s="276"/>
-      <c r="Y1" s="265" t="s">
+      <c r="V1" s="277"/>
+      <c r="W1" s="277"/>
+      <c r="X1" s="277"/>
+      <c r="Y1" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" s="265"/>
-      <c r="AA1" s="265"/>
-      <c r="AB1" s="265"/>
-      <c r="AC1" s="276" t="s">
+      <c r="Z1" s="266"/>
+      <c r="AA1" s="266"/>
+      <c r="AB1" s="266"/>
+      <c r="AC1" s="277" t="s">
         <v>83</v>
       </c>
-      <c r="AD1" s="276"/>
-      <c r="AE1" s="276"/>
-      <c r="AF1" s="276"/>
-      <c r="AG1" s="265" t="s">
+      <c r="AD1" s="277"/>
+      <c r="AE1" s="277"/>
+      <c r="AF1" s="277"/>
+      <c r="AG1" s="266" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="265"/>
-      <c r="AI1" s="265"/>
-      <c r="AJ1" s="265"/>
-      <c r="AK1" s="276" t="s">
+      <c r="AH1" s="266"/>
+      <c r="AI1" s="266"/>
+      <c r="AJ1" s="266"/>
+      <c r="AK1" s="277" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="276"/>
-      <c r="AM1" s="276"/>
-      <c r="AN1" s="276"/>
-      <c r="AO1" s="265" t="s">
+      <c r="AL1" s="277"/>
+      <c r="AM1" s="277"/>
+      <c r="AN1" s="277"/>
+      <c r="AO1" s="266" t="s">
         <v>86</v>
       </c>
-      <c r="AP1" s="265"/>
-      <c r="AQ1" s="265"/>
-      <c r="AR1" s="265"/>
-      <c r="AS1" s="276" t="s">
+      <c r="AP1" s="266"/>
+      <c r="AQ1" s="266"/>
+      <c r="AR1" s="266"/>
+      <c r="AS1" s="277" t="s">
         <v>87</v>
       </c>
-      <c r="AT1" s="276"/>
-      <c r="AU1" s="276"/>
-      <c r="AV1" s="276"/>
-      <c r="AW1" s="265" t="s">
+      <c r="AT1" s="277"/>
+      <c r="AU1" s="277"/>
+      <c r="AV1" s="277"/>
+      <c r="AW1" s="266" t="s">
         <v>88</v>
       </c>
-      <c r="AX1" s="265"/>
-      <c r="AY1" s="265"/>
-      <c r="AZ1" s="265"/>
-      <c r="BA1" s="276" t="s">
+      <c r="AX1" s="266"/>
+      <c r="AY1" s="266"/>
+      <c r="AZ1" s="266"/>
+      <c r="BA1" s="277" t="s">
         <v>89</v>
       </c>
-      <c r="BB1" s="276"/>
-      <c r="BC1" s="276"/>
-      <c r="BD1" s="276"/>
-      <c r="BE1" s="265" t="s">
+      <c r="BB1" s="277"/>
+      <c r="BC1" s="277"/>
+      <c r="BD1" s="277"/>
+      <c r="BE1" s="266" t="s">
         <v>90</v>
       </c>
-      <c r="BF1" s="265"/>
-      <c r="BG1" s="265"/>
-      <c r="BH1" s="265"/>
+      <c r="BF1" s="266"/>
+      <c r="BG1" s="266"/>
+      <c r="BH1" s="266"/>
     </row>
     <row r="2" spans="1:60" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -36359,94 +36359,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.4">
-      <c r="A1" s="265" t="s">
+      <c r="A1" s="266" t="s">
         <v>678</v>
       </c>
-      <c r="B1" s="265"/>
-      <c r="C1" s="265"/>
-      <c r="D1" s="265"/>
-      <c r="E1" s="266" t="s">
+      <c r="B1" s="266"/>
+      <c r="C1" s="266"/>
+      <c r="D1" s="266"/>
+      <c r="E1" s="267" t="s">
         <v>679</v>
       </c>
-      <c r="F1" s="267"/>
-      <c r="G1" s="267"/>
-      <c r="H1" s="267"/>
-      <c r="I1" s="267"/>
-      <c r="J1" s="267"/>
-      <c r="K1" s="267"/>
-      <c r="L1" s="268"/>
-      <c r="M1" s="276" t="s">
+      <c r="F1" s="268"/>
+      <c r="G1" s="268"/>
+      <c r="H1" s="268"/>
+      <c r="I1" s="268"/>
+      <c r="J1" s="268"/>
+      <c r="K1" s="268"/>
+      <c r="L1" s="269"/>
+      <c r="M1" s="277" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="276"/>
-      <c r="O1" s="276"/>
-      <c r="P1" s="276"/>
-      <c r="Q1" s="266" t="s">
+      <c r="N1" s="277"/>
+      <c r="O1" s="277"/>
+      <c r="P1" s="277"/>
+      <c r="Q1" s="267" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="267"/>
-      <c r="S1" s="267"/>
-      <c r="T1" s="267"/>
-      <c r="U1" s="276" t="s">
+      <c r="R1" s="268"/>
+      <c r="S1" s="268"/>
+      <c r="T1" s="268"/>
+      <c r="U1" s="277" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="276"/>
-      <c r="W1" s="276"/>
-      <c r="X1" s="276"/>
-      <c r="Y1" s="266" t="s">
+      <c r="V1" s="277"/>
+      <c r="W1" s="277"/>
+      <c r="X1" s="277"/>
+      <c r="Y1" s="267" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" s="267"/>
-      <c r="AA1" s="267"/>
-      <c r="AB1" s="267"/>
-      <c r="AC1" s="276" t="s">
+      <c r="Z1" s="268"/>
+      <c r="AA1" s="268"/>
+      <c r="AB1" s="268"/>
+      <c r="AC1" s="277" t="s">
         <v>83</v>
       </c>
-      <c r="AD1" s="276"/>
-      <c r="AE1" s="276"/>
-      <c r="AF1" s="276"/>
-      <c r="AG1" s="266" t="s">
+      <c r="AD1" s="277"/>
+      <c r="AE1" s="277"/>
+      <c r="AF1" s="277"/>
+      <c r="AG1" s="267" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="267"/>
-      <c r="AI1" s="267"/>
-      <c r="AJ1" s="267"/>
-      <c r="AK1" s="276" t="s">
+      <c r="AH1" s="268"/>
+      <c r="AI1" s="268"/>
+      <c r="AJ1" s="268"/>
+      <c r="AK1" s="277" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="276"/>
-      <c r="AM1" s="276"/>
-      <c r="AN1" s="276"/>
-      <c r="AO1" s="266" t="s">
+      <c r="AL1" s="277"/>
+      <c r="AM1" s="277"/>
+      <c r="AN1" s="277"/>
+      <c r="AO1" s="267" t="s">
         <v>86</v>
       </c>
-      <c r="AP1" s="267"/>
-      <c r="AQ1" s="267"/>
-      <c r="AR1" s="267"/>
-      <c r="AS1" s="276" t="s">
+      <c r="AP1" s="268"/>
+      <c r="AQ1" s="268"/>
+      <c r="AR1" s="268"/>
+      <c r="AS1" s="277" t="s">
         <v>87</v>
       </c>
-      <c r="AT1" s="276"/>
-      <c r="AU1" s="276"/>
-      <c r="AV1" s="276"/>
-      <c r="AW1" s="266" t="s">
+      <c r="AT1" s="277"/>
+      <c r="AU1" s="277"/>
+      <c r="AV1" s="277"/>
+      <c r="AW1" s="267" t="s">
         <v>88</v>
       </c>
-      <c r="AX1" s="267"/>
-      <c r="AY1" s="267"/>
-      <c r="AZ1" s="267"/>
-      <c r="BA1" s="276" t="s">
+      <c r="AX1" s="268"/>
+      <c r="AY1" s="268"/>
+      <c r="AZ1" s="268"/>
+      <c r="BA1" s="277" t="s">
         <v>89</v>
       </c>
-      <c r="BB1" s="276"/>
-      <c r="BC1" s="276"/>
-      <c r="BD1" s="276"/>
-      <c r="BE1" s="266" t="s">
+      <c r="BB1" s="277"/>
+      <c r="BC1" s="277"/>
+      <c r="BD1" s="277"/>
+      <c r="BE1" s="267" t="s">
         <v>90</v>
       </c>
-      <c r="BF1" s="267"/>
-      <c r="BG1" s="267"/>
-      <c r="BH1" s="267"/>
+      <c r="BF1" s="268"/>
+      <c r="BG1" s="268"/>
+      <c r="BH1" s="268"/>
     </row>
     <row r="2" spans="1:60" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -38327,7 +38327,7 @@
       <c r="B2" s="158" t="s">
         <v>493</v>
       </c>
-      <c r="C2" s="277" t="s">
+      <c r="C2" s="278" t="s">
         <v>514</v>
       </c>
       <c r="D2" s="159" t="s">
@@ -38341,7 +38341,7 @@
       <c r="B3" s="161" t="s">
         <v>494</v>
       </c>
-      <c r="C3" s="278"/>
+      <c r="C3" s="280"/>
       <c r="D3" s="162" t="s">
         <v>516</v>
       </c>
@@ -38353,7 +38353,7 @@
       <c r="B4" s="161" t="s">
         <v>495</v>
       </c>
-      <c r="C4" s="278"/>
+      <c r="C4" s="280"/>
       <c r="D4" s="162" t="s">
         <v>11</v>
       </c>
@@ -38365,7 +38365,7 @@
       <c r="B5" s="161" t="s">
         <v>496</v>
       </c>
-      <c r="C5" s="278"/>
+      <c r="C5" s="280"/>
       <c r="D5" s="162" t="s">
         <v>11</v>
       </c>
@@ -38377,7 +38377,7 @@
       <c r="B6" s="161" t="s">
         <v>497</v>
       </c>
-      <c r="C6" s="278"/>
+      <c r="C6" s="280"/>
       <c r="D6" s="162" t="s">
         <v>11</v>
       </c>
@@ -38389,7 +38389,7 @@
       <c r="B7" s="161" t="s">
         <v>498</v>
       </c>
-      <c r="C7" s="278"/>
+      <c r="C7" s="280"/>
       <c r="D7" s="162" t="s">
         <v>11</v>
       </c>
@@ -38401,7 +38401,7 @@
       <c r="B8" s="161" t="s">
         <v>499</v>
       </c>
-      <c r="C8" s="278"/>
+      <c r="C8" s="280"/>
       <c r="D8" s="162" t="s">
         <v>11</v>
       </c>
@@ -38413,7 +38413,7 @@
       <c r="B9" s="161" t="s">
         <v>500</v>
       </c>
-      <c r="C9" s="278"/>
+      <c r="C9" s="280"/>
       <c r="D9" s="162" t="s">
         <v>11</v>
       </c>
@@ -38425,7 +38425,7 @@
       <c r="B10" s="161" t="s">
         <v>501</v>
       </c>
-      <c r="C10" s="278"/>
+      <c r="C10" s="280"/>
       <c r="D10" s="162" t="s">
         <v>11</v>
       </c>
@@ -38449,7 +38449,7 @@
       <c r="B12" s="166" t="s">
         <v>240</v>
       </c>
-      <c r="C12" s="277" t="s">
+      <c r="C12" s="278" t="s">
         <v>517</v>
       </c>
       <c r="D12" s="159" t="s">
@@ -38463,7 +38463,7 @@
       <c r="B13" s="167" t="s">
         <v>241</v>
       </c>
-      <c r="C13" s="278"/>
+      <c r="C13" s="280"/>
       <c r="D13" s="162" t="s">
         <v>519</v>
       </c>
@@ -38475,7 +38475,7 @@
       <c r="B14" s="167" t="s">
         <v>242</v>
       </c>
-      <c r="C14" s="278"/>
+      <c r="C14" s="280"/>
       <c r="D14" s="162" t="s">
         <v>11</v>
       </c>
@@ -38487,7 +38487,7 @@
       <c r="B15" s="167" t="s">
         <v>243</v>
       </c>
-      <c r="C15" s="278"/>
+      <c r="C15" s="280"/>
       <c r="D15" s="162" t="s">
         <v>11</v>
       </c>
@@ -38499,7 +38499,7 @@
       <c r="B16" s="167" t="s">
         <v>244</v>
       </c>
-      <c r="C16" s="278"/>
+      <c r="C16" s="280"/>
       <c r="D16" s="162" t="s">
         <v>11</v>
       </c>
@@ -38523,7 +38523,7 @@
       <c r="B18" s="169" t="s">
         <v>246</v>
       </c>
-      <c r="C18" s="277" t="s">
+      <c r="C18" s="278" t="s">
         <v>109</v>
       </c>
       <c r="D18" s="159" t="s">
@@ -38537,7 +38537,7 @@
       <c r="B19" s="171" t="s">
         <v>247</v>
       </c>
-      <c r="C19" s="278"/>
+      <c r="C19" s="280"/>
       <c r="D19" s="162" t="s">
         <v>521</v>
       </c>
@@ -38549,7 +38549,7 @@
       <c r="B20" s="170" t="s">
         <v>248</v>
       </c>
-      <c r="C20" s="278"/>
+      <c r="C20" s="280"/>
       <c r="D20" s="162" t="s">
         <v>522</v>
       </c>
@@ -38561,7 +38561,7 @@
       <c r="B21" s="170" t="s">
         <v>249</v>
       </c>
-      <c r="C21" s="278"/>
+      <c r="C21" s="280"/>
       <c r="D21" s="162" t="s">
         <v>523</v>
       </c>
@@ -38573,7 +38573,7 @@
       <c r="B22" s="170" t="s">
         <v>250</v>
       </c>
-      <c r="C22" s="278"/>
+      <c r="C22" s="280"/>
       <c r="D22" s="162" t="s">
         <v>524</v>
       </c>
@@ -38585,7 +38585,7 @@
       <c r="B23" s="170" t="s">
         <v>251</v>
       </c>
-      <c r="C23" s="278"/>
+      <c r="C23" s="280"/>
       <c r="D23" s="162" t="s">
         <v>525</v>
       </c>
@@ -38597,7 +38597,7 @@
       <c r="B24" s="170" t="s">
         <v>491</v>
       </c>
-      <c r="C24" s="278"/>
+      <c r="C24" s="280"/>
       <c r="D24" s="162" t="s">
         <v>11</v>
       </c>
@@ -38609,7 +38609,7 @@
       <c r="B25" s="170" t="s">
         <v>492</v>
       </c>
-      <c r="C25" s="278"/>
+      <c r="C25" s="280"/>
       <c r="D25" s="162" t="s">
         <v>526</v>
       </c>
@@ -38621,7 +38621,7 @@
       <c r="B26" s="170" t="s">
         <v>252</v>
       </c>
-      <c r="C26" s="278"/>
+      <c r="C26" s="280"/>
       <c r="D26" s="162" t="s">
         <v>11</v>
       </c>
@@ -38633,7 +38633,7 @@
       <c r="B27" s="171" t="s">
         <v>502</v>
       </c>
-      <c r="C27" s="278"/>
+      <c r="C27" s="280"/>
       <c r="D27" s="162" t="s">
         <v>527</v>
       </c>
@@ -38657,7 +38657,7 @@
       <c r="B29" s="173" t="s">
         <v>253</v>
       </c>
-      <c r="C29" s="277" t="s">
+      <c r="C29" s="278" t="s">
         <v>529</v>
       </c>
       <c r="D29" s="159" t="s">
@@ -38671,7 +38671,7 @@
       <c r="B30" s="175" t="s">
         <v>254</v>
       </c>
-      <c r="C30" s="278"/>
+      <c r="C30" s="280"/>
       <c r="D30" s="177" t="s">
         <v>675</v>
       </c>
@@ -38683,7 +38683,7 @@
       <c r="B31" s="176" t="s">
         <v>255</v>
       </c>
-      <c r="C31" s="278"/>
+      <c r="C31" s="280"/>
       <c r="D31" s="162" t="s">
         <v>531</v>
       </c>
@@ -38695,7 +38695,7 @@
       <c r="B32" s="176" t="s">
         <v>256</v>
       </c>
-      <c r="C32" s="278"/>
+      <c r="C32" s="280"/>
       <c r="D32" s="162" t="s">
         <v>532</v>
       </c>
@@ -38707,7 +38707,7 @@
       <c r="B33" s="176" t="s">
         <v>257</v>
       </c>
-      <c r="C33" s="278"/>
+      <c r="C33" s="280"/>
       <c r="D33" s="177" t="s">
         <v>533</v>
       </c>
@@ -38719,7 +38719,7 @@
       <c r="B34" s="175" t="s">
         <v>258</v>
       </c>
-      <c r="C34" s="278"/>
+      <c r="C34" s="280"/>
       <c r="D34" s="162" t="s">
         <v>534</v>
       </c>
@@ -38731,7 +38731,7 @@
       <c r="B35" s="176" t="s">
         <v>259</v>
       </c>
-      <c r="C35" s="278"/>
+      <c r="C35" s="280"/>
       <c r="D35" s="162" t="s">
         <v>535</v>
       </c>
@@ -38743,7 +38743,7 @@
       <c r="B36" s="175" t="s">
         <v>260</v>
       </c>
-      <c r="C36" s="278"/>
+      <c r="C36" s="280"/>
       <c r="D36" s="162" t="s">
         <v>535</v>
       </c>
@@ -38755,7 +38755,7 @@
       <c r="B37" s="176" t="s">
         <v>261</v>
       </c>
-      <c r="C37" s="278"/>
+      <c r="C37" s="280"/>
       <c r="D37" s="162" t="s">
         <v>536</v>
       </c>
@@ -38767,7 +38767,7 @@
       <c r="B38" s="175" t="s">
         <v>262</v>
       </c>
-      <c r="C38" s="278"/>
+      <c r="C38" s="280"/>
       <c r="D38" s="162" t="s">
         <v>536</v>
       </c>
@@ -38779,7 +38779,7 @@
       <c r="B39" s="176" t="s">
         <v>263</v>
       </c>
-      <c r="C39" s="278"/>
+      <c r="C39" s="280"/>
       <c r="D39" s="177" t="s">
         <v>670</v>
       </c>
@@ -38791,7 +38791,7 @@
       <c r="B40" s="175" t="s">
         <v>264</v>
       </c>
-      <c r="C40" s="278"/>
+      <c r="C40" s="280"/>
       <c r="D40" s="162" t="s">
         <v>537</v>
       </c>
@@ -38803,7 +38803,7 @@
       <c r="B41" s="176" t="s">
         <v>265</v>
       </c>
-      <c r="C41" s="278"/>
+      <c r="C41" s="280"/>
       <c r="D41" s="162" t="s">
         <v>538</v>
       </c>
@@ -38840,7 +38840,7 @@
       <c r="B44" s="185" t="s">
         <v>266</v>
       </c>
-      <c r="C44" s="277" t="s">
+      <c r="C44" s="278" t="s">
         <v>541</v>
       </c>
       <c r="D44" s="186" t="s">
@@ -38854,7 +38854,7 @@
       <c r="B45" s="188" t="s">
         <v>267</v>
       </c>
-      <c r="C45" s="278"/>
+      <c r="C45" s="280"/>
       <c r="D45" s="162" t="s">
         <v>11</v>
       </c>
@@ -38866,7 +38866,7 @@
       <c r="B46" s="188" t="s">
         <v>268</v>
       </c>
-      <c r="C46" s="278"/>
+      <c r="C46" s="280"/>
       <c r="D46" s="162" t="s">
         <v>542</v>
       </c>
@@ -38878,7 +38878,7 @@
       <c r="B47" s="188" t="s">
         <v>269</v>
       </c>
-      <c r="C47" s="278"/>
+      <c r="C47" s="280"/>
       <c r="D47" s="177" t="s">
         <v>543</v>
       </c>
@@ -38890,7 +38890,7 @@
       <c r="B48" s="188" t="s">
         <v>270</v>
       </c>
-      <c r="C48" s="278"/>
+      <c r="C48" s="280"/>
       <c r="D48" s="162" t="s">
         <v>11</v>
       </c>
@@ -38902,7 +38902,7 @@
       <c r="B49" s="188" t="s">
         <v>271</v>
       </c>
-      <c r="C49" s="278"/>
+      <c r="C49" s="280"/>
       <c r="D49" s="162" t="s">
         <v>544</v>
       </c>
@@ -38914,7 +38914,7 @@
       <c r="B50" s="188" t="s">
         <v>272</v>
       </c>
-      <c r="C50" s="278"/>
+      <c r="C50" s="280"/>
       <c r="D50" s="162" t="s">
         <v>11</v>
       </c>
@@ -38926,7 +38926,7 @@
       <c r="B51" s="188" t="s">
         <v>273</v>
       </c>
-      <c r="C51" s="278"/>
+      <c r="C51" s="280"/>
       <c r="D51" s="177" t="s">
         <v>676</v>
       </c>
@@ -38938,7 +38938,7 @@
       <c r="B52" s="188" t="s">
         <v>274</v>
       </c>
-      <c r="C52" s="278"/>
+      <c r="C52" s="280"/>
       <c r="D52" s="177" t="s">
         <v>543</v>
       </c>
@@ -38962,7 +38962,7 @@
       <c r="B54" s="191" t="s">
         <v>276</v>
       </c>
-      <c r="C54" s="277" t="s">
+      <c r="C54" s="278" t="s">
         <v>545</v>
       </c>
       <c r="D54" s="177" t="s">
@@ -38976,7 +38976,7 @@
       <c r="B55" s="191" t="s">
         <v>277</v>
       </c>
-      <c r="C55" s="278"/>
+      <c r="C55" s="280"/>
       <c r="D55" s="162" t="s">
         <v>547</v>
       </c>
@@ -38988,7 +38988,7 @@
       <c r="B56" s="191" t="s">
         <v>278</v>
       </c>
-      <c r="C56" s="278"/>
+      <c r="C56" s="280"/>
       <c r="D56" s="162" t="s">
         <v>548</v>
       </c>
@@ -39012,7 +39012,7 @@
       <c r="B58" s="254" t="s">
         <v>280</v>
       </c>
-      <c r="C58" s="277" t="s">
+      <c r="C58" s="278" t="s">
         <v>550</v>
       </c>
       <c r="D58" s="159" t="s">
@@ -39038,7 +39038,7 @@
       <c r="B60" s="193" t="s">
         <v>281</v>
       </c>
-      <c r="C60" s="277" t="s">
+      <c r="C60" s="278" t="s">
         <v>552</v>
       </c>
       <c r="D60" s="162" t="s">
@@ -39052,7 +39052,7 @@
       <c r="B61" s="193" t="s">
         <v>282</v>
       </c>
-      <c r="C61" s="278"/>
+      <c r="C61" s="280"/>
       <c r="D61" s="162" t="s">
         <v>554</v>
       </c>
@@ -39064,7 +39064,7 @@
       <c r="B62" s="193" t="s">
         <v>283</v>
       </c>
-      <c r="C62" s="278"/>
+      <c r="C62" s="280"/>
       <c r="D62" s="162" t="s">
         <v>555</v>
       </c>
@@ -39076,7 +39076,7 @@
       <c r="B63" s="193" t="s">
         <v>284</v>
       </c>
-      <c r="C63" s="278"/>
+      <c r="C63" s="280"/>
       <c r="D63" s="162" t="s">
         <v>556</v>
       </c>
@@ -39088,7 +39088,7 @@
       <c r="B64" s="193" t="s">
         <v>285</v>
       </c>
-      <c r="C64" s="278"/>
+      <c r="C64" s="280"/>
       <c r="D64" s="162" t="s">
         <v>557</v>
       </c>
@@ -39100,7 +39100,7 @@
       <c r="B65" s="193" t="s">
         <v>286</v>
       </c>
-      <c r="C65" s="278"/>
+      <c r="C65" s="280"/>
       <c r="D65" s="162" t="s">
         <v>558</v>
       </c>
@@ -39112,7 +39112,7 @@
       <c r="B66" s="193" t="s">
         <v>287</v>
       </c>
-      <c r="C66" s="278"/>
+      <c r="C66" s="280"/>
       <c r="D66" s="162" t="s">
         <v>559</v>
       </c>
@@ -39136,7 +39136,7 @@
       <c r="B68" s="197" t="s">
         <v>289</v>
       </c>
-      <c r="C68" s="277" t="s">
+      <c r="C68" s="278" t="s">
         <v>561</v>
       </c>
       <c r="D68" s="159" t="s">
@@ -39150,7 +39150,7 @@
       <c r="B69" s="199" t="s">
         <v>290</v>
       </c>
-      <c r="C69" s="278"/>
+      <c r="C69" s="280"/>
       <c r="D69" s="162" t="s">
         <v>11</v>
       </c>
@@ -39162,7 +39162,7 @@
       <c r="B70" s="199" t="s">
         <v>291</v>
       </c>
-      <c r="C70" s="278"/>
+      <c r="C70" s="280"/>
       <c r="D70" s="162" t="s">
         <v>11</v>
       </c>
@@ -39174,7 +39174,7 @@
       <c r="B71" s="199" t="s">
         <v>292</v>
       </c>
-      <c r="C71" s="278"/>
+      <c r="C71" s="280"/>
       <c r="D71" s="162" t="s">
         <v>11</v>
       </c>
@@ -39186,7 +39186,7 @@
       <c r="B72" s="199" t="s">
         <v>293</v>
       </c>
-      <c r="C72" s="278"/>
+      <c r="C72" s="280"/>
       <c r="D72" s="162" t="s">
         <v>563</v>
       </c>
@@ -39198,7 +39198,7 @@
       <c r="B73" s="199" t="s">
         <v>294</v>
       </c>
-      <c r="C73" s="278"/>
+      <c r="C73" s="280"/>
       <c r="D73" s="162" t="s">
         <v>11</v>
       </c>
@@ -39210,7 +39210,7 @@
       <c r="B74" s="199" t="s">
         <v>295</v>
       </c>
-      <c r="C74" s="278"/>
+      <c r="C74" s="280"/>
       <c r="D74" s="162" t="s">
         <v>11</v>
       </c>
@@ -39222,7 +39222,7 @@
       <c r="B75" s="199" t="s">
         <v>296</v>
       </c>
-      <c r="C75" s="278"/>
+      <c r="C75" s="280"/>
       <c r="D75" s="162" t="s">
         <v>11</v>
       </c>
@@ -39234,7 +39234,7 @@
       <c r="B76" s="199" t="s">
         <v>297</v>
       </c>
-      <c r="C76" s="278"/>
+      <c r="C76" s="280"/>
       <c r="D76" s="162" t="s">
         <v>11</v>
       </c>
@@ -39246,7 +39246,7 @@
       <c r="B77" s="199" t="s">
         <v>298</v>
       </c>
-      <c r="C77" s="278"/>
+      <c r="C77" s="280"/>
       <c r="D77" s="162" t="s">
         <v>563</v>
       </c>
@@ -39258,7 +39258,7 @@
       <c r="B78" s="199" t="s">
         <v>299</v>
       </c>
-      <c r="C78" s="278"/>
+      <c r="C78" s="280"/>
       <c r="D78" s="162" t="s">
         <v>11</v>
       </c>
@@ -39270,7 +39270,7 @@
       <c r="B79" s="199" t="s">
         <v>300</v>
       </c>
-      <c r="C79" s="278"/>
+      <c r="C79" s="280"/>
       <c r="D79" s="162" t="s">
         <v>11</v>
       </c>
@@ -39282,7 +39282,7 @@
       <c r="B80" s="200" t="s">
         <v>301</v>
       </c>
-      <c r="C80" s="278"/>
+      <c r="C80" s="280"/>
       <c r="D80" s="162" t="s">
         <v>11</v>
       </c>
@@ -39294,7 +39294,7 @@
       <c r="B81" s="200" t="s">
         <v>302</v>
       </c>
-      <c r="C81" s="278"/>
+      <c r="C81" s="280"/>
       <c r="D81" s="162" t="s">
         <v>11</v>
       </c>
@@ -39306,7 +39306,7 @@
       <c r="B82" s="200" t="s">
         <v>303</v>
       </c>
-      <c r="C82" s="278"/>
+      <c r="C82" s="280"/>
       <c r="D82" s="162" t="s">
         <v>563</v>
       </c>
@@ -39318,7 +39318,7 @@
       <c r="B83" s="200" t="s">
         <v>304</v>
       </c>
-      <c r="C83" s="278"/>
+      <c r="C83" s="280"/>
       <c r="D83" s="162" t="s">
         <v>564</v>
       </c>
@@ -39330,7 +39330,7 @@
       <c r="B84" s="201" t="s">
         <v>305</v>
       </c>
-      <c r="C84" s="278"/>
+      <c r="C84" s="280"/>
       <c r="D84" s="162" t="s">
         <v>565</v>
       </c>
@@ -39342,7 +39342,7 @@
       <c r="B85" s="201" t="s">
         <v>306</v>
       </c>
-      <c r="C85" s="278"/>
+      <c r="C85" s="280"/>
       <c r="D85" s="162" t="s">
         <v>566</v>
       </c>
@@ -39354,7 +39354,7 @@
       <c r="B86" s="201" t="s">
         <v>307</v>
       </c>
-      <c r="C86" s="278"/>
+      <c r="C86" s="280"/>
       <c r="D86" s="162" t="s">
         <v>567</v>
       </c>
@@ -39366,7 +39366,7 @@
       <c r="B87" s="201" t="s">
         <v>308</v>
       </c>
-      <c r="C87" s="278"/>
+      <c r="C87" s="280"/>
       <c r="D87" s="162" t="s">
         <v>568</v>
       </c>
@@ -39390,7 +39390,7 @@
       <c r="B89" s="205" t="s">
         <v>310</v>
       </c>
-      <c r="C89" s="277" t="s">
+      <c r="C89" s="278" t="s">
         <v>570</v>
       </c>
       <c r="D89" s="162" t="s">
@@ -39404,7 +39404,7 @@
       <c r="B90" s="205" t="s">
         <v>438</v>
       </c>
-      <c r="C90" s="278"/>
+      <c r="C90" s="280"/>
       <c r="D90" s="206" t="s">
         <v>572</v>
       </c>
@@ -39416,7 +39416,7 @@
       <c r="B91" s="205" t="s">
         <v>311</v>
       </c>
-      <c r="C91" s="278"/>
+      <c r="C91" s="280"/>
       <c r="D91" s="207" t="s">
         <v>573</v>
       </c>
@@ -39440,7 +39440,7 @@
       <c r="B93" s="185" t="s">
         <v>313</v>
       </c>
-      <c r="C93" s="277" t="s">
+      <c r="C93" s="278" t="s">
         <v>575</v>
       </c>
       <c r="D93" s="186" t="s">
@@ -39454,7 +39454,7 @@
       <c r="B94" s="188" t="s">
         <v>319</v>
       </c>
-      <c r="C94" s="278"/>
+      <c r="C94" s="280"/>
       <c r="D94" s="177" t="s">
         <v>577</v>
       </c>
@@ -39466,7 +39466,7 @@
       <c r="B95" s="188" t="s">
         <v>488</v>
       </c>
-      <c r="C95" s="278"/>
+      <c r="C95" s="280"/>
       <c r="D95" s="162" t="s">
         <v>578</v>
       </c>
@@ -39478,7 +39478,7 @@
       <c r="B96" s="188" t="s">
         <v>489</v>
       </c>
-      <c r="C96" s="278"/>
+      <c r="C96" s="280"/>
       <c r="D96" s="162" t="s">
         <v>579</v>
       </c>
@@ -39490,7 +39490,7 @@
       <c r="B97" s="188" t="s">
         <v>490</v>
       </c>
-      <c r="C97" s="278"/>
+      <c r="C97" s="280"/>
       <c r="D97" s="162" t="s">
         <v>580</v>
       </c>
@@ -39514,7 +39514,7 @@
       <c r="B99" s="211" t="s">
         <v>454</v>
       </c>
-      <c r="C99" s="277" t="s">
+      <c r="C99" s="278" t="s">
         <v>581</v>
       </c>
       <c r="D99" s="159" t="s">
@@ -39528,7 +39528,7 @@
       <c r="B100" s="213" t="s">
         <v>314</v>
       </c>
-      <c r="C100" s="278"/>
+      <c r="C100" s="280"/>
       <c r="D100" s="162" t="s">
         <v>583</v>
       </c>
@@ -39540,7 +39540,7 @@
       <c r="B101" s="213" t="s">
         <v>315</v>
       </c>
-      <c r="C101" s="278"/>
+      <c r="C101" s="280"/>
       <c r="D101" s="162" t="s">
         <v>584</v>
       </c>
@@ -39552,7 +39552,7 @@
       <c r="B102" s="213" t="s">
         <v>316</v>
       </c>
-      <c r="C102" s="278"/>
+      <c r="C102" s="280"/>
       <c r="D102" s="162" t="s">
         <v>584</v>
       </c>
@@ -39564,7 +39564,7 @@
       <c r="B103" s="213" t="s">
         <v>317</v>
       </c>
-      <c r="C103" s="278"/>
+      <c r="C103" s="280"/>
       <c r="D103" s="162" t="s">
         <v>585</v>
       </c>
@@ -39588,7 +39588,7 @@
       <c r="B105" s="216" t="s">
         <v>439</v>
       </c>
-      <c r="C105" s="277" t="s">
+      <c r="C105" s="278" t="s">
         <v>586</v>
       </c>
       <c r="D105" s="186" t="s">
@@ -39602,7 +39602,7 @@
       <c r="B106" s="217" t="s">
         <v>440</v>
       </c>
-      <c r="C106" s="278"/>
+      <c r="C106" s="280"/>
       <c r="D106" s="162" t="s">
         <v>11</v>
       </c>
@@ -39614,7 +39614,7 @@
       <c r="B107" s="217" t="s">
         <v>441</v>
       </c>
-      <c r="C107" s="278"/>
+      <c r="C107" s="280"/>
       <c r="D107" s="162" t="s">
         <v>11</v>
       </c>
@@ -39626,7 +39626,7 @@
       <c r="B108" s="217" t="s">
         <v>442</v>
       </c>
-      <c r="C108" s="278"/>
+      <c r="C108" s="280"/>
       <c r="D108" s="162" t="s">
         <v>11</v>
       </c>
@@ -39638,7 +39638,7 @@
       <c r="B109" s="217" t="s">
         <v>443</v>
       </c>
-      <c r="C109" s="278"/>
+      <c r="C109" s="280"/>
       <c r="D109" s="162" t="s">
         <v>563</v>
       </c>
@@ -39650,7 +39650,7 @@
       <c r="B110" s="217" t="s">
         <v>444</v>
       </c>
-      <c r="C110" s="278"/>
+      <c r="C110" s="280"/>
       <c r="D110" s="162" t="s">
         <v>11</v>
       </c>
@@ -39662,7 +39662,7 @@
       <c r="B111" s="217" t="s">
         <v>445</v>
       </c>
-      <c r="C111" s="278"/>
+      <c r="C111" s="280"/>
       <c r="D111" s="162" t="s">
         <v>11</v>
       </c>
@@ -39674,7 +39674,7 @@
       <c r="B112" s="217" t="s">
         <v>506</v>
       </c>
-      <c r="C112" s="278"/>
+      <c r="C112" s="280"/>
       <c r="D112" s="162" t="s">
         <v>11</v>
       </c>
@@ -39686,7 +39686,7 @@
       <c r="B113" s="217" t="s">
         <v>507</v>
       </c>
-      <c r="C113" s="278"/>
+      <c r="C113" s="280"/>
       <c r="D113" s="162" t="s">
         <v>11</v>
       </c>
@@ -39698,7 +39698,7 @@
       <c r="B114" s="217" t="s">
         <v>508</v>
       </c>
-      <c r="C114" s="278"/>
+      <c r="C114" s="280"/>
       <c r="D114" s="162" t="s">
         <v>11</v>
       </c>
@@ -39710,7 +39710,7 @@
       <c r="B115" s="217" t="s">
         <v>509</v>
       </c>
-      <c r="C115" s="278"/>
+      <c r="C115" s="280"/>
       <c r="D115" s="162" t="s">
         <v>11</v>
       </c>
@@ -39722,7 +39722,7 @@
       <c r="B116" s="217" t="s">
         <v>446</v>
       </c>
-      <c r="C116" s="278"/>
+      <c r="C116" s="280"/>
       <c r="D116" s="162" t="s">
         <v>588</v>
       </c>
@@ -39734,7 +39734,7 @@
       <c r="B117" s="217" t="s">
         <v>447</v>
       </c>
-      <c r="C117" s="278"/>
+      <c r="C117" s="280"/>
       <c r="D117" s="162" t="s">
         <v>589</v>
       </c>
@@ -39746,7 +39746,7 @@
       <c r="B118" s="217" t="s">
         <v>477</v>
       </c>
-      <c r="C118" s="278"/>
+      <c r="C118" s="280"/>
       <c r="D118" s="162" t="s">
         <v>590</v>
       </c>
@@ -39758,7 +39758,7 @@
       <c r="B119" s="217" t="s">
         <v>478</v>
       </c>
-      <c r="C119" s="278"/>
+      <c r="C119" s="280"/>
       <c r="D119" s="162" t="s">
         <v>591</v>
       </c>
@@ -39770,7 +39770,7 @@
       <c r="B120" s="217" t="s">
         <v>510</v>
       </c>
-      <c r="C120" s="278"/>
+      <c r="C120" s="280"/>
       <c r="D120" s="162" t="s">
         <v>592</v>
       </c>
@@ -39782,7 +39782,7 @@
       <c r="B121" s="217" t="s">
         <v>513</v>
       </c>
-      <c r="C121" s="278"/>
+      <c r="C121" s="280"/>
       <c r="D121" s="162" t="s">
         <v>593</v>
       </c>
@@ -39794,7 +39794,7 @@
       <c r="B122" s="217" t="s">
         <v>512</v>
       </c>
-      <c r="C122" s="278"/>
+      <c r="C122" s="280"/>
       <c r="D122" s="177" t="s">
         <v>594</v>
       </c>
@@ -39806,7 +39806,7 @@
       <c r="B123" s="217" t="s">
         <v>320</v>
       </c>
-      <c r="C123" s="278"/>
+      <c r="C123" s="280"/>
       <c r="D123" s="162" t="s">
         <v>595</v>
       </c>
@@ -39818,7 +39818,7 @@
       <c r="B124" s="217" t="s">
         <v>321</v>
       </c>
-      <c r="C124" s="278"/>
+      <c r="C124" s="280"/>
       <c r="D124" s="162" t="s">
         <v>595</v>
       </c>
@@ -39830,7 +39830,7 @@
       <c r="B125" s="217" t="s">
         <v>322</v>
       </c>
-      <c r="C125" s="278"/>
+      <c r="C125" s="280"/>
       <c r="D125" s="177" t="s">
         <v>672</v>
       </c>
@@ -39842,7 +39842,7 @@
       <c r="B126" s="217" t="s">
         <v>323</v>
       </c>
-      <c r="C126" s="278"/>
+      <c r="C126" s="280"/>
       <c r="D126" s="162" t="s">
         <v>596</v>
       </c>
@@ -39854,7 +39854,7 @@
       <c r="B127" s="217" t="s">
         <v>448</v>
       </c>
-      <c r="C127" s="278"/>
+      <c r="C127" s="280"/>
       <c r="D127" s="177" t="s">
         <v>673</v>
       </c>
@@ -39866,7 +39866,7 @@
       <c r="B128" s="217" t="s">
         <v>449</v>
       </c>
-      <c r="C128" s="278"/>
+      <c r="C128" s="280"/>
       <c r="D128" s="177" t="s">
         <v>669</v>
       </c>
@@ -39878,7 +39878,7 @@
       <c r="B129" s="217" t="s">
         <v>324</v>
       </c>
-      <c r="C129" s="278"/>
+      <c r="C129" s="280"/>
       <c r="D129" s="177" t="s">
         <v>597</v>
       </c>
@@ -39890,7 +39890,7 @@
       <c r="B130" s="217" t="s">
         <v>480</v>
       </c>
-      <c r="C130" s="278"/>
+      <c r="C130" s="280"/>
       <c r="D130" s="177" t="s">
         <v>598</v>
       </c>
@@ -39902,7 +39902,7 @@
       <c r="B131" s="217" t="s">
         <v>325</v>
       </c>
-      <c r="C131" s="278"/>
+      <c r="C131" s="280"/>
       <c r="D131" s="162" t="s">
         <v>599</v>
       </c>
@@ -39914,7 +39914,7 @@
       <c r="B132" s="217" t="s">
         <v>326</v>
       </c>
-      <c r="C132" s="278"/>
+      <c r="C132" s="280"/>
       <c r="D132" s="162" t="s">
         <v>600</v>
       </c>
@@ -39926,7 +39926,7 @@
       <c r="B133" s="217" t="s">
         <v>327</v>
       </c>
-      <c r="C133" s="278"/>
+      <c r="C133" s="280"/>
       <c r="D133" s="218" t="s">
         <v>601</v>
       </c>
@@ -39938,7 +39938,7 @@
       <c r="B134" s="217" t="s">
         <v>328</v>
       </c>
-      <c r="C134" s="278"/>
+      <c r="C134" s="280"/>
       <c r="D134" s="218" t="s">
         <v>601</v>
       </c>
@@ -39950,7 +39950,7 @@
       <c r="B135" s="217" t="s">
         <v>329</v>
       </c>
-      <c r="C135" s="278"/>
+      <c r="C135" s="280"/>
       <c r="D135" s="162" t="s">
         <v>602</v>
       </c>
@@ -39962,7 +39962,7 @@
       <c r="B136" s="217" t="s">
         <v>330</v>
       </c>
-      <c r="C136" s="278"/>
+      <c r="C136" s="280"/>
       <c r="D136" s="162" t="s">
         <v>603</v>
       </c>
@@ -39974,7 +39974,7 @@
       <c r="B137" s="217" t="s">
         <v>463</v>
       </c>
-      <c r="C137" s="278"/>
+      <c r="C137" s="280"/>
       <c r="D137" s="162" t="s">
         <v>604</v>
       </c>
@@ -39998,7 +39998,7 @@
       <c r="B139" s="221" t="s">
         <v>331</v>
       </c>
-      <c r="C139" s="277" t="s">
+      <c r="C139" s="278" t="s">
         <v>606</v>
       </c>
       <c r="D139" s="162" t="s">
@@ -40012,7 +40012,7 @@
       <c r="B140" s="221" t="s">
         <v>332</v>
       </c>
-      <c r="C140" s="278"/>
+      <c r="C140" s="280"/>
       <c r="D140" s="177" t="s">
         <v>608</v>
       </c>
@@ -40024,7 +40024,7 @@
       <c r="B141" s="221" t="s">
         <v>333</v>
       </c>
-      <c r="C141" s="278"/>
+      <c r="C141" s="280"/>
       <c r="D141" s="162" t="s">
         <v>11</v>
       </c>
@@ -40036,7 +40036,7 @@
       <c r="B142" s="221" t="s">
         <v>334</v>
       </c>
-      <c r="C142" s="278"/>
+      <c r="C142" s="280"/>
       <c r="D142" s="162" t="s">
         <v>11</v>
       </c>
@@ -40048,7 +40048,7 @@
       <c r="B143" s="221" t="s">
         <v>450</v>
       </c>
-      <c r="C143" s="278"/>
+      <c r="C143" s="280"/>
       <c r="D143" s="177" t="s">
         <v>609</v>
       </c>
@@ -40060,7 +40060,7 @@
       <c r="B144" s="221" t="s">
         <v>451</v>
       </c>
-      <c r="C144" s="278"/>
+      <c r="C144" s="280"/>
       <c r="D144" s="177" t="s">
         <v>610</v>
       </c>
@@ -40072,7 +40072,7 @@
       <c r="B145" s="221" t="s">
         <v>335</v>
       </c>
-      <c r="C145" s="278"/>
+      <c r="C145" s="280"/>
       <c r="D145" s="162" t="s">
         <v>611</v>
       </c>
@@ -40084,7 +40084,7 @@
       <c r="B146" s="221" t="s">
         <v>336</v>
       </c>
-      <c r="C146" s="278"/>
+      <c r="C146" s="280"/>
       <c r="D146" s="162" t="s">
         <v>11</v>
       </c>
@@ -40096,7 +40096,7 @@
       <c r="B147" s="221" t="s">
         <v>337</v>
       </c>
-      <c r="C147" s="278"/>
+      <c r="C147" s="280"/>
       <c r="D147" s="162" t="s">
         <v>11</v>
       </c>
@@ -40108,7 +40108,7 @@
       <c r="B148" s="221" t="s">
         <v>338</v>
       </c>
-      <c r="C148" s="278"/>
+      <c r="C148" s="280"/>
       <c r="D148" s="162" t="s">
         <v>11</v>
       </c>
@@ -40120,7 +40120,7 @@
       <c r="B149" s="221" t="s">
         <v>339</v>
       </c>
-      <c r="C149" s="278"/>
+      <c r="C149" s="280"/>
       <c r="D149" s="162" t="s">
         <v>612</v>
       </c>
@@ -40132,7 +40132,7 @@
       <c r="B150" s="221" t="s">
         <v>340</v>
       </c>
-      <c r="C150" s="278"/>
+      <c r="C150" s="280"/>
       <c r="D150" s="162" t="s">
         <v>613</v>
       </c>
@@ -40144,7 +40144,7 @@
       <c r="B151" s="221" t="s">
         <v>341</v>
       </c>
-      <c r="C151" s="278"/>
+      <c r="C151" s="280"/>
       <c r="D151" s="162" t="s">
         <v>614</v>
       </c>
@@ -40178,6 +40178,13 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="C139:C152"/>
+    <mergeCell ref="C60:C67"/>
+    <mergeCell ref="C68:C88"/>
+    <mergeCell ref="C89:C92"/>
+    <mergeCell ref="C93:C98"/>
+    <mergeCell ref="C99:C104"/>
+    <mergeCell ref="C105:C138"/>
     <mergeCell ref="C58:C59"/>
     <mergeCell ref="C54:C57"/>
     <mergeCell ref="C2:C11"/>
@@ -40185,13 +40192,6 @@
     <mergeCell ref="C18:C28"/>
     <mergeCell ref="C29:C41"/>
     <mergeCell ref="C44:C53"/>
-    <mergeCell ref="C139:C152"/>
-    <mergeCell ref="C60:C67"/>
-    <mergeCell ref="C68:C88"/>
-    <mergeCell ref="C89:C92"/>
-    <mergeCell ref="C93:C98"/>
-    <mergeCell ref="C99:C104"/>
-    <mergeCell ref="C105:C138"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -40237,7 +40237,7 @@
       <c r="B2" s="197" t="s">
         <v>344</v>
       </c>
-      <c r="C2" s="277" t="s">
+      <c r="C2" s="278" t="s">
         <v>561</v>
       </c>
       <c r="D2" s="159" t="s">
@@ -40251,7 +40251,7 @@
       <c r="B3" s="199" t="s">
         <v>345</v>
       </c>
-      <c r="C3" s="278"/>
+      <c r="C3" s="280"/>
       <c r="D3" s="162" t="s">
         <v>11</v>
       </c>
@@ -40263,7 +40263,7 @@
       <c r="B4" s="199" t="s">
         <v>346</v>
       </c>
-      <c r="C4" s="278"/>
+      <c r="C4" s="280"/>
       <c r="D4" s="162" t="s">
         <v>11</v>
       </c>
@@ -40275,7 +40275,7 @@
       <c r="B5" s="199" t="s">
         <v>347</v>
       </c>
-      <c r="C5" s="278"/>
+      <c r="C5" s="280"/>
       <c r="D5" s="162" t="s">
         <v>11</v>
       </c>
@@ -40287,7 +40287,7 @@
       <c r="B6" s="199" t="s">
         <v>348</v>
       </c>
-      <c r="C6" s="278"/>
+      <c r="C6" s="280"/>
       <c r="D6" s="162" t="s">
         <v>11</v>
       </c>
@@ -40299,7 +40299,7 @@
       <c r="B7" s="199" t="s">
         <v>349</v>
       </c>
-      <c r="C7" s="278"/>
+      <c r="C7" s="280"/>
       <c r="D7" s="162" t="s">
         <v>11</v>
       </c>
@@ -40311,7 +40311,7 @@
       <c r="B8" s="199" t="s">
         <v>350</v>
       </c>
-      <c r="C8" s="278"/>
+      <c r="C8" s="280"/>
       <c r="D8" s="162" t="s">
         <v>11</v>
       </c>
@@ -40323,7 +40323,7 @@
       <c r="B9" s="199" t="s">
         <v>351</v>
       </c>
-      <c r="C9" s="278"/>
+      <c r="C9" s="280"/>
       <c r="D9" s="162" t="s">
         <v>11</v>
       </c>
@@ -40335,7 +40335,7 @@
       <c r="B10" s="199" t="s">
         <v>352</v>
       </c>
-      <c r="C10" s="278"/>
+      <c r="C10" s="280"/>
       <c r="D10" s="162" t="s">
         <v>11</v>
       </c>
@@ -40347,7 +40347,7 @@
       <c r="B11" s="199" t="s">
         <v>353</v>
       </c>
-      <c r="C11" s="278"/>
+      <c r="C11" s="280"/>
       <c r="D11" s="162" t="s">
         <v>11</v>
       </c>
@@ -40359,7 +40359,7 @@
       <c r="B12" s="199" t="s">
         <v>354</v>
       </c>
-      <c r="C12" s="278"/>
+      <c r="C12" s="280"/>
       <c r="D12" s="162" t="s">
         <v>11</v>
       </c>
@@ -40371,7 +40371,7 @@
       <c r="B13" s="199" t="s">
         <v>355</v>
       </c>
-      <c r="C13" s="278"/>
+      <c r="C13" s="280"/>
       <c r="D13" s="162" t="s">
         <v>11</v>
       </c>
@@ -40383,7 +40383,7 @@
       <c r="B14" s="199" t="s">
         <v>356</v>
       </c>
-      <c r="C14" s="278"/>
+      <c r="C14" s="280"/>
       <c r="D14" s="162" t="s">
         <v>619</v>
       </c>
@@ -40395,7 +40395,7 @@
       <c r="B15" s="199" t="s">
         <v>357</v>
       </c>
-      <c r="C15" s="278"/>
+      <c r="C15" s="280"/>
       <c r="D15" s="162" t="s">
         <v>619</v>
       </c>
@@ -40419,7 +40419,7 @@
       <c r="B17" s="227" t="s">
         <v>358</v>
       </c>
-      <c r="C17" s="277" t="s">
+      <c r="C17" s="278" t="s">
         <v>621</v>
       </c>
       <c r="D17" s="159" t="s">
@@ -40433,7 +40433,7 @@
       <c r="B18" s="228" t="s">
         <v>359</v>
       </c>
-      <c r="C18" s="278"/>
+      <c r="C18" s="280"/>
       <c r="D18" s="162" t="s">
         <v>623</v>
       </c>
@@ -40445,7 +40445,7 @@
       <c r="B19" s="228" t="s">
         <v>360</v>
       </c>
-      <c r="C19" s="278"/>
+      <c r="C19" s="280"/>
       <c r="D19" s="162" t="s">
         <v>624</v>
       </c>
@@ -40457,7 +40457,7 @@
       <c r="B20" s="228" t="s">
         <v>361</v>
       </c>
-      <c r="C20" s="278"/>
+      <c r="C20" s="280"/>
       <c r="D20" s="162" t="s">
         <v>553</v>
       </c>
@@ -40469,7 +40469,7 @@
       <c r="B21" s="228" t="s">
         <v>362</v>
       </c>
-      <c r="C21" s="278"/>
+      <c r="C21" s="280"/>
       <c r="D21" s="162" t="s">
         <v>554</v>
       </c>
@@ -40481,7 +40481,7 @@
       <c r="B22" s="228" t="s">
         <v>363</v>
       </c>
-      <c r="C22" s="278"/>
+      <c r="C22" s="280"/>
       <c r="D22" s="162" t="s">
         <v>555</v>
       </c>
@@ -40493,7 +40493,7 @@
       <c r="B23" s="228" t="s">
         <v>364</v>
       </c>
-      <c r="C23" s="278"/>
+      <c r="C23" s="280"/>
       <c r="D23" s="162" t="s">
         <v>556</v>
       </c>
@@ -40505,7 +40505,7 @@
       <c r="B24" s="228" t="s">
         <v>365</v>
       </c>
-      <c r="C24" s="278"/>
+      <c r="C24" s="280"/>
       <c r="D24" s="162" t="s">
         <v>557</v>
       </c>
@@ -40529,7 +40529,7 @@
       <c r="B26" s="173" t="s">
         <v>367</v>
       </c>
-      <c r="C26" s="277" t="s">
+      <c r="C26" s="278" t="s">
         <v>625</v>
       </c>
       <c r="D26" s="159" t="s">
@@ -40543,7 +40543,7 @@
       <c r="B27" s="176" t="s">
         <v>368</v>
       </c>
-      <c r="C27" s="278"/>
+      <c r="C27" s="280"/>
       <c r="D27" s="162" t="s">
         <v>627</v>
       </c>
@@ -40555,7 +40555,7 @@
       <c r="B28" s="176" t="s">
         <v>369</v>
       </c>
-      <c r="C28" s="278"/>
+      <c r="C28" s="280"/>
       <c r="D28" s="162" t="s">
         <v>628</v>
       </c>
@@ -40567,7 +40567,7 @@
       <c r="B29" s="176" t="s">
         <v>370</v>
       </c>
-      <c r="C29" s="278"/>
+      <c r="C29" s="280"/>
       <c r="D29" s="162" t="s">
         <v>629</v>
       </c>
@@ -40579,7 +40579,7 @@
       <c r="B30" s="176" t="s">
         <v>371</v>
       </c>
-      <c r="C30" s="278"/>
+      <c r="C30" s="280"/>
       <c r="D30" s="162" t="s">
         <v>630</v>
       </c>
@@ -40591,7 +40591,7 @@
       <c r="B31" s="176" t="s">
         <v>372</v>
       </c>
-      <c r="C31" s="278"/>
+      <c r="C31" s="280"/>
       <c r="D31" s="162" t="s">
         <v>630</v>
       </c>
@@ -40603,7 +40603,7 @@
       <c r="B32" s="176" t="s">
         <v>373</v>
       </c>
-      <c r="C32" s="278"/>
+      <c r="C32" s="280"/>
       <c r="D32" s="162" t="s">
         <v>631</v>
       </c>
@@ -40615,7 +40615,7 @@
       <c r="B33" s="176" t="s">
         <v>374</v>
       </c>
-      <c r="C33" s="278"/>
+      <c r="C33" s="280"/>
       <c r="D33" s="162" t="s">
         <v>631</v>
       </c>
@@ -40627,7 +40627,7 @@
       <c r="B34" s="176" t="s">
         <v>375</v>
       </c>
-      <c r="C34" s="278"/>
+      <c r="C34" s="280"/>
       <c r="D34" s="162" t="s">
         <v>631</v>
       </c>
@@ -40639,7 +40639,7 @@
       <c r="B35" s="176" t="s">
         <v>376</v>
       </c>
-      <c r="C35" s="278"/>
+      <c r="C35" s="280"/>
       <c r="D35" s="162" t="s">
         <v>631</v>
       </c>
@@ -40663,7 +40663,7 @@
       <c r="B37" s="232" t="s">
         <v>481</v>
       </c>
-      <c r="C37" s="277" t="s">
+      <c r="C37" s="278" t="s">
         <v>632</v>
       </c>
       <c r="D37" s="186" t="s">
@@ -40677,7 +40677,7 @@
       <c r="B38" s="220" t="s">
         <v>482</v>
       </c>
-      <c r="C38" s="278"/>
+      <c r="C38" s="280"/>
       <c r="D38" s="177" t="s">
         <v>610</v>
       </c>
@@ -40689,7 +40689,7 @@
       <c r="B39" s="220" t="s">
         <v>483</v>
       </c>
-      <c r="C39" s="278"/>
+      <c r="C39" s="280"/>
       <c r="D39" s="177" t="s">
         <v>633</v>
       </c>
@@ -40719,6 +40719,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004FD8CECCB51EC843BF514AFE68379818" ma:contentTypeVersion="18" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="eda339f53f012ceb64677667a741b441">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="107e75b3-53cc-4838-92d2-ebc011bd4832" xmlns:ns3="888ccf44-0d39-41a2-ab17-f7efb2bf6977" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04a86f3db711706e561c315688f1c464" ns2:_="" ns3:_="">
     <xsd:import namespace="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
@@ -40967,15 +40976,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -40988,6 +40988,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F91B7B9-75FF-4624-B506-952B5B54766C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41002,14 +41010,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Downloaded the "old" version from main
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/prw_energinet_dk/Documents/Dokumenter/GitHub/MTB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="11_65313A6E4C5506009E52DA9B1CE17435CB52B360" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C97A57C7-5E32-4B71-AAC0-EEDCD587FBCB}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="11_65313A6E4C5506009E52DA9B1CE17435CB52B360" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADAE1870-AFBD-4A5B-B92E-E02D13B5CF6A}"/>
   <bookViews>
-    <workbookView xWindow="-19335" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16700" yWindow="-21710" windowWidth="51420" windowHeight="21100" tabRatio="822" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -3943,7 +3943,6 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3998,10 +3997,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4013,6 +4012,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -4576,8 +4576,8 @@
   </sheetPr>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4700,16 +4700,16 @@
         <v>435</v>
       </c>
       <c r="H7" s="144"/>
-      <c r="I7" s="261" t="s">
+      <c r="I7" s="260" t="s">
         <v>466</v>
       </c>
-      <c r="J7" s="261"/>
-      <c r="K7" s="261"/>
-      <c r="L7" s="261" t="s">
+      <c r="J7" s="260"/>
+      <c r="K7" s="260"/>
+      <c r="L7" s="260" t="s">
         <v>467</v>
       </c>
-      <c r="M7" s="261"/>
-      <c r="N7" s="262"/>
+      <c r="M7" s="260"/>
+      <c r="N7" s="261"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" s="27" t="s">
@@ -4752,7 +4752,7 @@
       <c r="C9" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="E9" s="260" t="s">
+      <c r="E9" s="283" t="s">
         <v>680</v>
       </c>
       <c r="H9" s="145"/>
@@ -5134,7 +5134,7 @@
       <c r="B2" s="237" t="s">
         <v>378</v>
       </c>
-      <c r="C2" s="278" t="s">
+      <c r="C2" s="277" t="s">
         <v>514</v>
       </c>
       <c r="D2" s="186" t="s">
@@ -5148,7 +5148,7 @@
       <c r="B3" s="239" t="s">
         <v>379</v>
       </c>
-      <c r="C3" s="280"/>
+      <c r="C3" s="278"/>
       <c r="D3" s="177" t="s">
         <v>11</v>
       </c>
@@ -5160,7 +5160,7 @@
       <c r="B4" s="239" t="s">
         <v>380</v>
       </c>
-      <c r="C4" s="280"/>
+      <c r="C4" s="278"/>
       <c r="D4" s="177" t="s">
         <v>11</v>
       </c>
@@ -5172,7 +5172,7 @@
       <c r="B5" s="239" t="s">
         <v>381</v>
       </c>
-      <c r="C5" s="280"/>
+      <c r="C5" s="278"/>
       <c r="D5" s="177" t="s">
         <v>11</v>
       </c>
@@ -5184,7 +5184,7 @@
       <c r="B6" s="239" t="s">
         <v>382</v>
       </c>
-      <c r="C6" s="280"/>
+      <c r="C6" s="278"/>
       <c r="D6" s="177" t="s">
         <v>11</v>
       </c>
@@ -5222,7 +5222,7 @@
       <c r="B9" s="173" t="s">
         <v>385</v>
       </c>
-      <c r="C9" s="281" t="s">
+      <c r="C9" s="280" t="s">
         <v>637</v>
       </c>
       <c r="D9" s="186" t="s">
@@ -5236,7 +5236,7 @@
       <c r="B10" s="230" t="s">
         <v>386</v>
       </c>
-      <c r="C10" s="282"/>
+      <c r="C10" s="281"/>
       <c r="D10" s="182" t="s">
         <v>639</v>
       </c>
@@ -5248,7 +5248,7 @@
       <c r="B11" s="227" t="s">
         <v>387</v>
       </c>
-      <c r="C11" s="278" t="s">
+      <c r="C11" s="277" t="s">
         <v>640</v>
       </c>
       <c r="D11" s="186" t="s">
@@ -5262,7 +5262,7 @@
       <c r="B12" s="228" t="s">
         <v>388</v>
       </c>
-      <c r="C12" s="280"/>
+      <c r="C12" s="278"/>
       <c r="D12" s="177" t="s">
         <v>642</v>
       </c>
@@ -5286,7 +5286,7 @@
       <c r="B14" s="197" t="s">
         <v>390</v>
       </c>
-      <c r="C14" s="281" t="s">
+      <c r="C14" s="280" t="s">
         <v>561</v>
       </c>
       <c r="D14" s="186" t="s">
@@ -5300,7 +5300,7 @@
       <c r="B15" s="199" t="s">
         <v>391</v>
       </c>
-      <c r="C15" s="283"/>
+      <c r="C15" s="282"/>
       <c r="D15" s="177" t="s">
         <v>11</v>
       </c>
@@ -5312,7 +5312,7 @@
       <c r="B16" s="199" t="s">
         <v>392</v>
       </c>
-      <c r="C16" s="283"/>
+      <c r="C16" s="282"/>
       <c r="D16" s="177" t="s">
         <v>11</v>
       </c>
@@ -5324,7 +5324,7 @@
       <c r="B17" s="199" t="s">
         <v>393</v>
       </c>
-      <c r="C17" s="283"/>
+      <c r="C17" s="282"/>
       <c r="D17" s="177" t="s">
         <v>11</v>
       </c>
@@ -5336,7 +5336,7 @@
       <c r="B18" s="199" t="s">
         <v>394</v>
       </c>
-      <c r="C18" s="283"/>
+      <c r="C18" s="282"/>
       <c r="D18" s="177" t="s">
         <v>11</v>
       </c>
@@ -5348,7 +5348,7 @@
       <c r="B19" s="199" t="s">
         <v>395</v>
       </c>
-      <c r="C19" s="283"/>
+      <c r="C19" s="282"/>
       <c r="D19" s="177" t="s">
         <v>11</v>
       </c>
@@ -5360,7 +5360,7 @@
       <c r="B20" s="199" t="s">
         <v>396</v>
       </c>
-      <c r="C20" s="283"/>
+      <c r="C20" s="282"/>
       <c r="D20" s="177" t="s">
         <v>11</v>
       </c>
@@ -5372,7 +5372,7 @@
       <c r="B21" s="199" t="s">
         <v>397</v>
       </c>
-      <c r="C21" s="283"/>
+      <c r="C21" s="282"/>
       <c r="D21" s="177" t="s">
         <v>11</v>
       </c>
@@ -5384,7 +5384,7 @@
       <c r="B22" s="199" t="s">
         <v>398</v>
       </c>
-      <c r="C22" s="283"/>
+      <c r="C22" s="282"/>
       <c r="D22" s="177" t="s">
         <v>11</v>
       </c>
@@ -5396,7 +5396,7 @@
       <c r="B23" s="199" t="s">
         <v>399</v>
       </c>
-      <c r="C23" s="283"/>
+      <c r="C23" s="282"/>
       <c r="D23" s="177" t="s">
         <v>11</v>
       </c>
@@ -5408,7 +5408,7 @@
       <c r="B24" s="199" t="s">
         <v>400</v>
       </c>
-      <c r="C24" s="283"/>
+      <c r="C24" s="282"/>
       <c r="D24" s="177" t="s">
         <v>11</v>
       </c>
@@ -5420,7 +5420,7 @@
       <c r="B25" s="199" t="s">
         <v>401</v>
       </c>
-      <c r="C25" s="283"/>
+      <c r="C25" s="282"/>
       <c r="D25" s="177" t="s">
         <v>11</v>
       </c>
@@ -5432,7 +5432,7 @@
       <c r="B26" s="199" t="s">
         <v>402</v>
       </c>
-      <c r="C26" s="283"/>
+      <c r="C26" s="282"/>
       <c r="D26" s="177" t="s">
         <v>564</v>
       </c>
@@ -5444,7 +5444,7 @@
       <c r="B27" s="199" t="s">
         <v>403</v>
       </c>
-      <c r="C27" s="283"/>
+      <c r="C27" s="282"/>
       <c r="D27" s="177" t="s">
         <v>565</v>
       </c>
@@ -5456,7 +5456,7 @@
       <c r="B28" s="199" t="s">
         <v>404</v>
       </c>
-      <c r="C28" s="283"/>
+      <c r="C28" s="282"/>
       <c r="D28" s="177" t="s">
         <v>566</v>
       </c>
@@ -5468,7 +5468,7 @@
       <c r="B29" s="199" t="s">
         <v>405</v>
       </c>
-      <c r="C29" s="283"/>
+      <c r="C29" s="282"/>
       <c r="D29" s="177" t="s">
         <v>567</v>
       </c>
@@ -5480,7 +5480,7 @@
       <c r="B30" s="199" t="s">
         <v>406</v>
       </c>
-      <c r="C30" s="283"/>
+      <c r="C30" s="282"/>
       <c r="D30" s="183" t="s">
         <v>645</v>
       </c>
@@ -5492,7 +5492,7 @@
       <c r="B31" s="199" t="s">
         <v>407</v>
       </c>
-      <c r="C31" s="283"/>
+      <c r="C31" s="282"/>
       <c r="D31" s="183" t="s">
         <v>645</v>
       </c>
@@ -5504,7 +5504,7 @@
       <c r="B32" s="199" t="s">
         <v>408</v>
       </c>
-      <c r="C32" s="283"/>
+      <c r="C32" s="282"/>
       <c r="D32" s="177" t="s">
         <v>595</v>
       </c>
@@ -5516,7 +5516,7 @@
       <c r="B33" s="199" t="s">
         <v>409</v>
       </c>
-      <c r="C33" s="283"/>
+      <c r="C33" s="282"/>
       <c r="D33" s="177" t="s">
         <v>595</v>
       </c>
@@ -5528,7 +5528,7 @@
       <c r="B34" s="199" t="s">
         <v>410</v>
       </c>
-      <c r="C34" s="283"/>
+      <c r="C34" s="282"/>
       <c r="D34" s="177" t="s">
         <v>568</v>
       </c>
@@ -5540,7 +5540,7 @@
       <c r="B35" s="199" t="s">
         <v>411</v>
       </c>
-      <c r="C35" s="283"/>
+      <c r="C35" s="282"/>
       <c r="D35" s="177" t="s">
         <v>569</v>
       </c>
@@ -5552,7 +5552,7 @@
       <c r="B36" s="199" t="s">
         <v>412</v>
       </c>
-      <c r="C36" s="283"/>
+      <c r="C36" s="282"/>
       <c r="D36" s="177" t="s">
         <v>646</v>
       </c>
@@ -5564,7 +5564,7 @@
       <c r="B37" s="226" t="s">
         <v>487</v>
       </c>
-      <c r="C37" s="282"/>
+      <c r="C37" s="281"/>
       <c r="D37" s="177" t="s">
         <v>647</v>
       </c>
@@ -5576,7 +5576,7 @@
       <c r="B38" s="227" t="s">
         <v>413</v>
       </c>
-      <c r="C38" s="278" t="s">
+      <c r="C38" s="277" t="s">
         <v>640</v>
       </c>
       <c r="D38" s="186" t="s">
@@ -5590,7 +5590,7 @@
       <c r="B39" s="228" t="s">
         <v>414</v>
       </c>
-      <c r="C39" s="280"/>
+      <c r="C39" s="278"/>
       <c r="D39" s="177" t="s">
         <v>554</v>
       </c>
@@ -5602,7 +5602,7 @@
       <c r="B40" s="228" t="s">
         <v>415</v>
       </c>
-      <c r="C40" s="280"/>
+      <c r="C40" s="278"/>
       <c r="D40" s="177" t="s">
         <v>557</v>
       </c>
@@ -5626,7 +5626,7 @@
       <c r="B42" s="232" t="s">
         <v>461</v>
       </c>
-      <c r="C42" s="278" t="s">
+      <c r="C42" s="277" t="s">
         <v>648</v>
       </c>
       <c r="D42" s="186" t="s">
@@ -5640,7 +5640,7 @@
       <c r="B43" s="220" t="s">
         <v>462</v>
       </c>
-      <c r="C43" s="280"/>
+      <c r="C43" s="278"/>
       <c r="D43" s="177" t="s">
         <v>650</v>
       </c>
@@ -5652,7 +5652,7 @@
       <c r="B44" s="220" t="s">
         <v>417</v>
       </c>
-      <c r="C44" s="280"/>
+      <c r="C44" s="278"/>
       <c r="D44" s="177" t="s">
         <v>651</v>
       </c>
@@ -5664,7 +5664,7 @@
       <c r="B45" s="220" t="s">
         <v>418</v>
       </c>
-      <c r="C45" s="280"/>
+      <c r="C45" s="278"/>
       <c r="D45" s="177" t="s">
         <v>11</v>
       </c>
@@ -5676,7 +5676,7 @@
       <c r="B46" s="220" t="s">
         <v>419</v>
       </c>
-      <c r="C46" s="280"/>
+      <c r="C46" s="278"/>
       <c r="D46" s="177" t="s">
         <v>11</v>
       </c>
@@ -5688,7 +5688,7 @@
       <c r="B47" s="220" t="s">
         <v>420</v>
       </c>
-      <c r="C47" s="280"/>
+      <c r="C47" s="278"/>
       <c r="D47" s="177" t="s">
         <v>11</v>
       </c>
@@ -5700,7 +5700,7 @@
       <c r="B48" s="220" t="s">
         <v>452</v>
       </c>
-      <c r="C48" s="280"/>
+      <c r="C48" s="278"/>
       <c r="D48" s="177" t="s">
         <v>609</v>
       </c>
@@ -5712,7 +5712,7 @@
       <c r="B49" s="220" t="s">
         <v>453</v>
       </c>
-      <c r="C49" s="280"/>
+      <c r="C49" s="278"/>
       <c r="D49" s="177" t="s">
         <v>610</v>
       </c>
@@ -5724,7 +5724,7 @@
       <c r="B50" s="220" t="s">
         <v>485</v>
       </c>
-      <c r="C50" s="280"/>
+      <c r="C50" s="278"/>
       <c r="D50" s="177" t="s">
         <v>633</v>
       </c>
@@ -5736,7 +5736,7 @@
       <c r="B51" s="220" t="s">
         <v>486</v>
       </c>
-      <c r="C51" s="280"/>
+      <c r="C51" s="278"/>
       <c r="D51" s="177" t="s">
         <v>634</v>
       </c>
@@ -5748,7 +5748,7 @@
       <c r="B52" s="220" t="s">
         <v>460</v>
       </c>
-      <c r="C52" s="280"/>
+      <c r="C52" s="278"/>
       <c r="D52" s="177" t="s">
         <v>611</v>
       </c>
@@ -5760,7 +5760,7 @@
       <c r="B53" s="220" t="s">
         <v>456</v>
       </c>
-      <c r="C53" s="280"/>
+      <c r="C53" s="278"/>
       <c r="D53" s="177" t="s">
         <v>11</v>
       </c>
@@ -5772,7 +5772,7 @@
       <c r="B54" s="220" t="s">
         <v>457</v>
       </c>
-      <c r="C54" s="280"/>
+      <c r="C54" s="278"/>
       <c r="D54" s="177" t="s">
         <v>11</v>
       </c>
@@ -5784,7 +5784,7 @@
       <c r="B55" s="220" t="s">
         <v>459</v>
       </c>
-      <c r="C55" s="280"/>
+      <c r="C55" s="278"/>
       <c r="D55" s="177" t="s">
         <v>11</v>
       </c>
@@ -5796,7 +5796,7 @@
       <c r="B56" s="220" t="s">
         <v>458</v>
       </c>
-      <c r="C56" s="280"/>
+      <c r="C56" s="278"/>
       <c r="D56" s="177" t="s">
         <v>11</v>
       </c>
@@ -5808,7 +5808,7 @@
       <c r="B57" s="220" t="s">
         <v>421</v>
       </c>
-      <c r="C57" s="280"/>
+      <c r="C57" s="278"/>
       <c r="D57" s="177" t="s">
         <v>612</v>
       </c>
@@ -5820,7 +5820,7 @@
       <c r="B58" s="220" t="s">
         <v>422</v>
       </c>
-      <c r="C58" s="280"/>
+      <c r="C58" s="278"/>
       <c r="D58" s="177" t="s">
         <v>613</v>
       </c>
@@ -5832,7 +5832,7 @@
       <c r="B59" s="220" t="s">
         <v>423</v>
       </c>
-      <c r="C59" s="280"/>
+      <c r="C59" s="278"/>
       <c r="D59" s="177" t="s">
         <v>614</v>
       </c>
@@ -6015,16 +6015,16 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="48"/>
-      <c r="B1" s="263" t="s">
+      <c r="B1" s="262" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="264"/>
-      <c r="D1" s="265"/>
-      <c r="E1" s="263" t="s">
+      <c r="C1" s="263"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="262" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="264"/>
-      <c r="G1" s="264"/>
+      <c r="F1" s="263"/>
+      <c r="G1" s="263"/>
       <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
@@ -7001,15 +7001,15 @@
   </sheetPr>
   <dimension ref="A1:CN196"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="3" width="12.69140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="34.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.69140625" style="1" customWidth="1"/>
     <col min="5" max="6" width="10.69140625" style="1" customWidth="1"/>
     <col min="7" max="9" width="12.69140625" style="1" customWidth="1"/>
     <col min="10" max="11" width="10.69140625" style="1" customWidth="1"/>
@@ -7066,94 +7066,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.4">
-      <c r="A1" s="266" t="s">
+      <c r="A1" s="265" t="s">
         <v>678</v>
       </c>
-      <c r="B1" s="266"/>
-      <c r="C1" s="266"/>
-      <c r="D1" s="266"/>
-      <c r="E1" s="267" t="s">
+      <c r="B1" s="265"/>
+      <c r="C1" s="265"/>
+      <c r="D1" s="265"/>
+      <c r="E1" s="266" t="s">
         <v>679</v>
       </c>
-      <c r="F1" s="268"/>
-      <c r="G1" s="268"/>
-      <c r="H1" s="268"/>
-      <c r="I1" s="268"/>
-      <c r="J1" s="268"/>
-      <c r="K1" s="268"/>
-      <c r="L1" s="269"/>
-      <c r="M1" s="270" t="s">
+      <c r="F1" s="267"/>
+      <c r="G1" s="267"/>
+      <c r="H1" s="267"/>
+      <c r="I1" s="267"/>
+      <c r="J1" s="267"/>
+      <c r="K1" s="267"/>
+      <c r="L1" s="268"/>
+      <c r="M1" s="269" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="270"/>
-      <c r="O1" s="270"/>
-      <c r="P1" s="270"/>
-      <c r="Q1" s="266" t="s">
+      <c r="N1" s="269"/>
+      <c r="O1" s="269"/>
+      <c r="P1" s="269"/>
+      <c r="Q1" s="265" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="266"/>
-      <c r="S1" s="266"/>
-      <c r="T1" s="266"/>
-      <c r="U1" s="270" t="s">
+      <c r="R1" s="265"/>
+      <c r="S1" s="265"/>
+      <c r="T1" s="265"/>
+      <c r="U1" s="269" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="270"/>
-      <c r="W1" s="270"/>
-      <c r="X1" s="270"/>
-      <c r="Y1" s="266" t="s">
+      <c r="V1" s="269"/>
+      <c r="W1" s="269"/>
+      <c r="X1" s="269"/>
+      <c r="Y1" s="265" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" s="266"/>
-      <c r="AA1" s="266"/>
-      <c r="AB1" s="266"/>
-      <c r="AC1" s="270" t="s">
+      <c r="Z1" s="265"/>
+      <c r="AA1" s="265"/>
+      <c r="AB1" s="265"/>
+      <c r="AC1" s="269" t="s">
         <v>83</v>
       </c>
-      <c r="AD1" s="270"/>
-      <c r="AE1" s="270"/>
-      <c r="AF1" s="270"/>
-      <c r="AG1" s="266" t="s">
+      <c r="AD1" s="269"/>
+      <c r="AE1" s="269"/>
+      <c r="AF1" s="269"/>
+      <c r="AG1" s="265" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="266"/>
-      <c r="AI1" s="266"/>
-      <c r="AJ1" s="266"/>
-      <c r="AK1" s="270" t="s">
+      <c r="AH1" s="265"/>
+      <c r="AI1" s="265"/>
+      <c r="AJ1" s="265"/>
+      <c r="AK1" s="269" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="270"/>
-      <c r="AM1" s="270"/>
-      <c r="AN1" s="270"/>
-      <c r="AO1" s="266" t="s">
+      <c r="AL1" s="269"/>
+      <c r="AM1" s="269"/>
+      <c r="AN1" s="269"/>
+      <c r="AO1" s="265" t="s">
         <v>86</v>
       </c>
-      <c r="AP1" s="266"/>
-      <c r="AQ1" s="266"/>
-      <c r="AR1" s="266"/>
-      <c r="AS1" s="270" t="s">
+      <c r="AP1" s="265"/>
+      <c r="AQ1" s="265"/>
+      <c r="AR1" s="265"/>
+      <c r="AS1" s="269" t="s">
         <v>87</v>
       </c>
-      <c r="AT1" s="270"/>
-      <c r="AU1" s="270"/>
-      <c r="AV1" s="270"/>
-      <c r="AW1" s="266" t="s">
+      <c r="AT1" s="269"/>
+      <c r="AU1" s="269"/>
+      <c r="AV1" s="269"/>
+      <c r="AW1" s="265" t="s">
         <v>88</v>
       </c>
-      <c r="AX1" s="266"/>
-      <c r="AY1" s="266"/>
-      <c r="AZ1" s="266"/>
-      <c r="BA1" s="270" t="s">
+      <c r="AX1" s="265"/>
+      <c r="AY1" s="265"/>
+      <c r="AZ1" s="265"/>
+      <c r="BA1" s="269" t="s">
         <v>89</v>
       </c>
-      <c r="BB1" s="270"/>
-      <c r="BC1" s="270"/>
-      <c r="BD1" s="270"/>
-      <c r="BE1" s="266" t="s">
+      <c r="BB1" s="269"/>
+      <c r="BC1" s="269"/>
+      <c r="BD1" s="269"/>
+      <c r="BE1" s="265" t="s">
         <v>90</v>
       </c>
-      <c r="BF1" s="266"/>
-      <c r="BG1" s="266"/>
-      <c r="BH1" s="266"/>
+      <c r="BF1" s="265"/>
+      <c r="BG1" s="265"/>
+      <c r="BH1" s="265"/>
     </row>
     <row r="2" spans="1:60" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -24323,7 +24323,7 @@
   </sheetPr>
   <dimension ref="A1:CN171"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="BE1" sqref="BE1:BH1"/>
     </sheetView>
@@ -24388,94 +24388,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:92" x14ac:dyDescent="0.4">
-      <c r="A1" s="266" t="s">
+      <c r="A1" s="265" t="s">
         <v>678</v>
       </c>
-      <c r="B1" s="266"/>
-      <c r="C1" s="266"/>
-      <c r="D1" s="266"/>
-      <c r="E1" s="267" t="s">
+      <c r="B1" s="265"/>
+      <c r="C1" s="265"/>
+      <c r="D1" s="265"/>
+      <c r="E1" s="266" t="s">
         <v>679</v>
       </c>
-      <c r="F1" s="268"/>
-      <c r="G1" s="268"/>
-      <c r="H1" s="268"/>
-      <c r="I1" s="268"/>
-      <c r="J1" s="268"/>
-      <c r="K1" s="268"/>
-      <c r="L1" s="269"/>
-      <c r="M1" s="274" t="s">
+      <c r="F1" s="267"/>
+      <c r="G1" s="267"/>
+      <c r="H1" s="267"/>
+      <c r="I1" s="267"/>
+      <c r="J1" s="267"/>
+      <c r="K1" s="267"/>
+      <c r="L1" s="268"/>
+      <c r="M1" s="273" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="275"/>
-      <c r="O1" s="275"/>
-      <c r="P1" s="276"/>
-      <c r="Q1" s="267" t="s">
+      <c r="N1" s="274"/>
+      <c r="O1" s="274"/>
+      <c r="P1" s="275"/>
+      <c r="Q1" s="266" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="268"/>
-      <c r="S1" s="268"/>
-      <c r="T1" s="268"/>
-      <c r="U1" s="274" t="s">
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="267"/>
+      <c r="U1" s="273" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="275"/>
-      <c r="W1" s="275"/>
-      <c r="X1" s="276"/>
-      <c r="Y1" s="271" t="s">
+      <c r="V1" s="274"/>
+      <c r="W1" s="274"/>
+      <c r="X1" s="275"/>
+      <c r="Y1" s="270" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" s="272"/>
-      <c r="AA1" s="272"/>
-      <c r="AB1" s="273"/>
-      <c r="AC1" s="274" t="s">
+      <c r="Z1" s="271"/>
+      <c r="AA1" s="271"/>
+      <c r="AB1" s="272"/>
+      <c r="AC1" s="273" t="s">
         <v>83</v>
       </c>
-      <c r="AD1" s="275"/>
-      <c r="AE1" s="275"/>
-      <c r="AF1" s="276"/>
-      <c r="AG1" s="271" t="s">
+      <c r="AD1" s="274"/>
+      <c r="AE1" s="274"/>
+      <c r="AF1" s="275"/>
+      <c r="AG1" s="270" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="272"/>
-      <c r="AI1" s="272"/>
-      <c r="AJ1" s="273"/>
-      <c r="AK1" s="274" t="s">
+      <c r="AH1" s="271"/>
+      <c r="AI1" s="271"/>
+      <c r="AJ1" s="272"/>
+      <c r="AK1" s="273" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="275"/>
-      <c r="AM1" s="275"/>
-      <c r="AN1" s="276"/>
-      <c r="AO1" s="271" t="s">
+      <c r="AL1" s="274"/>
+      <c r="AM1" s="274"/>
+      <c r="AN1" s="275"/>
+      <c r="AO1" s="270" t="s">
         <v>86</v>
       </c>
-      <c r="AP1" s="272"/>
-      <c r="AQ1" s="272"/>
-      <c r="AR1" s="273"/>
-      <c r="AS1" s="274" t="s">
+      <c r="AP1" s="271"/>
+      <c r="AQ1" s="271"/>
+      <c r="AR1" s="272"/>
+      <c r="AS1" s="273" t="s">
         <v>87</v>
       </c>
-      <c r="AT1" s="275"/>
-      <c r="AU1" s="275"/>
-      <c r="AV1" s="276"/>
-      <c r="AW1" s="271" t="s">
+      <c r="AT1" s="274"/>
+      <c r="AU1" s="274"/>
+      <c r="AV1" s="275"/>
+      <c r="AW1" s="270" t="s">
         <v>88</v>
       </c>
-      <c r="AX1" s="272"/>
-      <c r="AY1" s="272"/>
-      <c r="AZ1" s="273"/>
-      <c r="BA1" s="274" t="s">
+      <c r="AX1" s="271"/>
+      <c r="AY1" s="271"/>
+      <c r="AZ1" s="272"/>
+      <c r="BA1" s="273" t="s">
         <v>89</v>
       </c>
-      <c r="BB1" s="275"/>
-      <c r="BC1" s="275"/>
-      <c r="BD1" s="276"/>
-      <c r="BE1" s="271" t="s">
+      <c r="BB1" s="274"/>
+      <c r="BC1" s="274"/>
+      <c r="BD1" s="275"/>
+      <c r="BE1" s="270" t="s">
         <v>90</v>
       </c>
-      <c r="BF1" s="272"/>
-      <c r="BG1" s="272"/>
-      <c r="BH1" s="273"/>
+      <c r="BF1" s="271"/>
+      <c r="BG1" s="271"/>
+      <c r="BH1" s="272"/>
     </row>
     <row r="2" spans="1:92" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -29612,7 +29612,7 @@
   </sheetPr>
   <dimension ref="A1:BH62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="BH2" sqref="BH1:BH1048576"/>
     </sheetView>
@@ -29677,94 +29677,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.4">
-      <c r="A1" s="266" t="s">
+      <c r="A1" s="265" t="s">
         <v>678</v>
       </c>
-      <c r="B1" s="266"/>
-      <c r="C1" s="266"/>
-      <c r="D1" s="266"/>
-      <c r="E1" s="267" t="s">
+      <c r="B1" s="265"/>
+      <c r="C1" s="265"/>
+      <c r="D1" s="265"/>
+      <c r="E1" s="266" t="s">
         <v>679</v>
       </c>
-      <c r="F1" s="268"/>
-      <c r="G1" s="268"/>
-      <c r="H1" s="268"/>
-      <c r="I1" s="268"/>
-      <c r="J1" s="268"/>
-      <c r="K1" s="268"/>
-      <c r="L1" s="269"/>
-      <c r="M1" s="277" t="s">
+      <c r="F1" s="267"/>
+      <c r="G1" s="267"/>
+      <c r="H1" s="267"/>
+      <c r="I1" s="267"/>
+      <c r="J1" s="267"/>
+      <c r="K1" s="267"/>
+      <c r="L1" s="268"/>
+      <c r="M1" s="276" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="277"/>
-      <c r="O1" s="277"/>
-      <c r="P1" s="277"/>
-      <c r="Q1" s="266" t="s">
+      <c r="N1" s="276"/>
+      <c r="O1" s="276"/>
+      <c r="P1" s="276"/>
+      <c r="Q1" s="265" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="266"/>
-      <c r="S1" s="266"/>
-      <c r="T1" s="266"/>
-      <c r="U1" s="277" t="s">
+      <c r="R1" s="265"/>
+      <c r="S1" s="265"/>
+      <c r="T1" s="265"/>
+      <c r="U1" s="276" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="277"/>
-      <c r="W1" s="277"/>
-      <c r="X1" s="277"/>
-      <c r="Y1" s="266" t="s">
+      <c r="V1" s="276"/>
+      <c r="W1" s="276"/>
+      <c r="X1" s="276"/>
+      <c r="Y1" s="265" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" s="266"/>
-      <c r="AA1" s="266"/>
-      <c r="AB1" s="266"/>
-      <c r="AC1" s="277" t="s">
+      <c r="Z1" s="265"/>
+      <c r="AA1" s="265"/>
+      <c r="AB1" s="265"/>
+      <c r="AC1" s="276" t="s">
         <v>83</v>
       </c>
-      <c r="AD1" s="277"/>
-      <c r="AE1" s="277"/>
-      <c r="AF1" s="277"/>
-      <c r="AG1" s="266" t="s">
+      <c r="AD1" s="276"/>
+      <c r="AE1" s="276"/>
+      <c r="AF1" s="276"/>
+      <c r="AG1" s="265" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="266"/>
-      <c r="AI1" s="266"/>
-      <c r="AJ1" s="266"/>
-      <c r="AK1" s="277" t="s">
+      <c r="AH1" s="265"/>
+      <c r="AI1" s="265"/>
+      <c r="AJ1" s="265"/>
+      <c r="AK1" s="276" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="277"/>
-      <c r="AM1" s="277"/>
-      <c r="AN1" s="277"/>
-      <c r="AO1" s="266" t="s">
+      <c r="AL1" s="276"/>
+      <c r="AM1" s="276"/>
+      <c r="AN1" s="276"/>
+      <c r="AO1" s="265" t="s">
         <v>86</v>
       </c>
-      <c r="AP1" s="266"/>
-      <c r="AQ1" s="266"/>
-      <c r="AR1" s="266"/>
-      <c r="AS1" s="277" t="s">
+      <c r="AP1" s="265"/>
+      <c r="AQ1" s="265"/>
+      <c r="AR1" s="265"/>
+      <c r="AS1" s="276" t="s">
         <v>87</v>
       </c>
-      <c r="AT1" s="277"/>
-      <c r="AU1" s="277"/>
-      <c r="AV1" s="277"/>
-      <c r="AW1" s="266" t="s">
+      <c r="AT1" s="276"/>
+      <c r="AU1" s="276"/>
+      <c r="AV1" s="276"/>
+      <c r="AW1" s="265" t="s">
         <v>88</v>
       </c>
-      <c r="AX1" s="266"/>
-      <c r="AY1" s="266"/>
-      <c r="AZ1" s="266"/>
-      <c r="BA1" s="277" t="s">
+      <c r="AX1" s="265"/>
+      <c r="AY1" s="265"/>
+      <c r="AZ1" s="265"/>
+      <c r="BA1" s="276" t="s">
         <v>89</v>
       </c>
-      <c r="BB1" s="277"/>
-      <c r="BC1" s="277"/>
-      <c r="BD1" s="277"/>
-      <c r="BE1" s="266" t="s">
+      <c r="BB1" s="276"/>
+      <c r="BC1" s="276"/>
+      <c r="BD1" s="276"/>
+      <c r="BE1" s="265" t="s">
         <v>90</v>
       </c>
-      <c r="BF1" s="266"/>
-      <c r="BG1" s="266"/>
-      <c r="BH1" s="266"/>
+      <c r="BF1" s="265"/>
+      <c r="BG1" s="265"/>
+      <c r="BH1" s="265"/>
     </row>
     <row r="2" spans="1:60" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -36359,94 +36359,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.4">
-      <c r="A1" s="266" t="s">
+      <c r="A1" s="265" t="s">
         <v>678</v>
       </c>
-      <c r="B1" s="266"/>
-      <c r="C1" s="266"/>
-      <c r="D1" s="266"/>
-      <c r="E1" s="267" t="s">
+      <c r="B1" s="265"/>
+      <c r="C1" s="265"/>
+      <c r="D1" s="265"/>
+      <c r="E1" s="266" t="s">
         <v>679</v>
       </c>
-      <c r="F1" s="268"/>
-      <c r="G1" s="268"/>
-      <c r="H1" s="268"/>
-      <c r="I1" s="268"/>
-      <c r="J1" s="268"/>
-      <c r="K1" s="268"/>
-      <c r="L1" s="269"/>
-      <c r="M1" s="277" t="s">
+      <c r="F1" s="267"/>
+      <c r="G1" s="267"/>
+      <c r="H1" s="267"/>
+      <c r="I1" s="267"/>
+      <c r="J1" s="267"/>
+      <c r="K1" s="267"/>
+      <c r="L1" s="268"/>
+      <c r="M1" s="276" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="277"/>
-      <c r="O1" s="277"/>
-      <c r="P1" s="277"/>
-      <c r="Q1" s="267" t="s">
+      <c r="N1" s="276"/>
+      <c r="O1" s="276"/>
+      <c r="P1" s="276"/>
+      <c r="Q1" s="266" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="268"/>
-      <c r="S1" s="268"/>
-      <c r="T1" s="268"/>
-      <c r="U1" s="277" t="s">
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="267"/>
+      <c r="U1" s="276" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="277"/>
-      <c r="W1" s="277"/>
-      <c r="X1" s="277"/>
-      <c r="Y1" s="267" t="s">
+      <c r="V1" s="276"/>
+      <c r="W1" s="276"/>
+      <c r="X1" s="276"/>
+      <c r="Y1" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" s="268"/>
-      <c r="AA1" s="268"/>
-      <c r="AB1" s="268"/>
-      <c r="AC1" s="277" t="s">
+      <c r="Z1" s="267"/>
+      <c r="AA1" s="267"/>
+      <c r="AB1" s="267"/>
+      <c r="AC1" s="276" t="s">
         <v>83</v>
       </c>
-      <c r="AD1" s="277"/>
-      <c r="AE1" s="277"/>
-      <c r="AF1" s="277"/>
-      <c r="AG1" s="267" t="s">
+      <c r="AD1" s="276"/>
+      <c r="AE1" s="276"/>
+      <c r="AF1" s="276"/>
+      <c r="AG1" s="266" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="268"/>
-      <c r="AI1" s="268"/>
-      <c r="AJ1" s="268"/>
-      <c r="AK1" s="277" t="s">
+      <c r="AH1" s="267"/>
+      <c r="AI1" s="267"/>
+      <c r="AJ1" s="267"/>
+      <c r="AK1" s="276" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="277"/>
-      <c r="AM1" s="277"/>
-      <c r="AN1" s="277"/>
-      <c r="AO1" s="267" t="s">
+      <c r="AL1" s="276"/>
+      <c r="AM1" s="276"/>
+      <c r="AN1" s="276"/>
+      <c r="AO1" s="266" t="s">
         <v>86</v>
       </c>
-      <c r="AP1" s="268"/>
-      <c r="AQ1" s="268"/>
-      <c r="AR1" s="268"/>
-      <c r="AS1" s="277" t="s">
+      <c r="AP1" s="267"/>
+      <c r="AQ1" s="267"/>
+      <c r="AR1" s="267"/>
+      <c r="AS1" s="276" t="s">
         <v>87</v>
       </c>
-      <c r="AT1" s="277"/>
-      <c r="AU1" s="277"/>
-      <c r="AV1" s="277"/>
-      <c r="AW1" s="267" t="s">
+      <c r="AT1" s="276"/>
+      <c r="AU1" s="276"/>
+      <c r="AV1" s="276"/>
+      <c r="AW1" s="266" t="s">
         <v>88</v>
       </c>
-      <c r="AX1" s="268"/>
-      <c r="AY1" s="268"/>
-      <c r="AZ1" s="268"/>
-      <c r="BA1" s="277" t="s">
+      <c r="AX1" s="267"/>
+      <c r="AY1" s="267"/>
+      <c r="AZ1" s="267"/>
+      <c r="BA1" s="276" t="s">
         <v>89</v>
       </c>
-      <c r="BB1" s="277"/>
-      <c r="BC1" s="277"/>
-      <c r="BD1" s="277"/>
-      <c r="BE1" s="267" t="s">
+      <c r="BB1" s="276"/>
+      <c r="BC1" s="276"/>
+      <c r="BD1" s="276"/>
+      <c r="BE1" s="266" t="s">
         <v>90</v>
       </c>
-      <c r="BF1" s="268"/>
-      <c r="BG1" s="268"/>
-      <c r="BH1" s="268"/>
+      <c r="BF1" s="267"/>
+      <c r="BG1" s="267"/>
+      <c r="BH1" s="267"/>
     </row>
     <row r="2" spans="1:60" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -38327,7 +38327,7 @@
       <c r="B2" s="158" t="s">
         <v>493</v>
       </c>
-      <c r="C2" s="278" t="s">
+      <c r="C2" s="277" t="s">
         <v>514</v>
       </c>
       <c r="D2" s="159" t="s">
@@ -38341,7 +38341,7 @@
       <c r="B3" s="161" t="s">
         <v>494</v>
       </c>
-      <c r="C3" s="280"/>
+      <c r="C3" s="278"/>
       <c r="D3" s="162" t="s">
         <v>516</v>
       </c>
@@ -38353,7 +38353,7 @@
       <c r="B4" s="161" t="s">
         <v>495</v>
       </c>
-      <c r="C4" s="280"/>
+      <c r="C4" s="278"/>
       <c r="D4" s="162" t="s">
         <v>11</v>
       </c>
@@ -38365,7 +38365,7 @@
       <c r="B5" s="161" t="s">
         <v>496</v>
       </c>
-      <c r="C5" s="280"/>
+      <c r="C5" s="278"/>
       <c r="D5" s="162" t="s">
         <v>11</v>
       </c>
@@ -38377,7 +38377,7 @@
       <c r="B6" s="161" t="s">
         <v>497</v>
       </c>
-      <c r="C6" s="280"/>
+      <c r="C6" s="278"/>
       <c r="D6" s="162" t="s">
         <v>11</v>
       </c>
@@ -38389,7 +38389,7 @@
       <c r="B7" s="161" t="s">
         <v>498</v>
       </c>
-      <c r="C7" s="280"/>
+      <c r="C7" s="278"/>
       <c r="D7" s="162" t="s">
         <v>11</v>
       </c>
@@ -38401,7 +38401,7 @@
       <c r="B8" s="161" t="s">
         <v>499</v>
       </c>
-      <c r="C8" s="280"/>
+      <c r="C8" s="278"/>
       <c r="D8" s="162" t="s">
         <v>11</v>
       </c>
@@ -38413,7 +38413,7 @@
       <c r="B9" s="161" t="s">
         <v>500</v>
       </c>
-      <c r="C9" s="280"/>
+      <c r="C9" s="278"/>
       <c r="D9" s="162" t="s">
         <v>11</v>
       </c>
@@ -38425,7 +38425,7 @@
       <c r="B10" s="161" t="s">
         <v>501</v>
       </c>
-      <c r="C10" s="280"/>
+      <c r="C10" s="278"/>
       <c r="D10" s="162" t="s">
         <v>11</v>
       </c>
@@ -38449,7 +38449,7 @@
       <c r="B12" s="166" t="s">
         <v>240</v>
       </c>
-      <c r="C12" s="278" t="s">
+      <c r="C12" s="277" t="s">
         <v>517</v>
       </c>
       <c r="D12" s="159" t="s">
@@ -38463,7 +38463,7 @@
       <c r="B13" s="167" t="s">
         <v>241</v>
       </c>
-      <c r="C13" s="280"/>
+      <c r="C13" s="278"/>
       <c r="D13" s="162" t="s">
         <v>519</v>
       </c>
@@ -38475,7 +38475,7 @@
       <c r="B14" s="167" t="s">
         <v>242</v>
       </c>
-      <c r="C14" s="280"/>
+      <c r="C14" s="278"/>
       <c r="D14" s="162" t="s">
         <v>11</v>
       </c>
@@ -38487,7 +38487,7 @@
       <c r="B15" s="167" t="s">
         <v>243</v>
       </c>
-      <c r="C15" s="280"/>
+      <c r="C15" s="278"/>
       <c r="D15" s="162" t="s">
         <v>11</v>
       </c>
@@ -38499,7 +38499,7 @@
       <c r="B16" s="167" t="s">
         <v>244</v>
       </c>
-      <c r="C16" s="280"/>
+      <c r="C16" s="278"/>
       <c r="D16" s="162" t="s">
         <v>11</v>
       </c>
@@ -38523,7 +38523,7 @@
       <c r="B18" s="169" t="s">
         <v>246</v>
       </c>
-      <c r="C18" s="278" t="s">
+      <c r="C18" s="277" t="s">
         <v>109</v>
       </c>
       <c r="D18" s="159" t="s">
@@ -38537,7 +38537,7 @@
       <c r="B19" s="171" t="s">
         <v>247</v>
       </c>
-      <c r="C19" s="280"/>
+      <c r="C19" s="278"/>
       <c r="D19" s="162" t="s">
         <v>521</v>
       </c>
@@ -38549,7 +38549,7 @@
       <c r="B20" s="170" t="s">
         <v>248</v>
       </c>
-      <c r="C20" s="280"/>
+      <c r="C20" s="278"/>
       <c r="D20" s="162" t="s">
         <v>522</v>
       </c>
@@ -38561,7 +38561,7 @@
       <c r="B21" s="170" t="s">
         <v>249</v>
       </c>
-      <c r="C21" s="280"/>
+      <c r="C21" s="278"/>
       <c r="D21" s="162" t="s">
         <v>523</v>
       </c>
@@ -38573,7 +38573,7 @@
       <c r="B22" s="170" t="s">
         <v>250</v>
       </c>
-      <c r="C22" s="280"/>
+      <c r="C22" s="278"/>
       <c r="D22" s="162" t="s">
         <v>524</v>
       </c>
@@ -38585,7 +38585,7 @@
       <c r="B23" s="170" t="s">
         <v>251</v>
       </c>
-      <c r="C23" s="280"/>
+      <c r="C23" s="278"/>
       <c r="D23" s="162" t="s">
         <v>525</v>
       </c>
@@ -38597,7 +38597,7 @@
       <c r="B24" s="170" t="s">
         <v>491</v>
       </c>
-      <c r="C24" s="280"/>
+      <c r="C24" s="278"/>
       <c r="D24" s="162" t="s">
         <v>11</v>
       </c>
@@ -38609,7 +38609,7 @@
       <c r="B25" s="170" t="s">
         <v>492</v>
       </c>
-      <c r="C25" s="280"/>
+      <c r="C25" s="278"/>
       <c r="D25" s="162" t="s">
         <v>526</v>
       </c>
@@ -38621,7 +38621,7 @@
       <c r="B26" s="170" t="s">
         <v>252</v>
       </c>
-      <c r="C26" s="280"/>
+      <c r="C26" s="278"/>
       <c r="D26" s="162" t="s">
         <v>11</v>
       </c>
@@ -38633,7 +38633,7 @@
       <c r="B27" s="171" t="s">
         <v>502</v>
       </c>
-      <c r="C27" s="280"/>
+      <c r="C27" s="278"/>
       <c r="D27" s="162" t="s">
         <v>527</v>
       </c>
@@ -38657,7 +38657,7 @@
       <c r="B29" s="173" t="s">
         <v>253</v>
       </c>
-      <c r="C29" s="278" t="s">
+      <c r="C29" s="277" t="s">
         <v>529</v>
       </c>
       <c r="D29" s="159" t="s">
@@ -38671,7 +38671,7 @@
       <c r="B30" s="175" t="s">
         <v>254</v>
       </c>
-      <c r="C30" s="280"/>
+      <c r="C30" s="278"/>
       <c r="D30" s="177" t="s">
         <v>675</v>
       </c>
@@ -38683,7 +38683,7 @@
       <c r="B31" s="176" t="s">
         <v>255</v>
       </c>
-      <c r="C31" s="280"/>
+      <c r="C31" s="278"/>
       <c r="D31" s="162" t="s">
         <v>531</v>
       </c>
@@ -38695,7 +38695,7 @@
       <c r="B32" s="176" t="s">
         <v>256</v>
       </c>
-      <c r="C32" s="280"/>
+      <c r="C32" s="278"/>
       <c r="D32" s="162" t="s">
         <v>532</v>
       </c>
@@ -38707,7 +38707,7 @@
       <c r="B33" s="176" t="s">
         <v>257</v>
       </c>
-      <c r="C33" s="280"/>
+      <c r="C33" s="278"/>
       <c r="D33" s="177" t="s">
         <v>533</v>
       </c>
@@ -38719,7 +38719,7 @@
       <c r="B34" s="175" t="s">
         <v>258</v>
       </c>
-      <c r="C34" s="280"/>
+      <c r="C34" s="278"/>
       <c r="D34" s="162" t="s">
         <v>534</v>
       </c>
@@ -38731,7 +38731,7 @@
       <c r="B35" s="176" t="s">
         <v>259</v>
       </c>
-      <c r="C35" s="280"/>
+      <c r="C35" s="278"/>
       <c r="D35" s="162" t="s">
         <v>535</v>
       </c>
@@ -38743,7 +38743,7 @@
       <c r="B36" s="175" t="s">
         <v>260</v>
       </c>
-      <c r="C36" s="280"/>
+      <c r="C36" s="278"/>
       <c r="D36" s="162" t="s">
         <v>535</v>
       </c>
@@ -38755,7 +38755,7 @@
       <c r="B37" s="176" t="s">
         <v>261</v>
       </c>
-      <c r="C37" s="280"/>
+      <c r="C37" s="278"/>
       <c r="D37" s="162" t="s">
         <v>536</v>
       </c>
@@ -38767,7 +38767,7 @@
       <c r="B38" s="175" t="s">
         <v>262</v>
       </c>
-      <c r="C38" s="280"/>
+      <c r="C38" s="278"/>
       <c r="D38" s="162" t="s">
         <v>536</v>
       </c>
@@ -38779,7 +38779,7 @@
       <c r="B39" s="176" t="s">
         <v>263</v>
       </c>
-      <c r="C39" s="280"/>
+      <c r="C39" s="278"/>
       <c r="D39" s="177" t="s">
         <v>670</v>
       </c>
@@ -38791,7 +38791,7 @@
       <c r="B40" s="175" t="s">
         <v>264</v>
       </c>
-      <c r="C40" s="280"/>
+      <c r="C40" s="278"/>
       <c r="D40" s="162" t="s">
         <v>537</v>
       </c>
@@ -38803,7 +38803,7 @@
       <c r="B41" s="176" t="s">
         <v>265</v>
       </c>
-      <c r="C41" s="280"/>
+      <c r="C41" s="278"/>
       <c r="D41" s="162" t="s">
         <v>538</v>
       </c>
@@ -38840,7 +38840,7 @@
       <c r="B44" s="185" t="s">
         <v>266</v>
       </c>
-      <c r="C44" s="278" t="s">
+      <c r="C44" s="277" t="s">
         <v>541</v>
       </c>
       <c r="D44" s="186" t="s">
@@ -38854,7 +38854,7 @@
       <c r="B45" s="188" t="s">
         <v>267</v>
       </c>
-      <c r="C45" s="280"/>
+      <c r="C45" s="278"/>
       <c r="D45" s="162" t="s">
         <v>11</v>
       </c>
@@ -38866,7 +38866,7 @@
       <c r="B46" s="188" t="s">
         <v>268</v>
       </c>
-      <c r="C46" s="280"/>
+      <c r="C46" s="278"/>
       <c r="D46" s="162" t="s">
         <v>542</v>
       </c>
@@ -38878,7 +38878,7 @@
       <c r="B47" s="188" t="s">
         <v>269</v>
       </c>
-      <c r="C47" s="280"/>
+      <c r="C47" s="278"/>
       <c r="D47" s="177" t="s">
         <v>543</v>
       </c>
@@ -38890,7 +38890,7 @@
       <c r="B48" s="188" t="s">
         <v>270</v>
       </c>
-      <c r="C48" s="280"/>
+      <c r="C48" s="278"/>
       <c r="D48" s="162" t="s">
         <v>11</v>
       </c>
@@ -38902,7 +38902,7 @@
       <c r="B49" s="188" t="s">
         <v>271</v>
       </c>
-      <c r="C49" s="280"/>
+      <c r="C49" s="278"/>
       <c r="D49" s="162" t="s">
         <v>544</v>
       </c>
@@ -38914,7 +38914,7 @@
       <c r="B50" s="188" t="s">
         <v>272</v>
       </c>
-      <c r="C50" s="280"/>
+      <c r="C50" s="278"/>
       <c r="D50" s="162" t="s">
         <v>11</v>
       </c>
@@ -38926,7 +38926,7 @@
       <c r="B51" s="188" t="s">
         <v>273</v>
       </c>
-      <c r="C51" s="280"/>
+      <c r="C51" s="278"/>
       <c r="D51" s="177" t="s">
         <v>676</v>
       </c>
@@ -38938,7 +38938,7 @@
       <c r="B52" s="188" t="s">
         <v>274</v>
       </c>
-      <c r="C52" s="280"/>
+      <c r="C52" s="278"/>
       <c r="D52" s="177" t="s">
         <v>543</v>
       </c>
@@ -38962,7 +38962,7 @@
       <c r="B54" s="191" t="s">
         <v>276</v>
       </c>
-      <c r="C54" s="278" t="s">
+      <c r="C54" s="277" t="s">
         <v>545</v>
       </c>
       <c r="D54" s="177" t="s">
@@ -38976,7 +38976,7 @@
       <c r="B55" s="191" t="s">
         <v>277</v>
       </c>
-      <c r="C55" s="280"/>
+      <c r="C55" s="278"/>
       <c r="D55" s="162" t="s">
         <v>547</v>
       </c>
@@ -38988,7 +38988,7 @@
       <c r="B56" s="191" t="s">
         <v>278</v>
       </c>
-      <c r="C56" s="280"/>
+      <c r="C56" s="278"/>
       <c r="D56" s="162" t="s">
         <v>548</v>
       </c>
@@ -39012,7 +39012,7 @@
       <c r="B58" s="254" t="s">
         <v>280</v>
       </c>
-      <c r="C58" s="278" t="s">
+      <c r="C58" s="277" t="s">
         <v>550</v>
       </c>
       <c r="D58" s="159" t="s">
@@ -39038,7 +39038,7 @@
       <c r="B60" s="193" t="s">
         <v>281</v>
       </c>
-      <c r="C60" s="278" t="s">
+      <c r="C60" s="277" t="s">
         <v>552</v>
       </c>
       <c r="D60" s="162" t="s">
@@ -39052,7 +39052,7 @@
       <c r="B61" s="193" t="s">
         <v>282</v>
       </c>
-      <c r="C61" s="280"/>
+      <c r="C61" s="278"/>
       <c r="D61" s="162" t="s">
         <v>554</v>
       </c>
@@ -39064,7 +39064,7 @@
       <c r="B62" s="193" t="s">
         <v>283</v>
       </c>
-      <c r="C62" s="280"/>
+      <c r="C62" s="278"/>
       <c r="D62" s="162" t="s">
         <v>555</v>
       </c>
@@ -39076,7 +39076,7 @@
       <c r="B63" s="193" t="s">
         <v>284</v>
       </c>
-      <c r="C63" s="280"/>
+      <c r="C63" s="278"/>
       <c r="D63" s="162" t="s">
         <v>556</v>
       </c>
@@ -39088,7 +39088,7 @@
       <c r="B64" s="193" t="s">
         <v>285</v>
       </c>
-      <c r="C64" s="280"/>
+      <c r="C64" s="278"/>
       <c r="D64" s="162" t="s">
         <v>557</v>
       </c>
@@ -39100,7 +39100,7 @@
       <c r="B65" s="193" t="s">
         <v>286</v>
       </c>
-      <c r="C65" s="280"/>
+      <c r="C65" s="278"/>
       <c r="D65" s="162" t="s">
         <v>558</v>
       </c>
@@ -39112,7 +39112,7 @@
       <c r="B66" s="193" t="s">
         <v>287</v>
       </c>
-      <c r="C66" s="280"/>
+      <c r="C66" s="278"/>
       <c r="D66" s="162" t="s">
         <v>559</v>
       </c>
@@ -39136,7 +39136,7 @@
       <c r="B68" s="197" t="s">
         <v>289</v>
       </c>
-      <c r="C68" s="278" t="s">
+      <c r="C68" s="277" t="s">
         <v>561</v>
       </c>
       <c r="D68" s="159" t="s">
@@ -39150,7 +39150,7 @@
       <c r="B69" s="199" t="s">
         <v>290</v>
       </c>
-      <c r="C69" s="280"/>
+      <c r="C69" s="278"/>
       <c r="D69" s="162" t="s">
         <v>11</v>
       </c>
@@ -39162,7 +39162,7 @@
       <c r="B70" s="199" t="s">
         <v>291</v>
       </c>
-      <c r="C70" s="280"/>
+      <c r="C70" s="278"/>
       <c r="D70" s="162" t="s">
         <v>11</v>
       </c>
@@ -39174,7 +39174,7 @@
       <c r="B71" s="199" t="s">
         <v>292</v>
       </c>
-      <c r="C71" s="280"/>
+      <c r="C71" s="278"/>
       <c r="D71" s="162" t="s">
         <v>11</v>
       </c>
@@ -39186,7 +39186,7 @@
       <c r="B72" s="199" t="s">
         <v>293</v>
       </c>
-      <c r="C72" s="280"/>
+      <c r="C72" s="278"/>
       <c r="D72" s="162" t="s">
         <v>563</v>
       </c>
@@ -39198,7 +39198,7 @@
       <c r="B73" s="199" t="s">
         <v>294</v>
       </c>
-      <c r="C73" s="280"/>
+      <c r="C73" s="278"/>
       <c r="D73" s="162" t="s">
         <v>11</v>
       </c>
@@ -39210,7 +39210,7 @@
       <c r="B74" s="199" t="s">
         <v>295</v>
       </c>
-      <c r="C74" s="280"/>
+      <c r="C74" s="278"/>
       <c r="D74" s="162" t="s">
         <v>11</v>
       </c>
@@ -39222,7 +39222,7 @@
       <c r="B75" s="199" t="s">
         <v>296</v>
       </c>
-      <c r="C75" s="280"/>
+      <c r="C75" s="278"/>
       <c r="D75" s="162" t="s">
         <v>11</v>
       </c>
@@ -39234,7 +39234,7 @@
       <c r="B76" s="199" t="s">
         <v>297</v>
       </c>
-      <c r="C76" s="280"/>
+      <c r="C76" s="278"/>
       <c r="D76" s="162" t="s">
         <v>11</v>
       </c>
@@ -39246,7 +39246,7 @@
       <c r="B77" s="199" t="s">
         <v>298</v>
       </c>
-      <c r="C77" s="280"/>
+      <c r="C77" s="278"/>
       <c r="D77" s="162" t="s">
         <v>563</v>
       </c>
@@ -39258,7 +39258,7 @@
       <c r="B78" s="199" t="s">
         <v>299</v>
       </c>
-      <c r="C78" s="280"/>
+      <c r="C78" s="278"/>
       <c r="D78" s="162" t="s">
         <v>11</v>
       </c>
@@ -39270,7 +39270,7 @@
       <c r="B79" s="199" t="s">
         <v>300</v>
       </c>
-      <c r="C79" s="280"/>
+      <c r="C79" s="278"/>
       <c r="D79" s="162" t="s">
         <v>11</v>
       </c>
@@ -39282,7 +39282,7 @@
       <c r="B80" s="200" t="s">
         <v>301</v>
       </c>
-      <c r="C80" s="280"/>
+      <c r="C80" s="278"/>
       <c r="D80" s="162" t="s">
         <v>11</v>
       </c>
@@ -39294,7 +39294,7 @@
       <c r="B81" s="200" t="s">
         <v>302</v>
       </c>
-      <c r="C81" s="280"/>
+      <c r="C81" s="278"/>
       <c r="D81" s="162" t="s">
         <v>11</v>
       </c>
@@ -39306,7 +39306,7 @@
       <c r="B82" s="200" t="s">
         <v>303</v>
       </c>
-      <c r="C82" s="280"/>
+      <c r="C82" s="278"/>
       <c r="D82" s="162" t="s">
         <v>563</v>
       </c>
@@ -39318,7 +39318,7 @@
       <c r="B83" s="200" t="s">
         <v>304</v>
       </c>
-      <c r="C83" s="280"/>
+      <c r="C83" s="278"/>
       <c r="D83" s="162" t="s">
         <v>564</v>
       </c>
@@ -39330,7 +39330,7 @@
       <c r="B84" s="201" t="s">
         <v>305</v>
       </c>
-      <c r="C84" s="280"/>
+      <c r="C84" s="278"/>
       <c r="D84" s="162" t="s">
         <v>565</v>
       </c>
@@ -39342,7 +39342,7 @@
       <c r="B85" s="201" t="s">
         <v>306</v>
       </c>
-      <c r="C85" s="280"/>
+      <c r="C85" s="278"/>
       <c r="D85" s="162" t="s">
         <v>566</v>
       </c>
@@ -39354,7 +39354,7 @@
       <c r="B86" s="201" t="s">
         <v>307</v>
       </c>
-      <c r="C86" s="280"/>
+      <c r="C86" s="278"/>
       <c r="D86" s="162" t="s">
         <v>567</v>
       </c>
@@ -39366,7 +39366,7 @@
       <c r="B87" s="201" t="s">
         <v>308</v>
       </c>
-      <c r="C87" s="280"/>
+      <c r="C87" s="278"/>
       <c r="D87" s="162" t="s">
         <v>568</v>
       </c>
@@ -39390,7 +39390,7 @@
       <c r="B89" s="205" t="s">
         <v>310</v>
       </c>
-      <c r="C89" s="278" t="s">
+      <c r="C89" s="277" t="s">
         <v>570</v>
       </c>
       <c r="D89" s="162" t="s">
@@ -39404,7 +39404,7 @@
       <c r="B90" s="205" t="s">
         <v>438</v>
       </c>
-      <c r="C90" s="280"/>
+      <c r="C90" s="278"/>
       <c r="D90" s="206" t="s">
         <v>572</v>
       </c>
@@ -39416,7 +39416,7 @@
       <c r="B91" s="205" t="s">
         <v>311</v>
       </c>
-      <c r="C91" s="280"/>
+      <c r="C91" s="278"/>
       <c r="D91" s="207" t="s">
         <v>573</v>
       </c>
@@ -39440,7 +39440,7 @@
       <c r="B93" s="185" t="s">
         <v>313</v>
       </c>
-      <c r="C93" s="278" t="s">
+      <c r="C93" s="277" t="s">
         <v>575</v>
       </c>
       <c r="D93" s="186" t="s">
@@ -39454,7 +39454,7 @@
       <c r="B94" s="188" t="s">
         <v>319</v>
       </c>
-      <c r="C94" s="280"/>
+      <c r="C94" s="278"/>
       <c r="D94" s="177" t="s">
         <v>577</v>
       </c>
@@ -39466,7 +39466,7 @@
       <c r="B95" s="188" t="s">
         <v>488</v>
       </c>
-      <c r="C95" s="280"/>
+      <c r="C95" s="278"/>
       <c r="D95" s="162" t="s">
         <v>578</v>
       </c>
@@ -39478,7 +39478,7 @@
       <c r="B96" s="188" t="s">
         <v>489</v>
       </c>
-      <c r="C96" s="280"/>
+      <c r="C96" s="278"/>
       <c r="D96" s="162" t="s">
         <v>579</v>
       </c>
@@ -39490,7 +39490,7 @@
       <c r="B97" s="188" t="s">
         <v>490</v>
       </c>
-      <c r="C97" s="280"/>
+      <c r="C97" s="278"/>
       <c r="D97" s="162" t="s">
         <v>580</v>
       </c>
@@ -39514,7 +39514,7 @@
       <c r="B99" s="211" t="s">
         <v>454</v>
       </c>
-      <c r="C99" s="278" t="s">
+      <c r="C99" s="277" t="s">
         <v>581</v>
       </c>
       <c r="D99" s="159" t="s">
@@ -39528,7 +39528,7 @@
       <c r="B100" s="213" t="s">
         <v>314</v>
       </c>
-      <c r="C100" s="280"/>
+      <c r="C100" s="278"/>
       <c r="D100" s="162" t="s">
         <v>583</v>
       </c>
@@ -39540,7 +39540,7 @@
       <c r="B101" s="213" t="s">
         <v>315</v>
       </c>
-      <c r="C101" s="280"/>
+      <c r="C101" s="278"/>
       <c r="D101" s="162" t="s">
         <v>584</v>
       </c>
@@ -39552,7 +39552,7 @@
       <c r="B102" s="213" t="s">
         <v>316</v>
       </c>
-      <c r="C102" s="280"/>
+      <c r="C102" s="278"/>
       <c r="D102" s="162" t="s">
         <v>584</v>
       </c>
@@ -39564,7 +39564,7 @@
       <c r="B103" s="213" t="s">
         <v>317</v>
       </c>
-      <c r="C103" s="280"/>
+      <c r="C103" s="278"/>
       <c r="D103" s="162" t="s">
         <v>585</v>
       </c>
@@ -39588,7 +39588,7 @@
       <c r="B105" s="216" t="s">
         <v>439</v>
       </c>
-      <c r="C105" s="278" t="s">
+      <c r="C105" s="277" t="s">
         <v>586</v>
       </c>
       <c r="D105" s="186" t="s">
@@ -39602,7 +39602,7 @@
       <c r="B106" s="217" t="s">
         <v>440</v>
       </c>
-      <c r="C106" s="280"/>
+      <c r="C106" s="278"/>
       <c r="D106" s="162" t="s">
         <v>11</v>
       </c>
@@ -39614,7 +39614,7 @@
       <c r="B107" s="217" t="s">
         <v>441</v>
       </c>
-      <c r="C107" s="280"/>
+      <c r="C107" s="278"/>
       <c r="D107" s="162" t="s">
         <v>11</v>
       </c>
@@ -39626,7 +39626,7 @@
       <c r="B108" s="217" t="s">
         <v>442</v>
       </c>
-      <c r="C108" s="280"/>
+      <c r="C108" s="278"/>
       <c r="D108" s="162" t="s">
         <v>11</v>
       </c>
@@ -39638,7 +39638,7 @@
       <c r="B109" s="217" t="s">
         <v>443</v>
       </c>
-      <c r="C109" s="280"/>
+      <c r="C109" s="278"/>
       <c r="D109" s="162" t="s">
         <v>563</v>
       </c>
@@ -39650,7 +39650,7 @@
       <c r="B110" s="217" t="s">
         <v>444</v>
       </c>
-      <c r="C110" s="280"/>
+      <c r="C110" s="278"/>
       <c r="D110" s="162" t="s">
         <v>11</v>
       </c>
@@ -39662,7 +39662,7 @@
       <c r="B111" s="217" t="s">
         <v>445</v>
       </c>
-      <c r="C111" s="280"/>
+      <c r="C111" s="278"/>
       <c r="D111" s="162" t="s">
         <v>11</v>
       </c>
@@ -39674,7 +39674,7 @@
       <c r="B112" s="217" t="s">
         <v>506</v>
       </c>
-      <c r="C112" s="280"/>
+      <c r="C112" s="278"/>
       <c r="D112" s="162" t="s">
         <v>11</v>
       </c>
@@ -39686,7 +39686,7 @@
       <c r="B113" s="217" t="s">
         <v>507</v>
       </c>
-      <c r="C113" s="280"/>
+      <c r="C113" s="278"/>
       <c r="D113" s="162" t="s">
         <v>11</v>
       </c>
@@ -39698,7 +39698,7 @@
       <c r="B114" s="217" t="s">
         <v>508</v>
       </c>
-      <c r="C114" s="280"/>
+      <c r="C114" s="278"/>
       <c r="D114" s="162" t="s">
         <v>11</v>
       </c>
@@ -39710,7 +39710,7 @@
       <c r="B115" s="217" t="s">
         <v>509</v>
       </c>
-      <c r="C115" s="280"/>
+      <c r="C115" s="278"/>
       <c r="D115" s="162" t="s">
         <v>11</v>
       </c>
@@ -39722,7 +39722,7 @@
       <c r="B116" s="217" t="s">
         <v>446</v>
       </c>
-      <c r="C116" s="280"/>
+      <c r="C116" s="278"/>
       <c r="D116" s="162" t="s">
         <v>588</v>
       </c>
@@ -39734,7 +39734,7 @@
       <c r="B117" s="217" t="s">
         <v>447</v>
       </c>
-      <c r="C117" s="280"/>
+      <c r="C117" s="278"/>
       <c r="D117" s="162" t="s">
         <v>589</v>
       </c>
@@ -39746,7 +39746,7 @@
       <c r="B118" s="217" t="s">
         <v>477</v>
       </c>
-      <c r="C118" s="280"/>
+      <c r="C118" s="278"/>
       <c r="D118" s="162" t="s">
         <v>590</v>
       </c>
@@ -39758,7 +39758,7 @@
       <c r="B119" s="217" t="s">
         <v>478</v>
       </c>
-      <c r="C119" s="280"/>
+      <c r="C119" s="278"/>
       <c r="D119" s="162" t="s">
         <v>591</v>
       </c>
@@ -39770,7 +39770,7 @@
       <c r="B120" s="217" t="s">
         <v>510</v>
       </c>
-      <c r="C120" s="280"/>
+      <c r="C120" s="278"/>
       <c r="D120" s="162" t="s">
         <v>592</v>
       </c>
@@ -39782,7 +39782,7 @@
       <c r="B121" s="217" t="s">
         <v>513</v>
       </c>
-      <c r="C121" s="280"/>
+      <c r="C121" s="278"/>
       <c r="D121" s="162" t="s">
         <v>593</v>
       </c>
@@ -39794,7 +39794,7 @@
       <c r="B122" s="217" t="s">
         <v>512</v>
       </c>
-      <c r="C122" s="280"/>
+      <c r="C122" s="278"/>
       <c r="D122" s="177" t="s">
         <v>594</v>
       </c>
@@ -39806,7 +39806,7 @@
       <c r="B123" s="217" t="s">
         <v>320</v>
       </c>
-      <c r="C123" s="280"/>
+      <c r="C123" s="278"/>
       <c r="D123" s="162" t="s">
         <v>595</v>
       </c>
@@ -39818,7 +39818,7 @@
       <c r="B124" s="217" t="s">
         <v>321</v>
       </c>
-      <c r="C124" s="280"/>
+      <c r="C124" s="278"/>
       <c r="D124" s="162" t="s">
         <v>595</v>
       </c>
@@ -39830,7 +39830,7 @@
       <c r="B125" s="217" t="s">
         <v>322</v>
       </c>
-      <c r="C125" s="280"/>
+      <c r="C125" s="278"/>
       <c r="D125" s="177" t="s">
         <v>672</v>
       </c>
@@ -39842,7 +39842,7 @@
       <c r="B126" s="217" t="s">
         <v>323</v>
       </c>
-      <c r="C126" s="280"/>
+      <c r="C126" s="278"/>
       <c r="D126" s="162" t="s">
         <v>596</v>
       </c>
@@ -39854,7 +39854,7 @@
       <c r="B127" s="217" t="s">
         <v>448</v>
       </c>
-      <c r="C127" s="280"/>
+      <c r="C127" s="278"/>
       <c r="D127" s="177" t="s">
         <v>673</v>
       </c>
@@ -39866,7 +39866,7 @@
       <c r="B128" s="217" t="s">
         <v>449</v>
       </c>
-      <c r="C128" s="280"/>
+      <c r="C128" s="278"/>
       <c r="D128" s="177" t="s">
         <v>669</v>
       </c>
@@ -39878,7 +39878,7 @@
       <c r="B129" s="217" t="s">
         <v>324</v>
       </c>
-      <c r="C129" s="280"/>
+      <c r="C129" s="278"/>
       <c r="D129" s="177" t="s">
         <v>597</v>
       </c>
@@ -39890,7 +39890,7 @@
       <c r="B130" s="217" t="s">
         <v>480</v>
       </c>
-      <c r="C130" s="280"/>
+      <c r="C130" s="278"/>
       <c r="D130" s="177" t="s">
         <v>598</v>
       </c>
@@ -39902,7 +39902,7 @@
       <c r="B131" s="217" t="s">
         <v>325</v>
       </c>
-      <c r="C131" s="280"/>
+      <c r="C131" s="278"/>
       <c r="D131" s="162" t="s">
         <v>599</v>
       </c>
@@ -39914,7 +39914,7 @@
       <c r="B132" s="217" t="s">
         <v>326</v>
       </c>
-      <c r="C132" s="280"/>
+      <c r="C132" s="278"/>
       <c r="D132" s="162" t="s">
         <v>600</v>
       </c>
@@ -39926,7 +39926,7 @@
       <c r="B133" s="217" t="s">
         <v>327</v>
       </c>
-      <c r="C133" s="280"/>
+      <c r="C133" s="278"/>
       <c r="D133" s="218" t="s">
         <v>601</v>
       </c>
@@ -39938,7 +39938,7 @@
       <c r="B134" s="217" t="s">
         <v>328</v>
       </c>
-      <c r="C134" s="280"/>
+      <c r="C134" s="278"/>
       <c r="D134" s="218" t="s">
         <v>601</v>
       </c>
@@ -39950,7 +39950,7 @@
       <c r="B135" s="217" t="s">
         <v>329</v>
       </c>
-      <c r="C135" s="280"/>
+      <c r="C135" s="278"/>
       <c r="D135" s="162" t="s">
         <v>602</v>
       </c>
@@ -39962,7 +39962,7 @@
       <c r="B136" s="217" t="s">
         <v>330</v>
       </c>
-      <c r="C136" s="280"/>
+      <c r="C136" s="278"/>
       <c r="D136" s="162" t="s">
         <v>603</v>
       </c>
@@ -39974,7 +39974,7 @@
       <c r="B137" s="217" t="s">
         <v>463</v>
       </c>
-      <c r="C137" s="280"/>
+      <c r="C137" s="278"/>
       <c r="D137" s="162" t="s">
         <v>604</v>
       </c>
@@ -39998,7 +39998,7 @@
       <c r="B139" s="221" t="s">
         <v>331</v>
       </c>
-      <c r="C139" s="278" t="s">
+      <c r="C139" s="277" t="s">
         <v>606</v>
       </c>
       <c r="D139" s="162" t="s">
@@ -40012,7 +40012,7 @@
       <c r="B140" s="221" t="s">
         <v>332</v>
       </c>
-      <c r="C140" s="280"/>
+      <c r="C140" s="278"/>
       <c r="D140" s="177" t="s">
         <v>608</v>
       </c>
@@ -40024,7 +40024,7 @@
       <c r="B141" s="221" t="s">
         <v>333</v>
       </c>
-      <c r="C141" s="280"/>
+      <c r="C141" s="278"/>
       <c r="D141" s="162" t="s">
         <v>11</v>
       </c>
@@ -40036,7 +40036,7 @@
       <c r="B142" s="221" t="s">
         <v>334</v>
       </c>
-      <c r="C142" s="280"/>
+      <c r="C142" s="278"/>
       <c r="D142" s="162" t="s">
         <v>11</v>
       </c>
@@ -40048,7 +40048,7 @@
       <c r="B143" s="221" t="s">
         <v>450</v>
       </c>
-      <c r="C143" s="280"/>
+      <c r="C143" s="278"/>
       <c r="D143" s="177" t="s">
         <v>609</v>
       </c>
@@ -40060,7 +40060,7 @@
       <c r="B144" s="221" t="s">
         <v>451</v>
       </c>
-      <c r="C144" s="280"/>
+      <c r="C144" s="278"/>
       <c r="D144" s="177" t="s">
         <v>610</v>
       </c>
@@ -40072,7 +40072,7 @@
       <c r="B145" s="221" t="s">
         <v>335</v>
       </c>
-      <c r="C145" s="280"/>
+      <c r="C145" s="278"/>
       <c r="D145" s="162" t="s">
         <v>611</v>
       </c>
@@ -40084,7 +40084,7 @@
       <c r="B146" s="221" t="s">
         <v>336</v>
       </c>
-      <c r="C146" s="280"/>
+      <c r="C146" s="278"/>
       <c r="D146" s="162" t="s">
         <v>11</v>
       </c>
@@ -40096,7 +40096,7 @@
       <c r="B147" s="221" t="s">
         <v>337</v>
       </c>
-      <c r="C147" s="280"/>
+      <c r="C147" s="278"/>
       <c r="D147" s="162" t="s">
         <v>11</v>
       </c>
@@ -40108,7 +40108,7 @@
       <c r="B148" s="221" t="s">
         <v>338</v>
       </c>
-      <c r="C148" s="280"/>
+      <c r="C148" s="278"/>
       <c r="D148" s="162" t="s">
         <v>11</v>
       </c>
@@ -40120,7 +40120,7 @@
       <c r="B149" s="221" t="s">
         <v>339</v>
       </c>
-      <c r="C149" s="280"/>
+      <c r="C149" s="278"/>
       <c r="D149" s="162" t="s">
         <v>612</v>
       </c>
@@ -40132,7 +40132,7 @@
       <c r="B150" s="221" t="s">
         <v>340</v>
       </c>
-      <c r="C150" s="280"/>
+      <c r="C150" s="278"/>
       <c r="D150" s="162" t="s">
         <v>613</v>
       </c>
@@ -40144,7 +40144,7 @@
       <c r="B151" s="221" t="s">
         <v>341</v>
       </c>
-      <c r="C151" s="280"/>
+      <c r="C151" s="278"/>
       <c r="D151" s="162" t="s">
         <v>614</v>
       </c>
@@ -40178,6 +40178,13 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="C18:C28"/>
+    <mergeCell ref="C29:C41"/>
+    <mergeCell ref="C44:C53"/>
     <mergeCell ref="C139:C152"/>
     <mergeCell ref="C60:C67"/>
     <mergeCell ref="C68:C88"/>
@@ -40185,13 +40192,6 @@
     <mergeCell ref="C93:C98"/>
     <mergeCell ref="C99:C104"/>
     <mergeCell ref="C105:C138"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="C18:C28"/>
-    <mergeCell ref="C29:C41"/>
-    <mergeCell ref="C44:C53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -40237,7 +40237,7 @@
       <c r="B2" s="197" t="s">
         <v>344</v>
       </c>
-      <c r="C2" s="278" t="s">
+      <c r="C2" s="277" t="s">
         <v>561</v>
       </c>
       <c r="D2" s="159" t="s">
@@ -40251,7 +40251,7 @@
       <c r="B3" s="199" t="s">
         <v>345</v>
       </c>
-      <c r="C3" s="280"/>
+      <c r="C3" s="278"/>
       <c r="D3" s="162" t="s">
         <v>11</v>
       </c>
@@ -40263,7 +40263,7 @@
       <c r="B4" s="199" t="s">
         <v>346</v>
       </c>
-      <c r="C4" s="280"/>
+      <c r="C4" s="278"/>
       <c r="D4" s="162" t="s">
         <v>11</v>
       </c>
@@ -40275,7 +40275,7 @@
       <c r="B5" s="199" t="s">
         <v>347</v>
       </c>
-      <c r="C5" s="280"/>
+      <c r="C5" s="278"/>
       <c r="D5" s="162" t="s">
         <v>11</v>
       </c>
@@ -40287,7 +40287,7 @@
       <c r="B6" s="199" t="s">
         <v>348</v>
       </c>
-      <c r="C6" s="280"/>
+      <c r="C6" s="278"/>
       <c r="D6" s="162" t="s">
         <v>11</v>
       </c>
@@ -40299,7 +40299,7 @@
       <c r="B7" s="199" t="s">
         <v>349</v>
       </c>
-      <c r="C7" s="280"/>
+      <c r="C7" s="278"/>
       <c r="D7" s="162" t="s">
         <v>11</v>
       </c>
@@ -40311,7 +40311,7 @@
       <c r="B8" s="199" t="s">
         <v>350</v>
       </c>
-      <c r="C8" s="280"/>
+      <c r="C8" s="278"/>
       <c r="D8" s="162" t="s">
         <v>11</v>
       </c>
@@ -40323,7 +40323,7 @@
       <c r="B9" s="199" t="s">
         <v>351</v>
       </c>
-      <c r="C9" s="280"/>
+      <c r="C9" s="278"/>
       <c r="D9" s="162" t="s">
         <v>11</v>
       </c>
@@ -40335,7 +40335,7 @@
       <c r="B10" s="199" t="s">
         <v>352</v>
       </c>
-      <c r="C10" s="280"/>
+      <c r="C10" s="278"/>
       <c r="D10" s="162" t="s">
         <v>11</v>
       </c>
@@ -40347,7 +40347,7 @@
       <c r="B11" s="199" t="s">
         <v>353</v>
       </c>
-      <c r="C11" s="280"/>
+      <c r="C11" s="278"/>
       <c r="D11" s="162" t="s">
         <v>11</v>
       </c>
@@ -40359,7 +40359,7 @@
       <c r="B12" s="199" t="s">
         <v>354</v>
       </c>
-      <c r="C12" s="280"/>
+      <c r="C12" s="278"/>
       <c r="D12" s="162" t="s">
         <v>11</v>
       </c>
@@ -40371,7 +40371,7 @@
       <c r="B13" s="199" t="s">
         <v>355</v>
       </c>
-      <c r="C13" s="280"/>
+      <c r="C13" s="278"/>
       <c r="D13" s="162" t="s">
         <v>11</v>
       </c>
@@ -40383,7 +40383,7 @@
       <c r="B14" s="199" t="s">
         <v>356</v>
       </c>
-      <c r="C14" s="280"/>
+      <c r="C14" s="278"/>
       <c r="D14" s="162" t="s">
         <v>619</v>
       </c>
@@ -40395,7 +40395,7 @@
       <c r="B15" s="199" t="s">
         <v>357</v>
       </c>
-      <c r="C15" s="280"/>
+      <c r="C15" s="278"/>
       <c r="D15" s="162" t="s">
         <v>619</v>
       </c>
@@ -40419,7 +40419,7 @@
       <c r="B17" s="227" t="s">
         <v>358</v>
       </c>
-      <c r="C17" s="278" t="s">
+      <c r="C17" s="277" t="s">
         <v>621</v>
       </c>
       <c r="D17" s="159" t="s">
@@ -40433,7 +40433,7 @@
       <c r="B18" s="228" t="s">
         <v>359</v>
       </c>
-      <c r="C18" s="280"/>
+      <c r="C18" s="278"/>
       <c r="D18" s="162" t="s">
         <v>623</v>
       </c>
@@ -40445,7 +40445,7 @@
       <c r="B19" s="228" t="s">
         <v>360</v>
       </c>
-      <c r="C19" s="280"/>
+      <c r="C19" s="278"/>
       <c r="D19" s="162" t="s">
         <v>624</v>
       </c>
@@ -40457,7 +40457,7 @@
       <c r="B20" s="228" t="s">
         <v>361</v>
       </c>
-      <c r="C20" s="280"/>
+      <c r="C20" s="278"/>
       <c r="D20" s="162" t="s">
         <v>553</v>
       </c>
@@ -40469,7 +40469,7 @@
       <c r="B21" s="228" t="s">
         <v>362</v>
       </c>
-      <c r="C21" s="280"/>
+      <c r="C21" s="278"/>
       <c r="D21" s="162" t="s">
         <v>554</v>
       </c>
@@ -40481,7 +40481,7 @@
       <c r="B22" s="228" t="s">
         <v>363</v>
       </c>
-      <c r="C22" s="280"/>
+      <c r="C22" s="278"/>
       <c r="D22" s="162" t="s">
         <v>555</v>
       </c>
@@ -40493,7 +40493,7 @@
       <c r="B23" s="228" t="s">
         <v>364</v>
       </c>
-      <c r="C23" s="280"/>
+      <c r="C23" s="278"/>
       <c r="D23" s="162" t="s">
         <v>556</v>
       </c>
@@ -40505,7 +40505,7 @@
       <c r="B24" s="228" t="s">
         <v>365</v>
       </c>
-      <c r="C24" s="280"/>
+      <c r="C24" s="278"/>
       <c r="D24" s="162" t="s">
         <v>557</v>
       </c>
@@ -40529,7 +40529,7 @@
       <c r="B26" s="173" t="s">
         <v>367</v>
       </c>
-      <c r="C26" s="278" t="s">
+      <c r="C26" s="277" t="s">
         <v>625</v>
       </c>
       <c r="D26" s="159" t="s">
@@ -40543,7 +40543,7 @@
       <c r="B27" s="176" t="s">
         <v>368</v>
       </c>
-      <c r="C27" s="280"/>
+      <c r="C27" s="278"/>
       <c r="D27" s="162" t="s">
         <v>627</v>
       </c>
@@ -40555,7 +40555,7 @@
       <c r="B28" s="176" t="s">
         <v>369</v>
       </c>
-      <c r="C28" s="280"/>
+      <c r="C28" s="278"/>
       <c r="D28" s="162" t="s">
         <v>628</v>
       </c>
@@ -40567,7 +40567,7 @@
       <c r="B29" s="176" t="s">
         <v>370</v>
       </c>
-      <c r="C29" s="280"/>
+      <c r="C29" s="278"/>
       <c r="D29" s="162" t="s">
         <v>629</v>
       </c>
@@ -40579,7 +40579,7 @@
       <c r="B30" s="176" t="s">
         <v>371</v>
       </c>
-      <c r="C30" s="280"/>
+      <c r="C30" s="278"/>
       <c r="D30" s="162" t="s">
         <v>630</v>
       </c>
@@ -40591,7 +40591,7 @@
       <c r="B31" s="176" t="s">
         <v>372</v>
       </c>
-      <c r="C31" s="280"/>
+      <c r="C31" s="278"/>
       <c r="D31" s="162" t="s">
         <v>630</v>
       </c>
@@ -40603,7 +40603,7 @@
       <c r="B32" s="176" t="s">
         <v>373</v>
       </c>
-      <c r="C32" s="280"/>
+      <c r="C32" s="278"/>
       <c r="D32" s="162" t="s">
         <v>631</v>
       </c>
@@ -40615,7 +40615,7 @@
       <c r="B33" s="176" t="s">
         <v>374</v>
       </c>
-      <c r="C33" s="280"/>
+      <c r="C33" s="278"/>
       <c r="D33" s="162" t="s">
         <v>631</v>
       </c>
@@ -40627,7 +40627,7 @@
       <c r="B34" s="176" t="s">
         <v>375</v>
       </c>
-      <c r="C34" s="280"/>
+      <c r="C34" s="278"/>
       <c r="D34" s="162" t="s">
         <v>631</v>
       </c>
@@ -40639,7 +40639,7 @@
       <c r="B35" s="176" t="s">
         <v>376</v>
       </c>
-      <c r="C35" s="280"/>
+      <c r="C35" s="278"/>
       <c r="D35" s="162" t="s">
         <v>631</v>
       </c>
@@ -40663,7 +40663,7 @@
       <c r="B37" s="232" t="s">
         <v>481</v>
       </c>
-      <c r="C37" s="278" t="s">
+      <c r="C37" s="277" t="s">
         <v>632</v>
       </c>
       <c r="D37" s="186" t="s">
@@ -40677,7 +40677,7 @@
       <c r="B38" s="220" t="s">
         <v>482</v>
       </c>
-      <c r="C38" s="280"/>
+      <c r="C38" s="278"/>
       <c r="D38" s="177" t="s">
         <v>610</v>
       </c>
@@ -40689,7 +40689,7 @@
       <c r="B39" s="220" t="s">
         <v>483</v>
       </c>
-      <c r="C39" s="280"/>
+      <c r="C39" s="278"/>
       <c r="D39" s="177" t="s">
         <v>633</v>
       </c>
@@ -40719,15 +40719,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004FD8CECCB51EC843BF514AFE68379818" ma:contentTypeVersion="18" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="eda339f53f012ceb64677667a741b441">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="107e75b3-53cc-4838-92d2-ebc011bd4832" xmlns:ns3="888ccf44-0d39-41a2-ab17-f7efb2bf6977" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04a86f3db711706e561c315688f1c464" ns2:_="" ns3:_="">
     <xsd:import namespace="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
@@ -40976,6 +40967,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -40988,14 +40988,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F91B7B9-75FF-4624-B506-952B5B54766C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41010,6 +41002,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Removed MtrfrGnd Event. Similar to Pmode and Qmode, these Event will not be used.  This would require subscribers in PowerFactory
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/prw_energinet_dk/Documents/Dokumenter/GitHub/MTB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4C41DDB-07AC-4E37-9102-94DFEB104633}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF2C0BE2-8D6B-4D55-9B5A-AF425359AEB2}"/>
   <bookViews>
-    <workbookView xWindow="20790" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20790" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="822" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -359,7 +359,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4301" uniqueCount="937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4295" uniqueCount="934">
   <si>
     <t>Range</t>
   </si>
@@ -3506,15 +3506,6 @@
   </si>
   <si>
     <t>Grounded</t>
-  </si>
-  <si>
-    <t>MtrfrGnd</t>
-  </si>
-  <si>
-    <t>Change Main Transformer Grounding</t>
-  </si>
-  <si>
-    <t>&lt;= 0, Ungrounded / &gt; 0, Grounded</t>
   </si>
   <si>
     <t>RfG_SystemProtect_Q</t>
@@ -5780,8 +5771,8 @@
   </sheetPr>
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -9422,8 +9413,8 @@
   </sheetPr>
   <dimension ref="A1:CQ218"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
@@ -16596,7 +16587,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="87" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="E59" s="89">
         <f t="shared" si="18"/>
@@ -16731,7 +16722,7 @@
         <v>1</v>
       </c>
       <c r="D60" s="87" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="E60" s="89">
         <f t="shared" si="18"/>
@@ -16866,7 +16857,7 @@
         <v>1</v>
       </c>
       <c r="D61" s="87" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="E61" s="89">
         <f t="shared" si="18"/>
@@ -31378,27 +31369,27 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000003000000}">
           <x14:formula1>
-            <xm:f>'Event types'!$A$2:$A$942</xm:f>
+            <xm:f>'Event types'!$A$2:$A$941</xm:f>
           </x14:formula1>
-          <xm:sqref>T38 AZ106:AZ109 AF106:AF109 AB106:AB109 X106:X109 AV106:AV109 AJ106:AJ109 BL107:BL108 BH106:BH109 T106:T109 AR106:AR109 AF45:AF95 X45:X95 T45:T69 AB45:AB95 BL3:BL39 BL44:BL95 AN45:AN95 AJ40:AJ95 T71:T95 AV44:AV95 BD44:BD95 AZ3:AZ95 BH3:BH95 AR3:AR95 AB40:AB42 T40:T42 X40:X42 AF40:AF42 T136:T137 T3:T27 X3:X27 AV3:AV42 T30:T34 X30:X38 AB3:AB38 AN3:AN38 AJ3:AJ38 AF3:AF38 BD3:BD39 X97 AB97 AF97 T97 T36 T197:T216</xm:sqref>
+          <xm:sqref>T38 T197:T216 T36 T97 AF97 AB97 X97 BD3:BD39 AF3:AF38 AJ3:AJ38 AN3:AN38 AB3:AB38 X30:X38 T30:T34 AV3:AV42 X3:X27 T3:T27 T136:T137 AF40:AF42 X40:X42 T40:T42 AB40:AB42 AR3:AR95 BH3:BH95 AZ3:AZ95 BD44:BD95 AV44:AV95 T71:T95 AJ40:AJ95 AN45:AN95 BL44:BL95 BL3:BL39 AB45:AB95 T45:T69 X45:X95 AF45:AF95 AR106:AR109 T106:T109 BH106:BH109 BL107:BL108 AJ106:AJ109 AV106:AV109 X106:X109 AB106:AB109 AF106:AF109 AZ106:AZ109</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000004000000}">
           <x14:formula1>
-            <xm:f>'Event types'!$A$2:$A$275</xm:f>
+            <xm:f>'Event types'!$A$2:$A$274</xm:f>
           </x14:formula1>
-          <xm:sqref>T43:T44 BL96:BL105 BL110:BL151 BL43 AB110:AB151 T98:T105 BD96:BD105 AZ96:AZ105 BH96:BH105 AJ96:AJ105 AN96:AN105 AV96:AV105 AF98:AF105 AR96:AR105 AB98:AB105 X98:X105 X112:X151 BD110:BD151 T110:T135 X110 AZ110:AZ151 T138:T151 AR110:AR151 AF110:AF151 AV110:AV151 AN110:AN151 AJ110:AJ151 BH110:BH151 AF43:AF44 AV43 AN43:AN44 AF96 AB96 X96 T96 BD43 X28:X29 T28:T29 AB43:AB44 X43:X44</xm:sqref>
+          <xm:sqref>T43:T44 X43:X44 AB43:AB44 T28:T29 X28:X29 BD43 T96 X96 AB96 AF96 AN43:AN44 AV43 AF43:AF44 BH110:BH151 AJ110:AJ151 AN110:AN151 AV110:AV151 AF110:AF151 AR110:AR151 T138:T151 AZ110:AZ151 X110 T110:T135 BD110:BD151 X112:X151 X98:X105 AB98:AB105 AR96:AR105 AF98:AF105 AV96:AV105 AN96:AN105 AJ96:AJ105 BH96:BH105 AZ96:AZ105 BD96:BD105 T98:T105 AB110:AB151 BL43 BL110:BL151 BL96:BL105</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000005000000}">
           <x14:formula1>
-            <xm:f>'Event types'!$A$2:$A$103</xm:f>
+            <xm:f>'Event types'!$A$2:$A$102</xm:f>
           </x14:formula1>
-          <xm:sqref>T183:T196 BL152:BL197 T156:T161 T164:T177 X152:X197 AB152:AB197 BH152:BH197 AJ152:AJ195 AF152:AF197 AV152:AV195 AN152:AN194 BD152:BD197 AR152:AR195 AZ152:AZ196</xm:sqref>
+          <xm:sqref>T183:T196 AZ152:AZ196 AR152:AR195 BD152:BD197 AN152:AN194 AV152:AV195 AF152:AF197 AJ152:AJ195 BH152:BH197 AB152:AB197 X152:X197 T164:T177 T156:T161 BL152:BL197</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000006000000}">
           <x14:formula1>
-            <xm:f>'Event types'!$A$2:$A$95</xm:f>
+            <xm:f>'Event types'!$A$2:$A$94</xm:f>
           </x14:formula1>
-          <xm:sqref>T178:T186 P3:P1048576 T152:T163 X111 T70</xm:sqref>
+          <xm:sqref>T178:T186 T70 X111 T152:T163 P3:P1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -36801,15 +36792,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000003000000}">
           <x14:formula1>
-            <xm:f>'Event types'!$A$2:$A$942</xm:f>
+            <xm:f>'Event types'!$A$2:$A$941</xm:f>
           </x14:formula1>
-          <xm:sqref>N42:N1048576 R42:R66 R22 N22 V22 Z22 AD22 AH22</xm:sqref>
+          <xm:sqref>N42:N1048576 AH22 AD22 Z22 V22 N22 R22 R42:R66</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000004000000}">
           <x14:formula1>
-            <xm:f>'Event types'!$A$2:$A$275</xm:f>
+            <xm:f>'Event types'!$A$2:$A$274</xm:f>
           </x14:formula1>
-          <xm:sqref>AH23:AH37 R3:R21 N3:N21 BB3:BB37 AX3:AX37 AT3:AT37 AP3:AP37 AL3:AL37 V3:V21 Z3:Z21 AD3:AD21 AH3:AH21 BF3:BF37 N23:N37 R23:R37 V23:V37 Z23:Z37 AD23:AD37</xm:sqref>
+          <xm:sqref>AH23:AH37 AD23:AD37 Z23:Z37 V23:V37 R23:R37 N23:N37 BF3:BF37 AH3:AH21 AD3:AD21 Z3:Z21 V3:V21 AL3:AL37 AP3:AP37 AT3:AT37 AX3:AX37 BB3:BB37 N3:N21 R3:R21</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -43850,15 +43841,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000003000000}">
           <x14:formula1>
-            <xm:f>'Event types'!$A$2:$A$275</xm:f>
+            <xm:f>'Event types'!$A$2:$A$274</xm:f>
           </x14:formula1>
-          <xm:sqref>AI3:AI39 O3:O39 S3:S39 AI41:AI50 AE41:AE50 AA41:AA50 W41:W50 S41:S50 BG3:BG50 AM3:AM50 AQ3:AQ50 AU3:AU50 AY3:AY50 BC3:BC50 O41:O50 AE3:AE39 AA3:AA39 W3:W39 AI53:AI61 O53:O62 BC53:BC61 AY53:AY61 AU53:AU61 AQ53:AQ61 AM53:AM61 BG53:BG61 S53:S62 W53:W62 AA53:AA61 AE53:AE61</xm:sqref>
+          <xm:sqref>AI3:AI39 AE53:AE61 AA53:AA61 W53:W62 S53:S62 BG53:BG61 AM53:AM61 AQ53:AQ61 AU53:AU61 AY53:AY61 BC53:BC61 O53:O62 AI53:AI61 W3:W39 AA3:AA39 AE3:AE39 O41:O50 BC3:BC50 AY3:AY50 AU3:AU50 AQ3:AQ50 AM3:AM50 BG3:BG50 S41:S50 W41:W50 AA41:AA50 AE41:AE50 AI41:AI50 S3:S39 O3:O39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000004000000}">
           <x14:formula1>
-            <xm:f>'Event types'!$A$2:$A$942</xm:f>
+            <xm:f>'Event types'!$A$2:$A$941</xm:f>
           </x14:formula1>
-          <xm:sqref>AI40 O63:O1048576 S40 O40 W40 AA40 AE40</xm:sqref>
+          <xm:sqref>AI40 AE40 AA40 W40 O40 S40 O63:O1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -50279,19 +50270,19 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000003000000}">
           <x14:formula1>
-            <xm:f>'Event types'!$A$2:$A$942</xm:f>
+            <xm:f>'Event types'!$A$2:$A$941</xm:f>
           </x14:formula1>
-          <xm:sqref>O4:O13 O20:O38 O82:O1048576 AA56:AA61 AE36:AE38 W36:W38 W56:W61 AA14:AA19 S14:S19 W14:W19 AE14:AE19 AI15:AI19</xm:sqref>
+          <xm:sqref>O4:O13 AI15:AI19 AE14:AE19 W14:W19 S14:S19 AA14:AA19 W56:W61 W36:W38 AE36:AE38 AA56:AA61 O82:O1048576 O20:O38</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000004000000}">
           <x14:formula1>
-            <xm:f>'Event types'!$A$2:$A$49</xm:f>
+            <xm:f>'Event types'!$A$2:$A$48</xm:f>
           </x14:formula1>
-          <xm:sqref>S3:S13 O39:O81 S20:S1048576 AA36:AA38</xm:sqref>
+          <xm:sqref>S3:S13 AA36:AA38 S20:S1048576 O39:O81</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000005000000}">
           <x14:formula1>
-            <xm:f>'Event types'!$A$2:$A$95</xm:f>
+            <xm:f>'Event types'!$A$2:$A$94</xm:f>
           </x14:formula1>
           <xm:sqref>O14:O19 O3</xm:sqref>
         </x14:dataValidation>
@@ -50303,11 +50294,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView zoomScale="82" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K38" sqref="K38"/>
+      <selection pane="bottomLeft" activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -50521,30 +50512,30 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="113" t="s">
-        <v>931</v>
+        <v>116</v>
       </c>
       <c r="B11" s="113" t="s">
-        <v>932</v>
+        <v>155</v>
       </c>
       <c r="C11" s="113" t="s">
-        <v>933</v>
-      </c>
-      <c r="D11" s="114" t="s">
-        <v>11</v>
+        <v>156</v>
+      </c>
+      <c r="D11" s="113" t="s">
+        <v>140</v>
       </c>
       <c r="E11" s="113" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="114" t="s">
-        <v>11</v>
+        <v>157</v>
+      </c>
+      <c r="F11" s="113" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="113" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B12" s="113" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C12" s="113" t="s">
         <v>156</v>
@@ -50561,10 +50552,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="113" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B13" s="113" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C13" s="113" t="s">
         <v>156</v>
@@ -50581,10 +50572,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" s="113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B14" s="113" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C14" s="113" t="s">
         <v>156</v>
@@ -50601,30 +50592,30 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="113" t="s">
-        <v>118</v>
+        <v>161</v>
       </c>
       <c r="B15" s="113" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C15" s="113" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D15" s="113" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="E15" s="113" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="F15" s="113" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="113" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B16" s="113" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C16" s="113" t="s">
         <v>162</v>
@@ -50641,10 +50632,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="113" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B17" s="113" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C17" s="113" t="s">
         <v>162</v>
@@ -50661,10 +50652,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="113" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="B18" s="113" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C18" s="113" t="s">
         <v>162</v>
@@ -50681,50 +50672,50 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="113" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B19" s="113" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C19" s="113" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="D19" s="113" t="s">
-        <v>19</v>
+        <v>167</v>
       </c>
       <c r="E19" s="113" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="F19" s="113" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A20" s="113" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" s="113" t="s">
-        <v>166</v>
-      </c>
-      <c r="C20" s="113" t="s">
         <v>167</v>
       </c>
-      <c r="D20" s="113" t="s">
+    </row>
+    <row r="20" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A20" s="115" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" s="116" t="s">
+        <v>169</v>
+      </c>
+      <c r="C20" s="115" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="115" t="s">
         <v>167</v>
       </c>
-      <c r="E20" s="113" t="s">
-        <v>167</v>
-      </c>
-      <c r="F20" s="113" t="s">
-        <v>167</v>
+      <c r="E20" s="115" t="s">
+        <v>171</v>
+      </c>
+      <c r="F20" s="117" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A21" s="115" t="s">
-        <v>168</v>
+        <v>129</v>
       </c>
       <c r="B21" s="116" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C21" s="115" t="s">
         <v>170</v>
@@ -50741,10 +50732,10 @@
     </row>
     <row r="22" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A22" s="115" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B22" s="116" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C22" s="115" t="s">
         <v>170</v>
@@ -50761,10 +50752,10 @@
     </row>
     <row r="23" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A23" s="115" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B23" s="116" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C23" s="115" t="s">
         <v>170</v>
@@ -50781,10 +50772,10 @@
     </row>
     <row r="24" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A24" s="115" t="s">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="B24" s="116" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C24" s="115" t="s">
         <v>170</v>
@@ -50799,12 +50790,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="115" t="s">
-        <v>175</v>
+        <v>122</v>
       </c>
       <c r="B25" s="116" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C25" s="115" t="s">
         <v>170</v>
@@ -50819,32 +50810,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="115" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B26" s="116" t="s">
-        <v>177</v>
+        <v>228</v>
       </c>
       <c r="C26" s="115" t="s">
-        <v>170</v>
-      </c>
-      <c r="D26" s="115" t="s">
-        <v>167</v>
+        <v>178</v>
+      </c>
+      <c r="D26" s="117" t="s">
+        <v>179</v>
       </c>
       <c r="E26" s="115" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="F26" s="117" t="s">
-        <v>11</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="115" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="B27" s="116" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C27" s="115" t="s">
         <v>178</v>
@@ -50861,10 +50852,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="115" t="s">
-        <v>124</v>
+        <v>181</v>
       </c>
       <c r="B28" s="116" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C28" s="115" t="s">
         <v>178</v>
@@ -50881,10 +50872,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="115" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B29" s="116" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C29" s="115" t="s">
         <v>178</v>
@@ -50901,10 +50892,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="115" t="s">
-        <v>182</v>
+        <v>130</v>
       </c>
       <c r="B30" s="116" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C30" s="115" t="s">
         <v>178</v>
@@ -50921,10 +50912,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="115" t="s">
-        <v>130</v>
+        <v>183</v>
       </c>
       <c r="B31" s="116" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C31" s="115" t="s">
         <v>178</v>
@@ -50941,10 +50932,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" s="115" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B32" s="116" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C32" s="115" t="s">
         <v>178</v>
@@ -50961,10 +50952,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" s="115" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B33" s="116" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C33" s="115" t="s">
         <v>178</v>
@@ -50981,10 +50972,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" s="115" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B34" s="116" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C34" s="115" t="s">
         <v>178</v>
@@ -51001,10 +50992,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" s="115" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B35" s="116" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C35" s="115" t="s">
         <v>178</v>
@@ -51019,32 +51010,32 @@
         <v>180</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A36" s="115" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B36" s="116" t="s">
-        <v>237</v>
+        <v>189</v>
       </c>
       <c r="C36" s="115" t="s">
-        <v>178</v>
-      </c>
-      <c r="D36" s="117" t="s">
-        <v>179</v>
+        <v>170</v>
+      </c>
+      <c r="D36" s="115" t="s">
+        <v>167</v>
       </c>
       <c r="E36" s="115" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="F36" s="117" t="s">
-        <v>180</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A37" s="115" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B37" s="116" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C37" s="115" t="s">
         <v>170</v>
@@ -51061,10 +51052,10 @@
     </row>
     <row r="38" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A38" s="115" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B38" s="116" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C38" s="115" t="s">
         <v>170</v>
@@ -51081,10 +51072,10 @@
     </row>
     <row r="39" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A39" s="115" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B39" s="116" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C39" s="115" t="s">
         <v>170</v>
@@ -51101,10 +51092,10 @@
     </row>
     <row r="40" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A40" s="115" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B40" s="116" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C40" s="115" t="s">
         <v>170</v>
@@ -51121,10 +51112,10 @@
     </row>
     <row r="41" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A41" s="115" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B41" s="116" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C41" s="115" t="s">
         <v>170</v>
@@ -51141,10 +51132,10 @@
     </row>
     <row r="42" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A42" s="115" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B42" s="116" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C42" s="115" t="s">
         <v>170</v>
@@ -51161,10 +51152,10 @@
     </row>
     <row r="43" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A43" s="115" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B43" s="116" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C43" s="115" t="s">
         <v>170</v>
@@ -51181,10 +51172,10 @@
     </row>
     <row r="44" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A44" s="115" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B44" s="116" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C44" s="115" t="s">
         <v>170</v>
@@ -51201,10 +51192,10 @@
     </row>
     <row r="45" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A45" s="115" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B45" s="116" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C45" s="115" t="s">
         <v>170</v>
@@ -51220,31 +51211,31 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A46" s="115" t="s">
-        <v>206</v>
-      </c>
-      <c r="B46" s="116" t="s">
-        <v>207</v>
-      </c>
-      <c r="C46" s="115" t="s">
-        <v>170</v>
-      </c>
-      <c r="D46" s="115" t="s">
+      <c r="A46" s="118" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="119" t="s">
+        <v>208</v>
+      </c>
+      <c r="C46" s="118" t="s">
         <v>167</v>
       </c>
-      <c r="E46" s="115" t="s">
-        <v>171</v>
-      </c>
-      <c r="F46" s="117" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="D46" s="118" t="s">
+        <v>167</v>
+      </c>
+      <c r="E46" s="118" t="s">
+        <v>167</v>
+      </c>
+      <c r="F46" s="118" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A47" s="118" t="s">
-        <v>121</v>
+        <v>209</v>
       </c>
       <c r="B47" s="119" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C47" s="118" t="s">
         <v>167</v>
@@ -51256,26 +51247,6 @@
         <v>167</v>
       </c>
       <c r="F47" s="118" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A48" s="118" t="s">
-        <v>209</v>
-      </c>
-      <c r="B48" s="119" t="s">
-        <v>210</v>
-      </c>
-      <c r="C48" s="118" t="s">
-        <v>167</v>
-      </c>
-      <c r="D48" s="118" t="s">
-        <v>167</v>
-      </c>
-      <c r="E48" s="118" t="s">
-        <v>167</v>
-      </c>
-      <c r="F48" s="118" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Case 59, RfG_SystemProtect+fault, Event 4
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/prw_energinet_dk/Documents/Dokumenter/GitHub/MTB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF2C0BE2-8D6B-4D55-9B5A-AF425359AEB2}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F1E3183-5B20-4AD9-A50C-B77EA513BEC9}"/>
   <bookViews>
-    <workbookView xWindow="20790" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="822" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14480" yWindow="-21710" windowWidth="51420" windowHeight="21100" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -5132,6 +5132,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5201,13 +5208,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -5771,8 +5771,8 @@
   </sheetPr>
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5917,16 +5917,16 @@
         <v>429</v>
       </c>
       <c r="H8" s="137"/>
-      <c r="I8" s="291" t="s">
+      <c r="I8" s="294" t="s">
         <v>460</v>
       </c>
-      <c r="J8" s="291"/>
-      <c r="K8" s="291"/>
-      <c r="L8" s="291" t="s">
+      <c r="J8" s="294"/>
+      <c r="K8" s="294"/>
+      <c r="L8" s="294" t="s">
         <v>461</v>
       </c>
-      <c r="M8" s="291"/>
-      <c r="N8" s="292"/>
+      <c r="M8" s="294"/>
+      <c r="N8" s="295"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" s="27" t="s">
@@ -6107,16 +6107,16 @@
       <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A19" s="314" t="s">
+      <c r="A19" s="291" t="s">
         <v>928</v>
       </c>
       <c r="B19" s="283" t="b">
         <v>0</v>
       </c>
-      <c r="C19" s="315" t="s">
+      <c r="C19" s="292" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="316" t="s">
+      <c r="E19" s="293" t="s">
         <v>927</v>
       </c>
       <c r="G19" s="14"/>
@@ -6341,7 +6341,7 @@
       <c r="B2" s="218" t="s">
         <v>374</v>
       </c>
-      <c r="C2" s="308" t="s">
+      <c r="C2" s="311" t="s">
         <v>508</v>
       </c>
       <c r="D2" s="175" t="s">
@@ -6355,7 +6355,7 @@
       <c r="B3" s="220" t="s">
         <v>375</v>
       </c>
-      <c r="C3" s="309"/>
+      <c r="C3" s="312"/>
       <c r="D3" s="168" t="s">
         <v>11</v>
       </c>
@@ -6367,7 +6367,7 @@
       <c r="B4" s="220" t="s">
         <v>376</v>
       </c>
-      <c r="C4" s="309"/>
+      <c r="C4" s="312"/>
       <c r="D4" s="168" t="s">
         <v>11</v>
       </c>
@@ -6379,7 +6379,7 @@
       <c r="B5" s="220" t="s">
         <v>377</v>
       </c>
-      <c r="C5" s="309"/>
+      <c r="C5" s="312"/>
       <c r="D5" s="168" t="s">
         <v>11</v>
       </c>
@@ -6391,7 +6391,7 @@
       <c r="B6" s="220" t="s">
         <v>378</v>
       </c>
-      <c r="C6" s="309"/>
+      <c r="C6" s="312"/>
       <c r="D6" s="168" t="s">
         <v>11</v>
       </c>
@@ -6403,7 +6403,7 @@
       <c r="B7" s="222" t="s">
         <v>379</v>
       </c>
-      <c r="C7" s="310"/>
+      <c r="C7" s="313"/>
       <c r="D7" s="172" t="s">
         <v>11</v>
       </c>
@@ -6429,7 +6429,7 @@
       <c r="B9" s="164" t="s">
         <v>381</v>
       </c>
-      <c r="C9" s="311" t="s">
+      <c r="C9" s="314" t="s">
         <v>628</v>
       </c>
       <c r="D9" s="175" t="s">
@@ -6443,7 +6443,7 @@
       <c r="B10" s="211" t="s">
         <v>382</v>
       </c>
-      <c r="C10" s="312"/>
+      <c r="C10" s="315"/>
       <c r="D10" s="172" t="s">
         <v>630</v>
       </c>
@@ -6455,7 +6455,7 @@
       <c r="B11" s="208" t="s">
         <v>383</v>
       </c>
-      <c r="C11" s="308" t="s">
+      <c r="C11" s="311" t="s">
         <v>631</v>
       </c>
       <c r="D11" s="175" t="s">
@@ -6469,7 +6469,7 @@
       <c r="B12" s="209" t="s">
         <v>384</v>
       </c>
-      <c r="C12" s="309"/>
+      <c r="C12" s="312"/>
       <c r="D12" s="168" t="s">
         <v>633</v>
       </c>
@@ -6481,7 +6481,7 @@
       <c r="B13" s="210" t="s">
         <v>385</v>
       </c>
-      <c r="C13" s="310"/>
+      <c r="C13" s="313"/>
       <c r="D13" s="172" t="s">
         <v>634</v>
       </c>
@@ -6493,7 +6493,7 @@
       <c r="B14" s="183" t="s">
         <v>386</v>
       </c>
-      <c r="C14" s="311" t="s">
+      <c r="C14" s="314" t="s">
         <v>554</v>
       </c>
       <c r="D14" s="175" t="s">
@@ -6507,7 +6507,7 @@
       <c r="B15" s="185" t="s">
         <v>387</v>
       </c>
-      <c r="C15" s="313"/>
+      <c r="C15" s="316"/>
       <c r="D15" s="168" t="s">
         <v>11</v>
       </c>
@@ -6519,7 +6519,7 @@
       <c r="B16" s="185" t="s">
         <v>388</v>
       </c>
-      <c r="C16" s="313"/>
+      <c r="C16" s="316"/>
       <c r="D16" s="168" t="s">
         <v>11</v>
       </c>
@@ -6531,7 +6531,7 @@
       <c r="B17" s="185" t="s">
         <v>389</v>
       </c>
-      <c r="C17" s="313"/>
+      <c r="C17" s="316"/>
       <c r="D17" s="168" t="s">
         <v>11</v>
       </c>
@@ -6543,7 +6543,7 @@
       <c r="B18" s="185" t="s">
         <v>390</v>
       </c>
-      <c r="C18" s="313"/>
+      <c r="C18" s="316"/>
       <c r="D18" s="168" t="s">
         <v>11</v>
       </c>
@@ -6555,7 +6555,7 @@
       <c r="B19" s="185" t="s">
         <v>391</v>
       </c>
-      <c r="C19" s="313"/>
+      <c r="C19" s="316"/>
       <c r="D19" s="168" t="s">
         <v>11</v>
       </c>
@@ -6567,7 +6567,7 @@
       <c r="B20" s="185" t="s">
         <v>392</v>
       </c>
-      <c r="C20" s="313"/>
+      <c r="C20" s="316"/>
       <c r="D20" s="168" t="s">
         <v>11</v>
       </c>
@@ -6579,7 +6579,7 @@
       <c r="B21" s="185" t="s">
         <v>393</v>
       </c>
-      <c r="C21" s="313"/>
+      <c r="C21" s="316"/>
       <c r="D21" s="168" t="s">
         <v>11</v>
       </c>
@@ -6591,7 +6591,7 @@
       <c r="B22" s="185" t="s">
         <v>394</v>
       </c>
-      <c r="C22" s="313"/>
+      <c r="C22" s="316"/>
       <c r="D22" s="168" t="s">
         <v>11</v>
       </c>
@@ -6603,7 +6603,7 @@
       <c r="B23" s="185" t="s">
         <v>395</v>
       </c>
-      <c r="C23" s="313"/>
+      <c r="C23" s="316"/>
       <c r="D23" s="168" t="s">
         <v>11</v>
       </c>
@@ -6615,7 +6615,7 @@
       <c r="B24" s="185" t="s">
         <v>396</v>
       </c>
-      <c r="C24" s="313"/>
+      <c r="C24" s="316"/>
       <c r="D24" s="168" t="s">
         <v>11</v>
       </c>
@@ -6627,7 +6627,7 @@
       <c r="B25" s="185" t="s">
         <v>397</v>
       </c>
-      <c r="C25" s="313"/>
+      <c r="C25" s="316"/>
       <c r="D25" s="168" t="s">
         <v>11</v>
       </c>
@@ -6639,7 +6639,7 @@
       <c r="B26" s="185" t="s">
         <v>398</v>
       </c>
-      <c r="C26" s="313"/>
+      <c r="C26" s="316"/>
       <c r="D26" s="168" t="s">
         <v>557</v>
       </c>
@@ -6651,7 +6651,7 @@
       <c r="B27" s="185" t="s">
         <v>399</v>
       </c>
-      <c r="C27" s="313"/>
+      <c r="C27" s="316"/>
       <c r="D27" s="168" t="s">
         <v>558</v>
       </c>
@@ -6663,7 +6663,7 @@
       <c r="B28" s="185" t="s">
         <v>400</v>
       </c>
-      <c r="C28" s="313"/>
+      <c r="C28" s="316"/>
       <c r="D28" s="168" t="s">
         <v>559</v>
       </c>
@@ -6675,7 +6675,7 @@
       <c r="B29" s="185" t="s">
         <v>401</v>
       </c>
-      <c r="C29" s="313"/>
+      <c r="C29" s="316"/>
       <c r="D29" s="168" t="s">
         <v>560</v>
       </c>
@@ -6687,7 +6687,7 @@
       <c r="B30" s="185" t="s">
         <v>402</v>
       </c>
-      <c r="C30" s="313"/>
+      <c r="C30" s="316"/>
       <c r="D30" s="173" t="s">
         <v>636</v>
       </c>
@@ -6699,7 +6699,7 @@
       <c r="B31" s="185" t="s">
         <v>403</v>
       </c>
-      <c r="C31" s="313"/>
+      <c r="C31" s="316"/>
       <c r="D31" s="173" t="s">
         <v>636</v>
       </c>
@@ -6711,7 +6711,7 @@
       <c r="B32" s="185" t="s">
         <v>404</v>
       </c>
-      <c r="C32" s="313"/>
+      <c r="C32" s="316"/>
       <c r="D32" s="168" t="s">
         <v>587</v>
       </c>
@@ -6723,7 +6723,7 @@
       <c r="B33" s="185" t="s">
         <v>405</v>
       </c>
-      <c r="C33" s="313"/>
+      <c r="C33" s="316"/>
       <c r="D33" s="168" t="s">
         <v>587</v>
       </c>
@@ -6735,7 +6735,7 @@
       <c r="B34" s="185" t="s">
         <v>406</v>
       </c>
-      <c r="C34" s="313"/>
+      <c r="C34" s="316"/>
       <c r="D34" s="168" t="s">
         <v>561</v>
       </c>
@@ -6747,7 +6747,7 @@
       <c r="B35" s="185" t="s">
         <v>407</v>
       </c>
-      <c r="C35" s="313"/>
+      <c r="C35" s="316"/>
       <c r="D35" s="168" t="s">
         <v>562</v>
       </c>
@@ -6759,7 +6759,7 @@
       <c r="B36" s="185" t="s">
         <v>408</v>
       </c>
-      <c r="C36" s="313"/>
+      <c r="C36" s="316"/>
       <c r="D36" s="168" t="s">
         <v>637</v>
       </c>
@@ -6771,7 +6771,7 @@
       <c r="B37" s="207" t="s">
         <v>481</v>
       </c>
-      <c r="C37" s="312"/>
+      <c r="C37" s="315"/>
       <c r="D37" s="168" t="s">
         <v>638</v>
       </c>
@@ -6783,7 +6783,7 @@
       <c r="B38" s="208" t="s">
         <v>409</v>
       </c>
-      <c r="C38" s="308" t="s">
+      <c r="C38" s="311" t="s">
         <v>631</v>
       </c>
       <c r="D38" s="175" t="s">
@@ -6797,7 +6797,7 @@
       <c r="B39" s="209" t="s">
         <v>410</v>
       </c>
-      <c r="C39" s="309"/>
+      <c r="C39" s="312"/>
       <c r="D39" s="168" t="s">
         <v>547</v>
       </c>
@@ -6809,7 +6809,7 @@
       <c r="B40" s="209" t="s">
         <v>411</v>
       </c>
-      <c r="C40" s="309"/>
+      <c r="C40" s="312"/>
       <c r="D40" s="168" t="s">
         <v>550</v>
       </c>
@@ -6821,7 +6821,7 @@
       <c r="B41" s="210" t="s">
         <v>412</v>
       </c>
-      <c r="C41" s="310"/>
+      <c r="C41" s="313"/>
       <c r="D41" s="172" t="s">
         <v>551</v>
       </c>
@@ -6833,7 +6833,7 @@
       <c r="B42" s="213" t="s">
         <v>455</v>
       </c>
-      <c r="C42" s="308" t="s">
+      <c r="C42" s="311" t="s">
         <v>639</v>
       </c>
       <c r="D42" s="175" t="s">
@@ -6847,7 +6847,7 @@
       <c r="B43" s="202" t="s">
         <v>456</v>
       </c>
-      <c r="C43" s="309"/>
+      <c r="C43" s="312"/>
       <c r="D43" s="168" t="s">
         <v>641</v>
       </c>
@@ -6859,7 +6859,7 @@
       <c r="B44" s="202" t="s">
         <v>413</v>
       </c>
-      <c r="C44" s="309"/>
+      <c r="C44" s="312"/>
       <c r="D44" s="168" t="s">
         <v>642</v>
       </c>
@@ -6871,7 +6871,7 @@
       <c r="B45" s="202" t="s">
         <v>414</v>
       </c>
-      <c r="C45" s="309"/>
+      <c r="C45" s="312"/>
       <c r="D45" s="168" t="s">
         <v>11</v>
       </c>
@@ -6883,7 +6883,7 @@
       <c r="B46" s="202" t="s">
         <v>415</v>
       </c>
-      <c r="C46" s="309"/>
+      <c r="C46" s="312"/>
       <c r="D46" s="168" t="s">
         <v>11</v>
       </c>
@@ -6895,7 +6895,7 @@
       <c r="B47" s="202" t="s">
         <v>416</v>
       </c>
-      <c r="C47" s="309"/>
+      <c r="C47" s="312"/>
       <c r="D47" s="168" t="s">
         <v>11</v>
       </c>
@@ -6907,7 +6907,7 @@
       <c r="B48" s="202" t="s">
         <v>446</v>
       </c>
-      <c r="C48" s="309"/>
+      <c r="C48" s="312"/>
       <c r="D48" s="168" t="s">
         <v>600</v>
       </c>
@@ -6919,7 +6919,7 @@
       <c r="B49" s="202" t="s">
         <v>447</v>
       </c>
-      <c r="C49" s="309"/>
+      <c r="C49" s="312"/>
       <c r="D49" s="168" t="s">
         <v>601</v>
       </c>
@@ -6931,7 +6931,7 @@
       <c r="B50" s="202" t="s">
         <v>479</v>
       </c>
-      <c r="C50" s="309"/>
+      <c r="C50" s="312"/>
       <c r="D50" s="168" t="s">
         <v>624</v>
       </c>
@@ -6943,7 +6943,7 @@
       <c r="B51" s="202" t="s">
         <v>480</v>
       </c>
-      <c r="C51" s="309"/>
+      <c r="C51" s="312"/>
       <c r="D51" s="168" t="s">
         <v>625</v>
       </c>
@@ -6955,7 +6955,7 @@
       <c r="B52" s="202" t="s">
         <v>454</v>
       </c>
-      <c r="C52" s="309"/>
+      <c r="C52" s="312"/>
       <c r="D52" s="168" t="s">
         <v>602</v>
       </c>
@@ -6967,7 +6967,7 @@
       <c r="B53" s="202" t="s">
         <v>450</v>
       </c>
-      <c r="C53" s="309"/>
+      <c r="C53" s="312"/>
       <c r="D53" s="168" t="s">
         <v>11</v>
       </c>
@@ -6979,7 +6979,7 @@
       <c r="B54" s="202" t="s">
         <v>451</v>
       </c>
-      <c r="C54" s="309"/>
+      <c r="C54" s="312"/>
       <c r="D54" s="168" t="s">
         <v>11</v>
       </c>
@@ -6991,7 +6991,7 @@
       <c r="B55" s="202" t="s">
         <v>453</v>
       </c>
-      <c r="C55" s="309"/>
+      <c r="C55" s="312"/>
       <c r="D55" s="168" t="s">
         <v>11</v>
       </c>
@@ -7003,7 +7003,7 @@
       <c r="B56" s="202" t="s">
         <v>452</v>
       </c>
-      <c r="C56" s="309"/>
+      <c r="C56" s="312"/>
       <c r="D56" s="168" t="s">
         <v>11</v>
       </c>
@@ -7015,7 +7015,7 @@
       <c r="B57" s="202" t="s">
         <v>417</v>
       </c>
-      <c r="C57" s="309"/>
+      <c r="C57" s="312"/>
       <c r="D57" s="168" t="s">
         <v>603</v>
       </c>
@@ -7027,7 +7027,7 @@
       <c r="B58" s="202" t="s">
         <v>418</v>
       </c>
-      <c r="C58" s="309"/>
+      <c r="C58" s="312"/>
       <c r="D58" s="168" t="s">
         <v>604</v>
       </c>
@@ -7039,7 +7039,7 @@
       <c r="B59" s="202" t="s">
         <v>419</v>
       </c>
-      <c r="C59" s="309"/>
+      <c r="C59" s="312"/>
       <c r="D59" s="168" t="s">
         <v>605</v>
       </c>
@@ -7051,7 +7051,7 @@
       <c r="B60" s="216" t="s">
         <v>420</v>
       </c>
-      <c r="C60" s="310"/>
+      <c r="C60" s="313"/>
       <c r="D60" s="172" t="s">
         <v>606</v>
       </c>
@@ -7140,7 +7140,7 @@
         <f>'Custom cases'!D4</f>
         <v>Custom_RfG_Fault_3_FRTtrig_0.87pu</v>
       </c>
-      <c r="C3" s="308" t="s">
+      <c r="C3" s="311" t="s">
         <v>701</v>
       </c>
       <c r="D3" s="244" t="s">
@@ -7155,7 +7155,7 @@
         <f>'Custom cases'!D5</f>
         <v>Custom_RfG_Fault_3_FRTtrig_0.86pu</v>
       </c>
-      <c r="C4" s="309"/>
+      <c r="C4" s="312"/>
       <c r="D4" s="244" t="s">
         <v>11</v>
       </c>
@@ -7168,7 +7168,7 @@
         <f>'Custom cases'!D6</f>
         <v>Custom_RfG_Fault_3_FRTtrig_0.85pu</v>
       </c>
-      <c r="C5" s="309"/>
+      <c r="C5" s="312"/>
       <c r="D5" s="168" t="s">
         <v>703</v>
       </c>
@@ -7181,7 +7181,7 @@
         <f>'Custom cases'!D7</f>
         <v>Custom_RfG_Fault_3_FRTtrig_0.84pu</v>
       </c>
-      <c r="C6" s="309"/>
+      <c r="C6" s="312"/>
       <c r="D6" s="244" t="s">
         <v>11</v>
       </c>
@@ -7194,7 +7194,7 @@
         <f>'Custom cases'!D8</f>
         <v>Custom_RfG_Fault_3_FRTtrig_0.83pu</v>
       </c>
-      <c r="C7" s="309"/>
+      <c r="C7" s="312"/>
       <c r="D7" s="244" t="s">
         <v>11</v>
       </c>
@@ -7207,7 +7207,7 @@
         <f>'Custom cases'!D9</f>
         <v>Custom_RfG_Fault_3_FRTtrig_0.82pu</v>
       </c>
-      <c r="C8" s="309"/>
+      <c r="C8" s="312"/>
       <c r="D8" s="244" t="s">
         <v>11</v>
       </c>
@@ -7220,7 +7220,7 @@
         <f>'Custom cases'!D10</f>
         <v>Custom_RfG_Fault_3_FRTtrig_0.81pu</v>
       </c>
-      <c r="C9" s="309"/>
+      <c r="C9" s="312"/>
       <c r="D9" s="244" t="s">
         <v>11</v>
       </c>
@@ -7233,7 +7233,7 @@
         <f>'Custom cases'!D11</f>
         <v>Custom_RfG_Fault_3_FRTtrig_0.80pu</v>
       </c>
-      <c r="C10" s="309"/>
+      <c r="C10" s="312"/>
       <c r="D10" s="244" t="s">
         <v>11</v>
       </c>
@@ -7246,7 +7246,7 @@
         <f>'Custom cases'!D12</f>
         <v>Custom_RfG_Fault_3_FRTtrig_0.79pu</v>
       </c>
-      <c r="C11" s="309"/>
+      <c r="C11" s="312"/>
       <c r="D11" s="244" t="s">
         <v>11</v>
       </c>
@@ -7259,7 +7259,7 @@
         <f>'Custom cases'!D13</f>
         <v>Custom_RfG_Fault_3_FRTtrig_0.78pu</v>
       </c>
-      <c r="C12" s="310"/>
+      <c r="C12" s="313"/>
       <c r="D12" s="245" t="s">
         <v>11</v>
       </c>
@@ -7272,7 +7272,7 @@
         <f>'Custom cases'!D14</f>
         <v>Custom_RfG_LVRT_FRTexit_0.84pu</v>
       </c>
-      <c r="C13" s="308" t="s">
+      <c r="C13" s="311" t="s">
         <v>700</v>
       </c>
       <c r="D13" s="244" t="s">
@@ -7287,7 +7287,7 @@
         <f>'Custom cases'!D15</f>
         <v>Custom_RfG_LVRT_FRTexit_0.85pu</v>
       </c>
-      <c r="C14" s="309"/>
+      <c r="C14" s="312"/>
       <c r="D14" s="168" t="s">
         <v>702</v>
       </c>
@@ -7300,7 +7300,7 @@
         <f>'Custom cases'!D16</f>
         <v>Custom_RfG_LVRT_FRTexit_0.86pu</v>
       </c>
-      <c r="C15" s="309"/>
+      <c r="C15" s="312"/>
       <c r="D15" s="244" t="s">
         <v>11</v>
       </c>
@@ -7313,7 +7313,7 @@
         <f>'Custom cases'!D17</f>
         <v>Custom_RfG_LVRT_FRTexit_0.87pu</v>
       </c>
-      <c r="C16" s="309"/>
+      <c r="C16" s="312"/>
       <c r="D16" s="244" t="s">
         <v>11</v>
       </c>
@@ -7326,7 +7326,7 @@
         <f>'Custom cases'!D18</f>
         <v>Custom_RfG_LVRT_FRTexit_0.88pu</v>
       </c>
-      <c r="C17" s="309"/>
+      <c r="C17" s="312"/>
       <c r="D17" s="244" t="s">
         <v>11</v>
       </c>
@@ -7339,7 +7339,7 @@
         <f>'Custom cases'!D19</f>
         <v>Custom_RfG_LVRT_FRTexit_0.89pu</v>
       </c>
-      <c r="C18" s="310"/>
+      <c r="C18" s="313"/>
       <c r="D18" s="245" t="s">
         <v>11</v>
       </c>
@@ -7352,7 +7352,7 @@
         <f>'Custom cases'!D20</f>
         <v>Custom_RfG_Fault_3_MaxIQ_0.24pu</v>
       </c>
-      <c r="C19" s="308" t="s">
+      <c r="C19" s="311" t="s">
         <v>729</v>
       </c>
       <c r="D19" s="244" t="s">
@@ -7367,7 +7367,7 @@
         <f>'Custom cases'!D21</f>
         <v>Custom_RfG_Fault_3_MaxIQ_0.23pu</v>
       </c>
-      <c r="C20" s="309"/>
+      <c r="C20" s="312"/>
       <c r="D20" s="244" t="s">
         <v>11</v>
       </c>
@@ -7380,7 +7380,7 @@
         <f>'Custom cases'!D22</f>
         <v>Custom_RfG_Fault_3_MaxIQ_0.22pu</v>
       </c>
-      <c r="C21" s="309"/>
+      <c r="C21" s="312"/>
       <c r="D21" s="244" t="s">
         <v>11</v>
       </c>
@@ -7393,7 +7393,7 @@
         <f>'Custom cases'!D23</f>
         <v>Custom_RfG_Fault_3_MaxIQ_0.21pu</v>
       </c>
-      <c r="C22" s="309"/>
+      <c r="C22" s="312"/>
       <c r="D22" s="244" t="s">
         <v>11</v>
       </c>
@@ -7406,7 +7406,7 @@
         <f>'Custom cases'!D24</f>
         <v>Custom_RfG_Fault_3_MaxIQ_0.20pu</v>
       </c>
-      <c r="C23" s="309"/>
+      <c r="C23" s="312"/>
       <c r="D23" s="168" t="s">
         <v>730</v>
       </c>
@@ -7419,7 +7419,7 @@
         <f>'Custom cases'!D25</f>
         <v>Custom_RfG_Fault_3_MaxIQ_0.19pu</v>
       </c>
-      <c r="C24" s="309"/>
+      <c r="C24" s="312"/>
       <c r="D24" s="244" t="s">
         <v>11</v>
       </c>
@@ -7432,7 +7432,7 @@
         <f>'Custom cases'!D26</f>
         <v>Custom_RfG_Fault_3_MaxIQ_0.18pu</v>
       </c>
-      <c r="C25" s="309"/>
+      <c r="C25" s="312"/>
       <c r="D25" s="244" t="s">
         <v>11</v>
       </c>
@@ -7445,7 +7445,7 @@
         <f>'Custom cases'!D27</f>
         <v>Custom_RfG_Fault_3_MaxIQ_0.17pu</v>
       </c>
-      <c r="C26" s="309"/>
+      <c r="C26" s="312"/>
       <c r="D26" s="244" t="s">
         <v>11</v>
       </c>
@@ -7458,7 +7458,7 @@
         <f>'Custom cases'!D28</f>
         <v>Custom_RfG_Fault_3_MaxIQ_0.16pu</v>
       </c>
-      <c r="C27" s="309"/>
+      <c r="C27" s="312"/>
       <c r="D27" s="244" t="s">
         <v>11</v>
       </c>
@@ -7471,7 +7471,7 @@
         <f>'Custom cases'!D29</f>
         <v>Custom_RfG_Fault_3_MaxIQ_0.15pu</v>
       </c>
-      <c r="C28" s="310"/>
+      <c r="C28" s="313"/>
       <c r="D28" s="245" t="s">
         <v>11</v>
       </c>
@@ -7484,7 +7484,7 @@
         <f>'Custom cases'!D30</f>
         <v>Custom_RfG_Fault_3_0.2pu_Plim_0.5pu</v>
       </c>
-      <c r="C29" s="308" t="s">
+      <c r="C29" s="311" t="s">
         <v>704</v>
       </c>
       <c r="D29" s="168" t="s">
@@ -7499,7 +7499,7 @@
         <f>'Custom cases'!D31</f>
         <v>Custom_RfG_Fault_2_0.2pu_Plim_0.5pu</v>
       </c>
-      <c r="C30" s="309"/>
+      <c r="C30" s="312"/>
       <c r="D30" s="244" t="s">
         <v>11</v>
       </c>
@@ -7512,7 +7512,7 @@
         <f>'Custom cases'!D32</f>
         <v>Custom_RfG_Fault_1_0.2pu_Plim_0.5pu</v>
       </c>
-      <c r="C31" s="309"/>
+      <c r="C31" s="312"/>
       <c r="D31" s="244" t="s">
         <v>11</v>
       </c>
@@ -7525,7 +7525,7 @@
         <f>'Custom cases'!D33</f>
         <v>Custom_RfG_Fault_3_0.2pu_Plim_0.15pu</v>
       </c>
-      <c r="C32" s="309"/>
+      <c r="C32" s="312"/>
       <c r="D32" s="168" t="s">
         <v>705</v>
       </c>
@@ -7538,7 +7538,7 @@
         <f>'Custom cases'!D34</f>
         <v>Custom_RfG_Fault_2_0.2pu_Plim_0.15pu</v>
       </c>
-      <c r="C33" s="309"/>
+      <c r="C33" s="312"/>
       <c r="D33" s="244" t="s">
         <v>11</v>
       </c>
@@ -7551,7 +7551,7 @@
         <f>'Custom cases'!D35</f>
         <v>Custom_RfG_Fault_1_0.2pu_Plim_0.15pu</v>
       </c>
-      <c r="C34" s="310"/>
+      <c r="C34" s="313"/>
       <c r="D34" s="245" t="s">
         <v>11</v>
       </c>
@@ -7564,7 +7564,7 @@
         <f>'Custom cases'!D36</f>
         <v>Custom_RfG_Ucontrol_Plim_1.00pu</v>
       </c>
-      <c r="C35" s="308" t="s">
+      <c r="C35" s="311" t="s">
         <v>709</v>
       </c>
       <c r="D35" s="168" t="s">
@@ -7579,7 +7579,7 @@
         <f>'Custom cases'!D37</f>
         <v>Custom_RfG_Ucontrol_Plim_0.50pu</v>
       </c>
-      <c r="C36" s="309"/>
+      <c r="C36" s="312"/>
       <c r="D36" s="168" t="s">
         <v>706</v>
       </c>
@@ -7592,7 +7592,7 @@
         <f>'Custom cases'!D38</f>
         <v>Custom_RfG_Ucontrol_Plim_0.15pu</v>
       </c>
-      <c r="C37" s="310"/>
+      <c r="C37" s="313"/>
       <c r="D37" s="172" t="s">
         <v>708</v>
       </c>
@@ -7605,7 +7605,7 @@
         <f>'Custom cases'!D39</f>
         <v>Custom_Fault_3_0.20pu_U0_1.118pu</v>
       </c>
-      <c r="C38" s="308" t="s">
+      <c r="C38" s="311" t="s">
         <v>719</v>
       </c>
       <c r="D38" s="175" t="s">
@@ -7620,7 +7620,7 @@
         <f>'Custom cases'!D40</f>
         <v>Custom_Fault_2_0.20pu_U0_1.118pu</v>
       </c>
-      <c r="C39" s="309"/>
+      <c r="C39" s="312"/>
       <c r="D39" s="244" t="s">
         <v>11</v>
       </c>
@@ -7633,7 +7633,7 @@
         <f>'Custom cases'!D41</f>
         <v>Custom_Fault_1_0.20pu_U0_1.118pu</v>
       </c>
-      <c r="C40" s="309"/>
+      <c r="C40" s="312"/>
       <c r="D40" s="244" t="s">
         <v>11</v>
       </c>
@@ -7646,7 +7646,7 @@
         <f>'Custom cases'!D42</f>
         <v>Custom_Fault_3_0.20pu_U0_0.968pu</v>
       </c>
-      <c r="C41" s="309"/>
+      <c r="C41" s="312"/>
       <c r="D41" s="168" t="s">
         <v>711</v>
       </c>
@@ -7659,7 +7659,7 @@
         <f>'Custom cases'!D43</f>
         <v>Custom_Fault_2_0.20pu_U0_0.968pu</v>
       </c>
-      <c r="C42" s="309"/>
+      <c r="C42" s="312"/>
       <c r="D42" s="244" t="s">
         <v>11</v>
       </c>
@@ -7672,7 +7672,7 @@
         <f>'Custom cases'!D44</f>
         <v>Custom_Fault_1_0.20pu_U0_0.968pu</v>
       </c>
-      <c r="C43" s="310"/>
+      <c r="C43" s="313"/>
       <c r="D43" s="245" t="s">
         <v>11</v>
       </c>
@@ -7685,7 +7685,7 @@
         <f>'Custom cases'!D45</f>
         <v>Custom_Fault_3_U0_1.118_Uend_1.065</v>
       </c>
-      <c r="C44" s="308" t="s">
+      <c r="C44" s="311" t="s">
         <v>720</v>
       </c>
       <c r="D44" s="175" t="s">
@@ -7700,7 +7700,7 @@
         <f>'Custom cases'!D46</f>
         <v>Custom_Fault_2_U0_1.118_Uend_1.065</v>
       </c>
-      <c r="C45" s="309"/>
+      <c r="C45" s="312"/>
       <c r="D45" s="244" t="s">
         <v>11</v>
       </c>
@@ -7713,7 +7713,7 @@
         <f>'Custom cases'!D47</f>
         <v>Custom_Fault_1_U0_1.118_Uend_1.065</v>
       </c>
-      <c r="C46" s="309"/>
+      <c r="C46" s="312"/>
       <c r="D46" s="244" t="s">
         <v>11</v>
       </c>
@@ -7726,7 +7726,7 @@
         <f>'Custom cases'!D48</f>
         <v>Custom_Fault_3_U0_1.118_Uend_0.968</v>
       </c>
-      <c r="C47" s="309"/>
+      <c r="C47" s="312"/>
       <c r="D47" s="244" t="s">
         <v>11</v>
       </c>
@@ -7739,7 +7739,7 @@
         <f>'Custom cases'!D49</f>
         <v>Custom_Fault_3_U0_0.959_Uend_1.065</v>
       </c>
-      <c r="C48" s="309"/>
+      <c r="C48" s="312"/>
       <c r="D48" s="168" t="s">
         <v>712</v>
       </c>
@@ -7752,7 +7752,7 @@
         <f>'Custom cases'!D50</f>
         <v>Custom_Fault_2_U0_0.959_Uend_1.065</v>
       </c>
-      <c r="C49" s="309"/>
+      <c r="C49" s="312"/>
       <c r="D49" s="244" t="s">
         <v>11</v>
       </c>
@@ -7765,7 +7765,7 @@
         <f>'Custom cases'!D51</f>
         <v>Custom_Fault_1_U0_0.959_Uend_1.065</v>
       </c>
-      <c r="C50" s="309"/>
+      <c r="C50" s="312"/>
       <c r="D50" s="244" t="s">
         <v>11</v>
       </c>
@@ -7778,7 +7778,7 @@
         <f>'Custom cases'!D52</f>
         <v>Custom_Fault_3_U0_0.959_Uend_1.118</v>
       </c>
-      <c r="C51" s="309"/>
+      <c r="C51" s="312"/>
       <c r="D51" s="244" t="s">
         <v>11</v>
       </c>
@@ -7791,7 +7791,7 @@
         <f>'Custom cases'!D53</f>
         <v>Custom_Fault_3_U0_1.118_Uend_0.900</v>
       </c>
-      <c r="C52" s="309"/>
+      <c r="C52" s="312"/>
       <c r="D52" s="168" t="s">
         <v>714</v>
       </c>
@@ -7804,7 +7804,7 @@
         <f>'Custom cases'!D54</f>
         <v>Custom_Fault_3_U0_1.065_Uend_0.900</v>
       </c>
-      <c r="C53" s="309"/>
+      <c r="C53" s="312"/>
       <c r="D53" s="244" t="s">
         <v>11</v>
       </c>
@@ -7817,7 +7817,7 @@
         <f>'Custom cases'!D55</f>
         <v>Custom_Fault_3_U0_0.959_Uend_0.900</v>
       </c>
-      <c r="C54" s="310"/>
+      <c r="C54" s="313"/>
       <c r="D54" s="245" t="s">
         <v>11</v>
       </c>
@@ -7830,7 +7830,7 @@
         <f>'Custom cases'!D56</f>
         <v>Custom_Fault_3_U0_1.065pu_OVRT_1.15</v>
       </c>
-      <c r="C55" s="308" t="s">
+      <c r="C55" s="311" t="s">
         <v>721</v>
       </c>
       <c r="D55" s="175" t="s">
@@ -7845,7 +7845,7 @@
         <f>'Custom cases'!D57</f>
         <v>Custom_Fault_3_U0_1.065pu_OVRT_1.20</v>
       </c>
-      <c r="C56" s="309"/>
+      <c r="C56" s="312"/>
       <c r="D56" s="168" t="s">
         <v>716</v>
       </c>
@@ -7858,7 +7858,7 @@
         <f>'Custom cases'!D58</f>
         <v>Custom_Fault_3_U0_1.065pu_OVRT_1.30</v>
       </c>
-      <c r="C57" s="309"/>
+      <c r="C57" s="312"/>
       <c r="D57" s="168" t="s">
         <v>715</v>
       </c>
@@ -7871,7 +7871,7 @@
         <f>'Custom cases'!D59</f>
         <v>Custom_Fault_3_U0_1.065pu_OVRT_1.15</v>
       </c>
-      <c r="C58" s="309"/>
+      <c r="C58" s="312"/>
       <c r="D58" s="168" t="s">
         <v>717</v>
       </c>
@@ -7884,7 +7884,7 @@
         <f>'Custom cases'!D60</f>
         <v>Custom_Fault_3_U0_1.065pu_OVRT_1.20</v>
       </c>
-      <c r="C59" s="309"/>
+      <c r="C59" s="312"/>
       <c r="D59" s="168" t="s">
         <v>717</v>
       </c>
@@ -7897,7 +7897,7 @@
         <f>'Custom cases'!D61</f>
         <v>Custom_Fault_3_U0_1.065pu_OVRT_1.30</v>
       </c>
-      <c r="C60" s="310"/>
+      <c r="C60" s="313"/>
       <c r="D60" s="172" t="s">
         <v>718</v>
       </c>
@@ -7910,7 +7910,7 @@
         <f>'Custom cases'!D62</f>
         <v>Custom_Fault_3_0.20pu_SCR_2</v>
       </c>
-      <c r="C61" s="308" t="s">
+      <c r="C61" s="311" t="s">
         <v>722</v>
       </c>
       <c r="D61" s="175" t="s">
@@ -7925,7 +7925,7 @@
         <f>'Custom cases'!D63</f>
         <v>Custom_Fault_3_0.20pu_SCR_3</v>
       </c>
-      <c r="C62" s="309"/>
+      <c r="C62" s="312"/>
       <c r="D62" s="244" t="s">
         <v>11</v>
       </c>
@@ -7938,7 +7938,7 @@
         <f>'Custom cases'!D64</f>
         <v>Custom_Fault_3_0.20pu_SCR_4</v>
       </c>
-      <c r="C63" s="309"/>
+      <c r="C63" s="312"/>
       <c r="D63" s="244" t="s">
         <v>11</v>
       </c>
@@ -7951,7 +7951,7 @@
         <f>'Custom cases'!D65</f>
         <v>Custom_Fault_3_0.20pu_SCR_5</v>
       </c>
-      <c r="C64" s="309"/>
+      <c r="C64" s="312"/>
       <c r="D64" s="244" t="s">
         <v>11</v>
       </c>
@@ -7964,7 +7964,7 @@
         <f>'Custom cases'!D66</f>
         <v>Custom_Fault_3_0.20pu_SCR_6</v>
       </c>
-      <c r="C65" s="309"/>
+      <c r="C65" s="312"/>
       <c r="D65" s="244" t="s">
         <v>11</v>
       </c>
@@ -7977,7 +7977,7 @@
         <f>'Custom cases'!D67</f>
         <v>Custom_Fault_2_0.20pu_SCR_2</v>
       </c>
-      <c r="C66" s="309"/>
+      <c r="C66" s="312"/>
       <c r="D66" s="244" t="s">
         <v>11</v>
       </c>
@@ -7990,7 +7990,7 @@
         <f>'Custom cases'!D68</f>
         <v>Custom_Fault_2_0.20pu_SCR_3</v>
       </c>
-      <c r="C67" s="309"/>
+      <c r="C67" s="312"/>
       <c r="D67" s="244" t="s">
         <v>11</v>
       </c>
@@ -8003,7 +8003,7 @@
         <f>'Custom cases'!D69</f>
         <v>Custom_Fault_2_0.20pu_SCR_4</v>
       </c>
-      <c r="C68" s="309"/>
+      <c r="C68" s="312"/>
       <c r="D68" s="244" t="s">
         <v>11</v>
       </c>
@@ -8016,7 +8016,7 @@
         <f>'Custom cases'!D70</f>
         <v>Custom_Fault_2_0.20pu_SCR_5</v>
       </c>
-      <c r="C69" s="309"/>
+      <c r="C69" s="312"/>
       <c r="D69" s="244" t="s">
         <v>11</v>
       </c>
@@ -8029,7 +8029,7 @@
         <f>'Custom cases'!D71</f>
         <v>Custom_Fault_2_0.20pu_SCR_6</v>
       </c>
-      <c r="C70" s="309"/>
+      <c r="C70" s="312"/>
       <c r="D70" s="244" t="s">
         <v>11</v>
       </c>
@@ -8042,7 +8042,7 @@
         <f>'Custom cases'!D72</f>
         <v>Custom_Fault_3_0.70pu_SCR_2</v>
       </c>
-      <c r="C71" s="309"/>
+      <c r="C71" s="312"/>
       <c r="D71" s="244" t="s">
         <v>11</v>
       </c>
@@ -8055,7 +8055,7 @@
         <f>'Custom cases'!D73</f>
         <v>Custom_Fault_3_0.70pu_SCR_3</v>
       </c>
-      <c r="C72" s="309"/>
+      <c r="C72" s="312"/>
       <c r="D72" s="244" t="s">
         <v>11</v>
       </c>
@@ -8068,7 +8068,7 @@
         <f>'Custom cases'!D74</f>
         <v>Custom_Fault_3_0.70pu_SCR_4</v>
       </c>
-      <c r="C73" s="309"/>
+      <c r="C73" s="312"/>
       <c r="D73" s="244" t="s">
         <v>11</v>
       </c>
@@ -8081,7 +8081,7 @@
         <f>'Custom cases'!D75</f>
         <v>Custom_Fault_3_0.70pu_SCR_5</v>
       </c>
-      <c r="C74" s="309"/>
+      <c r="C74" s="312"/>
       <c r="D74" s="244" t="s">
         <v>11</v>
       </c>
@@ -8094,7 +8094,7 @@
         <f>'Custom cases'!D76</f>
         <v>Custom_Fault_3_0.70pu_SCR_6</v>
       </c>
-      <c r="C75" s="309"/>
+      <c r="C75" s="312"/>
       <c r="D75" s="244" t="s">
         <v>11</v>
       </c>
@@ -8107,7 +8107,7 @@
         <f>'Custom cases'!D77</f>
         <v>Custom_Fault_2_0.70pu_SCR_2</v>
       </c>
-      <c r="C76" s="309"/>
+      <c r="C76" s="312"/>
       <c r="D76" s="244" t="s">
         <v>11</v>
       </c>
@@ -8120,7 +8120,7 @@
         <f>'Custom cases'!D78</f>
         <v>Custom_Fault_2_0.70pu_SCR_3</v>
       </c>
-      <c r="C77" s="309"/>
+      <c r="C77" s="312"/>
       <c r="D77" s="244" t="s">
         <v>11</v>
       </c>
@@ -8133,7 +8133,7 @@
         <f>'Custom cases'!D79</f>
         <v>Custom_Fault_2_0.70pu_SCR_4</v>
       </c>
-      <c r="C78" s="309"/>
+      <c r="C78" s="312"/>
       <c r="D78" s="244" t="s">
         <v>11</v>
       </c>
@@ -8146,7 +8146,7 @@
         <f>'Custom cases'!D80</f>
         <v>Custom_Fault_2_0.70pu_SCR_5</v>
       </c>
-      <c r="C79" s="309"/>
+      <c r="C79" s="312"/>
       <c r="D79" s="244" t="s">
         <v>11</v>
       </c>
@@ -8159,7 +8159,7 @@
         <f>'Custom cases'!D81</f>
         <v>Custom_Fault_2_0.70pu_SCR_6</v>
       </c>
-      <c r="C80" s="310"/>
+      <c r="C80" s="313"/>
       <c r="D80" s="245" t="s">
         <v>11</v>
       </c>
@@ -8172,7 +8172,7 @@
         <f>'Custom cases'!D82</f>
         <v>Custom_Fault_3_0.20pu_Duration_80</v>
       </c>
-      <c r="C81" s="308" t="s">
+      <c r="C81" s="311" t="s">
         <v>724</v>
       </c>
       <c r="D81" s="168" t="s">
@@ -8187,7 +8187,7 @@
         <f>'Custom cases'!D83</f>
         <v>Custom_Fault_3_0.20pu_Duration_60</v>
       </c>
-      <c r="C82" s="309"/>
+      <c r="C82" s="312"/>
       <c r="D82" s="244" t="s">
         <v>11</v>
       </c>
@@ -8200,7 +8200,7 @@
         <f>'Custom cases'!D84</f>
         <v>Custom_Fault_3_0.20pu_Duration_40</v>
       </c>
-      <c r="C83" s="309"/>
+      <c r="C83" s="312"/>
       <c r="D83" s="244" t="s">
         <v>11</v>
       </c>
@@ -8213,7 +8213,7 @@
         <f>'Custom cases'!D85</f>
         <v>Custom_Shift_10_Fault_3_0.20pu</v>
       </c>
-      <c r="C84" s="309"/>
+      <c r="C84" s="312"/>
       <c r="D84" s="168" t="s">
         <v>726</v>
       </c>
@@ -8226,7 +8226,7 @@
         <f>'Custom cases'!D86</f>
         <v>Custom_Shift_20_Fault_3_0.20pu</v>
       </c>
-      <c r="C85" s="309"/>
+      <c r="C85" s="312"/>
       <c r="D85" s="244" t="s">
         <v>11</v>
       </c>
@@ -8239,7 +8239,7 @@
         <f>'Custom cases'!D87</f>
         <v>Custom_Shift_30_Fault_3_0.20pu</v>
       </c>
-      <c r="C86" s="309"/>
+      <c r="C86" s="312"/>
       <c r="D86" s="244" t="s">
         <v>11</v>
       </c>
@@ -8252,7 +8252,7 @@
         <f>'Custom cases'!D88</f>
         <v>Custom_Shift_40_Fault_3_0.20pu</v>
       </c>
-      <c r="C87" s="309"/>
+      <c r="C87" s="312"/>
       <c r="D87" s="244" t="s">
         <v>11</v>
       </c>
@@ -8265,7 +8265,7 @@
         <f>'Custom cases'!D89</f>
         <v>Custom_Shift_50_Fault_3_0.20pu</v>
       </c>
-      <c r="C88" s="310"/>
+      <c r="C88" s="313"/>
       <c r="D88" s="245" t="s">
         <v>11</v>
       </c>
@@ -8427,16 +8427,16 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="41"/>
-      <c r="B1" s="293" t="s">
+      <c r="B1" s="296" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="294"/>
-      <c r="D1" s="295"/>
-      <c r="E1" s="293" t="s">
+      <c r="C1" s="297"/>
+      <c r="D1" s="298"/>
+      <c r="E1" s="296" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="294"/>
-      <c r="G1" s="294"/>
+      <c r="F1" s="297"/>
+      <c r="G1" s="297"/>
       <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
@@ -9413,9 +9413,9 @@
   </sheetPr>
   <dimension ref="A1:CQ218"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AD62" sqref="AD62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -9480,103 +9480,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.4">
-      <c r="A1" s="297" t="s">
+      <c r="A1" s="300" t="s">
         <v>659</v>
       </c>
-      <c r="B1" s="297"/>
-      <c r="C1" s="297"/>
-      <c r="D1" s="297"/>
-      <c r="E1" s="298" t="s">
+      <c r="B1" s="300"/>
+      <c r="C1" s="300"/>
+      <c r="D1" s="300"/>
+      <c r="E1" s="301" t="s">
         <v>660</v>
       </c>
-      <c r="F1" s="299"/>
-      <c r="G1" s="299"/>
-      <c r="H1" s="299"/>
-      <c r="I1" s="299"/>
-      <c r="J1" s="299"/>
-      <c r="K1" s="299"/>
-      <c r="L1" s="299"/>
-      <c r="M1" s="299"/>
-      <c r="N1" s="299"/>
-      <c r="O1" s="300"/>
-      <c r="P1" s="296" t="s">
+      <c r="F1" s="302"/>
+      <c r="G1" s="302"/>
+      <c r="H1" s="302"/>
+      <c r="I1" s="302"/>
+      <c r="J1" s="302"/>
+      <c r="K1" s="302"/>
+      <c r="L1" s="302"/>
+      <c r="M1" s="302"/>
+      <c r="N1" s="302"/>
+      <c r="O1" s="303"/>
+      <c r="P1" s="299" t="s">
         <v>78</v>
       </c>
-      <c r="Q1" s="296"/>
-      <c r="R1" s="296"/>
-      <c r="S1" s="296"/>
-      <c r="T1" s="297" t="s">
+      <c r="Q1" s="299"/>
+      <c r="R1" s="299"/>
+      <c r="S1" s="299"/>
+      <c r="T1" s="300" t="s">
         <v>79</v>
       </c>
-      <c r="U1" s="297"/>
-      <c r="V1" s="297"/>
-      <c r="W1" s="297"/>
-      <c r="X1" s="296" t="s">
+      <c r="U1" s="300"/>
+      <c r="V1" s="300"/>
+      <c r="W1" s="300"/>
+      <c r="X1" s="299" t="s">
         <v>80</v>
       </c>
-      <c r="Y1" s="296"/>
-      <c r="Z1" s="296"/>
-      <c r="AA1" s="296"/>
-      <c r="AB1" s="297" t="s">
+      <c r="Y1" s="299"/>
+      <c r="Z1" s="299"/>
+      <c r="AA1" s="299"/>
+      <c r="AB1" s="300" t="s">
         <v>81</v>
       </c>
-      <c r="AC1" s="297"/>
-      <c r="AD1" s="297"/>
-      <c r="AE1" s="297"/>
-      <c r="AF1" s="296" t="s">
+      <c r="AC1" s="300"/>
+      <c r="AD1" s="300"/>
+      <c r="AE1" s="300"/>
+      <c r="AF1" s="299" t="s">
         <v>82</v>
       </c>
-      <c r="AG1" s="296"/>
-      <c r="AH1" s="296"/>
-      <c r="AI1" s="296"/>
-      <c r="AJ1" s="297" t="s">
+      <c r="AG1" s="299"/>
+      <c r="AH1" s="299"/>
+      <c r="AI1" s="299"/>
+      <c r="AJ1" s="300" t="s">
         <v>83</v>
       </c>
-      <c r="AK1" s="297"/>
-      <c r="AL1" s="297"/>
-      <c r="AM1" s="297"/>
-      <c r="AN1" s="296" t="s">
+      <c r="AK1" s="300"/>
+      <c r="AL1" s="300"/>
+      <c r="AM1" s="300"/>
+      <c r="AN1" s="299" t="s">
         <v>84</v>
       </c>
-      <c r="AO1" s="296"/>
-      <c r="AP1" s="296"/>
-      <c r="AQ1" s="296"/>
-      <c r="AR1" s="297" t="s">
+      <c r="AO1" s="299"/>
+      <c r="AP1" s="299"/>
+      <c r="AQ1" s="299"/>
+      <c r="AR1" s="300" t="s">
         <v>85</v>
       </c>
-      <c r="AS1" s="297"/>
-      <c r="AT1" s="297"/>
-      <c r="AU1" s="297"/>
-      <c r="AV1" s="296" t="s">
+      <c r="AS1" s="300"/>
+      <c r="AT1" s="300"/>
+      <c r="AU1" s="300"/>
+      <c r="AV1" s="299" t="s">
         <v>86</v>
       </c>
-      <c r="AW1" s="296"/>
-      <c r="AX1" s="296"/>
-      <c r="AY1" s="296"/>
-      <c r="AZ1" s="297" t="s">
+      <c r="AW1" s="299"/>
+      <c r="AX1" s="299"/>
+      <c r="AY1" s="299"/>
+      <c r="AZ1" s="300" t="s">
         <v>87</v>
       </c>
-      <c r="BA1" s="297"/>
-      <c r="BB1" s="297"/>
-      <c r="BC1" s="297"/>
-      <c r="BD1" s="296" t="s">
+      <c r="BA1" s="300"/>
+      <c r="BB1" s="300"/>
+      <c r="BC1" s="300"/>
+      <c r="BD1" s="299" t="s">
         <v>88</v>
       </c>
-      <c r="BE1" s="296"/>
-      <c r="BF1" s="296"/>
-      <c r="BG1" s="296"/>
-      <c r="BH1" s="297" t="s">
+      <c r="BE1" s="299"/>
+      <c r="BF1" s="299"/>
+      <c r="BG1" s="299"/>
+      <c r="BH1" s="300" t="s">
         <v>89</v>
       </c>
-      <c r="BI1" s="297"/>
-      <c r="BJ1" s="297"/>
-      <c r="BK1" s="297"/>
-      <c r="BL1" s="296" t="s">
+      <c r="BI1" s="300"/>
+      <c r="BJ1" s="300"/>
+      <c r="BK1" s="300"/>
+      <c r="BL1" s="299" t="s">
         <v>688</v>
       </c>
-      <c r="BM1" s="296"/>
-      <c r="BN1" s="296"/>
-      <c r="BO1" s="296"/>
+      <c r="BM1" s="299"/>
+      <c r="BN1" s="299"/>
+      <c r="BO1" s="299"/>
     </row>
     <row r="2" spans="1:67" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -16936,7 +16936,7 @@
         <v>1.65</v>
       </c>
       <c r="AD61" s="89">
-        <v>0.25</v>
+        <v>4</v>
       </c>
       <c r="AE61" s="89"/>
       <c r="AF61" s="97" t="s">
@@ -31470,95 +31470,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:93" x14ac:dyDescent="0.4">
-      <c r="A1" s="297" t="s">
+      <c r="A1" s="300" t="s">
         <v>659</v>
       </c>
-      <c r="B1" s="297"/>
-      <c r="C1" s="297"/>
-      <c r="D1" s="297"/>
-      <c r="E1" s="298" t="s">
+      <c r="B1" s="300"/>
+      <c r="C1" s="300"/>
+      <c r="D1" s="300"/>
+      <c r="E1" s="301" t="s">
         <v>660</v>
       </c>
-      <c r="F1" s="299"/>
-      <c r="G1" s="299"/>
-      <c r="H1" s="299"/>
-      <c r="I1" s="299"/>
-      <c r="J1" s="299"/>
-      <c r="K1" s="299"/>
-      <c r="L1" s="299"/>
-      <c r="M1" s="300"/>
-      <c r="N1" s="304" t="s">
+      <c r="F1" s="302"/>
+      <c r="G1" s="302"/>
+      <c r="H1" s="302"/>
+      <c r="I1" s="302"/>
+      <c r="J1" s="302"/>
+      <c r="K1" s="302"/>
+      <c r="L1" s="302"/>
+      <c r="M1" s="303"/>
+      <c r="N1" s="307" t="s">
         <v>78</v>
       </c>
-      <c r="O1" s="305"/>
-      <c r="P1" s="305"/>
-      <c r="Q1" s="306"/>
-      <c r="R1" s="298" t="s">
+      <c r="O1" s="308"/>
+      <c r="P1" s="308"/>
+      <c r="Q1" s="309"/>
+      <c r="R1" s="301" t="s">
         <v>79</v>
       </c>
-      <c r="S1" s="299"/>
-      <c r="T1" s="299"/>
-      <c r="U1" s="299"/>
-      <c r="V1" s="304" t="s">
+      <c r="S1" s="302"/>
+      <c r="T1" s="302"/>
+      <c r="U1" s="302"/>
+      <c r="V1" s="307" t="s">
         <v>80</v>
       </c>
-      <c r="W1" s="305"/>
-      <c r="X1" s="305"/>
-      <c r="Y1" s="306"/>
-      <c r="Z1" s="301" t="s">
+      <c r="W1" s="308"/>
+      <c r="X1" s="308"/>
+      <c r="Y1" s="309"/>
+      <c r="Z1" s="304" t="s">
         <v>81</v>
       </c>
-      <c r="AA1" s="302"/>
-      <c r="AB1" s="302"/>
-      <c r="AC1" s="303"/>
-      <c r="AD1" s="304" t="s">
+      <c r="AA1" s="305"/>
+      <c r="AB1" s="305"/>
+      <c r="AC1" s="306"/>
+      <c r="AD1" s="307" t="s">
         <v>82</v>
       </c>
-      <c r="AE1" s="305"/>
-      <c r="AF1" s="305"/>
-      <c r="AG1" s="306"/>
-      <c r="AH1" s="301" t="s">
+      <c r="AE1" s="308"/>
+      <c r="AF1" s="308"/>
+      <c r="AG1" s="309"/>
+      <c r="AH1" s="304" t="s">
         <v>83</v>
       </c>
-      <c r="AI1" s="302"/>
-      <c r="AJ1" s="302"/>
-      <c r="AK1" s="303"/>
-      <c r="AL1" s="304" t="s">
+      <c r="AI1" s="305"/>
+      <c r="AJ1" s="305"/>
+      <c r="AK1" s="306"/>
+      <c r="AL1" s="307" t="s">
         <v>84</v>
       </c>
-      <c r="AM1" s="305"/>
-      <c r="AN1" s="305"/>
-      <c r="AO1" s="306"/>
-      <c r="AP1" s="301" t="s">
+      <c r="AM1" s="308"/>
+      <c r="AN1" s="308"/>
+      <c r="AO1" s="309"/>
+      <c r="AP1" s="304" t="s">
         <v>85</v>
       </c>
-      <c r="AQ1" s="302"/>
-      <c r="AR1" s="302"/>
-      <c r="AS1" s="303"/>
-      <c r="AT1" s="304" t="s">
+      <c r="AQ1" s="305"/>
+      <c r="AR1" s="305"/>
+      <c r="AS1" s="306"/>
+      <c r="AT1" s="307" t="s">
         <v>86</v>
       </c>
-      <c r="AU1" s="305"/>
-      <c r="AV1" s="305"/>
-      <c r="AW1" s="306"/>
-      <c r="AX1" s="301" t="s">
+      <c r="AU1" s="308"/>
+      <c r="AV1" s="308"/>
+      <c r="AW1" s="309"/>
+      <c r="AX1" s="304" t="s">
         <v>87</v>
       </c>
-      <c r="AY1" s="302"/>
-      <c r="AZ1" s="302"/>
-      <c r="BA1" s="303"/>
-      <c r="BB1" s="304" t="s">
+      <c r="AY1" s="305"/>
+      <c r="AZ1" s="305"/>
+      <c r="BA1" s="306"/>
+      <c r="BB1" s="307" t="s">
         <v>88</v>
       </c>
-      <c r="BC1" s="305"/>
-      <c r="BD1" s="305"/>
-      <c r="BE1" s="306"/>
-      <c r="BF1" s="301" t="s">
+      <c r="BC1" s="308"/>
+      <c r="BD1" s="308"/>
+      <c r="BE1" s="309"/>
+      <c r="BF1" s="304" t="s">
         <v>89</v>
       </c>
-      <c r="BG1" s="302"/>
-      <c r="BH1" s="302"/>
-      <c r="BI1" s="303"/>
+      <c r="BG1" s="305"/>
+      <c r="BH1" s="305"/>
+      <c r="BI1" s="306"/>
     </row>
     <row r="2" spans="1:93" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -31589,7 +31589,7 @@
         <v>98</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>734</v>
+        <v>742</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>99</v>
@@ -36817,7 +36817,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3:G62"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -36880,96 +36880,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.4">
-      <c r="A1" s="297" t="s">
+      <c r="A1" s="300" t="s">
         <v>659</v>
       </c>
-      <c r="B1" s="297"/>
-      <c r="C1" s="297"/>
-      <c r="D1" s="297"/>
-      <c r="E1" s="298" t="s">
+      <c r="B1" s="300"/>
+      <c r="C1" s="300"/>
+      <c r="D1" s="300"/>
+      <c r="E1" s="301" t="s">
         <v>660</v>
       </c>
-      <c r="F1" s="299"/>
-      <c r="G1" s="299"/>
-      <c r="H1" s="299"/>
-      <c r="I1" s="299"/>
-      <c r="J1" s="299"/>
-      <c r="K1" s="299"/>
-      <c r="L1" s="299"/>
-      <c r="M1" s="299"/>
-      <c r="N1" s="300"/>
-      <c r="O1" s="307" t="s">
+      <c r="F1" s="302"/>
+      <c r="G1" s="302"/>
+      <c r="H1" s="302"/>
+      <c r="I1" s="302"/>
+      <c r="J1" s="302"/>
+      <c r="K1" s="302"/>
+      <c r="L1" s="302"/>
+      <c r="M1" s="302"/>
+      <c r="N1" s="303"/>
+      <c r="O1" s="310" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="307"/>
-      <c r="Q1" s="307"/>
-      <c r="R1" s="307"/>
-      <c r="S1" s="297" t="s">
+      <c r="P1" s="310"/>
+      <c r="Q1" s="310"/>
+      <c r="R1" s="310"/>
+      <c r="S1" s="300" t="s">
         <v>79</v>
       </c>
-      <c r="T1" s="297"/>
-      <c r="U1" s="297"/>
-      <c r="V1" s="297"/>
-      <c r="W1" s="307" t="s">
+      <c r="T1" s="300"/>
+      <c r="U1" s="300"/>
+      <c r="V1" s="300"/>
+      <c r="W1" s="310" t="s">
         <v>80</v>
       </c>
-      <c r="X1" s="307"/>
-      <c r="Y1" s="307"/>
-      <c r="Z1" s="307"/>
-      <c r="AA1" s="297" t="s">
+      <c r="X1" s="310"/>
+      <c r="Y1" s="310"/>
+      <c r="Z1" s="310"/>
+      <c r="AA1" s="300" t="s">
         <v>81</v>
       </c>
-      <c r="AB1" s="297"/>
-      <c r="AC1" s="297"/>
-      <c r="AD1" s="297"/>
-      <c r="AE1" s="307" t="s">
+      <c r="AB1" s="300"/>
+      <c r="AC1" s="300"/>
+      <c r="AD1" s="300"/>
+      <c r="AE1" s="310" t="s">
         <v>82</v>
       </c>
-      <c r="AF1" s="307"/>
-      <c r="AG1" s="307"/>
-      <c r="AH1" s="307"/>
-      <c r="AI1" s="297" t="s">
+      <c r="AF1" s="310"/>
+      <c r="AG1" s="310"/>
+      <c r="AH1" s="310"/>
+      <c r="AI1" s="300" t="s">
         <v>83</v>
       </c>
-      <c r="AJ1" s="297"/>
-      <c r="AK1" s="297"/>
-      <c r="AL1" s="297"/>
-      <c r="AM1" s="307" t="s">
+      <c r="AJ1" s="300"/>
+      <c r="AK1" s="300"/>
+      <c r="AL1" s="300"/>
+      <c r="AM1" s="310" t="s">
         <v>84</v>
       </c>
-      <c r="AN1" s="307"/>
-      <c r="AO1" s="307"/>
-      <c r="AP1" s="307"/>
-      <c r="AQ1" s="297" t="s">
+      <c r="AN1" s="310"/>
+      <c r="AO1" s="310"/>
+      <c r="AP1" s="310"/>
+      <c r="AQ1" s="300" t="s">
         <v>85</v>
       </c>
-      <c r="AR1" s="297"/>
-      <c r="AS1" s="297"/>
-      <c r="AT1" s="297"/>
-      <c r="AU1" s="307" t="s">
+      <c r="AR1" s="300"/>
+      <c r="AS1" s="300"/>
+      <c r="AT1" s="300"/>
+      <c r="AU1" s="310" t="s">
         <v>86</v>
       </c>
-      <c r="AV1" s="307"/>
-      <c r="AW1" s="307"/>
-      <c r="AX1" s="307"/>
-      <c r="AY1" s="297" t="s">
+      <c r="AV1" s="310"/>
+      <c r="AW1" s="310"/>
+      <c r="AX1" s="310"/>
+      <c r="AY1" s="300" t="s">
         <v>87</v>
       </c>
-      <c r="AZ1" s="297"/>
-      <c r="BA1" s="297"/>
-      <c r="BB1" s="297"/>
-      <c r="BC1" s="307" t="s">
+      <c r="AZ1" s="300"/>
+      <c r="BA1" s="300"/>
+      <c r="BB1" s="300"/>
+      <c r="BC1" s="310" t="s">
         <v>88</v>
       </c>
-      <c r="BD1" s="307"/>
-      <c r="BE1" s="307"/>
-      <c r="BF1" s="307"/>
-      <c r="BG1" s="297" t="s">
+      <c r="BD1" s="310"/>
+      <c r="BE1" s="310"/>
+      <c r="BF1" s="310"/>
+      <c r="BG1" s="300" t="s">
         <v>89</v>
       </c>
-      <c r="BH1" s="297"/>
-      <c r="BI1" s="297"/>
-      <c r="BJ1" s="297"/>
+      <c r="BH1" s="300"/>
+      <c r="BI1" s="300"/>
+      <c r="BJ1" s="300"/>
     </row>
     <row r="2" spans="1:62" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -37003,7 +37003,7 @@
         <v>98</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>734</v>
+        <v>742</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>99</v>
@@ -43930,96 +43930,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.4">
-      <c r="A1" s="297" t="s">
+      <c r="A1" s="300" t="s">
         <v>659</v>
       </c>
-      <c r="B1" s="297"/>
-      <c r="C1" s="297"/>
-      <c r="D1" s="297"/>
-      <c r="E1" s="298" t="s">
+      <c r="B1" s="300"/>
+      <c r="C1" s="300"/>
+      <c r="D1" s="300"/>
+      <c r="E1" s="301" t="s">
         <v>660</v>
       </c>
-      <c r="F1" s="299"/>
-      <c r="G1" s="299"/>
-      <c r="H1" s="299"/>
-      <c r="I1" s="299"/>
-      <c r="J1" s="299"/>
-      <c r="K1" s="299"/>
-      <c r="L1" s="299"/>
-      <c r="M1" s="299"/>
-      <c r="N1" s="300"/>
-      <c r="O1" s="307" t="s">
+      <c r="F1" s="302"/>
+      <c r="G1" s="302"/>
+      <c r="H1" s="302"/>
+      <c r="I1" s="302"/>
+      <c r="J1" s="302"/>
+      <c r="K1" s="302"/>
+      <c r="L1" s="302"/>
+      <c r="M1" s="302"/>
+      <c r="N1" s="303"/>
+      <c r="O1" s="310" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="307"/>
-      <c r="Q1" s="307"/>
-      <c r="R1" s="307"/>
-      <c r="S1" s="298" t="s">
+      <c r="P1" s="310"/>
+      <c r="Q1" s="310"/>
+      <c r="R1" s="310"/>
+      <c r="S1" s="301" t="s">
         <v>79</v>
       </c>
-      <c r="T1" s="299"/>
-      <c r="U1" s="299"/>
-      <c r="V1" s="299"/>
-      <c r="W1" s="307" t="s">
+      <c r="T1" s="302"/>
+      <c r="U1" s="302"/>
+      <c r="V1" s="302"/>
+      <c r="W1" s="310" t="s">
         <v>80</v>
       </c>
-      <c r="X1" s="307"/>
-      <c r="Y1" s="307"/>
-      <c r="Z1" s="307"/>
-      <c r="AA1" s="298" t="s">
+      <c r="X1" s="310"/>
+      <c r="Y1" s="310"/>
+      <c r="Z1" s="310"/>
+      <c r="AA1" s="301" t="s">
         <v>81</v>
       </c>
-      <c r="AB1" s="299"/>
-      <c r="AC1" s="299"/>
-      <c r="AD1" s="299"/>
-      <c r="AE1" s="307" t="s">
+      <c r="AB1" s="302"/>
+      <c r="AC1" s="302"/>
+      <c r="AD1" s="302"/>
+      <c r="AE1" s="310" t="s">
         <v>82</v>
       </c>
-      <c r="AF1" s="307"/>
-      <c r="AG1" s="307"/>
-      <c r="AH1" s="307"/>
-      <c r="AI1" s="298" t="s">
+      <c r="AF1" s="310"/>
+      <c r="AG1" s="310"/>
+      <c r="AH1" s="310"/>
+      <c r="AI1" s="301" t="s">
         <v>83</v>
       </c>
-      <c r="AJ1" s="299"/>
-      <c r="AK1" s="299"/>
-      <c r="AL1" s="299"/>
-      <c r="AM1" s="307" t="s">
+      <c r="AJ1" s="302"/>
+      <c r="AK1" s="302"/>
+      <c r="AL1" s="302"/>
+      <c r="AM1" s="310" t="s">
         <v>84</v>
       </c>
-      <c r="AN1" s="307"/>
-      <c r="AO1" s="307"/>
-      <c r="AP1" s="307"/>
-      <c r="AQ1" s="298" t="s">
+      <c r="AN1" s="310"/>
+      <c r="AO1" s="310"/>
+      <c r="AP1" s="310"/>
+      <c r="AQ1" s="301" t="s">
         <v>85</v>
       </c>
-      <c r="AR1" s="299"/>
-      <c r="AS1" s="299"/>
-      <c r="AT1" s="299"/>
-      <c r="AU1" s="307" t="s">
+      <c r="AR1" s="302"/>
+      <c r="AS1" s="302"/>
+      <c r="AT1" s="302"/>
+      <c r="AU1" s="310" t="s">
         <v>86</v>
       </c>
-      <c r="AV1" s="307"/>
-      <c r="AW1" s="307"/>
-      <c r="AX1" s="307"/>
-      <c r="AY1" s="298" t="s">
+      <c r="AV1" s="310"/>
+      <c r="AW1" s="310"/>
+      <c r="AX1" s="310"/>
+      <c r="AY1" s="301" t="s">
         <v>87</v>
       </c>
-      <c r="AZ1" s="299"/>
-      <c r="BA1" s="299"/>
-      <c r="BB1" s="299"/>
-      <c r="BC1" s="307" t="s">
+      <c r="AZ1" s="302"/>
+      <c r="BA1" s="302"/>
+      <c r="BB1" s="302"/>
+      <c r="BC1" s="310" t="s">
         <v>88</v>
       </c>
-      <c r="BD1" s="307"/>
-      <c r="BE1" s="307"/>
-      <c r="BF1" s="307"/>
-      <c r="BG1" s="298" t="s">
+      <c r="BD1" s="310"/>
+      <c r="BE1" s="310"/>
+      <c r="BF1" s="310"/>
+      <c r="BG1" s="301" t="s">
         <v>89</v>
       </c>
-      <c r="BH1" s="299"/>
-      <c r="BI1" s="299"/>
-      <c r="BJ1" s="299"/>
+      <c r="BH1" s="302"/>
+      <c r="BI1" s="302"/>
+      <c r="BJ1" s="302"/>
     </row>
     <row r="2" spans="1:62" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
@@ -51296,7 +51296,7 @@
       <c r="B2" s="150" t="s">
         <v>487</v>
       </c>
-      <c r="C2" s="308" t="s">
+      <c r="C2" s="311" t="s">
         <v>508</v>
       </c>
       <c r="D2" s="175" t="s">
@@ -51310,7 +51310,7 @@
       <c r="B3" s="152" t="s">
         <v>488</v>
       </c>
-      <c r="C3" s="309"/>
+      <c r="C3" s="312"/>
       <c r="D3" s="168" t="s">
         <v>510</v>
       </c>
@@ -51322,7 +51322,7 @@
       <c r="B4" s="152" t="s">
         <v>489</v>
       </c>
-      <c r="C4" s="309"/>
+      <c r="C4" s="312"/>
       <c r="D4" s="168" t="s">
         <v>11</v>
       </c>
@@ -51334,7 +51334,7 @@
       <c r="B5" s="152" t="s">
         <v>490</v>
       </c>
-      <c r="C5" s="309"/>
+      <c r="C5" s="312"/>
       <c r="D5" s="168" t="s">
         <v>11</v>
       </c>
@@ -51346,7 +51346,7 @@
       <c r="B6" s="152" t="s">
         <v>491</v>
       </c>
-      <c r="C6" s="309"/>
+      <c r="C6" s="312"/>
       <c r="D6" s="168" t="s">
         <v>11</v>
       </c>
@@ -51358,7 +51358,7 @@
       <c r="B7" s="152" t="s">
         <v>492</v>
       </c>
-      <c r="C7" s="309"/>
+      <c r="C7" s="312"/>
       <c r="D7" s="168" t="s">
         <v>11</v>
       </c>
@@ -51370,7 +51370,7 @@
       <c r="B8" s="152" t="s">
         <v>493</v>
       </c>
-      <c r="C8" s="309"/>
+      <c r="C8" s="312"/>
       <c r="D8" s="168" t="s">
         <v>11</v>
       </c>
@@ -51382,7 +51382,7 @@
       <c r="B9" s="152" t="s">
         <v>494</v>
       </c>
-      <c r="C9" s="309"/>
+      <c r="C9" s="312"/>
       <c r="D9" s="168" t="s">
         <v>11</v>
       </c>
@@ -51394,7 +51394,7 @@
       <c r="B10" s="152" t="s">
         <v>495</v>
       </c>
-      <c r="C10" s="309"/>
+      <c r="C10" s="312"/>
       <c r="D10" s="168" t="s">
         <v>11</v>
       </c>
@@ -51406,7 +51406,7 @@
       <c r="B11" s="155" t="s">
         <v>505</v>
       </c>
-      <c r="C11" s="310"/>
+      <c r="C11" s="313"/>
       <c r="D11" s="172" t="s">
         <v>11</v>
       </c>
@@ -51418,7 +51418,7 @@
       <c r="B12" s="157" t="s">
         <v>239</v>
       </c>
-      <c r="C12" s="308" t="s">
+      <c r="C12" s="311" t="s">
         <v>511</v>
       </c>
       <c r="D12" s="175" t="s">
@@ -51432,7 +51432,7 @@
       <c r="B13" s="158" t="s">
         <v>240</v>
       </c>
-      <c r="C13" s="309"/>
+      <c r="C13" s="312"/>
       <c r="D13" s="168" t="s">
         <v>513</v>
       </c>
@@ -51444,7 +51444,7 @@
       <c r="B14" s="158" t="s">
         <v>241</v>
       </c>
-      <c r="C14" s="309"/>
+      <c r="C14" s="312"/>
       <c r="D14" s="168" t="s">
         <v>11</v>
       </c>
@@ -51456,7 +51456,7 @@
       <c r="B15" s="158" t="s">
         <v>242</v>
       </c>
-      <c r="C15" s="309"/>
+      <c r="C15" s="312"/>
       <c r="D15" s="168" t="s">
         <v>11</v>
       </c>
@@ -51468,7 +51468,7 @@
       <c r="B16" s="158" t="s">
         <v>243</v>
       </c>
-      <c r="C16" s="309"/>
+      <c r="C16" s="312"/>
       <c r="D16" s="168" t="s">
         <v>11</v>
       </c>
@@ -51480,7 +51480,7 @@
       <c r="B17" s="159" t="s">
         <v>244</v>
       </c>
-      <c r="C17" s="310"/>
+      <c r="C17" s="313"/>
       <c r="D17" s="172" t="s">
         <v>11</v>
       </c>
@@ -51492,7 +51492,7 @@
       <c r="B18" s="160" t="s">
         <v>245</v>
       </c>
-      <c r="C18" s="308" t="s">
+      <c r="C18" s="311" t="s">
         <v>108</v>
       </c>
       <c r="D18" s="175" t="s">
@@ -51506,7 +51506,7 @@
       <c r="B19" s="162" t="s">
         <v>246</v>
       </c>
-      <c r="C19" s="309"/>
+      <c r="C19" s="312"/>
       <c r="D19" s="168" t="s">
         <v>515</v>
       </c>
@@ -51518,7 +51518,7 @@
       <c r="B20" s="161" t="s">
         <v>247</v>
       </c>
-      <c r="C20" s="309"/>
+      <c r="C20" s="312"/>
       <c r="D20" s="168" t="s">
         <v>516</v>
       </c>
@@ -51530,7 +51530,7 @@
       <c r="B21" s="161" t="s">
         <v>248</v>
       </c>
-      <c r="C21" s="309"/>
+      <c r="C21" s="312"/>
       <c r="D21" s="168" t="s">
         <v>517</v>
       </c>
@@ -51542,7 +51542,7 @@
       <c r="B22" s="161" t="s">
         <v>249</v>
       </c>
-      <c r="C22" s="309"/>
+      <c r="C22" s="312"/>
       <c r="D22" s="168" t="s">
         <v>518</v>
       </c>
@@ -51554,7 +51554,7 @@
       <c r="B23" s="161" t="s">
         <v>250</v>
       </c>
-      <c r="C23" s="309"/>
+      <c r="C23" s="312"/>
       <c r="D23" s="168" t="s">
         <v>519</v>
       </c>
@@ -51566,7 +51566,7 @@
       <c r="B24" s="161" t="s">
         <v>485</v>
       </c>
-      <c r="C24" s="309"/>
+      <c r="C24" s="312"/>
       <c r="D24" s="168" t="s">
         <v>11</v>
       </c>
@@ -51578,7 +51578,7 @@
       <c r="B25" s="161" t="s">
         <v>486</v>
       </c>
-      <c r="C25" s="309"/>
+      <c r="C25" s="312"/>
       <c r="D25" s="168" t="s">
         <v>520</v>
       </c>
@@ -51590,7 +51590,7 @@
       <c r="B26" s="161" t="s">
         <v>251</v>
       </c>
-      <c r="C26" s="309"/>
+      <c r="C26" s="312"/>
       <c r="D26" s="168" t="s">
         <v>11</v>
       </c>
@@ -51602,7 +51602,7 @@
       <c r="B27" s="162" t="s">
         <v>496</v>
       </c>
-      <c r="C27" s="309"/>
+      <c r="C27" s="312"/>
       <c r="D27" s="168" t="s">
         <v>521</v>
       </c>
@@ -51614,7 +51614,7 @@
       <c r="B28" s="162" t="s">
         <v>497</v>
       </c>
-      <c r="C28" s="310"/>
+      <c r="C28" s="313"/>
       <c r="D28" s="168" t="s">
         <v>522</v>
       </c>
@@ -51626,7 +51626,7 @@
       <c r="B29" s="164" t="s">
         <v>252</v>
       </c>
-      <c r="C29" s="308" t="s">
+      <c r="C29" s="311" t="s">
         <v>523</v>
       </c>
       <c r="D29" s="175" t="s">
@@ -51640,7 +51640,7 @@
       <c r="B30" s="166" t="s">
         <v>253</v>
       </c>
-      <c r="C30" s="309"/>
+      <c r="C30" s="312"/>
       <c r="D30" s="168" t="s">
         <v>656</v>
       </c>
@@ -51652,7 +51652,7 @@
       <c r="B31" s="167" t="s">
         <v>254</v>
       </c>
-      <c r="C31" s="309"/>
+      <c r="C31" s="312"/>
       <c r="D31" s="168" t="s">
         <v>525</v>
       </c>
@@ -51664,7 +51664,7 @@
       <c r="B32" s="167" t="s">
         <v>255</v>
       </c>
-      <c r="C32" s="309"/>
+      <c r="C32" s="312"/>
       <c r="D32" s="168" t="s">
         <v>526</v>
       </c>
@@ -51676,7 +51676,7 @@
       <c r="B33" s="167" t="s">
         <v>256</v>
       </c>
-      <c r="C33" s="309"/>
+      <c r="C33" s="312"/>
       <c r="D33" s="168" t="s">
         <v>527</v>
       </c>
@@ -51688,7 +51688,7 @@
       <c r="B34" s="166" t="s">
         <v>257</v>
       </c>
-      <c r="C34" s="309"/>
+      <c r="C34" s="312"/>
       <c r="D34" s="168" t="s">
         <v>528</v>
       </c>
@@ -51700,7 +51700,7 @@
       <c r="B35" s="167" t="s">
         <v>258</v>
       </c>
-      <c r="C35" s="309"/>
+      <c r="C35" s="312"/>
       <c r="D35" s="168" t="s">
         <v>529</v>
       </c>
@@ -51712,7 +51712,7 @@
       <c r="B36" s="166" t="s">
         <v>259</v>
       </c>
-      <c r="C36" s="309"/>
+      <c r="C36" s="312"/>
       <c r="D36" s="168" t="s">
         <v>529</v>
       </c>
@@ -51724,7 +51724,7 @@
       <c r="B37" s="167" t="s">
         <v>260</v>
       </c>
-      <c r="C37" s="309"/>
+      <c r="C37" s="312"/>
       <c r="D37" s="168" t="s">
         <v>530</v>
       </c>
@@ -51736,7 +51736,7 @@
       <c r="B38" s="166" t="s">
         <v>261</v>
       </c>
-      <c r="C38" s="309"/>
+      <c r="C38" s="312"/>
       <c r="D38" s="168" t="s">
         <v>530</v>
       </c>
@@ -51748,7 +51748,7 @@
       <c r="B39" s="167" t="s">
         <v>262</v>
       </c>
-      <c r="C39" s="309"/>
+      <c r="C39" s="312"/>
       <c r="D39" s="168" t="s">
         <v>651</v>
       </c>
@@ -51760,7 +51760,7 @@
       <c r="B40" s="166" t="s">
         <v>263</v>
       </c>
-      <c r="C40" s="309"/>
+      <c r="C40" s="312"/>
       <c r="D40" s="168" t="s">
         <v>531</v>
       </c>
@@ -51772,7 +51772,7 @@
       <c r="B41" s="167" t="s">
         <v>264</v>
       </c>
-      <c r="C41" s="309"/>
+      <c r="C41" s="312"/>
       <c r="D41" s="168" t="s">
         <v>532</v>
       </c>
@@ -51784,7 +51784,7 @@
       <c r="B42" s="166" t="s">
         <v>498</v>
       </c>
-      <c r="C42" s="309"/>
+      <c r="C42" s="312"/>
       <c r="D42" s="168" t="s">
         <v>533</v>
       </c>
@@ -51796,7 +51796,7 @@
       <c r="B43" s="170" t="s">
         <v>499</v>
       </c>
-      <c r="C43" s="310"/>
+      <c r="C43" s="313"/>
       <c r="D43" s="172" t="s">
         <v>534</v>
       </c>
@@ -51809,7 +51809,7 @@
       <c r="B44" s="174" t="s">
         <v>265</v>
       </c>
-      <c r="C44" s="308" t="s">
+      <c r="C44" s="311" t="s">
         <v>535</v>
       </c>
       <c r="D44" s="175" t="s">
@@ -51823,7 +51823,7 @@
       <c r="B45" s="176" t="s">
         <v>266</v>
       </c>
-      <c r="C45" s="309"/>
+      <c r="C45" s="312"/>
       <c r="D45" s="168" t="s">
         <v>11</v>
       </c>
@@ -51835,7 +51835,7 @@
       <c r="B46" s="176" t="s">
         <v>267</v>
       </c>
-      <c r="C46" s="309"/>
+      <c r="C46" s="312"/>
       <c r="D46" s="168" t="s">
         <v>536</v>
       </c>
@@ -51847,7 +51847,7 @@
       <c r="B47" s="176" t="s">
         <v>268</v>
       </c>
-      <c r="C47" s="309"/>
+      <c r="C47" s="312"/>
       <c r="D47" s="168" t="s">
         <v>537</v>
       </c>
@@ -51859,7 +51859,7 @@
       <c r="B48" s="176" t="s">
         <v>269</v>
       </c>
-      <c r="C48" s="309"/>
+      <c r="C48" s="312"/>
       <c r="D48" s="168" t="s">
         <v>11</v>
       </c>
@@ -51871,7 +51871,7 @@
       <c r="B49" s="176" t="s">
         <v>270</v>
       </c>
-      <c r="C49" s="309"/>
+      <c r="C49" s="312"/>
       <c r="D49" s="168" t="s">
         <v>538</v>
       </c>
@@ -51883,7 +51883,7 @@
       <c r="B50" s="176" t="s">
         <v>271</v>
       </c>
-      <c r="C50" s="309"/>
+      <c r="C50" s="312"/>
       <c r="D50" s="168" t="s">
         <v>11</v>
       </c>
@@ -51895,7 +51895,7 @@
       <c r="B51" s="176" t="s">
         <v>272</v>
       </c>
-      <c r="C51" s="309"/>
+      <c r="C51" s="312"/>
       <c r="D51" s="168" t="s">
         <v>657</v>
       </c>
@@ -51907,7 +51907,7 @@
       <c r="B52" s="176" t="s">
         <v>273</v>
       </c>
-      <c r="C52" s="309"/>
+      <c r="C52" s="312"/>
       <c r="D52" s="168" t="s">
         <v>537</v>
       </c>
@@ -51919,7 +51919,7 @@
       <c r="B53" s="177" t="s">
         <v>274</v>
       </c>
-      <c r="C53" s="310"/>
+      <c r="C53" s="313"/>
       <c r="D53" s="172" t="s">
         <v>11</v>
       </c>
@@ -51931,7 +51931,7 @@
       <c r="B54" s="178" t="s">
         <v>275</v>
       </c>
-      <c r="C54" s="308" t="s">
+      <c r="C54" s="311" t="s">
         <v>539</v>
       </c>
       <c r="D54" s="168" t="s">
@@ -51945,7 +51945,7 @@
       <c r="B55" s="178" t="s">
         <v>276</v>
       </c>
-      <c r="C55" s="309"/>
+      <c r="C55" s="312"/>
       <c r="D55" s="168" t="s">
         <v>541</v>
       </c>
@@ -51957,7 +51957,7 @@
       <c r="B56" s="178" t="s">
         <v>277</v>
       </c>
-      <c r="C56" s="309"/>
+      <c r="C56" s="312"/>
       <c r="D56" s="168" t="s">
         <v>542</v>
       </c>
@@ -51969,7 +51969,7 @@
       <c r="B57" s="178" t="s">
         <v>278</v>
       </c>
-      <c r="C57" s="310"/>
+      <c r="C57" s="313"/>
       <c r="D57" s="168" t="s">
         <v>543</v>
       </c>
@@ -51981,7 +51981,7 @@
       <c r="B58" s="231" t="s">
         <v>731</v>
       </c>
-      <c r="C58" s="308" t="s">
+      <c r="C58" s="311" t="s">
         <v>544</v>
       </c>
       <c r="D58" s="175" t="s">
@@ -51995,7 +51995,7 @@
       <c r="B59" s="277" t="s">
         <v>732</v>
       </c>
-      <c r="C59" s="309"/>
+      <c r="C59" s="312"/>
       <c r="D59" s="279" t="s">
         <v>737</v>
       </c>
@@ -52007,7 +52007,7 @@
       <c r="B60" s="179" t="s">
         <v>652</v>
       </c>
-      <c r="C60" s="310"/>
+      <c r="C60" s="313"/>
       <c r="D60" s="172" t="s">
         <v>655</v>
       </c>
@@ -52019,7 +52019,7 @@
       <c r="B61" s="180" t="s">
         <v>279</v>
       </c>
-      <c r="C61" s="308" t="s">
+      <c r="C61" s="311" t="s">
         <v>545</v>
       </c>
       <c r="D61" s="168" t="s">
@@ -52033,7 +52033,7 @@
       <c r="B62" s="180" t="s">
         <v>280</v>
       </c>
-      <c r="C62" s="309"/>
+      <c r="C62" s="312"/>
       <c r="D62" s="168" t="s">
         <v>547</v>
       </c>
@@ -52045,7 +52045,7 @@
       <c r="B63" s="180" t="s">
         <v>281</v>
       </c>
-      <c r="C63" s="309"/>
+      <c r="C63" s="312"/>
       <c r="D63" s="168" t="s">
         <v>548</v>
       </c>
@@ -52057,7 +52057,7 @@
       <c r="B64" s="180" t="s">
         <v>282</v>
       </c>
-      <c r="C64" s="309"/>
+      <c r="C64" s="312"/>
       <c r="D64" s="168" t="s">
         <v>549</v>
       </c>
@@ -52069,7 +52069,7 @@
       <c r="B65" s="180" t="s">
         <v>283</v>
       </c>
-      <c r="C65" s="309"/>
+      <c r="C65" s="312"/>
       <c r="D65" s="168" t="s">
         <v>550</v>
       </c>
@@ -52081,7 +52081,7 @@
       <c r="B66" s="180" t="s">
         <v>284</v>
       </c>
-      <c r="C66" s="309"/>
+      <c r="C66" s="312"/>
       <c r="D66" s="168" t="s">
         <v>551</v>
       </c>
@@ -52093,7 +52093,7 @@
       <c r="B67" s="180" t="s">
         <v>285</v>
       </c>
-      <c r="C67" s="309"/>
+      <c r="C67" s="312"/>
       <c r="D67" s="168" t="s">
         <v>552</v>
       </c>
@@ -52105,7 +52105,7 @@
       <c r="B68" s="180" t="s">
         <v>664</v>
       </c>
-      <c r="C68" s="309"/>
+      <c r="C68" s="312"/>
       <c r="D68" s="168" t="s">
         <v>689</v>
       </c>
@@ -52117,7 +52117,7 @@
       <c r="B69" s="239" t="s">
         <v>674</v>
       </c>
-      <c r="C69" s="309"/>
+      <c r="C69" s="312"/>
       <c r="D69" s="168" t="s">
         <v>690</v>
       </c>
@@ -52129,7 +52129,7 @@
       <c r="B70" s="181" t="s">
         <v>286</v>
       </c>
-      <c r="C70" s="310"/>
+      <c r="C70" s="313"/>
       <c r="D70" s="172" t="s">
         <v>553</v>
       </c>
@@ -52141,7 +52141,7 @@
       <c r="B71" s="183" t="s">
         <v>287</v>
       </c>
-      <c r="C71" s="308" t="s">
+      <c r="C71" s="311" t="s">
         <v>554</v>
       </c>
       <c r="D71" s="175" t="s">
@@ -52155,7 +52155,7 @@
       <c r="B72" s="185" t="s">
         <v>288</v>
       </c>
-      <c r="C72" s="309"/>
+      <c r="C72" s="312"/>
       <c r="D72" s="168" t="s">
         <v>11</v>
       </c>
@@ -52167,7 +52167,7 @@
       <c r="B73" s="185" t="s">
         <v>289</v>
       </c>
-      <c r="C73" s="309"/>
+      <c r="C73" s="312"/>
       <c r="D73" s="168" t="s">
         <v>11</v>
       </c>
@@ -52179,7 +52179,7 @@
       <c r="B74" s="185" t="s">
         <v>666</v>
       </c>
-      <c r="C74" s="309"/>
+      <c r="C74" s="312"/>
       <c r="D74" s="168" t="s">
         <v>11</v>
       </c>
@@ -52191,7 +52191,7 @@
       <c r="B75" s="185" t="s">
         <v>290</v>
       </c>
-      <c r="C75" s="309"/>
+      <c r="C75" s="312"/>
       <c r="D75" s="168" t="s">
         <v>11</v>
       </c>
@@ -52203,7 +52203,7 @@
       <c r="B76" s="185" t="s">
         <v>291</v>
       </c>
-      <c r="C76" s="309"/>
+      <c r="C76" s="312"/>
       <c r="D76" s="168" t="s">
         <v>556</v>
       </c>
@@ -52215,7 +52215,7 @@
       <c r="B77" s="185" t="s">
         <v>292</v>
       </c>
-      <c r="C77" s="309"/>
+      <c r="C77" s="312"/>
       <c r="D77" s="168" t="s">
         <v>11</v>
       </c>
@@ -52227,7 +52227,7 @@
       <c r="B78" s="185" t="s">
         <v>293</v>
       </c>
-      <c r="C78" s="309"/>
+      <c r="C78" s="312"/>
       <c r="D78" s="168" t="s">
         <v>11</v>
       </c>
@@ -52239,7 +52239,7 @@
       <c r="B79" s="185" t="s">
         <v>294</v>
       </c>
-      <c r="C79" s="309"/>
+      <c r="C79" s="312"/>
       <c r="D79" s="168" t="s">
         <v>11</v>
       </c>
@@ -52251,7 +52251,7 @@
       <c r="B80" s="185" t="s">
         <v>667</v>
       </c>
-      <c r="C80" s="309"/>
+      <c r="C80" s="312"/>
       <c r="D80" s="168" t="s">
         <v>11</v>
       </c>
@@ -52263,7 +52263,7 @@
       <c r="B81" s="185" t="s">
         <v>295</v>
       </c>
-      <c r="C81" s="309"/>
+      <c r="C81" s="312"/>
       <c r="D81" s="168" t="s">
         <v>11</v>
       </c>
@@ -52275,7 +52275,7 @@
       <c r="B82" s="185" t="s">
         <v>296</v>
       </c>
-      <c r="C82" s="309"/>
+      <c r="C82" s="312"/>
       <c r="D82" s="168" t="s">
         <v>556</v>
       </c>
@@ -52287,7 +52287,7 @@
       <c r="B83" s="185" t="s">
         <v>297</v>
       </c>
-      <c r="C83" s="309"/>
+      <c r="C83" s="312"/>
       <c r="D83" s="168" t="s">
         <v>11</v>
       </c>
@@ -52299,7 +52299,7 @@
       <c r="B84" s="185" t="s">
         <v>298</v>
       </c>
-      <c r="C84" s="309"/>
+      <c r="C84" s="312"/>
       <c r="D84" s="168" t="s">
         <v>11</v>
       </c>
@@ -52311,7 +52311,7 @@
       <c r="B85" s="186" t="s">
         <v>299</v>
       </c>
-      <c r="C85" s="309"/>
+      <c r="C85" s="312"/>
       <c r="D85" s="168" t="s">
         <v>11</v>
       </c>
@@ -52323,7 +52323,7 @@
       <c r="B86" s="186" t="s">
         <v>665</v>
       </c>
-      <c r="C86" s="309"/>
+      <c r="C86" s="312"/>
       <c r="D86" s="168" t="s">
         <v>11</v>
       </c>
@@ -52335,7 +52335,7 @@
       <c r="B87" s="186" t="s">
         <v>300</v>
       </c>
-      <c r="C87" s="309"/>
+      <c r="C87" s="312"/>
       <c r="D87" s="168" t="s">
         <v>11</v>
       </c>
@@ -52347,7 +52347,7 @@
       <c r="B88" s="186" t="s">
         <v>301</v>
       </c>
-      <c r="C88" s="309"/>
+      <c r="C88" s="312"/>
       <c r="D88" s="168" t="s">
         <v>556</v>
       </c>
@@ -52359,7 +52359,7 @@
       <c r="B89" s="186" t="s">
         <v>302</v>
       </c>
-      <c r="C89" s="309"/>
+      <c r="C89" s="312"/>
       <c r="D89" s="168" t="s">
         <v>557</v>
       </c>
@@ -52371,7 +52371,7 @@
       <c r="B90" s="187" t="s">
         <v>303</v>
       </c>
-      <c r="C90" s="309"/>
+      <c r="C90" s="312"/>
       <c r="D90" s="168" t="s">
         <v>558</v>
       </c>
@@ -52383,7 +52383,7 @@
       <c r="B91" s="187" t="s">
         <v>304</v>
       </c>
-      <c r="C91" s="309"/>
+      <c r="C91" s="312"/>
       <c r="D91" s="168" t="s">
         <v>559</v>
       </c>
@@ -52395,7 +52395,7 @@
       <c r="B92" s="187" t="s">
         <v>305</v>
       </c>
-      <c r="C92" s="309"/>
+      <c r="C92" s="312"/>
       <c r="D92" s="168" t="s">
         <v>560</v>
       </c>
@@ -52407,7 +52407,7 @@
       <c r="B93" s="187" t="s">
         <v>306</v>
       </c>
-      <c r="C93" s="309"/>
+      <c r="C93" s="312"/>
       <c r="D93" s="168" t="s">
         <v>561</v>
       </c>
@@ -52419,7 +52419,7 @@
       <c r="B94" s="189" t="s">
         <v>307</v>
       </c>
-      <c r="C94" s="310"/>
+      <c r="C94" s="313"/>
       <c r="D94" s="172" t="s">
         <v>562</v>
       </c>
@@ -52431,7 +52431,7 @@
       <c r="B95" s="190" t="s">
         <v>308</v>
       </c>
-      <c r="C95" s="308" t="s">
+      <c r="C95" s="311" t="s">
         <v>563</v>
       </c>
       <c r="D95" s="168" t="s">
@@ -52445,7 +52445,7 @@
       <c r="B96" s="190" t="s">
         <v>432</v>
       </c>
-      <c r="C96" s="309"/>
+      <c r="C96" s="312"/>
       <c r="D96" s="278" t="s">
         <v>565</v>
       </c>
@@ -52457,7 +52457,7 @@
       <c r="B97" s="190" t="s">
         <v>309</v>
       </c>
-      <c r="C97" s="309"/>
+      <c r="C97" s="312"/>
       <c r="D97" s="191" t="s">
         <v>566</v>
       </c>
@@ -52469,7 +52469,7 @@
       <c r="B98" s="192" t="s">
         <v>310</v>
       </c>
-      <c r="C98" s="310"/>
+      <c r="C98" s="313"/>
       <c r="D98" s="172" t="s">
         <v>567</v>
       </c>
@@ -52481,7 +52481,7 @@
       <c r="B99" s="174" t="s">
         <v>311</v>
       </c>
-      <c r="C99" s="308" t="s">
+      <c r="C99" s="311" t="s">
         <v>568</v>
       </c>
       <c r="D99" s="175" t="s">
@@ -52495,7 +52495,7 @@
       <c r="B100" s="176" t="s">
         <v>317</v>
       </c>
-      <c r="C100" s="309"/>
+      <c r="C100" s="312"/>
       <c r="D100" s="168" t="s">
         <v>570</v>
       </c>
@@ -52507,7 +52507,7 @@
       <c r="B101" s="176" t="s">
         <v>482</v>
       </c>
-      <c r="C101" s="309"/>
+      <c r="C101" s="312"/>
       <c r="D101" s="168" t="s">
         <v>571</v>
       </c>
@@ -52519,7 +52519,7 @@
       <c r="B102" s="176" t="s">
         <v>483</v>
       </c>
-      <c r="C102" s="309"/>
+      <c r="C102" s="312"/>
       <c r="D102" s="168" t="s">
         <v>572</v>
       </c>
@@ -52531,7 +52531,7 @@
       <c r="B103" s="176" t="s">
         <v>484</v>
       </c>
-      <c r="C103" s="309"/>
+      <c r="C103" s="312"/>
       <c r="D103" s="168" t="s">
         <v>573</v>
       </c>
@@ -52543,7 +52543,7 @@
       <c r="B104" s="176" t="s">
         <v>647</v>
       </c>
-      <c r="C104" s="309"/>
+      <c r="C104" s="312"/>
       <c r="D104" s="168" t="s">
         <v>648</v>
       </c>
@@ -52555,7 +52555,7 @@
       <c r="B105" s="176" t="s">
         <v>671</v>
       </c>
-      <c r="C105" s="309"/>
+      <c r="C105" s="312"/>
       <c r="D105" s="168" t="s">
         <v>691</v>
       </c>
@@ -52567,7 +52567,7 @@
       <c r="B106" s="176" t="s">
         <v>672</v>
       </c>
-      <c r="C106" s="309"/>
+      <c r="C106" s="312"/>
       <c r="D106" s="168" t="s">
         <v>692</v>
       </c>
@@ -52579,7 +52579,7 @@
       <c r="B107" s="176" t="s">
         <v>673</v>
       </c>
-      <c r="C107" s="309"/>
+      <c r="C107" s="312"/>
       <c r="D107" s="168" t="s">
         <v>693</v>
       </c>
@@ -52591,7 +52591,7 @@
       <c r="B108" s="176" t="s">
         <v>687</v>
       </c>
-      <c r="C108" s="310"/>
+      <c r="C108" s="313"/>
       <c r="D108" s="168" t="s">
         <v>694</v>
       </c>
@@ -52603,7 +52603,7 @@
       <c r="B109" s="194" t="s">
         <v>448</v>
       </c>
-      <c r="C109" s="308" t="s">
+      <c r="C109" s="311" t="s">
         <v>574</v>
       </c>
       <c r="D109" s="175" t="s">
@@ -52617,7 +52617,7 @@
       <c r="B110" s="196" t="s">
         <v>736</v>
       </c>
-      <c r="C110" s="309"/>
+      <c r="C110" s="312"/>
       <c r="D110" s="168" t="s">
         <v>735</v>
       </c>
@@ -52629,7 +52629,7 @@
       <c r="B111" s="196" t="s">
         <v>312</v>
       </c>
-      <c r="C111" s="309"/>
+      <c r="C111" s="312"/>
       <c r="D111" s="168" t="s">
         <v>575</v>
       </c>
@@ -52641,7 +52641,7 @@
       <c r="B112" s="196" t="s">
         <v>313</v>
       </c>
-      <c r="C112" s="309"/>
+      <c r="C112" s="312"/>
       <c r="D112" s="168" t="s">
         <v>576</v>
       </c>
@@ -52653,7 +52653,7 @@
       <c r="B113" s="196" t="s">
         <v>314</v>
       </c>
-      <c r="C113" s="309"/>
+      <c r="C113" s="312"/>
       <c r="D113" s="168" t="s">
         <v>576</v>
       </c>
@@ -52665,7 +52665,7 @@
       <c r="B114" s="196" t="s">
         <v>315</v>
       </c>
-      <c r="C114" s="309"/>
+      <c r="C114" s="312"/>
       <c r="D114" s="168" t="s">
         <v>577</v>
       </c>
@@ -52677,7 +52677,7 @@
       <c r="B115" s="198" t="s">
         <v>316</v>
       </c>
-      <c r="C115" s="310"/>
+      <c r="C115" s="313"/>
       <c r="D115" s="172" t="s">
         <v>577</v>
       </c>
@@ -52689,7 +52689,7 @@
       <c r="B116" s="199" t="s">
         <v>433</v>
       </c>
-      <c r="C116" s="308" t="s">
+      <c r="C116" s="311" t="s">
         <v>578</v>
       </c>
       <c r="D116" s="175" t="s">
@@ -52703,7 +52703,7 @@
       <c r="B117" s="200" t="s">
         <v>434</v>
       </c>
-      <c r="C117" s="309"/>
+      <c r="C117" s="312"/>
       <c r="D117" s="168" t="s">
         <v>11</v>
       </c>
@@ -52715,7 +52715,7 @@
       <c r="B118" s="200" t="s">
         <v>435</v>
       </c>
-      <c r="C118" s="309"/>
+      <c r="C118" s="312"/>
       <c r="D118" s="168" t="s">
         <v>11</v>
       </c>
@@ -52727,7 +52727,7 @@
       <c r="B119" s="200" t="s">
         <v>683</v>
       </c>
-      <c r="C119" s="309"/>
+      <c r="C119" s="312"/>
       <c r="D119" s="168" t="s">
         <v>11</v>
       </c>
@@ -52739,7 +52739,7 @@
       <c r="B120" s="200" t="s">
         <v>436</v>
       </c>
-      <c r="C120" s="309"/>
+      <c r="C120" s="312"/>
       <c r="D120" s="168" t="s">
         <v>11</v>
       </c>
@@ -52751,7 +52751,7 @@
       <c r="B121" s="200" t="s">
         <v>437</v>
       </c>
-      <c r="C121" s="309"/>
+      <c r="C121" s="312"/>
       <c r="D121" s="168" t="s">
         <v>556</v>
       </c>
@@ -52763,7 +52763,7 @@
       <c r="B122" s="200" t="s">
         <v>438</v>
       </c>
-      <c r="C122" s="309"/>
+      <c r="C122" s="312"/>
       <c r="D122" s="168" t="s">
         <v>11</v>
       </c>
@@ -52775,7 +52775,7 @@
       <c r="B123" s="200" t="s">
         <v>439</v>
       </c>
-      <c r="C123" s="309"/>
+      <c r="C123" s="312"/>
       <c r="D123" s="168" t="s">
         <v>11</v>
       </c>
@@ -52787,7 +52787,7 @@
       <c r="B124" s="200" t="s">
         <v>684</v>
       </c>
-      <c r="C124" s="309"/>
+      <c r="C124" s="312"/>
       <c r="D124" s="168" t="s">
         <v>11</v>
       </c>
@@ -52799,7 +52799,7 @@
       <c r="B125" s="200" t="s">
         <v>500</v>
       </c>
-      <c r="C125" s="309"/>
+      <c r="C125" s="312"/>
       <c r="D125" s="168" t="s">
         <v>11</v>
       </c>
@@ -52811,7 +52811,7 @@
       <c r="B126" s="200" t="s">
         <v>501</v>
       </c>
-      <c r="C126" s="309"/>
+      <c r="C126" s="312"/>
       <c r="D126" s="168" t="s">
         <v>11</v>
       </c>
@@ -52823,7 +52823,7 @@
       <c r="B127" s="200" t="s">
         <v>502</v>
       </c>
-      <c r="C127" s="309"/>
+      <c r="C127" s="312"/>
       <c r="D127" s="168" t="s">
         <v>11</v>
       </c>
@@ -52835,7 +52835,7 @@
       <c r="B128" s="200" t="s">
         <v>685</v>
       </c>
-      <c r="C128" s="309"/>
+      <c r="C128" s="312"/>
       <c r="D128" s="168" t="s">
         <v>11</v>
       </c>
@@ -52847,7 +52847,7 @@
       <c r="B129" s="200" t="s">
         <v>503</v>
       </c>
-      <c r="C129" s="309"/>
+      <c r="C129" s="312"/>
       <c r="D129" s="168" t="s">
         <v>11</v>
       </c>
@@ -52859,7 +52859,7 @@
       <c r="B130" s="200" t="s">
         <v>440</v>
       </c>
-      <c r="C130" s="309"/>
+      <c r="C130" s="312"/>
       <c r="D130" s="168" t="s">
         <v>580</v>
       </c>
@@ -52871,7 +52871,7 @@
       <c r="B131" s="200" t="s">
         <v>441</v>
       </c>
-      <c r="C131" s="309"/>
+      <c r="C131" s="312"/>
       <c r="D131" s="168" t="s">
         <v>581</v>
       </c>
@@ -52883,7 +52883,7 @@
       <c r="B132" s="200" t="s">
         <v>471</v>
       </c>
-      <c r="C132" s="309"/>
+      <c r="C132" s="312"/>
       <c r="D132" s="168" t="s">
         <v>582</v>
       </c>
@@ -52895,7 +52895,7 @@
       <c r="B133" s="200" t="s">
         <v>472</v>
       </c>
-      <c r="C133" s="309"/>
+      <c r="C133" s="312"/>
       <c r="D133" s="168" t="s">
         <v>583</v>
       </c>
@@ -52907,7 +52907,7 @@
       <c r="B134" s="200" t="s">
         <v>504</v>
       </c>
-      <c r="C134" s="309"/>
+      <c r="C134" s="312"/>
       <c r="D134" s="168" t="s">
         <v>584</v>
       </c>
@@ -52919,7 +52919,7 @@
       <c r="B135" s="200" t="s">
         <v>507</v>
       </c>
-      <c r="C135" s="309"/>
+      <c r="C135" s="312"/>
       <c r="D135" s="168" t="s">
         <v>585</v>
       </c>
@@ -52931,7 +52931,7 @@
       <c r="B136" s="200" t="s">
         <v>506</v>
       </c>
-      <c r="C136" s="309"/>
+      <c r="C136" s="312"/>
       <c r="D136" s="168" t="s">
         <v>586</v>
       </c>
@@ -52943,7 +52943,7 @@
       <c r="B137" s="200" t="s">
         <v>318</v>
       </c>
-      <c r="C137" s="309"/>
+      <c r="C137" s="312"/>
       <c r="D137" s="168" t="s">
         <v>587</v>
       </c>
@@ -52955,7 +52955,7 @@
       <c r="B138" s="200" t="s">
         <v>319</v>
       </c>
-      <c r="C138" s="309"/>
+      <c r="C138" s="312"/>
       <c r="D138" s="168" t="s">
         <v>587</v>
       </c>
@@ -52967,7 +52967,7 @@
       <c r="B139" s="200" t="s">
         <v>320</v>
       </c>
-      <c r="C139" s="309"/>
+      <c r="C139" s="312"/>
       <c r="D139" s="168" t="s">
         <v>653</v>
       </c>
@@ -52979,7 +52979,7 @@
       <c r="B140" s="200" t="s">
         <v>321</v>
       </c>
-      <c r="C140" s="309"/>
+      <c r="C140" s="312"/>
       <c r="D140" s="168" t="s">
         <v>588</v>
       </c>
@@ -52991,7 +52991,7 @@
       <c r="B141" s="200" t="s">
         <v>442</v>
       </c>
-      <c r="C141" s="309"/>
+      <c r="C141" s="312"/>
       <c r="D141" s="168" t="s">
         <v>654</v>
       </c>
@@ -53003,7 +53003,7 @@
       <c r="B142" s="200" t="s">
         <v>443</v>
       </c>
-      <c r="C142" s="309"/>
+      <c r="C142" s="312"/>
       <c r="D142" s="168" t="s">
         <v>650</v>
       </c>
@@ -53015,7 +53015,7 @@
       <c r="B143" s="200" t="s">
         <v>322</v>
       </c>
-      <c r="C143" s="309"/>
+      <c r="C143" s="312"/>
       <c r="D143" s="168" t="s">
         <v>589</v>
       </c>
@@ -53027,7 +53027,7 @@
       <c r="B144" s="200" t="s">
         <v>474</v>
       </c>
-      <c r="C144" s="309"/>
+      <c r="C144" s="312"/>
       <c r="D144" s="168" t="s">
         <v>590</v>
       </c>
@@ -53039,7 +53039,7 @@
       <c r="B145" s="200" t="s">
         <v>323</v>
       </c>
-      <c r="C145" s="309"/>
+      <c r="C145" s="312"/>
       <c r="D145" s="168" t="s">
         <v>591</v>
       </c>
@@ -53051,7 +53051,7 @@
       <c r="B146" s="200" t="s">
         <v>324</v>
       </c>
-      <c r="C146" s="309"/>
+      <c r="C146" s="312"/>
       <c r="D146" s="168" t="s">
         <v>592</v>
       </c>
@@ -53063,7 +53063,7 @@
       <c r="B147" s="200" t="s">
         <v>325</v>
       </c>
-      <c r="C147" s="309"/>
+      <c r="C147" s="312"/>
       <c r="D147" s="168" t="s">
         <v>593</v>
       </c>
@@ -53075,7 +53075,7 @@
       <c r="B148" s="200" t="s">
         <v>326</v>
       </c>
-      <c r="C148" s="309"/>
+      <c r="C148" s="312"/>
       <c r="D148" s="168" t="s">
         <v>594</v>
       </c>
@@ -53087,7 +53087,7 @@
       <c r="B149" s="200" t="s">
         <v>457</v>
       </c>
-      <c r="C149" s="309"/>
+      <c r="C149" s="312"/>
       <c r="D149" s="168" t="s">
         <v>595</v>
       </c>
@@ -53099,7 +53099,7 @@
       <c r="B150" s="200" t="s">
         <v>458</v>
       </c>
-      <c r="C150" s="309"/>
+      <c r="C150" s="312"/>
       <c r="D150" s="168" t="s">
         <v>596</v>
       </c>
@@ -53111,7 +53111,7 @@
       <c r="B151" s="200" t="s">
         <v>675</v>
       </c>
-      <c r="C151" s="309"/>
+      <c r="C151" s="312"/>
       <c r="D151" s="168" t="s">
         <v>695</v>
       </c>
@@ -53123,7 +53123,7 @@
       <c r="B152" s="200" t="s">
         <v>676</v>
       </c>
-      <c r="C152" s="309"/>
+      <c r="C152" s="312"/>
       <c r="D152" s="168" t="s">
         <v>11</v>
       </c>
@@ -53135,7 +53135,7 @@
       <c r="B153" s="200" t="s">
         <v>677</v>
       </c>
-      <c r="C153" s="309"/>
+      <c r="C153" s="312"/>
       <c r="D153" s="168" t="s">
         <v>11</v>
       </c>
@@ -53147,7 +53147,7 @@
       <c r="B154" s="200" t="s">
         <v>678</v>
       </c>
-      <c r="C154" s="309"/>
+      <c r="C154" s="312"/>
       <c r="D154" s="168" t="s">
         <v>11</v>
       </c>
@@ -53159,7 +53159,7 @@
       <c r="B155" s="200" t="s">
         <v>679</v>
       </c>
-      <c r="C155" s="309"/>
+      <c r="C155" s="312"/>
       <c r="D155" s="168" t="s">
         <v>11</v>
       </c>
@@ -53171,7 +53171,7 @@
       <c r="B156" s="200" t="s">
         <v>680</v>
       </c>
-      <c r="C156" s="309"/>
+      <c r="C156" s="312"/>
       <c r="D156" s="168" t="s">
         <v>11</v>
       </c>
@@ -53183,7 +53183,7 @@
       <c r="B157" s="200" t="s">
         <v>681</v>
       </c>
-      <c r="C157" s="309"/>
+      <c r="C157" s="312"/>
       <c r="D157" s="168" t="s">
         <v>11</v>
       </c>
@@ -53195,7 +53195,7 @@
       <c r="B158" s="200" t="s">
         <v>682</v>
       </c>
-      <c r="C158" s="309"/>
+      <c r="C158" s="312"/>
       <c r="D158" s="168" t="s">
         <v>11</v>
       </c>
@@ -53207,7 +53207,7 @@
       <c r="B159" s="200" t="s">
         <v>663</v>
       </c>
-      <c r="C159" s="309"/>
+      <c r="C159" s="312"/>
       <c r="D159" s="168" t="s">
         <v>696</v>
       </c>
@@ -53219,7 +53219,7 @@
       <c r="B160" s="200" t="s">
         <v>670</v>
       </c>
-      <c r="C160" s="309"/>
+      <c r="C160" s="312"/>
       <c r="D160" s="168" t="s">
         <v>697</v>
       </c>
@@ -53231,7 +53231,7 @@
       <c r="B161" s="200" t="s">
         <v>668</v>
       </c>
-      <c r="C161" s="309"/>
+      <c r="C161" s="312"/>
       <c r="D161" s="168" t="s">
         <v>698</v>
       </c>
@@ -53243,7 +53243,7 @@
       <c r="B162" s="201" t="s">
         <v>669</v>
       </c>
-      <c r="C162" s="310"/>
+      <c r="C162" s="313"/>
       <c r="D162" s="245" t="s">
         <v>11</v>
       </c>
@@ -53255,7 +53255,7 @@
       <c r="B163" s="203" t="s">
         <v>327</v>
       </c>
-      <c r="C163" s="308" t="s">
+      <c r="C163" s="311" t="s">
         <v>597</v>
       </c>
       <c r="D163" s="168" t="s">
@@ -53269,7 +53269,7 @@
       <c r="B164" s="203" t="s">
         <v>328</v>
       </c>
-      <c r="C164" s="309"/>
+      <c r="C164" s="312"/>
       <c r="D164" s="168" t="s">
         <v>599</v>
       </c>
@@ -53281,7 +53281,7 @@
       <c r="B165" s="203" t="s">
         <v>329</v>
       </c>
-      <c r="C165" s="309"/>
+      <c r="C165" s="312"/>
       <c r="D165" s="168" t="s">
         <v>11</v>
       </c>
@@ -53293,7 +53293,7 @@
       <c r="B166" s="203" t="s">
         <v>330</v>
       </c>
-      <c r="C166" s="309"/>
+      <c r="C166" s="312"/>
       <c r="D166" s="168" t="s">
         <v>11</v>
       </c>
@@ -53305,7 +53305,7 @@
       <c r="B167" s="203" t="s">
         <v>444</v>
       </c>
-      <c r="C167" s="309"/>
+      <c r="C167" s="312"/>
       <c r="D167" s="168" t="s">
         <v>600</v>
       </c>
@@ -53317,7 +53317,7 @@
       <c r="B168" s="203" t="s">
         <v>445</v>
       </c>
-      <c r="C168" s="309"/>
+      <c r="C168" s="312"/>
       <c r="D168" s="168" t="s">
         <v>601</v>
       </c>
@@ -53329,7 +53329,7 @@
       <c r="B169" s="203" t="s">
         <v>331</v>
       </c>
-      <c r="C169" s="309"/>
+      <c r="C169" s="312"/>
       <c r="D169" s="168" t="s">
         <v>602</v>
       </c>
@@ -53341,7 +53341,7 @@
       <c r="B170" s="203" t="s">
         <v>332</v>
       </c>
-      <c r="C170" s="309"/>
+      <c r="C170" s="312"/>
       <c r="D170" s="168" t="s">
         <v>11</v>
       </c>
@@ -53353,7 +53353,7 @@
       <c r="B171" s="203" t="s">
         <v>333</v>
       </c>
-      <c r="C171" s="309"/>
+      <c r="C171" s="312"/>
       <c r="D171" s="168" t="s">
         <v>11</v>
       </c>
@@ -53365,7 +53365,7 @@
       <c r="B172" s="203" t="s">
         <v>334</v>
       </c>
-      <c r="C172" s="309"/>
+      <c r="C172" s="312"/>
       <c r="D172" s="168" t="s">
         <v>11</v>
       </c>
@@ -53377,7 +53377,7 @@
       <c r="B173" s="203" t="s">
         <v>335</v>
       </c>
-      <c r="C173" s="309"/>
+      <c r="C173" s="312"/>
       <c r="D173" s="168" t="s">
         <v>603</v>
       </c>
@@ -53389,7 +53389,7 @@
       <c r="B174" s="203" t="s">
         <v>336</v>
       </c>
-      <c r="C174" s="309"/>
+      <c r="C174" s="312"/>
       <c r="D174" s="168" t="s">
         <v>604</v>
       </c>
@@ -53401,7 +53401,7 @@
       <c r="B175" s="203" t="s">
         <v>337</v>
       </c>
-      <c r="C175" s="309"/>
+      <c r="C175" s="312"/>
       <c r="D175" s="168" t="s">
         <v>605</v>
       </c>
@@ -53413,7 +53413,7 @@
       <c r="B176" s="204" t="s">
         <v>338</v>
       </c>
-      <c r="C176" s="310"/>
+      <c r="C176" s="313"/>
       <c r="D176" s="172" t="s">
         <v>606</v>
       </c>
@@ -53434,6 +53434,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C163:C176"/>
+    <mergeCell ref="C61:C70"/>
+    <mergeCell ref="C71:C94"/>
+    <mergeCell ref="C95:C98"/>
+    <mergeCell ref="C99:C108"/>
+    <mergeCell ref="C109:C115"/>
+    <mergeCell ref="C116:C162"/>
     <mergeCell ref="C58:C60"/>
     <mergeCell ref="C54:C57"/>
     <mergeCell ref="C2:C11"/>
@@ -53441,13 +53448,6 @@
     <mergeCell ref="C18:C28"/>
     <mergeCell ref="C44:C53"/>
     <mergeCell ref="C29:C43"/>
-    <mergeCell ref="C163:C176"/>
-    <mergeCell ref="C61:C70"/>
-    <mergeCell ref="C71:C94"/>
-    <mergeCell ref="C95:C98"/>
-    <mergeCell ref="C99:C108"/>
-    <mergeCell ref="C109:C115"/>
-    <mergeCell ref="C116:C162"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -53493,7 +53493,7 @@
       <c r="B2" s="183" t="s">
         <v>340</v>
       </c>
-      <c r="C2" s="308" t="s">
+      <c r="C2" s="311" t="s">
         <v>554</v>
       </c>
       <c r="D2" s="151" t="s">
@@ -53507,7 +53507,7 @@
       <c r="B3" s="185" t="s">
         <v>341</v>
       </c>
-      <c r="C3" s="309"/>
+      <c r="C3" s="312"/>
       <c r="D3" s="153" t="s">
         <v>11</v>
       </c>
@@ -53519,7 +53519,7 @@
       <c r="B4" s="185" t="s">
         <v>342</v>
       </c>
-      <c r="C4" s="309"/>
+      <c r="C4" s="312"/>
       <c r="D4" s="153" t="s">
         <v>11</v>
       </c>
@@ -53531,7 +53531,7 @@
       <c r="B5" s="185" t="s">
         <v>343</v>
       </c>
-      <c r="C5" s="309"/>
+      <c r="C5" s="312"/>
       <c r="D5" s="153" t="s">
         <v>11</v>
       </c>
@@ -53543,7 +53543,7 @@
       <c r="B6" s="185" t="s">
         <v>344</v>
       </c>
-      <c r="C6" s="309"/>
+      <c r="C6" s="312"/>
       <c r="D6" s="153" t="s">
         <v>11</v>
       </c>
@@ -53555,7 +53555,7 @@
       <c r="B7" s="185" t="s">
         <v>345</v>
       </c>
-      <c r="C7" s="309"/>
+      <c r="C7" s="312"/>
       <c r="D7" s="153" t="s">
         <v>11</v>
       </c>
@@ -53567,7 +53567,7 @@
       <c r="B8" s="185" t="s">
         <v>346</v>
       </c>
-      <c r="C8" s="309"/>
+      <c r="C8" s="312"/>
       <c r="D8" s="153" t="s">
         <v>11</v>
       </c>
@@ -53579,7 +53579,7 @@
       <c r="B9" s="185" t="s">
         <v>347</v>
       </c>
-      <c r="C9" s="309"/>
+      <c r="C9" s="312"/>
       <c r="D9" s="153" t="s">
         <v>11</v>
       </c>
@@ -53591,7 +53591,7 @@
       <c r="B10" s="185" t="s">
         <v>348</v>
       </c>
-      <c r="C10" s="309"/>
+      <c r="C10" s="312"/>
       <c r="D10" s="153" t="s">
         <v>11</v>
       </c>
@@ -53603,7 +53603,7 @@
       <c r="B11" s="185" t="s">
         <v>349</v>
       </c>
-      <c r="C11" s="309"/>
+      <c r="C11" s="312"/>
       <c r="D11" s="153" t="s">
         <v>11</v>
       </c>
@@ -53615,7 +53615,7 @@
       <c r="B12" s="185" t="s">
         <v>350</v>
       </c>
-      <c r="C12" s="309"/>
+      <c r="C12" s="312"/>
       <c r="D12" s="153" t="s">
         <v>11</v>
       </c>
@@ -53627,7 +53627,7 @@
       <c r="B13" s="185" t="s">
         <v>351</v>
       </c>
-      <c r="C13" s="309"/>
+      <c r="C13" s="312"/>
       <c r="D13" s="153" t="s">
         <v>11</v>
       </c>
@@ -53639,7 +53639,7 @@
       <c r="B14" s="185" t="s">
         <v>352</v>
       </c>
-      <c r="C14" s="309"/>
+      <c r="C14" s="312"/>
       <c r="D14" s="153" t="s">
         <v>610</v>
       </c>
@@ -53651,7 +53651,7 @@
       <c r="B15" s="185" t="s">
         <v>353</v>
       </c>
-      <c r="C15" s="309"/>
+      <c r="C15" s="312"/>
       <c r="D15" s="153" t="s">
         <v>610</v>
       </c>
@@ -53663,7 +53663,7 @@
       <c r="B16" s="207" t="s">
         <v>473</v>
       </c>
-      <c r="C16" s="310"/>
+      <c r="C16" s="313"/>
       <c r="D16" s="156" t="s">
         <v>611</v>
       </c>
@@ -53675,7 +53675,7 @@
       <c r="B17" s="208" t="s">
         <v>354</v>
       </c>
-      <c r="C17" s="308" t="s">
+      <c r="C17" s="311" t="s">
         <v>612</v>
       </c>
       <c r="D17" s="151" t="s">
@@ -53689,7 +53689,7 @@
       <c r="B18" s="209" t="s">
         <v>355</v>
       </c>
-      <c r="C18" s="309"/>
+      <c r="C18" s="312"/>
       <c r="D18" s="153" t="s">
         <v>614</v>
       </c>
@@ -53701,7 +53701,7 @@
       <c r="B19" s="209" t="s">
         <v>356</v>
       </c>
-      <c r="C19" s="309"/>
+      <c r="C19" s="312"/>
       <c r="D19" s="153" t="s">
         <v>615</v>
       </c>
@@ -53713,7 +53713,7 @@
       <c r="B20" s="209" t="s">
         <v>357</v>
       </c>
-      <c r="C20" s="309"/>
+      <c r="C20" s="312"/>
       <c r="D20" s="153" t="s">
         <v>546</v>
       </c>
@@ -53725,7 +53725,7 @@
       <c r="B21" s="209" t="s">
         <v>358</v>
       </c>
-      <c r="C21" s="309"/>
+      <c r="C21" s="312"/>
       <c r="D21" s="153" t="s">
         <v>547</v>
       </c>
@@ -53737,7 +53737,7 @@
       <c r="B22" s="209" t="s">
         <v>359</v>
       </c>
-      <c r="C22" s="309"/>
+      <c r="C22" s="312"/>
       <c r="D22" s="153" t="s">
         <v>548</v>
       </c>
@@ -53749,7 +53749,7 @@
       <c r="B23" s="209" t="s">
         <v>360</v>
       </c>
-      <c r="C23" s="309"/>
+      <c r="C23" s="312"/>
       <c r="D23" s="153" t="s">
         <v>549</v>
       </c>
@@ -53761,7 +53761,7 @@
       <c r="B24" s="209" t="s">
         <v>361</v>
       </c>
-      <c r="C24" s="309"/>
+      <c r="C24" s="312"/>
       <c r="D24" s="153" t="s">
         <v>550</v>
       </c>
@@ -53773,7 +53773,7 @@
       <c r="B25" s="210" t="s">
         <v>362</v>
       </c>
-      <c r="C25" s="310"/>
+      <c r="C25" s="313"/>
       <c r="D25" s="156" t="s">
         <v>551</v>
       </c>
@@ -53785,7 +53785,7 @@
       <c r="B26" s="164" t="s">
         <v>363</v>
       </c>
-      <c r="C26" s="308" t="s">
+      <c r="C26" s="311" t="s">
         <v>616</v>
       </c>
       <c r="D26" s="151" t="s">
@@ -53799,7 +53799,7 @@
       <c r="B27" s="167" t="s">
         <v>364</v>
       </c>
-      <c r="C27" s="309"/>
+      <c r="C27" s="312"/>
       <c r="D27" s="153" t="s">
         <v>618</v>
       </c>
@@ -53811,7 +53811,7 @@
       <c r="B28" s="167" t="s">
         <v>365</v>
       </c>
-      <c r="C28" s="309"/>
+      <c r="C28" s="312"/>
       <c r="D28" s="153" t="s">
         <v>619</v>
       </c>
@@ -53823,7 +53823,7 @@
       <c r="B29" s="167" t="s">
         <v>366</v>
       </c>
-      <c r="C29" s="309"/>
+      <c r="C29" s="312"/>
       <c r="D29" s="153" t="s">
         <v>620</v>
       </c>
@@ -53835,7 +53835,7 @@
       <c r="B30" s="167" t="s">
         <v>367</v>
       </c>
-      <c r="C30" s="309"/>
+      <c r="C30" s="312"/>
       <c r="D30" s="153" t="s">
         <v>621</v>
       </c>
@@ -53847,7 +53847,7 @@
       <c r="B31" s="167" t="s">
         <v>368</v>
       </c>
-      <c r="C31" s="309"/>
+      <c r="C31" s="312"/>
       <c r="D31" s="153" t="s">
         <v>621</v>
       </c>
@@ -53859,7 +53859,7 @@
       <c r="B32" s="167" t="s">
         <v>369</v>
       </c>
-      <c r="C32" s="309"/>
+      <c r="C32" s="312"/>
       <c r="D32" s="153" t="s">
         <v>622</v>
       </c>
@@ -53871,7 +53871,7 @@
       <c r="B33" s="167" t="s">
         <v>370</v>
       </c>
-      <c r="C33" s="309"/>
+      <c r="C33" s="312"/>
       <c r="D33" s="153" t="s">
         <v>622</v>
       </c>
@@ -53883,7 +53883,7 @@
       <c r="B34" s="167" t="s">
         <v>371</v>
       </c>
-      <c r="C34" s="309"/>
+      <c r="C34" s="312"/>
       <c r="D34" s="153" t="s">
         <v>622</v>
       </c>
@@ -53895,7 +53895,7 @@
       <c r="B35" s="167" t="s">
         <v>372</v>
       </c>
-      <c r="C35" s="309"/>
+      <c r="C35" s="312"/>
       <c r="D35" s="153" t="s">
         <v>622</v>
       </c>
@@ -53907,7 +53907,7 @@
       <c r="B36" s="211" t="s">
         <v>373</v>
       </c>
-      <c r="C36" s="310"/>
+      <c r="C36" s="313"/>
       <c r="D36" s="153" t="s">
         <v>622</v>
       </c>
@@ -53919,7 +53919,7 @@
       <c r="B37" s="213" t="s">
         <v>475</v>
       </c>
-      <c r="C37" s="308" t="s">
+      <c r="C37" s="311" t="s">
         <v>623</v>
       </c>
       <c r="D37" s="175" t="s">
@@ -53933,7 +53933,7 @@
       <c r="B38" s="202" t="s">
         <v>476</v>
       </c>
-      <c r="C38" s="309"/>
+      <c r="C38" s="312"/>
       <c r="D38" s="168" t="s">
         <v>601</v>
       </c>
@@ -53945,7 +53945,7 @@
       <c r="B39" s="202" t="s">
         <v>477</v>
       </c>
-      <c r="C39" s="309"/>
+      <c r="C39" s="312"/>
       <c r="D39" s="168" t="s">
         <v>624</v>
       </c>
@@ -53957,7 +53957,7 @@
       <c r="B40" s="216" t="s">
         <v>478</v>
       </c>
-      <c r="C40" s="310"/>
+      <c r="C40" s="313"/>
       <c r="D40" s="172" t="s">
         <v>625</v>
       </c>
@@ -54224,15 +54224,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="107e75b3-53cc-4838-92d2-ebc011bd4832">
@@ -54241,6 +54232,15 @@
     <TaxCatchAll xmlns="888ccf44-0d39-41a2-ab17-f7efb2bf6977" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -54263,14 +54263,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2288FB7-E85A-4FE8-9E7A-FE572FF16064}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -54285,4 +54277,12 @@
     <ds:schemaRef ds:uri="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix bug with rankNameDict creation if 'Run custom cases' == False
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -9413,9 +9413,9 @@
   </sheetPr>
   <dimension ref="A1:CQ218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD62" sqref="AD62"/>
+      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Update bug in Rank 58 for Qref0
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/prw_energinet_dk/Documents/Dokumenter/GitHub/MTB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F1E3183-5B20-4AD9-A50C-B77EA513BEC9}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7784DD6-5403-4993-9B56-0D0A90D642B8}"/>
   <bookViews>
-    <workbookView xWindow="-14480" yWindow="-21710" windowWidth="51420" windowHeight="21100" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -9414,8 +9414,8 @@
   <dimension ref="A1:CQ218"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
+      <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -16741,8 +16741,8 @@
         <v>111</v>
       </c>
       <c r="J60" s="89">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <f t="shared" ref="J60" si="23">inp_Uc/inp_Un</f>
+        <v>1.0651315789473685</v>
       </c>
       <c r="K60" s="89" t="s">
         <v>106</v>
@@ -18190,11 +18190,11 @@
         <v>68</v>
       </c>
       <c r="B70" s="88" t="b">
-        <f t="shared" ref="B70:C71" si="23">inp_Un&gt;=110</f>
+        <f t="shared" ref="B70:C71" si="24">inp_Un&gt;=110</f>
         <v>1</v>
       </c>
       <c r="C70" s="88" t="b">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D70" s="87" t="s">
@@ -18341,11 +18341,11 @@
         <v>69</v>
       </c>
       <c r="B71" s="88" t="b">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="C71" s="88" t="b">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D71" s="87" t="s">
@@ -18498,11 +18498,11 @@
         <v>106</v>
       </c>
       <c r="L72" s="21">
-        <f t="shared" ref="L72:L93" si="24">inp_scr_min</f>
+        <f t="shared" ref="L72:L93" si="25">inp_scr_min</f>
         <v>10</v>
       </c>
       <c r="M72" s="21">
-        <f t="shared" ref="M72:M93" si="25">inp_xr_min</f>
+        <f t="shared" ref="M72:M93" si="26">inp_xr_min</f>
         <v>10</v>
       </c>
       <c r="N72" s="21" t="s">
@@ -18522,7 +18522,7 @@
         <v>0</v>
       </c>
       <c r="S72" s="96">
-        <f t="shared" ref="S72" si="26">IF(R72&lt;sel_ures,0,
+        <f t="shared" ref="S72" si="27">IF(R72&lt;sel_ures,0,
 IF(AND(sel_uclear&gt;=R72, R72&gt;=sel_ures),sel_tclear,
 IF(AND(sel_urec1&gt;=R72,R72&gt;sel_uclear),IF(sel_urec1&gt;sel_uclear,sel_tclear+(R72-sel_uclear)*(sel_trec1-sel_tclear)/(sel_urec1-sel_uclear),sel_tclear),
 IF(AND(sel_urec2&gt;=R72,R72&gt;sel_urec1),IF(sel_urec2&gt;sel_urec1,sel_trec2+(R72-sel_urec1)*(sel_trec3-sel_trec2)/(sel_urec2-sel_urec1),-99999),5
@@ -18615,11 +18615,11 @@
         <v>106</v>
       </c>
       <c r="L73" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M73" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N73" s="21" t="s">
@@ -18726,11 +18726,11 @@
         <v>106</v>
       </c>
       <c r="L74" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M74" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N74" s="21" t="s">
@@ -18837,11 +18837,11 @@
         <v>106</v>
       </c>
       <c r="L75" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M75" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N75" s="21" t="s">
@@ -18948,11 +18948,11 @@
         <v>106</v>
       </c>
       <c r="L76" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M76" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N76" s="21" t="s">
@@ -19059,11 +19059,11 @@
         <v>106</v>
       </c>
       <c r="L77" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M77" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N77" s="21" t="s">
@@ -19171,11 +19171,11 @@
         <v>106</v>
       </c>
       <c r="L78" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M78" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N78" s="21" t="s">
@@ -19195,7 +19195,7 @@
         <v>0</v>
       </c>
       <c r="S78" s="96">
-        <f t="shared" ref="S78" si="27">IF(R78&lt;sel_ures,0,
+        <f t="shared" ref="S78" si="28">IF(R78&lt;sel_ures,0,
 IF(AND(sel_uclear&gt;=R78, R78&gt;=sel_ures),sel_tclear,
 IF(AND(sel_urec1&gt;=R78,R78&gt;sel_uclear),IF(sel_urec1&gt;sel_uclear,sel_tclear+(R78-sel_uclear)*(sel_trec1-sel_tclear)/(sel_urec1-sel_uclear),sel_tclear),
 IF(AND(sel_urec2&gt;=R78,R78&gt;sel_urec1),IF(sel_urec2&gt;sel_urec1,sel_trec2+(R78-sel_urec1)*(sel_trec3-sel_trec2)/(sel_urec2-sel_urec1),-99999),5
@@ -19288,11 +19288,11 @@
         <v>106</v>
       </c>
       <c r="L79" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M79" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N79" s="21" t="s">
@@ -19399,11 +19399,11 @@
         <v>106</v>
       </c>
       <c r="L80" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M80" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N80" s="21" t="s">
@@ -19510,11 +19510,11 @@
         <v>106</v>
       </c>
       <c r="L81" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M81" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N81" s="21" t="s">
@@ -19621,11 +19621,11 @@
         <v>106</v>
       </c>
       <c r="L82" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M82" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N82" s="21" t="s">
@@ -19760,11 +19760,11 @@
         <v>106</v>
       </c>
       <c r="L83" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M83" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N83" s="21" t="s">
@@ -19900,11 +19900,11 @@
         <v>106</v>
       </c>
       <c r="L84" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M84" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N84" s="21" t="s">
@@ -19924,7 +19924,7 @@
         <v>0</v>
       </c>
       <c r="S84" s="96">
-        <f t="shared" ref="S84" si="28">IF(R84&lt;sel_ures,0,
+        <f t="shared" ref="S84" si="29">IF(R84&lt;sel_ures,0,
 IF(AND(sel_uclear&gt;=R84, R84&gt;=sel_ures),sel_tclear,
 IF(AND(sel_urec1&gt;=R84,R84&gt;sel_uclear),IF(sel_urec1&gt;sel_uclear,sel_tclear+(R84-sel_uclear)*(sel_trec1-sel_tclear)/(sel_urec1-sel_uclear),sel_tclear),
 IF(AND(sel_urec2&gt;=R84,R84&gt;sel_urec1),IF(sel_urec2&gt;sel_urec1,sel_trec2+(R84-sel_urec1)*(sel_trec3-sel_trec2)/(sel_urec2-sel_urec1),-99999),5
@@ -20045,11 +20045,11 @@
         <v>106</v>
       </c>
       <c r="L85" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M85" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N85" s="21" t="s">
@@ -20156,11 +20156,11 @@
         <v>106</v>
       </c>
       <c r="L86" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M86" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N86" s="21" t="s">
@@ -20267,11 +20267,11 @@
         <v>106</v>
       </c>
       <c r="L87" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M87" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N87" s="21" t="s">
@@ -20378,11 +20378,11 @@
         <v>106</v>
       </c>
       <c r="L88" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M88" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N88" s="21" t="s">
@@ -20489,11 +20489,11 @@
         <v>106</v>
       </c>
       <c r="L89" s="21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M89" s="21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N89" s="21" t="s">
@@ -20694,11 +20694,11 @@
         <v>89</v>
       </c>
       <c r="B91" s="88" t="b">
-        <f t="shared" ref="B91:C99" si="29">inp_Un&gt;=110</f>
+        <f t="shared" ref="B91:C99" si="30">inp_Un&gt;=110</f>
         <v>1</v>
       </c>
       <c r="C91" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="D91" s="87" t="s">
@@ -20728,11 +20728,11 @@
         <v>106</v>
       </c>
       <c r="L91" s="91">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M91" s="91">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N91" s="91" t="s">
@@ -20833,11 +20833,11 @@
         <v>90</v>
       </c>
       <c r="B92" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="C92" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="D92" s="87" t="s">
@@ -20867,11 +20867,11 @@
         <v>106</v>
       </c>
       <c r="L92" s="91">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M92" s="91">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N92" s="91" t="s">
@@ -20955,11 +20955,11 @@
         <v>91</v>
       </c>
       <c r="B93" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="C93" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="D93" s="87" t="s">
@@ -20989,11 +20989,11 @@
         <v>106</v>
       </c>
       <c r="L93" s="91">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10</v>
       </c>
       <c r="M93" s="91">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="N93" s="91" t="s">
@@ -21077,11 +21077,11 @@
         <v>92</v>
       </c>
       <c r="B94" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="C94" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="D94" s="87" t="s">
@@ -21201,11 +21201,11 @@
         <v>93</v>
       </c>
       <c r="B95" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="C95" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="D95" s="87" t="s">
@@ -21325,18 +21325,18 @@
         <v>94</v>
       </c>
       <c r="B96" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="C96" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="D96" s="87" t="s">
         <v>834</v>
       </c>
       <c r="E96" s="89">
-        <f t="shared" ref="E96:E99" si="30">inp_Uc/inp_Un</f>
+        <f t="shared" ref="E96:E99" si="31">inp_Uc/inp_Un</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="F96" s="89">
@@ -21359,11 +21359,11 @@
         <v>106</v>
       </c>
       <c r="L96" s="91">
-        <f t="shared" ref="L96:L99" si="31">inp_scr_min</f>
+        <f t="shared" ref="L96:L99" si="32">inp_scr_min</f>
         <v>10</v>
       </c>
       <c r="M96" s="91">
-        <f t="shared" ref="M96:M99" si="32">inp_xr_min</f>
+        <f t="shared" ref="M96:M99" si="33">inp_xr_min</f>
         <v>10</v>
       </c>
       <c r="N96" s="91" t="s">
@@ -21480,18 +21480,18 @@
         <v>95</v>
       </c>
       <c r="B97" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="C97" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="D97" s="87" t="s">
         <v>835</v>
       </c>
       <c r="E97" s="89">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F97" s="89">
@@ -21514,11 +21514,11 @@
         <v>106</v>
       </c>
       <c r="L97" s="91">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>10</v>
       </c>
       <c r="M97" s="91">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>10</v>
       </c>
       <c r="N97" s="91" t="s">
@@ -21607,18 +21607,18 @@
         <v>96</v>
       </c>
       <c r="B98" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="C98" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="D98" s="87" t="s">
         <v>836</v>
       </c>
       <c r="E98" s="89">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F98" s="89">
@@ -21641,11 +21641,11 @@
         <v>106</v>
       </c>
       <c r="L98" s="91">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>10</v>
       </c>
       <c r="M98" s="91">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>10</v>
       </c>
       <c r="N98" s="91" t="s">
@@ -21719,18 +21719,18 @@
         <v>97</v>
       </c>
       <c r="B99" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="C99" s="88" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="D99" s="87" t="s">
         <v>837</v>
       </c>
       <c r="E99" s="89">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F99" s="89">
@@ -21753,11 +21753,11 @@
         <v>106</v>
       </c>
       <c r="L99" s="91">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>10</v>
       </c>
       <c r="M99" s="91">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>10</v>
       </c>
       <c r="N99" s="91" t="s">
@@ -21853,18 +21853,18 @@
         <v>98</v>
       </c>
       <c r="B100" s="88" t="b">
-        <f t="shared" ref="B100:C140" si="33">inp_Un&gt;=110</f>
+        <f t="shared" ref="B100:C140" si="34">inp_Un&gt;=110</f>
         <v>1</v>
       </c>
       <c r="C100" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D100" s="87" t="s">
         <v>838</v>
       </c>
       <c r="E100" s="89">
-        <f t="shared" ref="E100:E130" si="34">inp_Uc/inp_Un</f>
+        <f t="shared" ref="E100:E130" si="35">inp_Uc/inp_Un</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="F100" s="89">
@@ -21977,18 +21977,18 @@
         <v>99</v>
       </c>
       <c r="B101" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C101" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D101" s="87" t="s">
         <v>839</v>
       </c>
       <c r="E101" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F101" s="89">
@@ -22004,7 +22004,7 @@
         <v>111</v>
       </c>
       <c r="J101" s="89">
-        <f t="shared" ref="J101:J109" si="35">inp_Uc/inp_Un</f>
+        <f t="shared" ref="J101:J109" si="36">inp_Uc/inp_Un</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="K101" s="89" t="s">
@@ -22120,18 +22120,18 @@
         <v>100</v>
       </c>
       <c r="B102" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C102" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D102" s="87" t="s">
         <v>840</v>
       </c>
       <c r="E102" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F102" s="89">
@@ -22147,7 +22147,7 @@
         <v>111</v>
       </c>
       <c r="J102" s="89">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="K102" s="89" t="s">
@@ -22241,18 +22241,18 @@
         <v>101</v>
       </c>
       <c r="B103" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C103" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D103" s="87" t="s">
         <v>841</v>
       </c>
       <c r="E103" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F103" s="89">
@@ -22268,7 +22268,7 @@
         <v>111</v>
       </c>
       <c r="J103" s="89">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="K103" s="89" t="s">
@@ -22366,18 +22366,18 @@
         <v>102</v>
       </c>
       <c r="B104" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C104" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D104" s="87" t="s">
         <v>842</v>
       </c>
       <c r="E104" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F104" s="89">
@@ -22393,7 +22393,7 @@
         <v>111</v>
       </c>
       <c r="J104" s="89">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="K104" s="89" t="s">
@@ -22490,18 +22490,18 @@
         <v>103</v>
       </c>
       <c r="B105" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C105" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D105" s="87" t="s">
         <v>843</v>
       </c>
       <c r="E105" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F105" s="89">
@@ -22517,7 +22517,7 @@
         <v>111</v>
       </c>
       <c r="J105" s="89">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="K105" s="89" t="s">
@@ -22611,18 +22611,18 @@
         <v>104</v>
       </c>
       <c r="B106" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C106" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D106" s="87" t="s">
         <v>844</v>
       </c>
       <c r="E106" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F106" s="89">
@@ -22638,7 +22638,7 @@
         <v>111</v>
       </c>
       <c r="J106" s="89">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="K106" s="280" t="s">
@@ -22794,18 +22794,18 @@
         <v>105</v>
       </c>
       <c r="B107" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C107" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D107" s="87" t="s">
         <v>845</v>
       </c>
       <c r="E107" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F107" s="89">
@@ -22821,7 +22821,7 @@
         <v>111</v>
       </c>
       <c r="J107" s="89">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="K107" s="280" t="s">
@@ -22977,18 +22977,18 @@
         <v>106</v>
       </c>
       <c r="B108" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C108" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D108" s="87" t="s">
         <v>846</v>
       </c>
       <c r="E108" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F108" s="89">
@@ -23004,7 +23004,7 @@
         <v>111</v>
       </c>
       <c r="J108" s="89">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="K108" s="280" t="s">
@@ -23160,18 +23160,18 @@
         <v>107</v>
       </c>
       <c r="B109" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C109" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D109" s="87" t="s">
         <v>847</v>
       </c>
       <c r="E109" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F109" s="89">
@@ -23187,7 +23187,7 @@
         <v>111</v>
       </c>
       <c r="J109" s="89">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="K109" s="89" t="s">
@@ -23268,18 +23268,18 @@
         <v>108</v>
       </c>
       <c r="B110" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C110" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D110" s="87" t="s">
         <v>848</v>
       </c>
       <c r="E110" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F110" s="89">
@@ -23295,18 +23295,18 @@
         <v>106</v>
       </c>
       <c r="J110" s="89">
-        <f t="shared" ref="J110:J116" si="36">IF(inp_default="Q(U)",E110,IF(inp_default="PF",1,0))</f>
+        <f t="shared" ref="J110:J116" si="37">IF(inp_default="Q(U)",E110,IF(inp_default="PF",1,0))</f>
         <v>0</v>
       </c>
       <c r="K110" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L110" s="91">
-        <f t="shared" ref="L110:L111" si="37">inp_scr_min</f>
+        <f t="shared" ref="L110:L111" si="38">inp_scr_min</f>
         <v>10</v>
       </c>
       <c r="M110" s="91">
-        <f t="shared" ref="M110:M111" si="38">inp_xr_min</f>
+        <f t="shared" ref="M110:M111" si="39">inp_xr_min</f>
         <v>10</v>
       </c>
       <c r="N110" s="91" t="s">
@@ -23389,18 +23389,18 @@
         <v>109</v>
       </c>
       <c r="B111" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C111" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D111" s="87" t="s">
         <v>921</v>
       </c>
       <c r="E111" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F111" s="89">
@@ -23416,18 +23416,18 @@
         <v>106</v>
       </c>
       <c r="J111" s="89">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="K111" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L111" s="91">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>10</v>
       </c>
       <c r="M111" s="91">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>10</v>
       </c>
       <c r="N111" s="91" t="s">
@@ -23508,18 +23508,18 @@
         <v>110</v>
       </c>
       <c r="B112" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C112" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D112" s="87" t="s">
         <v>849</v>
       </c>
       <c r="E112" s="89">
-        <f t="shared" ref="E112" si="39">inp_Uc/inp_Un</f>
+        <f t="shared" ref="E112" si="40">inp_Uc/inp_Un</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="F112" s="89">
@@ -23535,18 +23535,18 @@
         <v>106</v>
       </c>
       <c r="J112" s="89">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="K112" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L112" s="91">
-        <f t="shared" ref="L112" si="40">inp_scr_min</f>
+        <f t="shared" ref="L112" si="41">inp_scr_min</f>
         <v>10</v>
       </c>
       <c r="M112" s="91">
-        <f t="shared" ref="M112" si="41">inp_xr_min</f>
+        <f t="shared" ref="M112" si="42">inp_xr_min</f>
         <v>10</v>
       </c>
       <c r="N112" s="91" t="s">
@@ -23633,18 +23633,18 @@
         <v>111</v>
       </c>
       <c r="B113" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C113" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D113" s="87" t="s">
         <v>850</v>
       </c>
       <c r="E113" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F113" s="89">
@@ -23660,18 +23660,18 @@
         <v>106</v>
       </c>
       <c r="J113" s="89">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="K113" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L113" s="91">
-        <f t="shared" ref="L113:L116" si="42">inp_scr_min</f>
+        <f t="shared" ref="L113:L116" si="43">inp_scr_min</f>
         <v>10</v>
       </c>
       <c r="M113" s="91">
-        <f t="shared" ref="M113:M116" si="43">inp_xr_min</f>
+        <f t="shared" ref="M113:M116" si="44">inp_xr_min</f>
         <v>10</v>
       </c>
       <c r="N113" s="91" t="s">
@@ -23771,18 +23771,18 @@
         <v>112</v>
       </c>
       <c r="B114" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C114" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D114" s="87" t="s">
         <v>851</v>
       </c>
       <c r="E114" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F114" s="89">
@@ -23798,18 +23798,18 @@
         <v>106</v>
       </c>
       <c r="J114" s="89">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="K114" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L114" s="91">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>10</v>
       </c>
       <c r="M114" s="91">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>10</v>
       </c>
       <c r="N114" s="91" t="s">
@@ -23909,18 +23909,18 @@
         <v>113</v>
       </c>
       <c r="B115" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C115" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D115" s="87" t="s">
         <v>852</v>
       </c>
       <c r="E115" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F115" s="89">
@@ -23936,18 +23936,18 @@
         <v>106</v>
       </c>
       <c r="J115" s="89">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="K115" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L115" s="91">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>10</v>
       </c>
       <c r="M115" s="91">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>10</v>
       </c>
       <c r="N115" s="91" t="s">
@@ -24081,18 +24081,18 @@
         <v>114</v>
       </c>
       <c r="B116" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C116" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D116" s="87" t="s">
         <v>853</v>
       </c>
       <c r="E116" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F116" s="89">
@@ -24108,18 +24108,18 @@
         <v>106</v>
       </c>
       <c r="J116" s="89">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="K116" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L116" s="91">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>10</v>
       </c>
       <c r="M116" s="91">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>10</v>
       </c>
       <c r="N116" s="91" t="s">
@@ -24253,18 +24253,18 @@
         <v>115</v>
       </c>
       <c r="B117" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C117" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D117" s="87" t="s">
         <v>854</v>
       </c>
       <c r="E117" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F117" s="89">
@@ -24277,7 +24277,7 @@
         <v>220</v>
       </c>
       <c r="I117" s="90" t="str">
-        <f t="shared" ref="I117:I130" si="44">IF(inp_default="Q(U)","Q",IF(inp_default="Q","Q(U)",0))</f>
+        <f t="shared" ref="I117:I130" si="45">IF(inp_default="Q(U)","Q",IF(inp_default="Q","Q(U)",0))</f>
         <v>Q(U)</v>
       </c>
       <c r="J117" s="89">
@@ -24288,11 +24288,11 @@
         <v>106</v>
       </c>
       <c r="L117" s="91">
-        <f t="shared" ref="L117:L130" si="45">inp_scr_min</f>
+        <f t="shared" ref="L117:L130" si="46">inp_scr_min</f>
         <v>10</v>
       </c>
       <c r="M117" s="91">
-        <f t="shared" ref="M117:M130" si="46">inp_xr_min</f>
+        <f t="shared" ref="M117:M130" si="47">inp_xr_min</f>
         <v>10</v>
       </c>
       <c r="N117" s="91" t="s">
@@ -24312,7 +24312,7 @@
         <v>0</v>
       </c>
       <c r="S117" s="97">
-        <f t="shared" ref="S117" si="47">IF(R117&lt;sel_ures,0,
+        <f t="shared" ref="S117" si="48">IF(R117&lt;sel_ures,0,
 IF(AND(sel_uclear&gt;=R117, R117&gt;=sel_ures),sel_tclear,
 IF(AND(sel_urec1&gt;=R117,R117&gt;sel_uclear),IF(sel_urec1&gt;sel_uclear,sel_tclear+(R117-sel_uclear)*(sel_trec1-sel_tclear)/(sel_urec1-sel_uclear),sel_tclear),
 IF(AND(sel_urec2&gt;=R117,R117&gt;sel_urec1),IF(sel_urec2&gt;sel_urec1,sel_trec2+(R117-sel_urec1)*(sel_trec3-sel_trec2)/(sel_urec2-sel_urec1),-99999),5
@@ -24367,18 +24367,18 @@
         <v>116</v>
       </c>
       <c r="B118" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C118" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D118" s="87" t="s">
         <v>855</v>
       </c>
       <c r="E118" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F118" s="89">
@@ -24391,7 +24391,7 @@
         <v>220</v>
       </c>
       <c r="I118" s="90" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Q(U)</v>
       </c>
       <c r="J118" s="89">
@@ -24402,11 +24402,11 @@
         <v>106</v>
       </c>
       <c r="L118" s="91">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10</v>
       </c>
       <c r="M118" s="91">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>10</v>
       </c>
       <c r="N118" s="91" t="s">
@@ -24475,18 +24475,18 @@
         <v>117</v>
       </c>
       <c r="B119" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C119" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D119" s="87" t="s">
         <v>856</v>
       </c>
       <c r="E119" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F119" s="89">
@@ -24499,7 +24499,7 @@
         <v>220</v>
       </c>
       <c r="I119" s="90" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Q(U)</v>
       </c>
       <c r="J119" s="89">
@@ -24510,11 +24510,11 @@
         <v>106</v>
       </c>
       <c r="L119" s="91">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10</v>
       </c>
       <c r="M119" s="91">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>10</v>
       </c>
       <c r="N119" s="91" t="s">
@@ -24583,18 +24583,18 @@
         <v>118</v>
       </c>
       <c r="B120" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C120" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D120" s="87" t="s">
         <v>857</v>
       </c>
       <c r="E120" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F120" s="89">
@@ -24607,22 +24607,22 @@
         <v>220</v>
       </c>
       <c r="I120" s="90" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Q(U)</v>
       </c>
       <c r="J120" s="89">
-        <f t="shared" ref="J120" si="48">IF(inp_default="Q",E120,IF(inp_default="PF",1,0))</f>
+        <f t="shared" ref="J120" si="49">IF(inp_default="Q",E120,IF(inp_default="PF",1,0))</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="K120" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L120" s="91">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10</v>
       </c>
       <c r="M120" s="91">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>10</v>
       </c>
       <c r="N120" s="91" t="s">
@@ -24691,18 +24691,18 @@
         <v>119</v>
       </c>
       <c r="B121" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C121" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D121" s="87" t="s">
         <v>858</v>
       </c>
       <c r="E121" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F121" s="89">
@@ -24715,7 +24715,7 @@
         <v>220</v>
       </c>
       <c r="I121" s="90" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Q(U)</v>
       </c>
       <c r="J121" s="89">
@@ -24726,11 +24726,11 @@
         <v>106</v>
       </c>
       <c r="L121" s="91">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10</v>
       </c>
       <c r="M121" s="91">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>10</v>
       </c>
       <c r="N121" s="91" t="s">
@@ -24799,18 +24799,18 @@
         <v>120</v>
       </c>
       <c r="B122" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C122" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D122" s="87" t="s">
         <v>859</v>
       </c>
       <c r="E122" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F122" s="89">
@@ -24823,7 +24823,7 @@
         <v>220</v>
       </c>
       <c r="I122" s="90" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Q(U)</v>
       </c>
       <c r="J122" s="89">
@@ -24834,11 +24834,11 @@
         <v>106</v>
       </c>
       <c r="L122" s="91">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10</v>
       </c>
       <c r="M122" s="91">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>10</v>
       </c>
       <c r="N122" s="91" t="s">
@@ -24908,18 +24908,18 @@
         <v>121</v>
       </c>
       <c r="B123" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C123" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D123" s="87" t="s">
         <v>860</v>
       </c>
       <c r="E123" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F123" s="89">
@@ -24932,22 +24932,22 @@
         <v>220</v>
       </c>
       <c r="I123" s="90" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Q(U)</v>
       </c>
       <c r="J123" s="89">
-        <f t="shared" ref="J123:J124" si="49">IF(inp_default="Q",E123,IF(inp_default="PF",1,0))</f>
+        <f t="shared" ref="J123:J124" si="50">IF(inp_default="Q",E123,IF(inp_default="PF",1,0))</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="K123" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L123" s="91">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10</v>
       </c>
       <c r="M123" s="91">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>10</v>
       </c>
       <c r="N123" s="91" t="s">
@@ -25016,18 +25016,18 @@
         <v>122</v>
       </c>
       <c r="B124" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C124" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D124" s="87" t="s">
         <v>861</v>
       </c>
       <c r="E124" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F124" s="89">
@@ -25040,22 +25040,22 @@
         <v>220</v>
       </c>
       <c r="I124" s="90" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Q(U)</v>
       </c>
       <c r="J124" s="89">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="K124" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L124" s="91">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10</v>
       </c>
       <c r="M124" s="91">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>10</v>
       </c>
       <c r="N124" s="91" t="s">
@@ -25124,18 +25124,18 @@
         <v>123</v>
       </c>
       <c r="B125" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C125" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D125" s="87" t="s">
         <v>862</v>
       </c>
       <c r="E125" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F125" s="89">
@@ -25148,22 +25148,22 @@
         <v>220</v>
       </c>
       <c r="I125" s="90" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Q(U)</v>
       </c>
       <c r="J125" s="89">
-        <f t="shared" ref="J125" si="50">IF(inp_default="Q",E125,IF(inp_default="PF",1,0))</f>
+        <f t="shared" ref="J125" si="51">IF(inp_default="Q",E125,IF(inp_default="PF",1,0))</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="K125" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L125" s="91">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10</v>
       </c>
       <c r="M125" s="91">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>10</v>
       </c>
       <c r="N125" s="91" t="s">
@@ -25232,18 +25232,18 @@
         <v>124</v>
       </c>
       <c r="B126" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C126" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D126" s="87" t="s">
         <v>863</v>
       </c>
       <c r="E126" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F126" s="89">
@@ -25256,22 +25256,22 @@
         <v>220</v>
       </c>
       <c r="I126" s="90" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Q(U)</v>
       </c>
       <c r="J126" s="89">
-        <f t="shared" ref="J126:J128" si="51">IF(inp_default="Q",E126,IF(inp_default="PF",1,0))</f>
+        <f t="shared" ref="J126:J128" si="52">IF(inp_default="Q",E126,IF(inp_default="PF",1,0))</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="K126" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L126" s="91">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10</v>
       </c>
       <c r="M126" s="91">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>10</v>
       </c>
       <c r="N126" s="91" t="s">
@@ -25340,18 +25340,18 @@
         <v>125</v>
       </c>
       <c r="B127" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C127" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D127" s="87" t="s">
         <v>864</v>
       </c>
       <c r="E127" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F127" s="89">
@@ -25364,22 +25364,22 @@
         <v>220</v>
       </c>
       <c r="I127" s="90" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Q(U)</v>
       </c>
       <c r="J127" s="89">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="K127" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L127" s="91">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10</v>
       </c>
       <c r="M127" s="91">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>10</v>
       </c>
       <c r="N127" s="91" t="s">
@@ -25448,18 +25448,18 @@
         <v>126</v>
       </c>
       <c r="B128" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C128" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D128" s="87" t="s">
         <v>865</v>
       </c>
       <c r="E128" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F128" s="89">
@@ -25472,22 +25472,22 @@
         <v>220</v>
       </c>
       <c r="I128" s="90" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Q(U)</v>
       </c>
       <c r="J128" s="89">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="K128" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L128" s="91">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10</v>
       </c>
       <c r="M128" s="91">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>10</v>
       </c>
       <c r="N128" s="91" t="s">
@@ -25556,18 +25556,18 @@
         <v>127</v>
       </c>
       <c r="B129" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C129" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D129" s="87" t="s">
         <v>866</v>
       </c>
       <c r="E129" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F129" s="89">
@@ -25580,22 +25580,22 @@
         <v>220</v>
       </c>
       <c r="I129" s="90" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Q(U)</v>
       </c>
       <c r="J129" s="89">
-        <f t="shared" ref="J129" si="52">IF(inp_default="Q",E129,IF(inp_default="PF",1,0))</f>
+        <f t="shared" ref="J129" si="53">IF(inp_default="Q",E129,IF(inp_default="PF",1,0))</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="K129" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L129" s="91">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10</v>
       </c>
       <c r="M129" s="91">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>10</v>
       </c>
       <c r="N129" s="91" t="s">
@@ -25664,18 +25664,18 @@
         <v>128</v>
       </c>
       <c r="B130" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C130" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D130" s="87" t="s">
         <v>867</v>
       </c>
       <c r="E130" s="89">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F130" s="89">
@@ -25688,22 +25688,22 @@
         <v>220</v>
       </c>
       <c r="I130" s="90" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>Q(U)</v>
       </c>
       <c r="J130" s="89">
-        <f t="shared" ref="J130" si="53">IF(inp_default="Q",E130,IF(inp_default="PF",1,0))</f>
+        <f t="shared" ref="J130" si="54">IF(inp_default="Q",E130,IF(inp_default="PF",1,0))</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="K130" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L130" s="91">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10</v>
       </c>
       <c r="M130" s="91">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>10</v>
       </c>
       <c r="N130" s="91" t="s">
@@ -25772,18 +25772,18 @@
         <v>129</v>
       </c>
       <c r="B131" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C131" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D131" s="87" t="s">
         <v>868</v>
       </c>
       <c r="E131" s="89">
-        <f t="shared" ref="E131:E143" si="54">inp_Uc/inp_Un</f>
+        <f t="shared" ref="E131:E143" si="55">inp_Uc/inp_Un</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="F131" s="89">
@@ -25892,18 +25892,18 @@
         <v>130</v>
       </c>
       <c r="B132" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C132" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D132" s="87" t="s">
         <v>869</v>
       </c>
       <c r="E132" s="89">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F132" s="89">
@@ -26012,18 +26012,18 @@
         <v>131</v>
       </c>
       <c r="B133" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C133" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D133" s="87" t="s">
         <v>870</v>
       </c>
       <c r="E133" s="89">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F133" s="89">
@@ -26036,22 +26036,22 @@
         <v>220</v>
       </c>
       <c r="I133" s="90" t="str">
-        <f t="shared" ref="I133" si="55">IF(inp_default="Q(U)","Q",IF(inp_default="Q","Q(U)",0))</f>
+        <f t="shared" ref="I133" si="56">IF(inp_default="Q(U)","Q",IF(inp_default="Q","Q(U)",0))</f>
         <v>Q(U)</v>
       </c>
       <c r="J133" s="89">
-        <f t="shared" ref="J133" si="56">IF(inp_default="Q",E133,IF(inp_default="PF",1,0))</f>
+        <f t="shared" ref="J133" si="57">IF(inp_default="Q",E133,IF(inp_default="PF",1,0))</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="K133" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L133" s="91">
-        <f t="shared" ref="L133:L136" si="57">inp_scr_min</f>
+        <f t="shared" ref="L133:L136" si="58">inp_scr_min</f>
         <v>10</v>
       </c>
       <c r="M133" s="91">
-        <f t="shared" ref="M133:M136" si="58">inp_xr_min</f>
+        <f t="shared" ref="M133:M136" si="59">inp_xr_min</f>
         <v>10</v>
       </c>
       <c r="N133" s="91" t="s">
@@ -26122,18 +26122,18 @@
         <v>132</v>
       </c>
       <c r="B134" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C134" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D134" s="87" t="s">
         <v>871</v>
       </c>
       <c r="E134" s="89">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F134" s="89">
@@ -26156,11 +26156,11 @@
         <v>106</v>
       </c>
       <c r="L134" s="91">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>10</v>
       </c>
       <c r="M134" s="91">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>10</v>
       </c>
       <c r="N134" s="91" t="s">
@@ -26231,18 +26231,18 @@
         <v>133</v>
       </c>
       <c r="B135" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C135" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D135" s="87" t="s">
         <v>872</v>
       </c>
       <c r="E135" s="89">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F135" s="89">
@@ -26265,11 +26265,11 @@
         <v>106</v>
       </c>
       <c r="L135" s="91">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>10</v>
       </c>
       <c r="M135" s="91">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>10</v>
       </c>
       <c r="N135" s="91" t="s">
@@ -26340,18 +26340,18 @@
         <v>134</v>
       </c>
       <c r="B136" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C136" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D136" s="87" t="s">
         <v>873</v>
       </c>
       <c r="E136" s="89">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F136" s="89">
@@ -26364,22 +26364,22 @@
         <v>220</v>
       </c>
       <c r="I136" s="90" t="str">
-        <f t="shared" ref="I136" si="59">IF(inp_default="Q(U)","Q",IF(inp_default="Q","Q(U)",0))</f>
+        <f t="shared" ref="I136" si="60">IF(inp_default="Q(U)","Q",IF(inp_default="Q","Q(U)",0))</f>
         <v>Q(U)</v>
       </c>
       <c r="J136" s="89">
-        <f t="shared" ref="J136" si="60">IF(inp_default="Q",E136,IF(inp_default="PF",1,0))</f>
+        <f t="shared" ref="J136" si="61">IF(inp_default="Q",E136,IF(inp_default="PF",1,0))</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="K136" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L136" s="91">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>10</v>
       </c>
       <c r="M136" s="91">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>10</v>
       </c>
       <c r="N136" s="91" t="s">
@@ -26458,18 +26458,18 @@
         <v>135</v>
       </c>
       <c r="B137" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C137" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D137" s="87" t="s">
         <v>874</v>
       </c>
       <c r="E137" s="89">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F137" s="89">
@@ -26485,7 +26485,7 @@
         <v>106</v>
       </c>
       <c r="J137" s="89">
-        <f t="shared" ref="J137" si="61">IF(inp_default="Q(U)",E137,IF(inp_default="PF",1,0))</f>
+        <f t="shared" ref="J137" si="62">IF(inp_default="Q(U)",E137,IF(inp_default="PF",1,0))</f>
         <v>0</v>
       </c>
       <c r="K137" s="89" t="s">
@@ -26586,18 +26586,18 @@
         <v>136</v>
       </c>
       <c r="B138" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C138" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D138" s="87" t="s">
         <v>875</v>
       </c>
       <c r="E138" s="89">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F138" s="89">
@@ -26613,7 +26613,7 @@
         <v>106</v>
       </c>
       <c r="J138" s="89">
-        <f t="shared" ref="J138:J142" si="62">IF(inp_default="Q(U)",E138,IF(inp_default="PF",1,0))</f>
+        <f t="shared" ref="J138:J142" si="63">IF(inp_default="Q(U)",E138,IF(inp_default="PF",1,0))</f>
         <v>0</v>
       </c>
       <c r="K138" s="89" t="s">
@@ -26691,18 +26691,18 @@
         <v>137</v>
       </c>
       <c r="B139" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C139" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D139" s="87" t="s">
         <v>876</v>
       </c>
       <c r="E139" s="89">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F139" s="89">
@@ -26718,7 +26718,7 @@
         <v>106</v>
       </c>
       <c r="J139" s="89">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="K139" s="89" t="s">
@@ -26796,18 +26796,18 @@
         <v>138</v>
       </c>
       <c r="B140" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="C140" s="88" t="b">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="D140" s="87" t="s">
         <v>877</v>
       </c>
       <c r="E140" s="89">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F140" s="89">
@@ -26823,18 +26823,18 @@
         <v>106</v>
       </c>
       <c r="J140" s="89">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="K140" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L140" s="91">
-        <f t="shared" ref="L140:L141" si="63">inp_scr_min</f>
+        <f t="shared" ref="L140:L141" si="64">inp_scr_min</f>
         <v>10</v>
       </c>
       <c r="M140" s="91">
-        <f t="shared" ref="M140:M141" si="64">inp_xr_min</f>
+        <f t="shared" ref="M140:M141" si="65">inp_xr_min</f>
         <v>10</v>
       </c>
       <c r="N140" s="91" t="s">
@@ -26955,18 +26955,18 @@
         <v>139</v>
       </c>
       <c r="B141" s="88" t="b">
-        <f t="shared" ref="B141:C167" si="65">inp_Un&gt;=110</f>
+        <f t="shared" ref="B141:C167" si="66">inp_Un&gt;=110</f>
         <v>1</v>
       </c>
       <c r="C141" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D141" s="87" t="s">
         <v>878</v>
       </c>
       <c r="E141" s="89">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F141" s="89">
@@ -26982,18 +26982,18 @@
         <v>106</v>
       </c>
       <c r="J141" s="89">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="K141" s="89" t="s">
         <v>106</v>
       </c>
       <c r="L141" s="91">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>10</v>
       </c>
       <c r="M141" s="91">
-        <f t="shared" si="64"/>
+        <f t="shared" si="65"/>
         <v>10</v>
       </c>
       <c r="N141" s="91" t="s">
@@ -27114,18 +27114,18 @@
         <v>140</v>
       </c>
       <c r="B142" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C142" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D142" s="87" t="s">
         <v>879</v>
       </c>
       <c r="E142" s="89">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F142" s="89">
@@ -27141,7 +27141,7 @@
         <v>106</v>
       </c>
       <c r="J142" s="89">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="K142" s="89" t="s">
@@ -27247,18 +27247,18 @@
         <v>141</v>
       </c>
       <c r="B143" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C143" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D143" s="87" t="s">
         <v>880</v>
       </c>
       <c r="E143" s="89">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F143" s="89">
@@ -27274,7 +27274,7 @@
         <v>106</v>
       </c>
       <c r="J143" s="89">
-        <f t="shared" ref="J143" si="66">IF(inp_default="Q(U)",E143,IF(inp_default="PF",1,0))</f>
+        <f t="shared" ref="J143" si="67">IF(inp_default="Q(U)",E143,IF(inp_default="PF",1,0))</f>
         <v>0</v>
       </c>
       <c r="K143" s="89" t="s">
@@ -27380,18 +27380,18 @@
         <v>142</v>
       </c>
       <c r="B144" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C144" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D144" s="87" t="s">
         <v>919</v>
       </c>
       <c r="E144" s="89">
-        <f t="shared" ref="E144:E145" si="67">inp_Uc/inp_Un</f>
+        <f t="shared" ref="E144:E145" si="68">inp_Uc/inp_Un</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="F144" s="89">
@@ -27407,7 +27407,7 @@
         <v>106</v>
       </c>
       <c r="J144" s="89">
-        <f t="shared" ref="J144" si="68">IF(inp_default="Q(U)",E144,IF(inp_default="PF",1,0))</f>
+        <f t="shared" ref="J144" si="69">IF(inp_default="Q(U)",E144,IF(inp_default="PF",1,0))</f>
         <v>0</v>
       </c>
       <c r="K144" s="89" t="s">
@@ -27500,18 +27500,18 @@
         <v>143</v>
       </c>
       <c r="B145" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C145" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D145" s="87" t="s">
         <v>920</v>
       </c>
       <c r="E145" s="89">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F145" s="89">
@@ -27621,18 +27621,18 @@
         <v>144</v>
       </c>
       <c r="B146" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C146" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D146" s="87" t="s">
         <v>881</v>
       </c>
       <c r="E146" s="89">
-        <f t="shared" ref="E146:E178" si="69">inp_Uc/inp_Un</f>
+        <f t="shared" ref="E146:E178" si="70">inp_Uc/inp_Un</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="F146" s="89">
@@ -27671,7 +27671,7 @@
         <v>126</v>
       </c>
       <c r="S146" s="102">
-        <f t="shared" ref="S146:S151" si="70">inp_Uc/inp_Un</f>
+        <f t="shared" ref="S146:S151" si="71">inp_Uc/inp_Un</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="U146" s="89"/>
@@ -27722,18 +27722,18 @@
         <v>145</v>
       </c>
       <c r="B147" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C147" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D147" s="87" t="s">
         <v>882</v>
       </c>
       <c r="E147" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F147" s="89">
@@ -27749,7 +27749,7 @@
         <v>111</v>
       </c>
       <c r="J147" s="89">
-        <f t="shared" ref="J147" si="71">inp_Uc/inp_Un</f>
+        <f t="shared" ref="J147" si="72">inp_Uc/inp_Un</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="K147" s="89" t="s">
@@ -27773,7 +27773,7 @@
         <v>126</v>
       </c>
       <c r="S147" s="102">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="U147" s="89"/>
@@ -27824,18 +27824,18 @@
         <v>146</v>
       </c>
       <c r="B148" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C148" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D148" s="87" t="s">
         <v>883</v>
       </c>
       <c r="E148" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F148" s="89">
@@ -27874,7 +27874,7 @@
         <v>127</v>
       </c>
       <c r="S148" s="102">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="U148" s="89"/>
@@ -27925,18 +27925,18 @@
         <v>147</v>
       </c>
       <c r="B149" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C149" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D149" s="87" t="s">
         <v>884</v>
       </c>
       <c r="E149" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F149" s="89">
@@ -27952,7 +27952,7 @@
         <v>111</v>
       </c>
       <c r="J149" s="89">
-        <f t="shared" ref="J149:J151" si="72">inp_Uc/inp_Un</f>
+        <f t="shared" ref="J149:J151" si="73">inp_Uc/inp_Un</f>
         <v>1.0651315789473685</v>
       </c>
       <c r="K149" s="89" t="s">
@@ -27976,7 +27976,7 @@
         <v>127</v>
       </c>
       <c r="S149" s="102">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="T149" s="89"/>
@@ -28028,18 +28028,18 @@
         <v>148</v>
       </c>
       <c r="B150" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C150" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D150" s="87" t="s">
         <v>885</v>
       </c>
       <c r="E150" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F150" s="89">
@@ -28078,7 +28078,7 @@
         <v>459</v>
       </c>
       <c r="S150" s="102">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="U150" s="89"/>
@@ -28129,18 +28129,18 @@
         <v>149</v>
       </c>
       <c r="B151" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C151" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D151" s="87" t="s">
         <v>886</v>
       </c>
       <c r="E151" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F151" s="89">
@@ -28156,7 +28156,7 @@
         <v>111</v>
       </c>
       <c r="J151" s="89">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="K151" s="89" t="s">
@@ -28180,7 +28180,7 @@
         <v>459</v>
       </c>
       <c r="S151" s="102">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="T151" s="89"/>
@@ -28232,18 +28232,18 @@
         <v>150</v>
       </c>
       <c r="B152" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C152" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D152" s="87" t="s">
         <v>887</v>
       </c>
       <c r="E152" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F152" s="89">
@@ -28269,7 +28269,7 @@
         <v>10</v>
       </c>
       <c r="M152" s="91">
-        <f t="shared" ref="M152:M163" si="73">inp_xr_min</f>
+        <f t="shared" ref="M152:M163" si="74">inp_xr_min</f>
         <v>10</v>
       </c>
       <c r="N152" s="91" t="s">
@@ -28322,18 +28322,18 @@
         <v>151</v>
       </c>
       <c r="B153" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C153" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D153" s="87" t="s">
         <v>888</v>
       </c>
       <c r="E153" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F153" s="89">
@@ -28404,18 +28404,18 @@
         <v>152</v>
       </c>
       <c r="B154" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C154" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D154" s="87" t="s">
         <v>889</v>
       </c>
       <c r="E154" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F154" s="89">
@@ -28441,7 +28441,7 @@
         <v>10</v>
       </c>
       <c r="M154" s="91">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>10</v>
       </c>
       <c r="N154" s="91" t="s">
@@ -28484,18 +28484,18 @@
         <v>153</v>
       </c>
       <c r="B155" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C155" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D155" s="87" t="s">
         <v>890</v>
       </c>
       <c r="E155" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F155" s="89">
@@ -28558,18 +28558,18 @@
         <v>154</v>
       </c>
       <c r="B156" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C156" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D156" s="87" t="s">
         <v>891</v>
       </c>
       <c r="E156" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F156" s="89">
@@ -28595,7 +28595,7 @@
         <v>10</v>
       </c>
       <c r="M156" s="91">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>10</v>
       </c>
       <c r="N156" s="91" t="s">
@@ -28632,18 +28632,18 @@
         <v>155</v>
       </c>
       <c r="B157" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C157" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D157" s="87" t="s">
         <v>892</v>
       </c>
       <c r="E157" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F157" s="89">
@@ -28706,18 +28706,18 @@
         <v>156</v>
       </c>
       <c r="B158" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C158" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D158" s="87" t="s">
         <v>893</v>
       </c>
       <c r="E158" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F158" s="89">
@@ -28743,7 +28743,7 @@
         <v>10</v>
       </c>
       <c r="M158" s="91">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>10</v>
       </c>
       <c r="N158" s="91" t="s">
@@ -28780,18 +28780,18 @@
         <v>157</v>
       </c>
       <c r="B159" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C159" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D159" s="87" t="s">
         <v>894</v>
       </c>
       <c r="E159" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F159" s="89">
@@ -28854,18 +28854,18 @@
         <v>158</v>
       </c>
       <c r="B160" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C160" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D160" s="87" t="s">
         <v>895</v>
       </c>
       <c r="E160" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F160" s="89">
@@ -28891,7 +28891,7 @@
         <v>10</v>
       </c>
       <c r="M160" s="91">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>10</v>
       </c>
       <c r="N160" s="91" t="s">
@@ -28928,18 +28928,18 @@
         <v>159</v>
       </c>
       <c r="B161" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C161" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D161" s="87" t="s">
         <v>896</v>
       </c>
       <c r="E161" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F161" s="89">
@@ -28965,7 +28965,7 @@
         <v>10</v>
       </c>
       <c r="M161" s="91">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>10</v>
       </c>
       <c r="N161" s="91" t="s">
@@ -29002,18 +29002,18 @@
         <v>160</v>
       </c>
       <c r="B162" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C162" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D162" s="87" t="s">
         <v>897</v>
       </c>
       <c r="E162" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F162" s="89">
@@ -29039,7 +29039,7 @@
         <v>10</v>
       </c>
       <c r="M162" s="91">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>10</v>
       </c>
       <c r="N162" s="91" t="s">
@@ -29076,18 +29076,18 @@
         <v>161</v>
       </c>
       <c r="B163" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C163" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D163" s="87" t="s">
         <v>898</v>
       </c>
       <c r="E163" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F163" s="89">
@@ -29113,7 +29113,7 @@
         <v>10</v>
       </c>
       <c r="M163" s="91">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>10</v>
       </c>
       <c r="N163" s="91" t="s">
@@ -29150,18 +29150,18 @@
         <v>162</v>
       </c>
       <c r="B164" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C164" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D164" s="87" t="s">
         <v>899</v>
       </c>
       <c r="E164" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F164" s="89">
@@ -29183,11 +29183,11 @@
         <v>106</v>
       </c>
       <c r="L164" s="91">
-        <f t="shared" ref="L164:L168" si="74">inp_scr_min</f>
+        <f t="shared" ref="L164:L168" si="75">inp_scr_min</f>
         <v>10</v>
       </c>
       <c r="M164" s="91">
-        <f t="shared" ref="M164:M168" si="75">inp_xr_min</f>
+        <f t="shared" ref="M164:M168" si="76">inp_xr_min</f>
         <v>10</v>
       </c>
       <c r="N164" s="91" t="s">
@@ -29257,18 +29257,18 @@
         <v>163</v>
       </c>
       <c r="B165" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C165" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D165" s="87" t="s">
         <v>900</v>
       </c>
       <c r="E165" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F165" s="89">
@@ -29290,11 +29290,11 @@
         <v>106</v>
       </c>
       <c r="L165" s="91">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>10</v>
       </c>
       <c r="M165" s="91">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>10</v>
       </c>
       <c r="N165" s="91" t="s">
@@ -29364,18 +29364,18 @@
         <v>164</v>
       </c>
       <c r="B166" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C166" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D166" s="87" t="s">
         <v>901</v>
       </c>
       <c r="E166" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F166" s="89">
@@ -29397,11 +29397,11 @@
         <v>106</v>
       </c>
       <c r="L166" s="91">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>10</v>
       </c>
       <c r="M166" s="91">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>10</v>
       </c>
       <c r="N166" s="91" t="s">
@@ -29470,18 +29470,18 @@
         <v>165</v>
       </c>
       <c r="B167" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="C167" s="88" t="b">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="D167" s="87" t="s">
         <v>902</v>
       </c>
       <c r="E167" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F167" s="89">
@@ -29503,11 +29503,11 @@
         <v>106</v>
       </c>
       <c r="L167" s="91">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>10</v>
       </c>
       <c r="M167" s="91">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>10</v>
       </c>
       <c r="N167" s="91" t="s">
@@ -29576,18 +29576,18 @@
         <v>166</v>
       </c>
       <c r="B168" s="88" t="b">
-        <f t="shared" ref="B168:C178" si="76">inp_Un&gt;=110</f>
+        <f t="shared" ref="B168:C178" si="77">inp_Un&gt;=110</f>
         <v>1</v>
       </c>
       <c r="C168" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="D168" s="87" t="s">
         <v>903</v>
       </c>
       <c r="E168" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F168" s="89">
@@ -29609,11 +29609,11 @@
         <v>106</v>
       </c>
       <c r="L168" s="91">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>10</v>
       </c>
       <c r="M168" s="91">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>10</v>
       </c>
       <c r="N168" s="91" t="s">
@@ -29754,18 +29754,18 @@
         <v>167</v>
       </c>
       <c r="B169" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="C169" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="D169" s="87" t="s">
         <v>904</v>
       </c>
       <c r="E169" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F169" s="89">
@@ -29932,18 +29932,18 @@
         <v>168</v>
       </c>
       <c r="B170" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="C170" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="D170" s="87" t="s">
         <v>905</v>
       </c>
       <c r="E170" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F170" s="89">
@@ -29965,11 +29965,11 @@
         <v>106</v>
       </c>
       <c r="L170" s="91">
-        <f t="shared" ref="L170:L177" si="77">inp_scr_min</f>
+        <f t="shared" ref="L170:L177" si="78">inp_scr_min</f>
         <v>10</v>
       </c>
       <c r="M170" s="91">
-        <f t="shared" ref="M170:M178" si="78">inp_xr_min</f>
+        <f t="shared" ref="M170:M178" si="79">inp_xr_min</f>
         <v>10</v>
       </c>
       <c r="N170" s="91" t="s">
@@ -30039,18 +30039,18 @@
         <v>169</v>
       </c>
       <c r="B171" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="C171" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="D171" s="87" t="s">
         <v>906</v>
       </c>
       <c r="E171" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F171" s="89">
@@ -30072,11 +30072,11 @@
         <v>106</v>
       </c>
       <c r="L171" s="91">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>10</v>
       </c>
       <c r="M171" s="91">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>10</v>
       </c>
       <c r="N171" s="91" t="s">
@@ -30146,18 +30146,18 @@
         <v>170</v>
       </c>
       <c r="B172" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="C172" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="D172" s="87" t="s">
         <v>907</v>
       </c>
       <c r="E172" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F172" s="89">
@@ -30179,11 +30179,11 @@
         <v>106</v>
       </c>
       <c r="L172" s="91">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>10</v>
       </c>
       <c r="M172" s="91">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>10</v>
       </c>
       <c r="N172" s="91" t="s">
@@ -30253,18 +30253,18 @@
         <v>171</v>
       </c>
       <c r="B173" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="C173" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="D173" s="87" t="s">
         <v>908</v>
       </c>
       <c r="E173" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F173" s="89">
@@ -30286,11 +30286,11 @@
         <v>106</v>
       </c>
       <c r="L173" s="91">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>10</v>
       </c>
       <c r="M173" s="91">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>10</v>
       </c>
       <c r="N173" s="91" t="s">
@@ -30360,18 +30360,18 @@
         <v>172</v>
       </c>
       <c r="B174" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="C174" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="D174" s="87" t="s">
         <v>909</v>
       </c>
       <c r="E174" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F174" s="89">
@@ -30393,11 +30393,11 @@
         <v>106</v>
       </c>
       <c r="L174" s="91">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>10</v>
       </c>
       <c r="M174" s="91">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>10</v>
       </c>
       <c r="N174" s="91" t="s">
@@ -30465,18 +30465,18 @@
         <v>173</v>
       </c>
       <c r="B175" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="C175" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="D175" s="87" t="s">
         <v>910</v>
       </c>
       <c r="E175" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F175" s="89">
@@ -30498,11 +30498,11 @@
         <v>106</v>
       </c>
       <c r="L175" s="91">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>10</v>
       </c>
       <c r="M175" s="91">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>10</v>
       </c>
       <c r="N175" s="91" t="s">
@@ -30570,18 +30570,18 @@
         <v>174</v>
       </c>
       <c r="B176" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="C176" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="D176" s="87" t="s">
         <v>911</v>
       </c>
       <c r="E176" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F176" s="89">
@@ -30603,11 +30603,11 @@
         <v>106</v>
       </c>
       <c r="L176" s="91">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>10</v>
       </c>
       <c r="M176" s="91">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>10</v>
       </c>
       <c r="N176" s="91" t="s">
@@ -30708,18 +30708,18 @@
         <v>175</v>
       </c>
       <c r="B177" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="C177" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="D177" s="87" t="s">
         <v>926</v>
       </c>
       <c r="E177" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F177" s="89">
@@ -30741,11 +30741,11 @@
         <v>106</v>
       </c>
       <c r="L177" s="91">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>10</v>
       </c>
       <c r="M177" s="91">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>10</v>
       </c>
       <c r="N177" s="91" t="s">
@@ -30845,18 +30845,18 @@
         <v>176</v>
       </c>
       <c r="B178" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="C178" s="88" t="b">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="D178" s="87" t="s">
         <v>912</v>
       </c>
       <c r="E178" s="89">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.0651315789473685</v>
       </c>
       <c r="F178" s="89">
@@ -30882,7 +30882,7 @@
         <v>10</v>
       </c>
       <c r="M178" s="91">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>10</v>
       </c>
       <c r="N178" s="91" t="s">
@@ -31344,7 +31344,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="AC23:AD23 R71 E46 E51 J144 L169:M169 L153:M153 L155:M155 L157:M157 L159:M159" formula="1"/>
+    <ignoredError sqref="AC23:AD23 R71 E46 E51 J144 L169:M169 L153:M153 L155:M155 L157:M157 L159:M159 J60" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -53434,6 +53434,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="C18:C28"/>
+    <mergeCell ref="C44:C53"/>
+    <mergeCell ref="C29:C43"/>
     <mergeCell ref="C163:C176"/>
     <mergeCell ref="C61:C70"/>
     <mergeCell ref="C71:C94"/>
@@ -53441,13 +53448,6 @@
     <mergeCell ref="C99:C108"/>
     <mergeCell ref="C109:C115"/>
     <mergeCell ref="C116:C162"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="C18:C28"/>
-    <mergeCell ref="C44:C53"/>
-    <mergeCell ref="C29:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -54224,6 +54224,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="107e75b3-53cc-4838-92d2-ebc011bd4832">
@@ -54232,15 +54241,6 @@
     <TaxCatchAll xmlns="888ccf44-0d39-41a2-ab17-f7efb2bf6977" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -54263,6 +54263,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2288FB7-E85A-4FE8-9E7A-FE572FF16064}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -54277,12 +54285,4 @@
     <ds:schemaRef ds:uri="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update testcases.xlsx to reflect recent changes in plotting and guideFunction functionality
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/prw_energinet_dk/Documents/Dokumenter/GitHub/MTB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7784DD6-5403-4993-9B56-0D0A90D642B8}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A3B8C97-895B-41DC-8C6D-58B636181CF3}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20790" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -3346,12 +3346,6 @@
     <t>RfG_Fault_2_20_WG</t>
   </si>
   <si>
-    <t>RfG_Fault_3_ROCOF_curveOF</t>
-  </si>
-  <si>
-    <t>RfG_Fault_3_ROCOF_curveUF</t>
-  </si>
-  <si>
     <t>RfG_Fault_3_SCR_freqStep1</t>
   </si>
   <si>
@@ -3515,6 +3509,12 @@
   </si>
   <si>
     <t>RfG_SystemProtect+fault</t>
+  </si>
+  <si>
+    <t>RfG_Fault_3_RoCoF_curveOF</t>
+  </si>
+  <si>
+    <t>RfG_Fault_3_RoCoF_curveUF</t>
   </si>
 </sst>
 </file>
@@ -6108,7 +6108,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="291" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="B19" s="283" t="b">
         <v>0</v>
@@ -6117,7 +6117,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="293" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -9414,8 +9414,8 @@
   <dimension ref="A1:CQ218"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J60" sqref="J60"/>
+      <pane ySplit="2" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -9619,7 +9619,7 @@
         <v>100</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>101</v>
@@ -13508,7 +13508,9 @@
       <c r="R34" s="96">
         <v>0.5</v>
       </c>
-      <c r="S34" s="96"/>
+      <c r="S34" s="96">
+        <v>0</v>
+      </c>
       <c r="T34" s="5"/>
       <c r="U34" s="85"/>
       <c r="V34" s="85"/>
@@ -13646,7 +13648,9 @@
       <c r="R35" s="97">
         <v>0</v>
       </c>
-      <c r="S35" s="97"/>
+      <c r="S35" s="97">
+        <v>0</v>
+      </c>
       <c r="U35" s="89"/>
       <c r="V35" s="89"/>
       <c r="W35" s="108"/>
@@ -13753,7 +13757,9 @@
       <c r="R36" s="96">
         <v>0.5</v>
       </c>
-      <c r="S36" s="96"/>
+      <c r="S36" s="96">
+        <v>0</v>
+      </c>
       <c r="T36" s="5"/>
       <c r="U36" s="85"/>
       <c r="V36" s="85"/>
@@ -13863,7 +13869,9 @@
       <c r="R37" s="97">
         <v>0</v>
       </c>
-      <c r="S37" s="97"/>
+      <c r="S37" s="97">
+        <v>0</v>
+      </c>
       <c r="U37" s="89"/>
       <c r="V37" s="89"/>
       <c r="W37" s="108"/>
@@ -13970,7 +13978,9 @@
       <c r="R38" s="96">
         <v>0.5</v>
       </c>
-      <c r="S38" s="96"/>
+      <c r="S38" s="96">
+        <v>0</v>
+      </c>
       <c r="T38" s="5"/>
       <c r="U38" s="85"/>
       <c r="V38" s="85"/>
@@ -14080,7 +14090,9 @@
       <c r="R39" s="97">
         <v>0</v>
       </c>
-      <c r="S39" s="97"/>
+      <c r="S39" s="97">
+        <v>0</v>
+      </c>
       <c r="U39" s="89"/>
       <c r="V39" s="89"/>
       <c r="W39" s="89"/>
@@ -16333,7 +16345,7 @@
         <v>1</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="E57" s="5">
         <f t="shared" si="18"/>
@@ -16459,7 +16471,7 @@
         <v>1</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="E58" s="5">
         <f t="shared" si="18"/>
@@ -16587,7 +16599,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="87" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="E59" s="89">
         <f t="shared" si="18"/>
@@ -16722,7 +16734,7 @@
         <v>1</v>
       </c>
       <c r="D60" s="87" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="E60" s="89">
         <f t="shared" si="18"/>
@@ -16857,7 +16869,7 @@
         <v>1</v>
       </c>
       <c r="D61" s="87" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="E61" s="89">
         <f t="shared" si="18"/>
@@ -18035,7 +18047,7 @@
         <v>1</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="E69" s="5">
         <f t="shared" si="18"/>
@@ -18198,7 +18210,7 @@
         <v>1</v>
       </c>
       <c r="D70" s="87" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="E70" s="89">
         <f t="shared" si="18"/>
@@ -23316,7 +23328,7 @@
         <v>20</v>
       </c>
       <c r="P110" s="97" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="Q110" s="97">
         <v>1</v>
@@ -23326,7 +23338,7 @@
       </c>
       <c r="S110" s="97"/>
       <c r="T110" s="89" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="U110" s="89">
         <v>5</v>
@@ -23336,7 +23348,7 @@
       </c>
       <c r="W110" s="89"/>
       <c r="X110" s="97" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="Y110" s="97">
         <v>10</v>
@@ -23397,7 +23409,7 @@
         <v>1</v>
       </c>
       <c r="D111" s="87" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="E111" s="89">
         <f t="shared" si="35"/>
@@ -23449,7 +23461,7 @@
         <v>0</v>
       </c>
       <c r="T111" s="89" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="U111" s="89">
         <v>40</v>
@@ -26804,7 +26816,7 @@
         <v>1</v>
       </c>
       <c r="D140" s="87" t="s">
-        <v>877</v>
+        <v>932</v>
       </c>
       <c r="E140" s="89">
         <f t="shared" si="55"/>
@@ -26963,7 +26975,7 @@
         <v>1</v>
       </c>
       <c r="D141" s="87" t="s">
-        <v>878</v>
+        <v>933</v>
       </c>
       <c r="E141" s="89">
         <f t="shared" si="55"/>
@@ -27122,7 +27134,7 @@
         <v>1</v>
       </c>
       <c r="D142" s="87" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="E142" s="89">
         <f t="shared" si="55"/>
@@ -27255,7 +27267,7 @@
         <v>1</v>
       </c>
       <c r="D143" s="87" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="E143" s="89">
         <f t="shared" si="55"/>
@@ -27388,7 +27400,7 @@
         <v>1</v>
       </c>
       <c r="D144" s="87" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="E144" s="89">
         <f t="shared" ref="E144:E145" si="68">inp_Uc/inp_Un</f>
@@ -27508,7 +27520,7 @@
         <v>1</v>
       </c>
       <c r="D145" s="87" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="E145" s="89">
         <f t="shared" si="68"/>
@@ -27629,7 +27641,7 @@
         <v>1</v>
       </c>
       <c r="D146" s="87" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="E146" s="89">
         <f t="shared" ref="E146:E178" si="70">inp_Uc/inp_Un</f>
@@ -27730,7 +27742,7 @@
         <v>1</v>
       </c>
       <c r="D147" s="87" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="E147" s="89">
         <f t="shared" si="70"/>
@@ -27832,7 +27844,7 @@
         <v>1</v>
       </c>
       <c r="D148" s="87" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="E148" s="89">
         <f t="shared" si="70"/>
@@ -27933,7 +27945,7 @@
         <v>1</v>
       </c>
       <c r="D149" s="87" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="E149" s="89">
         <f t="shared" si="70"/>
@@ -28036,7 +28048,7 @@
         <v>1</v>
       </c>
       <c r="D150" s="87" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="E150" s="89">
         <f t="shared" si="70"/>
@@ -28137,7 +28149,7 @@
         <v>1</v>
       </c>
       <c r="D151" s="87" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="E151" s="89">
         <f t="shared" si="70"/>
@@ -28240,7 +28252,7 @@
         <v>1</v>
       </c>
       <c r="D152" s="87" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="E152" s="89">
         <f t="shared" si="70"/>
@@ -28273,7 +28285,7 @@
         <v>10</v>
       </c>
       <c r="N152" s="91" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="O152" s="109">
         <v>12</v>
@@ -28330,7 +28342,7 @@
         <v>1</v>
       </c>
       <c r="D153" s="87" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="E153" s="89">
         <f t="shared" si="70"/>
@@ -28363,7 +28375,7 @@
         <v>20</v>
       </c>
       <c r="N153" s="91" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="O153" s="109">
         <v>12</v>
@@ -28412,7 +28424,7 @@
         <v>1</v>
       </c>
       <c r="D154" s="87" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="E154" s="89">
         <f t="shared" si="70"/>
@@ -28445,7 +28457,7 @@
         <v>10</v>
       </c>
       <c r="N154" s="91" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="O154" s="109">
         <v>12</v>
@@ -28492,7 +28504,7 @@
         <v>1</v>
       </c>
       <c r="D155" s="87" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="E155" s="89">
         <f t="shared" si="70"/>
@@ -28525,7 +28537,7 @@
         <v>20</v>
       </c>
       <c r="N155" s="91" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="O155" s="109">
         <v>12</v>
@@ -28566,7 +28578,7 @@
         <v>1</v>
       </c>
       <c r="D156" s="87" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="E156" s="89">
         <f t="shared" si="70"/>
@@ -28599,7 +28611,7 @@
         <v>10</v>
       </c>
       <c r="N156" s="91" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="O156" s="109">
         <v>12</v>
@@ -28640,7 +28652,7 @@
         <v>1</v>
       </c>
       <c r="D157" s="87" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E157" s="89">
         <f t="shared" si="70"/>
@@ -28673,7 +28685,7 @@
         <v>20</v>
       </c>
       <c r="N157" s="91" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="O157" s="109">
         <v>12</v>
@@ -28714,7 +28726,7 @@
         <v>1</v>
       </c>
       <c r="D158" s="87" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E158" s="89">
         <f t="shared" si="70"/>
@@ -28747,7 +28759,7 @@
         <v>10</v>
       </c>
       <c r="N158" s="91" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="O158" s="109">
         <v>12</v>
@@ -28788,7 +28800,7 @@
         <v>1</v>
       </c>
       <c r="D159" s="87" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E159" s="89">
         <f t="shared" si="70"/>
@@ -28821,7 +28833,7 @@
         <v>20</v>
       </c>
       <c r="N159" s="91" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="O159" s="109">
         <v>12</v>
@@ -28862,7 +28874,7 @@
         <v>1</v>
       </c>
       <c r="D160" s="87" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="E160" s="89">
         <f t="shared" si="70"/>
@@ -28936,7 +28948,7 @@
         <v>1</v>
       </c>
       <c r="D161" s="87" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E161" s="89">
         <f t="shared" si="70"/>
@@ -29010,7 +29022,7 @@
         <v>1</v>
       </c>
       <c r="D162" s="87" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="E162" s="89">
         <f t="shared" si="70"/>
@@ -29084,7 +29096,7 @@
         <v>1</v>
       </c>
       <c r="D163" s="87" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="E163" s="89">
         <f t="shared" si="70"/>
@@ -29158,7 +29170,7 @@
         <v>1</v>
       </c>
       <c r="D164" s="87" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="E164" s="89">
         <f t="shared" si="70"/>
@@ -29265,7 +29277,7 @@
         <v>1</v>
       </c>
       <c r="D165" s="87" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="E165" s="89">
         <f t="shared" si="70"/>
@@ -29372,7 +29384,7 @@
         <v>1</v>
       </c>
       <c r="D166" s="87" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="E166" s="89">
         <f t="shared" si="70"/>
@@ -29478,7 +29490,7 @@
         <v>1</v>
       </c>
       <c r="D167" s="87" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="E167" s="89">
         <f t="shared" si="70"/>
@@ -29584,7 +29596,7 @@
         <v>1</v>
       </c>
       <c r="D168" s="87" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="E168" s="89">
         <f t="shared" si="70"/>
@@ -29762,7 +29774,7 @@
         <v>1</v>
       </c>
       <c r="D169" s="87" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="E169" s="89">
         <f t="shared" si="70"/>
@@ -29940,7 +29952,7 @@
         <v>1</v>
       </c>
       <c r="D170" s="87" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="E170" s="89">
         <f t="shared" si="70"/>
@@ -30047,7 +30059,7 @@
         <v>1</v>
       </c>
       <c r="D171" s="87" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="E171" s="89">
         <f t="shared" si="70"/>
@@ -30154,7 +30166,7 @@
         <v>1</v>
       </c>
       <c r="D172" s="87" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="E172" s="89">
         <f t="shared" si="70"/>
@@ -30261,7 +30273,7 @@
         <v>1</v>
       </c>
       <c r="D173" s="87" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="E173" s="89">
         <f t="shared" si="70"/>
@@ -30368,7 +30380,7 @@
         <v>1</v>
       </c>
       <c r="D174" s="87" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="E174" s="89">
         <f t="shared" si="70"/>
@@ -30473,7 +30485,7 @@
         <v>1</v>
       </c>
       <c r="D175" s="87" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="E175" s="89">
         <f t="shared" si="70"/>
@@ -30578,7 +30590,7 @@
         <v>1</v>
       </c>
       <c r="D176" s="87" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="E176" s="89">
         <f t="shared" si="70"/>
@@ -30716,7 +30728,7 @@
         <v>1</v>
       </c>
       <c r="D177" s="87" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="E177" s="89">
         <f t="shared" si="70"/>
@@ -30853,7 +30865,7 @@
         <v>1</v>
       </c>
       <c r="D178" s="87" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="E178" s="89">
         <f t="shared" si="70"/>
@@ -30886,7 +30898,7 @@
         <v>10</v>
       </c>
       <c r="N178" s="91" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="O178" s="109">
         <v>60</v>
@@ -50352,13 +50364,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="113" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="B3" s="113" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="C3" s="113" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D3" s="113" t="s">
         <v>140</v>
@@ -50392,13 +50404,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="113" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="B5" s="113" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C5" s="113" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="D5" s="113" t="s">
         <v>14</v>
@@ -53434,6 +53446,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C163:C176"/>
+    <mergeCell ref="C61:C70"/>
+    <mergeCell ref="C71:C94"/>
+    <mergeCell ref="C95:C98"/>
+    <mergeCell ref="C99:C108"/>
+    <mergeCell ref="C109:C115"/>
+    <mergeCell ref="C116:C162"/>
     <mergeCell ref="C58:C60"/>
     <mergeCell ref="C54:C57"/>
     <mergeCell ref="C2:C11"/>
@@ -53441,13 +53460,6 @@
     <mergeCell ref="C18:C28"/>
     <mergeCell ref="C44:C53"/>
     <mergeCell ref="C29:C43"/>
-    <mergeCell ref="C163:C176"/>
-    <mergeCell ref="C61:C70"/>
-    <mergeCell ref="C71:C94"/>
-    <mergeCell ref="C95:C98"/>
-    <mergeCell ref="C99:C108"/>
-    <mergeCell ref="C109:C115"/>
-    <mergeCell ref="C116:C162"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -54224,15 +54236,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="107e75b3-53cc-4838-92d2-ebc011bd4832">
@@ -54241,6 +54244,15 @@
     <TaxCatchAll xmlns="888ccf44-0d39-41a2-ab17-f7efb2bf6977" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -54263,14 +54275,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2288FB7-E85A-4FE8-9E7A-FE572FF16064}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -54285,4 +54289,12 @@
     <ds:schemaRef ds:uri="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update test cases in testcases.xlsx to reflect recent changes in guide functions
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/prw_energinet_dk/Documents/Dokumenter/GitHub/MTB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A3B8C97-895B-41DC-8C6D-58B636181CF3}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{509DD12B-C63D-4EFD-BF07-6F01ED60C84D}"/>
   <bookViews>
-    <workbookView xWindow="20790" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17610" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -5772,7 +5772,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -9408,14 +9408,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor rgb="FF00847C"/>
   </sheetPr>
   <dimension ref="A1:CQ218"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P39" sqref="P39"/>
+      <pane ySplit="2" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D171" sqref="D171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -9781,7 +9781,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -9885,7 +9885,7 @@
       <c r="BN3" s="96"/>
       <c r="BO3" s="96"/>
     </row>
-    <row r="4" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -9989,7 +9989,7 @@
       <c r="BN4" s="96"/>
       <c r="BO4" s="96"/>
     </row>
-    <row r="5" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -10093,7 +10093,7 @@
       <c r="BN5" s="96"/>
       <c r="BO5" s="96"/>
     </row>
-    <row r="6" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -10197,7 +10197,7 @@
       <c r="BN6" s="96"/>
       <c r="BO6" s="96"/>
     </row>
-    <row r="7" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -10301,7 +10301,7 @@
       <c r="BN7" s="96"/>
       <c r="BO7" s="96"/>
     </row>
-    <row r="8" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -10405,7 +10405,7 @@
       <c r="BN8" s="96"/>
       <c r="BO8" s="96"/>
     </row>
-    <row r="9" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -10508,7 +10508,7 @@
       <c r="BN9" s="96"/>
       <c r="BO9" s="96"/>
     </row>
-    <row r="10" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -10611,7 +10611,7 @@
       <c r="BN10" s="96"/>
       <c r="BO10" s="96"/>
     </row>
-    <row r="11" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -10715,7 +10715,7 @@
       <c r="BN11" s="96"/>
       <c r="BO11" s="96"/>
     </row>
-    <row r="12" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -10819,7 +10819,7 @@
       <c r="BN12" s="96"/>
       <c r="BO12" s="96"/>
     </row>
-    <row r="13" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -10930,7 +10930,7 @@
       <c r="BN13" s="96"/>
       <c r="BO13" s="96"/>
     </row>
-    <row r="14" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -11041,7 +11041,7 @@
       <c r="BN14" s="96"/>
       <c r="BO14" s="96"/>
     </row>
-    <row r="15" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -11152,7 +11152,7 @@
       <c r="BN15" s="96"/>
       <c r="BO15" s="96"/>
     </row>
-    <row r="16" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -11263,7 +11263,7 @@
       <c r="BN16" s="96"/>
       <c r="BO16" s="96"/>
     </row>
-    <row r="17" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -11374,7 +11374,7 @@
       <c r="BN17" s="96"/>
       <c r="BO17" s="96"/>
     </row>
-    <row r="18" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -11485,7 +11485,7 @@
       <c r="BN18" s="96"/>
       <c r="BO18" s="96"/>
     </row>
-    <row r="19" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -11614,7 +11614,7 @@
       <c r="BN19" s="96"/>
       <c r="BO19" s="96"/>
     </row>
-    <row r="20" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -11745,7 +11745,7 @@
       <c r="BN20" s="97"/>
       <c r="BO20" s="97"/>
     </row>
-    <row r="21" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -11878,7 +11878,7 @@
       <c r="BN21" s="96"/>
       <c r="BO21" s="96"/>
     </row>
-    <row r="22" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -12012,7 +12012,7 @@
       <c r="BN22" s="96"/>
       <c r="BO22" s="96"/>
     </row>
-    <row r="23" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -12146,7 +12146,7 @@
       <c r="BN23" s="96"/>
       <c r="BO23" s="96"/>
     </row>
-    <row r="24" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -12280,7 +12280,7 @@
       <c r="BN24" s="96"/>
       <c r="BO24" s="96"/>
     </row>
-    <row r="25" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -12414,7 +12414,7 @@
       <c r="BN25" s="96"/>
       <c r="BO25" s="96"/>
     </row>
-    <row r="26" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -12558,7 +12558,7 @@
       <c r="BN26" s="96"/>
       <c r="BO26" s="96"/>
     </row>
-    <row r="27" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -12702,7 +12702,7 @@
       <c r="BN27" s="96"/>
       <c r="BO27" s="96"/>
     </row>
-    <row r="28" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -12819,7 +12819,7 @@
       <c r="BN28" s="96"/>
       <c r="BO28" s="96"/>
     </row>
-    <row r="29" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -12936,7 +12936,7 @@
       <c r="BN29" s="96"/>
       <c r="BO29" s="96"/>
     </row>
-    <row r="30" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -13064,7 +13064,7 @@
       <c r="BN30" s="96"/>
       <c r="BO30" s="96"/>
     </row>
-    <row r="31" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -13194,7 +13194,7 @@
       <c r="BN31" s="97"/>
       <c r="BO31" s="97"/>
     </row>
-    <row r="32" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -13322,7 +13322,7 @@
       <c r="BN32" s="96"/>
       <c r="BO32" s="96"/>
     </row>
-    <row r="33" spans="1:95" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -13450,7 +13450,7 @@
       <c r="BN33" s="96"/>
       <c r="BO33" s="96"/>
     </row>
-    <row r="34" spans="1:95" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:95" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -13588,7 +13588,7 @@
       <c r="CP34" s="1"/>
       <c r="CQ34" s="1"/>
     </row>
-    <row r="35" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -13699,7 +13699,7 @@
       <c r="BN35" s="97"/>
       <c r="BO35" s="97"/>
     </row>
-    <row r="36" spans="1:95" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -13809,7 +13809,7 @@
       <c r="BN36" s="96"/>
       <c r="BO36" s="96"/>
     </row>
-    <row r="37" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -13920,7 +13920,7 @@
       <c r="BN37" s="97"/>
       <c r="BO37" s="97"/>
     </row>
-    <row r="38" spans="1:95" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -14030,7 +14030,7 @@
       <c r="BN38" s="96"/>
       <c r="BO38" s="96"/>
     </row>
-    <row r="39" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -14987,7 +14987,7 @@
       <c r="BN44" s="96"/>
       <c r="BO44" s="96"/>
     </row>
-    <row r="45" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -15096,7 +15096,7 @@
       <c r="BN45" s="97"/>
       <c r="BO45" s="97"/>
     </row>
-    <row r="46" spans="1:95" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -15205,7 +15205,7 @@
       <c r="BN46" s="96"/>
       <c r="BO46" s="96"/>
     </row>
-    <row r="47" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -15314,7 +15314,7 @@
       <c r="BN47" s="97"/>
       <c r="BO47" s="97"/>
     </row>
-    <row r="48" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -15423,7 +15423,7 @@
       <c r="BN48" s="97"/>
       <c r="BO48" s="97"/>
     </row>
-    <row r="49" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -15532,7 +15532,7 @@
       <c r="BN49" s="97"/>
       <c r="BO49" s="97"/>
     </row>
-    <row r="50" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -15642,7 +15642,7 @@
       <c r="BN50" s="97"/>
       <c r="BO50" s="97"/>
     </row>
-    <row r="51" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -15752,7 +15752,7 @@
       <c r="BN51" s="97"/>
       <c r="BO51" s="97"/>
     </row>
-    <row r="52" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -15862,7 +15862,7 @@
       <c r="BN52" s="97"/>
       <c r="BO52" s="97"/>
     </row>
-    <row r="53" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -15972,7 +15972,7 @@
       <c r="BN53" s="97"/>
       <c r="BO53" s="97"/>
     </row>
-    <row r="54" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -16082,7 +16082,7 @@
       <c r="BN54" s="97"/>
       <c r="BO54" s="97"/>
     </row>
-    <row r="55" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -16208,7 +16208,7 @@
       <c r="BN55" s="96"/>
       <c r="BO55" s="96"/>
     </row>
-    <row r="56" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -16334,7 +16334,7 @@
       <c r="BN56" s="96"/>
       <c r="BO56" s="96"/>
     </row>
-    <row r="57" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -16460,7 +16460,7 @@
       <c r="BN57" s="96"/>
       <c r="BO57" s="96"/>
     </row>
-    <row r="58" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -16586,7 +16586,7 @@
       <c r="BN58" s="96"/>
       <c r="BO58" s="96"/>
     </row>
-    <row r="59" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -16721,7 +16721,7 @@
       <c r="BN59" s="97"/>
       <c r="BO59" s="97"/>
     </row>
-    <row r="60" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -16856,7 +16856,7 @@
       <c r="BN60" s="97"/>
       <c r="BO60" s="97"/>
     </row>
-    <row r="61" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -16994,7 +16994,7 @@
       <c r="BN61" s="97"/>
       <c r="BO61" s="97"/>
     </row>
-    <row r="62" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -17121,7 +17121,7 @@
       <c r="BN62" s="96"/>
       <c r="BO62" s="96"/>
     </row>
-    <row r="63" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -17265,7 +17265,7 @@
       <c r="BN63" s="96"/>
       <c r="BO63" s="96"/>
     </row>
-    <row r="64" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -17408,7 +17408,7 @@
       <c r="BN64" s="96"/>
       <c r="BO64" s="96"/>
     </row>
-    <row r="65" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -17585,7 +17585,7 @@
       <c r="BN65" s="96"/>
       <c r="BO65" s="96"/>
     </row>
-    <row r="66" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -17730,7 +17730,7 @@
       <c r="BN66" s="96"/>
       <c r="BO66" s="96"/>
     </row>
-    <row r="67" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -17875,7 +17875,7 @@
       <c r="BN67" s="96"/>
       <c r="BO67" s="96"/>
     </row>
-    <row r="68" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -18036,7 +18036,7 @@
       <c r="BN68" s="96"/>
       <c r="BO68" s="96"/>
     </row>
-    <row r="69" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -18197,7 +18197,7 @@
       <c r="BN69" s="96"/>
       <c r="BO69" s="96"/>
     </row>
-    <row r="70" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -18348,7 +18348,7 @@
       <c r="BN70" s="96"/>
       <c r="BO70" s="96"/>
     </row>
-    <row r="71" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -18473,7 +18473,7 @@
       <c r="BN71" s="97"/>
       <c r="BO71" s="97"/>
     </row>
-    <row r="72" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -18590,7 +18590,7 @@
       <c r="BN72" s="96"/>
       <c r="BO72" s="96"/>
     </row>
-    <row r="73" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -18701,7 +18701,7 @@
       <c r="BN73" s="96"/>
       <c r="BO73" s="96"/>
     </row>
-    <row r="74" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -18812,7 +18812,7 @@
       <c r="BN74" s="96"/>
       <c r="BO74" s="96"/>
     </row>
-    <row r="75" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -18923,7 +18923,7 @@
       <c r="BN75" s="96"/>
       <c r="BO75" s="96"/>
     </row>
-    <row r="76" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -19034,7 +19034,7 @@
       <c r="BN76" s="96"/>
       <c r="BO76" s="96"/>
     </row>
-    <row r="77" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -19146,7 +19146,7 @@
       <c r="BN77" s="96"/>
       <c r="BO77" s="96"/>
     </row>
-    <row r="78" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -19263,7 +19263,7 @@
       <c r="BN78" s="96"/>
       <c r="BO78" s="96"/>
     </row>
-    <row r="79" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -19374,7 +19374,7 @@
       <c r="BN79" s="96"/>
       <c r="BO79" s="96"/>
     </row>
-    <row r="80" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -19485,7 +19485,7 @@
       <c r="BN80" s="96"/>
       <c r="BO80" s="96"/>
     </row>
-    <row r="81" spans="1:95" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -19596,7 +19596,7 @@
       <c r="BN81" s="96"/>
       <c r="BO81" s="96"/>
     </row>
-    <row r="82" spans="1:95" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:95" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -19735,7 +19735,7 @@
       <c r="CP82" s="1"/>
       <c r="CQ82" s="1"/>
     </row>
-    <row r="83" spans="1:95" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:95" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -19875,7 +19875,7 @@
       <c r="CP83" s="1"/>
       <c r="CQ83" s="1"/>
     </row>
-    <row r="84" spans="1:95" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:95" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -20020,7 +20020,7 @@
       <c r="CP84" s="1"/>
       <c r="CQ84" s="1"/>
     </row>
-    <row r="85" spans="1:95" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -20131,7 +20131,7 @@
       <c r="BN85" s="106"/>
       <c r="BO85" s="106"/>
     </row>
-    <row r="86" spans="1:95" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -20242,7 +20242,7 @@
       <c r="BN86" s="96"/>
       <c r="BO86" s="96"/>
     </row>
-    <row r="87" spans="1:95" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -20353,7 +20353,7 @@
       <c r="BN87" s="96"/>
       <c r="BO87" s="96"/>
     </row>
-    <row r="88" spans="1:95" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -20464,7 +20464,7 @@
       <c r="BN88" s="96"/>
       <c r="BO88" s="96"/>
     </row>
-    <row r="89" spans="1:95" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -20576,7 +20576,7 @@
       <c r="BN89" s="96"/>
       <c r="BO89" s="96"/>
     </row>
-    <row r="90" spans="1:95" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -20701,7 +20701,7 @@
       <c r="BN90" s="96"/>
       <c r="BO90" s="96"/>
     </row>
-    <row r="91" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -20840,7 +20840,7 @@
       <c r="BN91" s="97"/>
       <c r="BO91" s="97"/>
     </row>
-    <row r="92" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -20962,7 +20962,7 @@
       <c r="BN92" s="97"/>
       <c r="BO92" s="97"/>
     </row>
-    <row r="93" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -21084,7 +21084,7 @@
       <c r="BN93" s="97"/>
       <c r="BO93" s="97"/>
     </row>
-    <row r="94" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -21208,7 +21208,7 @@
       <c r="BN94" s="97"/>
       <c r="BO94" s="97"/>
     </row>
-    <row r="95" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -21332,7 +21332,7 @@
       <c r="BN95" s="97"/>
       <c r="BO95" s="97"/>
     </row>
-    <row r="96" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -21487,7 +21487,7 @@
       <c r="BN96" s="97"/>
       <c r="BO96" s="97"/>
     </row>
-    <row r="97" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -21614,7 +21614,7 @@
       <c r="BN97" s="97"/>
       <c r="BO97" s="97"/>
     </row>
-    <row r="98" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -21726,7 +21726,7 @@
       <c r="BN98" s="97"/>
       <c r="BO98" s="97"/>
     </row>
-    <row r="99" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -21860,7 +21860,7 @@
       <c r="BN99" s="97"/>
       <c r="BO99" s="97"/>
     </row>
-    <row r="100" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -23275,7 +23275,7 @@
       <c r="BN109" s="97"/>
       <c r="BO109" s="97"/>
     </row>
-    <row r="110" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -23396,7 +23396,7 @@
       <c r="BN110" s="97"/>
       <c r="BO110" s="97"/>
     </row>
-    <row r="111" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -23515,7 +23515,7 @@
       <c r="BN111" s="97"/>
       <c r="BO111" s="97"/>
     </row>
-    <row r="112" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -23640,7 +23640,7 @@
       <c r="BN112" s="97"/>
       <c r="BO112" s="97"/>
     </row>
-    <row r="113" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -23778,7 +23778,7 @@
       <c r="BN113" s="97"/>
       <c r="BO113" s="97"/>
     </row>
-    <row r="114" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -23916,7 +23916,7 @@
       <c r="BN114" s="97"/>
       <c r="BO114" s="97"/>
     </row>
-    <row r="115" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -24088,7 +24088,7 @@
       <c r="BN115" s="97"/>
       <c r="BO115" s="97"/>
     </row>
-    <row r="116" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -24260,7 +24260,7 @@
       <c r="BN116" s="97"/>
       <c r="BO116" s="97"/>
     </row>
-    <row r="117" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -24374,7 +24374,7 @@
       <c r="BN117" s="97"/>
       <c r="BO117" s="97"/>
     </row>
-    <row r="118" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -24482,7 +24482,7 @@
       <c r="BN118" s="97"/>
       <c r="BO118" s="97"/>
     </row>
-    <row r="119" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -24590,7 +24590,7 @@
       <c r="BN119" s="97"/>
       <c r="BO119" s="97"/>
     </row>
-    <row r="120" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -24698,7 +24698,7 @@
       <c r="BN120" s="97"/>
       <c r="BO120" s="97"/>
     </row>
-    <row r="121" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -24806,7 +24806,7 @@
       <c r="BN121" s="97"/>
       <c r="BO121" s="97"/>
     </row>
-    <row r="122" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -24915,7 +24915,7 @@
       <c r="BN122" s="97"/>
       <c r="BO122" s="97"/>
     </row>
-    <row r="123" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -25023,7 +25023,7 @@
       <c r="BN123" s="97"/>
       <c r="BO123" s="97"/>
     </row>
-    <row r="124" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -25131,7 +25131,7 @@
       <c r="BN124" s="97"/>
       <c r="BO124" s="97"/>
     </row>
-    <row r="125" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -25239,7 +25239,7 @@
       <c r="BN125" s="97"/>
       <c r="BO125" s="97"/>
     </row>
-    <row r="126" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -25347,7 +25347,7 @@
       <c r="BN126" s="97"/>
       <c r="BO126" s="97"/>
     </row>
-    <row r="127" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -25455,7 +25455,7 @@
       <c r="BN127" s="97"/>
       <c r="BO127" s="97"/>
     </row>
-    <row r="128" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -25563,7 +25563,7 @@
       <c r="BN128" s="97"/>
       <c r="BO128" s="97"/>
     </row>
-    <row r="129" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -25671,7 +25671,7 @@
       <c r="BN129" s="97"/>
       <c r="BO129" s="97"/>
     </row>
-    <row r="130" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -25779,7 +25779,7 @@
       <c r="BN130" s="97"/>
       <c r="BO130" s="97"/>
     </row>
-    <row r="131" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -25899,7 +25899,7 @@
       <c r="BN131" s="97"/>
       <c r="BO131" s="97"/>
     </row>
-    <row r="132" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -26019,7 +26019,7 @@
       <c r="BN132" s="97"/>
       <c r="BO132" s="97"/>
     </row>
-    <row r="133" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -26129,7 +26129,7 @@
       <c r="BN133" s="97"/>
       <c r="BO133" s="97"/>
     </row>
-    <row r="134" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -26238,7 +26238,7 @@
       <c r="BN134" s="97"/>
       <c r="BO134" s="97"/>
     </row>
-    <row r="135" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -26347,7 +26347,7 @@
       <c r="BN135" s="97"/>
       <c r="BO135" s="97"/>
     </row>
-    <row r="136" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -26465,7 +26465,7 @@
       <c r="BN136" s="97"/>
       <c r="BO136" s="97"/>
     </row>
-    <row r="137" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -26593,7 +26593,7 @@
       <c r="BN137" s="97"/>
       <c r="BO137" s="97"/>
     </row>
-    <row r="138" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -26698,7 +26698,7 @@
       <c r="BN138" s="97"/>
       <c r="BO138" s="97"/>
     </row>
-    <row r="139" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -26803,7 +26803,7 @@
       <c r="BN139" s="97"/>
       <c r="BO139" s="97"/>
     </row>
-    <row r="140" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -26962,7 +26962,7 @@
       <c r="BN140" s="97"/>
       <c r="BO140" s="97"/>
     </row>
-    <row r="141" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -27121,7 +27121,7 @@
       <c r="BN141" s="97"/>
       <c r="BO141" s="97"/>
     </row>
-    <row r="142" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -27254,7 +27254,7 @@
       <c r="BN142" s="97"/>
       <c r="BO142" s="97"/>
     </row>
-    <row r="143" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -27387,7 +27387,7 @@
       <c r="BN143" s="97"/>
       <c r="BO143" s="97"/>
     </row>
-    <row r="144" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -27507,7 +27507,7 @@
       <c r="BN144" s="97"/>
       <c r="BO144" s="97"/>
     </row>
-    <row r="145" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -27628,7 +27628,7 @@
       <c r="BN145" s="97"/>
       <c r="BO145" s="97"/>
     </row>
-    <row r="146" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -27729,7 +27729,7 @@
       <c r="BN146" s="97"/>
       <c r="BO146" s="97"/>
     </row>
-    <row r="147" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -27831,7 +27831,7 @@
       <c r="BN147" s="97"/>
       <c r="BO147" s="97"/>
     </row>
-    <row r="148" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -27932,7 +27932,7 @@
       <c r="BN148" s="97"/>
       <c r="BO148" s="97"/>
     </row>
-    <row r="149" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -28035,7 +28035,7 @@
       <c r="BN149" s="97"/>
       <c r="BO149" s="97"/>
     </row>
-    <row r="150" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -28136,7 +28136,7 @@
       <c r="BN150" s="97"/>
       <c r="BO150" s="97"/>
     </row>
-    <row r="151" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -28239,7 +28239,7 @@
       <c r="BN151" s="97"/>
       <c r="BO151" s="97"/>
     </row>
-    <row r="152" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -28329,7 +28329,7 @@
       <c r="BN152" s="96"/>
       <c r="BO152" s="96"/>
     </row>
-    <row r="153" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -28411,7 +28411,7 @@
       <c r="BN153" s="96"/>
       <c r="BO153" s="96"/>
     </row>
-    <row r="154" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -28491,7 +28491,7 @@
       <c r="BN154" s="96"/>
       <c r="BO154" s="96"/>
     </row>
-    <row r="155" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -28565,7 +28565,7 @@
       <c r="AH155" s="96"/>
       <c r="AI155" s="96"/>
     </row>
-    <row r="156" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -28639,7 +28639,7 @@
       <c r="AH156" s="96"/>
       <c r="AI156" s="96"/>
     </row>
-    <row r="157" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -28713,7 +28713,7 @@
       <c r="AH157" s="96"/>
       <c r="AI157" s="96"/>
     </row>
-    <row r="158" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -28787,7 +28787,7 @@
       <c r="AH158" s="96"/>
       <c r="AI158" s="96"/>
     </row>
-    <row r="159" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -28861,7 +28861,7 @@
       <c r="AH159" s="96"/>
       <c r="AI159" s="96"/>
     </row>
-    <row r="160" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -28935,7 +28935,7 @@
       <c r="AH160" s="96"/>
       <c r="AI160" s="96"/>
     </row>
-    <row r="161" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -29009,7 +29009,7 @@
       <c r="AH161" s="96"/>
       <c r="AI161" s="96"/>
     </row>
-    <row r="162" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -29083,7 +29083,7 @@
       <c r="AH162" s="96"/>
       <c r="AI162" s="96"/>
     </row>
-    <row r="163" spans="1:67" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -29157,7 +29157,7 @@
       <c r="AH163" s="96"/>
       <c r="AI163" s="96"/>
     </row>
-    <row r="164" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -29264,7 +29264,7 @@
       <c r="BN164" s="124"/>
       <c r="BO164" s="124"/>
     </row>
-    <row r="165" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -29371,7 +29371,7 @@
       <c r="BN165" s="124"/>
       <c r="BO165" s="124"/>
     </row>
-    <row r="166" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -29477,7 +29477,7 @@
       <c r="BN166" s="124"/>
       <c r="BO166" s="124"/>
     </row>
-    <row r="167" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -29583,7 +29583,7 @@
       <c r="BN167" s="124"/>
       <c r="BO167" s="124"/>
     </row>
-    <row r="168" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -29761,7 +29761,7 @@
       <c r="BN168" s="124"/>
       <c r="BO168" s="124"/>
     </row>
-    <row r="169" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -29939,7 +29939,7 @@
       <c r="BN169" s="124"/>
       <c r="BO169" s="124"/>
     </row>
-    <row r="170" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -30046,7 +30046,7 @@
       <c r="BN170" s="124"/>
       <c r="BO170" s="124"/>
     </row>
-    <row r="171" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -30153,7 +30153,7 @@
       <c r="BN171" s="124"/>
       <c r="BO171" s="124"/>
     </row>
-    <row r="172" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -30260,7 +30260,7 @@
       <c r="BN172" s="124"/>
       <c r="BO172" s="124"/>
     </row>
-    <row r="173" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -30367,7 +30367,7 @@
       <c r="BN173" s="124"/>
       <c r="BO173" s="124"/>
     </row>
-    <row r="174" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -30472,7 +30472,7 @@
       <c r="BN174" s="124"/>
       <c r="BO174" s="124"/>
     </row>
-    <row r="175" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -30577,7 +30577,7 @@
       <c r="BN175" s="124"/>
       <c r="BO175" s="124"/>
     </row>
-    <row r="176" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -30715,7 +30715,7 @@
       <c r="BN176" s="124"/>
       <c r="BO176" s="124"/>
     </row>
-    <row r="177" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -30852,7 +30852,7 @@
       <c r="BN177" s="124"/>
       <c r="BO177" s="124"/>
     </row>
-    <row r="178" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -31334,7 +31334,26 @@
       <c r="O218" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:BK178" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A2:BK178" xr:uid="{00000000-0009-0000-0000-000002000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="RfG_Ucontrol_Fault"/>
+        <filter val="RfG_Ucontrol_Fault_FRTlimit"/>
+        <filter val="RfG_Ucontrol_FRTsensitivity"/>
+        <filter val="RfG_Ucontrol_FRTsensitivity-ramp"/>
+        <filter val="RfG_Ucontrol_LFSM-O"/>
+        <filter val="RfG_Ucontrol_Phasejump"/>
+        <filter val="RfG_Ucontrol_rec"/>
+        <filter val="RfG_Ucontrol_Scmax"/>
+        <filter val="RfG_Ucontrol_Scmin"/>
+        <filter val="RfG_Ucontrol_Scmin_Droop_2"/>
+        <filter val="RfG_Ucontrol_Scmin_Droop_4"/>
+        <filter val="RfG_Ucontrol_Scmin_Droop_7"/>
+        <filter val="RfG_Ucontrol_SCR"/>
+        <filter val="RfG_Ucontrol_Sctune"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="15">
     <mergeCell ref="BL1:BO1"/>
     <mergeCell ref="A1:D1"/>
@@ -31360,7 +31379,7 @@
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>datavalidation!$E$1:$E$2</xm:f>
@@ -53446,6 +53465,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="C18:C28"/>
+    <mergeCell ref="C44:C53"/>
+    <mergeCell ref="C29:C43"/>
     <mergeCell ref="C163:C176"/>
     <mergeCell ref="C61:C70"/>
     <mergeCell ref="C71:C94"/>
@@ -53453,13 +53479,6 @@
     <mergeCell ref="C99:C108"/>
     <mergeCell ref="C109:C115"/>
     <mergeCell ref="C116:C162"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="C18:C28"/>
-    <mergeCell ref="C44:C53"/>
-    <mergeCell ref="C29:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -53987,6 +54006,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="107e75b3-53cc-4838-92d2-ebc011bd4832">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="888ccf44-0d39-41a2-ab17-f7efb2bf6977" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004FD8CECCB51EC843BF514AFE68379818" ma:contentTypeVersion="18" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="eda339f53f012ceb64677667a741b441">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="107e75b3-53cc-4838-92d2-ebc011bd4832" xmlns:ns3="888ccf44-0d39-41a2-ab17-f7efb2bf6977" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04a86f3db711706e561c315688f1c464" ns2:_="" ns3:_="">
     <xsd:import namespace="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
@@ -54235,41 +54274,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="107e75b3-53cc-4838-92d2-ebc011bd4832">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="888ccf44-0d39-41a2-ab17-f7efb2bf6977" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F91B7B9-75FF-4624-B506-952B5B54766C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
-    <ds:schemaRef ds:uri="888ccf44-0d39-41a2-ab17-f7efb2bf6977"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -54292,9 +54300,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F91B7B9-75FF-4624-B506-952B5B54766C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
+    <ds:schemaRef ds:uri="888ccf44-0d39-41a2-ab17-f7efb2bf6977"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update testcases.xlsx to include new test scenarios for guide functions
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/prw_energinet_dk/Documents/Dokumenter/GitHub/MTB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{509DD12B-C63D-4EFD-BF07-6F01ED60C84D}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D55F73F-7687-4A56-9060-6B99955C88B8}"/>
   <bookViews>
     <workbookView xWindow="-17610" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3484,9 +3484,6 @@
     <t>RfG_Qpf_Pref-change</t>
   </si>
   <si>
-    <t>RfG_Qpf_Qref-change</t>
-  </si>
-  <si>
     <t>RfG_proc_Freq_limit_down</t>
   </si>
   <si>
@@ -3515,6 +3512,9 @@
   </si>
   <si>
     <t>RfG_Fault_3_RoCoF_curveUF</t>
+  </si>
+  <si>
+    <t>RfG_Qpf_PFref-change</t>
   </si>
 </sst>
 </file>
@@ -6108,7 +6108,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="291" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B19" s="283" t="b">
         <v>0</v>
@@ -6117,7 +6117,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="293" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -9408,14 +9408,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <tabColor rgb="FF00847C"/>
   </sheetPr>
   <dimension ref="A1:CQ218"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D171" sqref="D171"/>
+      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -9619,7 +9619,7 @@
         <v>100</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>101</v>
@@ -9781,7 +9781,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -9885,7 +9885,7 @@
       <c r="BN3" s="96"/>
       <c r="BO3" s="96"/>
     </row>
-    <row r="4" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -9989,7 +9989,7 @@
       <c r="BN4" s="96"/>
       <c r="BO4" s="96"/>
     </row>
-    <row r="5" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -10093,7 +10093,7 @@
       <c r="BN5" s="96"/>
       <c r="BO5" s="96"/>
     </row>
-    <row r="6" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -10197,7 +10197,7 @@
       <c r="BN6" s="96"/>
       <c r="BO6" s="96"/>
     </row>
-    <row r="7" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -10301,7 +10301,7 @@
       <c r="BN7" s="96"/>
       <c r="BO7" s="96"/>
     </row>
-    <row r="8" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -10405,7 +10405,7 @@
       <c r="BN8" s="96"/>
       <c r="BO8" s="96"/>
     </row>
-    <row r="9" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -10508,7 +10508,7 @@
       <c r="BN9" s="96"/>
       <c r="BO9" s="96"/>
     </row>
-    <row r="10" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -10611,7 +10611,7 @@
       <c r="BN10" s="96"/>
       <c r="BO10" s="96"/>
     </row>
-    <row r="11" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -10715,7 +10715,7 @@
       <c r="BN11" s="96"/>
       <c r="BO11" s="96"/>
     </row>
-    <row r="12" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -10819,7 +10819,7 @@
       <c r="BN12" s="96"/>
       <c r="BO12" s="96"/>
     </row>
-    <row r="13" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -10930,7 +10930,7 @@
       <c r="BN13" s="96"/>
       <c r="BO13" s="96"/>
     </row>
-    <row r="14" spans="1:67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -11041,7 +11041,7 @@
       <c r="BN14" s="96"/>
       <c r="BO14" s="96"/>
     </row>
-    <row r="15" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -11152,7 +11152,7 @@
       <c r="BN15" s="96"/>
       <c r="BO15" s="96"/>
     </row>
-    <row r="16" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -11263,7 +11263,7 @@
       <c r="BN16" s="96"/>
       <c r="BO16" s="96"/>
     </row>
-    <row r="17" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -11374,7 +11374,7 @@
       <c r="BN17" s="96"/>
       <c r="BO17" s="96"/>
     </row>
-    <row r="18" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -11485,7 +11485,7 @@
       <c r="BN18" s="96"/>
       <c r="BO18" s="96"/>
     </row>
-    <row r="19" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -11614,7 +11614,7 @@
       <c r="BN19" s="96"/>
       <c r="BO19" s="96"/>
     </row>
-    <row r="20" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -11745,7 +11745,7 @@
       <c r="BN20" s="97"/>
       <c r="BO20" s="97"/>
     </row>
-    <row r="21" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -11878,7 +11878,7 @@
       <c r="BN21" s="96"/>
       <c r="BO21" s="96"/>
     </row>
-    <row r="22" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -12012,7 +12012,7 @@
       <c r="BN22" s="96"/>
       <c r="BO22" s="96"/>
     </row>
-    <row r="23" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -12146,7 +12146,7 @@
       <c r="BN23" s="96"/>
       <c r="BO23" s="96"/>
     </row>
-    <row r="24" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -12280,7 +12280,7 @@
       <c r="BN24" s="96"/>
       <c r="BO24" s="96"/>
     </row>
-    <row r="25" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -12414,7 +12414,7 @@
       <c r="BN25" s="96"/>
       <c r="BO25" s="96"/>
     </row>
-    <row r="26" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -12558,7 +12558,7 @@
       <c r="BN26" s="96"/>
       <c r="BO26" s="96"/>
     </row>
-    <row r="27" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -12702,7 +12702,7 @@
       <c r="BN27" s="96"/>
       <c r="BO27" s="96"/>
     </row>
-    <row r="28" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -12819,7 +12819,7 @@
       <c r="BN28" s="96"/>
       <c r="BO28" s="96"/>
     </row>
-    <row r="29" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -12936,7 +12936,7 @@
       <c r="BN29" s="96"/>
       <c r="BO29" s="96"/>
     </row>
-    <row r="30" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -13064,7 +13064,7 @@
       <c r="BN30" s="96"/>
       <c r="BO30" s="96"/>
     </row>
-    <row r="31" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -13194,7 +13194,7 @@
       <c r="BN31" s="97"/>
       <c r="BO31" s="97"/>
     </row>
-    <row r="32" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -13322,7 +13322,7 @@
       <c r="BN32" s="96"/>
       <c r="BO32" s="96"/>
     </row>
-    <row r="33" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:95" x14ac:dyDescent="0.4">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -13450,7 +13450,7 @@
       <c r="BN33" s="96"/>
       <c r="BO33" s="96"/>
     </row>
-    <row r="34" spans="1:95" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:95" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -13588,7 +13588,7 @@
       <c r="CP34" s="1"/>
       <c r="CQ34" s="1"/>
     </row>
-    <row r="35" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -13699,7 +13699,7 @@
       <c r="BN35" s="97"/>
       <c r="BO35" s="97"/>
     </row>
-    <row r="36" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:95" x14ac:dyDescent="0.4">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -13809,7 +13809,7 @@
       <c r="BN36" s="96"/>
       <c r="BO36" s="96"/>
     </row>
-    <row r="37" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -13920,7 +13920,7 @@
       <c r="BN37" s="97"/>
       <c r="BO37" s="97"/>
     </row>
-    <row r="38" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:95" x14ac:dyDescent="0.4">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -14030,7 +14030,7 @@
       <c r="BN38" s="96"/>
       <c r="BO38" s="96"/>
     </row>
-    <row r="39" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -14987,7 +14987,7 @@
       <c r="BN44" s="96"/>
       <c r="BO44" s="96"/>
     </row>
-    <row r="45" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -15096,7 +15096,7 @@
       <c r="BN45" s="97"/>
       <c r="BO45" s="97"/>
     </row>
-    <row r="46" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:95" x14ac:dyDescent="0.4">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -15205,7 +15205,7 @@
       <c r="BN46" s="96"/>
       <c r="BO46" s="96"/>
     </row>
-    <row r="47" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -15314,7 +15314,7 @@
       <c r="BN47" s="97"/>
       <c r="BO47" s="97"/>
     </row>
-    <row r="48" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -15423,7 +15423,7 @@
       <c r="BN48" s="97"/>
       <c r="BO48" s="97"/>
     </row>
-    <row r="49" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -15532,7 +15532,7 @@
       <c r="BN49" s="97"/>
       <c r="BO49" s="97"/>
     </row>
-    <row r="50" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -15642,7 +15642,7 @@
       <c r="BN50" s="97"/>
       <c r="BO50" s="97"/>
     </row>
-    <row r="51" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -15752,7 +15752,7 @@
       <c r="BN51" s="97"/>
       <c r="BO51" s="97"/>
     </row>
-    <row r="52" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -15862,7 +15862,7 @@
       <c r="BN52" s="97"/>
       <c r="BO52" s="97"/>
     </row>
-    <row r="53" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -15972,7 +15972,7 @@
       <c r="BN53" s="97"/>
       <c r="BO53" s="97"/>
     </row>
-    <row r="54" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -16082,7 +16082,7 @@
       <c r="BN54" s="97"/>
       <c r="BO54" s="97"/>
     </row>
-    <row r="55" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -16208,7 +16208,7 @@
       <c r="BN55" s="96"/>
       <c r="BO55" s="96"/>
     </row>
-    <row r="56" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -16334,7 +16334,7 @@
       <c r="BN56" s="96"/>
       <c r="BO56" s="96"/>
     </row>
-    <row r="57" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -16345,7 +16345,7 @@
         <v>1</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>923</v>
+        <v>933</v>
       </c>
       <c r="E57" s="5">
         <f t="shared" si="18"/>
@@ -16460,7 +16460,7 @@
       <c r="BN57" s="96"/>
       <c r="BO57" s="96"/>
     </row>
-    <row r="58" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -16586,7 +16586,7 @@
       <c r="BN58" s="96"/>
       <c r="BO58" s="96"/>
     </row>
-    <row r="59" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -16599,7 +16599,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="87" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="E59" s="89">
         <f t="shared" si="18"/>
@@ -16721,7 +16721,7 @@
       <c r="BN59" s="97"/>
       <c r="BO59" s="97"/>
     </row>
-    <row r="60" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -16734,7 +16734,7 @@
         <v>1</v>
       </c>
       <c r="D60" s="87" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E60" s="89">
         <f t="shared" si="18"/>
@@ -16856,7 +16856,7 @@
       <c r="BN60" s="97"/>
       <c r="BO60" s="97"/>
     </row>
-    <row r="61" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -16869,7 +16869,7 @@
         <v>1</v>
       </c>
       <c r="D61" s="87" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E61" s="89">
         <f t="shared" si="18"/>
@@ -16994,7 +16994,7 @@
       <c r="BN61" s="97"/>
       <c r="BO61" s="97"/>
     </row>
-    <row r="62" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -17121,7 +17121,7 @@
       <c r="BN62" s="96"/>
       <c r="BO62" s="96"/>
     </row>
-    <row r="63" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -17265,7 +17265,7 @@
       <c r="BN63" s="96"/>
       <c r="BO63" s="96"/>
     </row>
-    <row r="64" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -17408,7 +17408,7 @@
       <c r="BN64" s="96"/>
       <c r="BO64" s="96"/>
     </row>
-    <row r="65" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -17585,7 +17585,7 @@
       <c r="BN65" s="96"/>
       <c r="BO65" s="96"/>
     </row>
-    <row r="66" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -17730,7 +17730,7 @@
       <c r="BN66" s="96"/>
       <c r="BO66" s="96"/>
     </row>
-    <row r="67" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -17875,7 +17875,7 @@
       <c r="BN67" s="96"/>
       <c r="BO67" s="96"/>
     </row>
-    <row r="68" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -18036,7 +18036,7 @@
       <c r="BN68" s="96"/>
       <c r="BO68" s="96"/>
     </row>
-    <row r="69" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -18197,7 +18197,7 @@
       <c r="BN69" s="96"/>
       <c r="BO69" s="96"/>
     </row>
-    <row r="70" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -18348,7 +18348,7 @@
       <c r="BN70" s="96"/>
       <c r="BO70" s="96"/>
     </row>
-    <row r="71" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -18473,7 +18473,7 @@
       <c r="BN71" s="97"/>
       <c r="BO71" s="97"/>
     </row>
-    <row r="72" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -18590,7 +18590,7 @@
       <c r="BN72" s="96"/>
       <c r="BO72" s="96"/>
     </row>
-    <row r="73" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -18701,7 +18701,7 @@
       <c r="BN73" s="96"/>
       <c r="BO73" s="96"/>
     </row>
-    <row r="74" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -18812,7 +18812,7 @@
       <c r="BN74" s="96"/>
       <c r="BO74" s="96"/>
     </row>
-    <row r="75" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -18923,7 +18923,7 @@
       <c r="BN75" s="96"/>
       <c r="BO75" s="96"/>
     </row>
-    <row r="76" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -19034,7 +19034,7 @@
       <c r="BN76" s="96"/>
       <c r="BO76" s="96"/>
     </row>
-    <row r="77" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -19146,7 +19146,7 @@
       <c r="BN77" s="96"/>
       <c r="BO77" s="96"/>
     </row>
-    <row r="78" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -19263,7 +19263,7 @@
       <c r="BN78" s="96"/>
       <c r="BO78" s="96"/>
     </row>
-    <row r="79" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -19374,7 +19374,7 @@
       <c r="BN79" s="96"/>
       <c r="BO79" s="96"/>
     </row>
-    <row r="80" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -19485,7 +19485,7 @@
       <c r="BN80" s="96"/>
       <c r="BO80" s="96"/>
     </row>
-    <row r="81" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:95" x14ac:dyDescent="0.4">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -19596,7 +19596,7 @@
       <c r="BN81" s="96"/>
       <c r="BO81" s="96"/>
     </row>
-    <row r="82" spans="1:95" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:95" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -19735,7 +19735,7 @@
       <c r="CP82" s="1"/>
       <c r="CQ82" s="1"/>
     </row>
-    <row r="83" spans="1:95" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:95" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -19875,7 +19875,7 @@
       <c r="CP83" s="1"/>
       <c r="CQ83" s="1"/>
     </row>
-    <row r="84" spans="1:95" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:95" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -20020,7 +20020,7 @@
       <c r="CP84" s="1"/>
       <c r="CQ84" s="1"/>
     </row>
-    <row r="85" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:95" x14ac:dyDescent="0.4">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -20131,7 +20131,7 @@
       <c r="BN85" s="106"/>
       <c r="BO85" s="106"/>
     </row>
-    <row r="86" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:95" x14ac:dyDescent="0.4">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -20242,7 +20242,7 @@
       <c r="BN86" s="96"/>
       <c r="BO86" s="96"/>
     </row>
-    <row r="87" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:95" x14ac:dyDescent="0.4">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -20353,7 +20353,7 @@
       <c r="BN87" s="96"/>
       <c r="BO87" s="96"/>
     </row>
-    <row r="88" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:95" x14ac:dyDescent="0.4">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -20464,7 +20464,7 @@
       <c r="BN88" s="96"/>
       <c r="BO88" s="96"/>
     </row>
-    <row r="89" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:95" x14ac:dyDescent="0.4">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -20576,7 +20576,7 @@
       <c r="BN89" s="96"/>
       <c r="BO89" s="96"/>
     </row>
-    <row r="90" spans="1:95" hidden="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:95" x14ac:dyDescent="0.4">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -20701,7 +20701,7 @@
       <c r="BN90" s="96"/>
       <c r="BO90" s="96"/>
     </row>
-    <row r="91" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -20840,7 +20840,7 @@
       <c r="BN91" s="97"/>
       <c r="BO91" s="97"/>
     </row>
-    <row r="92" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -20962,7 +20962,7 @@
       <c r="BN92" s="97"/>
       <c r="BO92" s="97"/>
     </row>
-    <row r="93" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -21084,7 +21084,7 @@
       <c r="BN93" s="97"/>
       <c r="BO93" s="97"/>
     </row>
-    <row r="94" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -21208,7 +21208,7 @@
       <c r="BN94" s="97"/>
       <c r="BO94" s="97"/>
     </row>
-    <row r="95" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -21332,7 +21332,7 @@
       <c r="BN95" s="97"/>
       <c r="BO95" s="97"/>
     </row>
-    <row r="96" spans="1:95" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:95" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -21487,7 +21487,7 @@
       <c r="BN96" s="97"/>
       <c r="BO96" s="97"/>
     </row>
-    <row r="97" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -21614,7 +21614,7 @@
       <c r="BN97" s="97"/>
       <c r="BO97" s="97"/>
     </row>
-    <row r="98" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -21726,7 +21726,7 @@
       <c r="BN98" s="97"/>
       <c r="BO98" s="97"/>
     </row>
-    <row r="99" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -21860,7 +21860,7 @@
       <c r="BN99" s="97"/>
       <c r="BO99" s="97"/>
     </row>
-    <row r="100" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -23275,7 +23275,7 @@
       <c r="BN109" s="97"/>
       <c r="BO109" s="97"/>
     </row>
-    <row r="110" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -23396,7 +23396,7 @@
       <c r="BN110" s="97"/>
       <c r="BO110" s="97"/>
     </row>
-    <row r="111" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -23515,7 +23515,7 @@
       <c r="BN111" s="97"/>
       <c r="BO111" s="97"/>
     </row>
-    <row r="112" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -23640,7 +23640,7 @@
       <c r="BN112" s="97"/>
       <c r="BO112" s="97"/>
     </row>
-    <row r="113" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -23778,7 +23778,7 @@
       <c r="BN113" s="97"/>
       <c r="BO113" s="97"/>
     </row>
-    <row r="114" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -23916,7 +23916,7 @@
       <c r="BN114" s="97"/>
       <c r="BO114" s="97"/>
     </row>
-    <row r="115" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -24088,7 +24088,7 @@
       <c r="BN115" s="97"/>
       <c r="BO115" s="97"/>
     </row>
-    <row r="116" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -24260,7 +24260,7 @@
       <c r="BN116" s="97"/>
       <c r="BO116" s="97"/>
     </row>
-    <row r="117" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -24374,7 +24374,7 @@
       <c r="BN117" s="97"/>
       <c r="BO117" s="97"/>
     </row>
-    <row r="118" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -24482,7 +24482,7 @@
       <c r="BN118" s="97"/>
       <c r="BO118" s="97"/>
     </row>
-    <row r="119" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -24590,7 +24590,7 @@
       <c r="BN119" s="97"/>
       <c r="BO119" s="97"/>
     </row>
-    <row r="120" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -24698,7 +24698,7 @@
       <c r="BN120" s="97"/>
       <c r="BO120" s="97"/>
     </row>
-    <row r="121" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -24806,7 +24806,7 @@
       <c r="BN121" s="97"/>
       <c r="BO121" s="97"/>
     </row>
-    <row r="122" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -24915,7 +24915,7 @@
       <c r="BN122" s="97"/>
       <c r="BO122" s="97"/>
     </row>
-    <row r="123" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -25023,7 +25023,7 @@
       <c r="BN123" s="97"/>
       <c r="BO123" s="97"/>
     </row>
-    <row r="124" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -25131,7 +25131,7 @@
       <c r="BN124" s="97"/>
       <c r="BO124" s="97"/>
     </row>
-    <row r="125" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -25239,7 +25239,7 @@
       <c r="BN125" s="97"/>
       <c r="BO125" s="97"/>
     </row>
-    <row r="126" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -25347,7 +25347,7 @@
       <c r="BN126" s="97"/>
       <c r="BO126" s="97"/>
     </row>
-    <row r="127" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -25455,7 +25455,7 @@
       <c r="BN127" s="97"/>
       <c r="BO127" s="97"/>
     </row>
-    <row r="128" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -25563,7 +25563,7 @@
       <c r="BN128" s="97"/>
       <c r="BO128" s="97"/>
     </row>
-    <row r="129" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -25671,7 +25671,7 @@
       <c r="BN129" s="97"/>
       <c r="BO129" s="97"/>
     </row>
-    <row r="130" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -25779,7 +25779,7 @@
       <c r="BN130" s="97"/>
       <c r="BO130" s="97"/>
     </row>
-    <row r="131" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -25899,7 +25899,7 @@
       <c r="BN131" s="97"/>
       <c r="BO131" s="97"/>
     </row>
-    <row r="132" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -26019,7 +26019,7 @@
       <c r="BN132" s="97"/>
       <c r="BO132" s="97"/>
     </row>
-    <row r="133" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -26129,7 +26129,7 @@
       <c r="BN133" s="97"/>
       <c r="BO133" s="97"/>
     </row>
-    <row r="134" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -26238,7 +26238,7 @@
       <c r="BN134" s="97"/>
       <c r="BO134" s="97"/>
     </row>
-    <row r="135" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -26347,7 +26347,7 @@
       <c r="BN135" s="97"/>
       <c r="BO135" s="97"/>
     </row>
-    <row r="136" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -26465,7 +26465,7 @@
       <c r="BN136" s="97"/>
       <c r="BO136" s="97"/>
     </row>
-    <row r="137" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -26593,7 +26593,7 @@
       <c r="BN137" s="97"/>
       <c r="BO137" s="97"/>
     </row>
-    <row r="138" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -26698,7 +26698,7 @@
       <c r="BN138" s="97"/>
       <c r="BO138" s="97"/>
     </row>
-    <row r="139" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -26803,7 +26803,7 @@
       <c r="BN139" s="97"/>
       <c r="BO139" s="97"/>
     </row>
-    <row r="140" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -26816,7 +26816,7 @@
         <v>1</v>
       </c>
       <c r="D140" s="87" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="E140" s="89">
         <f t="shared" si="55"/>
@@ -26962,7 +26962,7 @@
       <c r="BN140" s="97"/>
       <c r="BO140" s="97"/>
     </row>
-    <row r="141" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -26975,7 +26975,7 @@
         <v>1</v>
       </c>
       <c r="D141" s="87" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="E141" s="89">
         <f t="shared" si="55"/>
@@ -27121,7 +27121,7 @@
       <c r="BN141" s="97"/>
       <c r="BO141" s="97"/>
     </row>
-    <row r="142" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -27254,7 +27254,7 @@
       <c r="BN142" s="97"/>
       <c r="BO142" s="97"/>
     </row>
-    <row r="143" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -27387,7 +27387,7 @@
       <c r="BN143" s="97"/>
       <c r="BO143" s="97"/>
     </row>
-    <row r="144" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -27507,7 +27507,7 @@
       <c r="BN144" s="97"/>
       <c r="BO144" s="97"/>
     </row>
-    <row r="145" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -27628,7 +27628,7 @@
       <c r="BN145" s="97"/>
       <c r="BO145" s="97"/>
     </row>
-    <row r="146" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -27729,7 +27729,7 @@
       <c r="BN146" s="97"/>
       <c r="BO146" s="97"/>
     </row>
-    <row r="147" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -27831,7 +27831,7 @@
       <c r="BN147" s="97"/>
       <c r="BO147" s="97"/>
     </row>
-    <row r="148" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -27932,7 +27932,7 @@
       <c r="BN148" s="97"/>
       <c r="BO148" s="97"/>
     </row>
-    <row r="149" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -28035,7 +28035,7 @@
       <c r="BN149" s="97"/>
       <c r="BO149" s="97"/>
     </row>
-    <row r="150" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -28136,7 +28136,7 @@
       <c r="BN150" s="97"/>
       <c r="BO150" s="97"/>
     </row>
-    <row r="151" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -28239,7 +28239,7 @@
       <c r="BN151" s="97"/>
       <c r="BO151" s="97"/>
     </row>
-    <row r="152" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -28285,7 +28285,7 @@
         <v>10</v>
       </c>
       <c r="N152" s="91" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="O152" s="109">
         <v>12</v>
@@ -28329,7 +28329,7 @@
       <c r="BN152" s="96"/>
       <c r="BO152" s="96"/>
     </row>
-    <row r="153" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -28375,7 +28375,7 @@
         <v>20</v>
       </c>
       <c r="N153" s="91" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="O153" s="109">
         <v>12</v>
@@ -28411,7 +28411,7 @@
       <c r="BN153" s="96"/>
       <c r="BO153" s="96"/>
     </row>
-    <row r="154" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -28457,7 +28457,7 @@
         <v>10</v>
       </c>
       <c r="N154" s="91" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="O154" s="109">
         <v>12</v>
@@ -28491,7 +28491,7 @@
       <c r="BN154" s="96"/>
       <c r="BO154" s="96"/>
     </row>
-    <row r="155" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -28537,7 +28537,7 @@
         <v>20</v>
       </c>
       <c r="N155" s="91" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="O155" s="109">
         <v>12</v>
@@ -28565,7 +28565,7 @@
       <c r="AH155" s="96"/>
       <c r="AI155" s="96"/>
     </row>
-    <row r="156" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -28611,7 +28611,7 @@
         <v>10</v>
       </c>
       <c r="N156" s="91" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="O156" s="109">
         <v>12</v>
@@ -28639,7 +28639,7 @@
       <c r="AH156" s="96"/>
       <c r="AI156" s="96"/>
     </row>
-    <row r="157" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -28685,7 +28685,7 @@
         <v>20</v>
       </c>
       <c r="N157" s="91" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="O157" s="109">
         <v>12</v>
@@ -28713,7 +28713,7 @@
       <c r="AH157" s="96"/>
       <c r="AI157" s="96"/>
     </row>
-    <row r="158" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -28759,7 +28759,7 @@
         <v>10</v>
       </c>
       <c r="N158" s="91" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="O158" s="109">
         <v>12</v>
@@ -28787,7 +28787,7 @@
       <c r="AH158" s="96"/>
       <c r="AI158" s="96"/>
     </row>
-    <row r="159" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -28833,7 +28833,7 @@
         <v>20</v>
       </c>
       <c r="N159" s="91" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="O159" s="109">
         <v>12</v>
@@ -28861,7 +28861,7 @@
       <c r="AH159" s="96"/>
       <c r="AI159" s="96"/>
     </row>
-    <row r="160" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -28935,7 +28935,7 @@
       <c r="AH160" s="96"/>
       <c r="AI160" s="96"/>
     </row>
-    <row r="161" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -29009,7 +29009,7 @@
       <c r="AH161" s="96"/>
       <c r="AI161" s="96"/>
     </row>
-    <row r="162" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -29083,7 +29083,7 @@
       <c r="AH162" s="96"/>
       <c r="AI162" s="96"/>
     </row>
-    <row r="163" spans="1:67" hidden="1" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -29157,7 +29157,7 @@
       <c r="AH163" s="96"/>
       <c r="AI163" s="96"/>
     </row>
-    <row r="164" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -29264,7 +29264,7 @@
       <c r="BN164" s="124"/>
       <c r="BO164" s="124"/>
     </row>
-    <row r="165" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -29371,7 +29371,7 @@
       <c r="BN165" s="124"/>
       <c r="BO165" s="124"/>
     </row>
-    <row r="166" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -29477,7 +29477,7 @@
       <c r="BN166" s="124"/>
       <c r="BO166" s="124"/>
     </row>
-    <row r="167" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -29583,7 +29583,7 @@
       <c r="BN167" s="124"/>
       <c r="BO167" s="124"/>
     </row>
-    <row r="168" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -29761,7 +29761,7 @@
       <c r="BN168" s="124"/>
       <c r="BO168" s="124"/>
     </row>
-    <row r="169" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -29939,7 +29939,7 @@
       <c r="BN169" s="124"/>
       <c r="BO169" s="124"/>
     </row>
-    <row r="170" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -30046,7 +30046,7 @@
       <c r="BN170" s="124"/>
       <c r="BO170" s="124"/>
     </row>
-    <row r="171" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -30153,7 +30153,7 @@
       <c r="BN171" s="124"/>
       <c r="BO171" s="124"/>
     </row>
-    <row r="172" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -30260,7 +30260,7 @@
       <c r="BN172" s="124"/>
       <c r="BO172" s="124"/>
     </row>
-    <row r="173" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -30367,7 +30367,7 @@
       <c r="BN173" s="124"/>
       <c r="BO173" s="124"/>
     </row>
-    <row r="174" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -30472,7 +30472,7 @@
       <c r="BN174" s="124"/>
       <c r="BO174" s="124"/>
     </row>
-    <row r="175" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -30577,7 +30577,7 @@
       <c r="BN175" s="124"/>
       <c r="BO175" s="124"/>
     </row>
-    <row r="176" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -30715,7 +30715,7 @@
       <c r="BN176" s="124"/>
       <c r="BO176" s="124"/>
     </row>
-    <row r="177" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -30728,7 +30728,7 @@
         <v>1</v>
       </c>
       <c r="D177" s="87" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="E177" s="89">
         <f t="shared" si="70"/>
@@ -30852,7 +30852,7 @@
       <c r="BN177" s="124"/>
       <c r="BO177" s="124"/>
     </row>
-    <row r="178" spans="1:67" s="87" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:67" s="87" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -30898,7 +30898,7 @@
         <v>10</v>
       </c>
       <c r="N178" s="91" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="O178" s="109">
         <v>60</v>
@@ -31334,26 +31334,7 @@
       <c r="O218" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:BK178" xr:uid="{00000000-0009-0000-0000-000002000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="RfG_Ucontrol_Fault"/>
-        <filter val="RfG_Ucontrol_Fault_FRTlimit"/>
-        <filter val="RfG_Ucontrol_FRTsensitivity"/>
-        <filter val="RfG_Ucontrol_FRTsensitivity-ramp"/>
-        <filter val="RfG_Ucontrol_LFSM-O"/>
-        <filter val="RfG_Ucontrol_Phasejump"/>
-        <filter val="RfG_Ucontrol_rec"/>
-        <filter val="RfG_Ucontrol_Scmax"/>
-        <filter val="RfG_Ucontrol_Scmin"/>
-        <filter val="RfG_Ucontrol_Scmin_Droop_2"/>
-        <filter val="RfG_Ucontrol_Scmin_Droop_4"/>
-        <filter val="RfG_Ucontrol_Scmin_Droop_7"/>
-        <filter val="RfG_Ucontrol_SCR"/>
-        <filter val="RfG_Ucontrol_Sctune"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:BK178" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="15">
     <mergeCell ref="BL1:BO1"/>
     <mergeCell ref="A1:D1"/>
@@ -53465,6 +53446,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C163:C176"/>
+    <mergeCell ref="C61:C70"/>
+    <mergeCell ref="C71:C94"/>
+    <mergeCell ref="C95:C98"/>
+    <mergeCell ref="C99:C108"/>
+    <mergeCell ref="C109:C115"/>
+    <mergeCell ref="C116:C162"/>
     <mergeCell ref="C58:C60"/>
     <mergeCell ref="C54:C57"/>
     <mergeCell ref="C2:C11"/>
@@ -53472,13 +53460,6 @@
     <mergeCell ref="C18:C28"/>
     <mergeCell ref="C44:C53"/>
     <mergeCell ref="C29:C43"/>
-    <mergeCell ref="C163:C176"/>
-    <mergeCell ref="C61:C70"/>
-    <mergeCell ref="C71:C94"/>
-    <mergeCell ref="C95:C98"/>
-    <mergeCell ref="C99:C108"/>
-    <mergeCell ref="C109:C115"/>
-    <mergeCell ref="C116:C162"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -54015,17 +53996,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="107e75b3-53cc-4838-92d2-ebc011bd4832">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="888ccf44-0d39-41a2-ab17-f7efb2bf6977" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004FD8CECCB51EC843BF514AFE68379818" ma:contentTypeVersion="18" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="eda339f53f012ceb64677667a741b441">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="107e75b3-53cc-4838-92d2-ebc011bd4832" xmlns:ns3="888ccf44-0d39-41a2-ab17-f7efb2bf6977" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04a86f3db711706e561c315688f1c464" ns2:_="" ns3:_="">
     <xsd:import namespace="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
@@ -54274,6 +54244,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="107e75b3-53cc-4838-92d2-ebc011bd4832">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="888ccf44-0d39-41a2-ab17-f7efb2bf6977" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
   <ds:schemaRefs>
@@ -54283,23 +54264,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2288FB7-E85A-4FE8-9E7A-FE572FF16064}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="888ccf44-0d39-41a2-ab17-f7efb2bf6977"/>
-    <ds:schemaRef ds:uri="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F91B7B9-75FF-4624-B506-952B5B54766C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -54316,4 +54280,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2288FB7-E85A-4FE8-9E7A-FE572FF16064}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="888ccf44-0d39-41a2-ab17-f7efb2bf6977"/>
+    <ds:schemaRef ds:uri="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update test cases in testcases.xlsx for enhanced coverage and accuracy
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/prw_energinet_dk/Documents/Dokumenter/GitHub/MTB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D55F73F-7687-4A56-9060-6B99955C88B8}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93899611-9B11-4DE4-9E63-5A6541A28DEB}"/>
   <bookViews>
     <workbookView xWindow="-17610" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3478,9 +3478,6 @@
     <t>RfG_LVFRT_profile_Pref_05</t>
   </si>
   <si>
-    <t>RfG_LVFRT_profil_Pref_05_Pavail</t>
-  </si>
-  <si>
     <t>RfG_Qpf_Pref-change</t>
   </si>
   <si>
@@ -3515,6 +3512,9 @@
   </si>
   <si>
     <t>RfG_Qpf_PFref-change</t>
+  </si>
+  <si>
+    <t>RfG_LVFRT_profile_Pref_05_Pavail</t>
   </si>
 </sst>
 </file>
@@ -6108,7 +6108,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="291" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B19" s="283" t="b">
         <v>0</v>
@@ -6117,7 +6117,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="293" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -9415,7 +9415,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
+      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -9619,7 +9619,7 @@
         <v>100</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>101</v>
@@ -16345,7 +16345,7 @@
         <v>1</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="E57" s="5">
         <f t="shared" si="18"/>
@@ -16471,7 +16471,7 @@
         <v>1</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E58" s="5">
         <f t="shared" si="18"/>
@@ -16599,7 +16599,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="87" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="E59" s="89">
         <f t="shared" si="18"/>
@@ -16734,7 +16734,7 @@
         <v>1</v>
       </c>
       <c r="D60" s="87" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="E60" s="89">
         <f t="shared" si="18"/>
@@ -16869,7 +16869,7 @@
         <v>1</v>
       </c>
       <c r="D61" s="87" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E61" s="89">
         <f t="shared" si="18"/>
@@ -18210,7 +18210,7 @@
         <v>1</v>
       </c>
       <c r="D70" s="87" t="s">
-        <v>921</v>
+        <v>933</v>
       </c>
       <c r="E70" s="89">
         <f t="shared" si="18"/>
@@ -26816,7 +26816,7 @@
         <v>1</v>
       </c>
       <c r="D140" s="87" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E140" s="89">
         <f t="shared" si="55"/>
@@ -26975,7 +26975,7 @@
         <v>1</v>
       </c>
       <c r="D141" s="87" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="E141" s="89">
         <f t="shared" si="55"/>
@@ -28285,7 +28285,7 @@
         <v>10</v>
       </c>
       <c r="N152" s="91" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="O152" s="109">
         <v>12</v>
@@ -28375,7 +28375,7 @@
         <v>20</v>
       </c>
       <c r="N153" s="91" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="O153" s="109">
         <v>12</v>
@@ -28457,7 +28457,7 @@
         <v>10</v>
       </c>
       <c r="N154" s="91" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="O154" s="109">
         <v>12</v>
@@ -28537,7 +28537,7 @@
         <v>20</v>
       </c>
       <c r="N155" s="91" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="O155" s="109">
         <v>12</v>
@@ -28611,7 +28611,7 @@
         <v>10</v>
       </c>
       <c r="N156" s="91" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="O156" s="109">
         <v>12</v>
@@ -28685,7 +28685,7 @@
         <v>20</v>
       </c>
       <c r="N157" s="91" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="O157" s="109">
         <v>12</v>
@@ -28759,7 +28759,7 @@
         <v>10</v>
       </c>
       <c r="N158" s="91" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="O158" s="109">
         <v>12</v>
@@ -28833,7 +28833,7 @@
         <v>20</v>
       </c>
       <c r="N159" s="91" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="O159" s="109">
         <v>12</v>
@@ -30728,7 +30728,7 @@
         <v>1</v>
       </c>
       <c r="D177" s="87" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="E177" s="89">
         <f t="shared" si="70"/>
@@ -30898,7 +30898,7 @@
         <v>10</v>
       </c>
       <c r="N178" s="91" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="O178" s="109">
         <v>60</v>
@@ -53446,6 +53446,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="C18:C28"/>
+    <mergeCell ref="C44:C53"/>
+    <mergeCell ref="C29:C43"/>
     <mergeCell ref="C163:C176"/>
     <mergeCell ref="C61:C70"/>
     <mergeCell ref="C71:C94"/>
@@ -53453,13 +53460,6 @@
     <mergeCell ref="C99:C108"/>
     <mergeCell ref="C109:C115"/>
     <mergeCell ref="C116:C162"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="C18:C28"/>
-    <mergeCell ref="C44:C53"/>
-    <mergeCell ref="C29:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -53987,15 +53987,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004FD8CECCB51EC843BF514AFE68379818" ma:contentTypeVersion="18" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="eda339f53f012ceb64677667a741b441">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="107e75b3-53cc-4838-92d2-ebc011bd4832" xmlns:ns3="888ccf44-0d39-41a2-ab17-f7efb2bf6977" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04a86f3db711706e561c315688f1c464" ns2:_="" ns3:_="">
     <xsd:import namespace="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
@@ -54244,6 +54235,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -54256,14 +54256,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F91B7B9-75FF-4624-B506-952B5B54766C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -54278,6 +54270,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update test cases in testcases.xlsx to improve coverage and accuracy
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/prw_energinet_dk/Documents/Dokumenter/GitHub/MTB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93899611-9B11-4DE4-9E63-5A6541A28DEB}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2822A63F-9E62-5889-8F7B-BDC091F69563}"/>
   <bookViews>
-    <workbookView xWindow="-17610" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14480" yWindow="-21710" windowWidth="51420" windowHeight="21100" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -3478,6 +3478,9 @@
     <t>RfG_LVFRT_profile_Pref_05</t>
   </si>
   <si>
+    <t>RfG_LVFRT_profil_Pref_05_Pavail</t>
+  </si>
+  <si>
     <t>RfG_Qpf_Pref-change</t>
   </si>
   <si>
@@ -3512,9 +3515,6 @@
   </si>
   <si>
     <t>RfG_Qpf_PFref-change</t>
-  </si>
-  <si>
-    <t>RfG_LVFRT_profile_Pref_05_Pavail</t>
   </si>
 </sst>
 </file>
@@ -6108,7 +6108,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="291" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B19" s="283" t="b">
         <v>0</v>
@@ -6117,7 +6117,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="293" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -9415,7 +9415,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
+      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -9619,7 +9619,7 @@
         <v>100</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>101</v>
@@ -16345,7 +16345,7 @@
         <v>1</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="E57" s="5">
         <f t="shared" si="18"/>
@@ -16471,7 +16471,7 @@
         <v>1</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="E58" s="5">
         <f t="shared" si="18"/>
@@ -16599,7 +16599,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="87" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="E59" s="89">
         <f t="shared" si="18"/>
@@ -16734,7 +16734,7 @@
         <v>1</v>
       </c>
       <c r="D60" s="87" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="E60" s="89">
         <f t="shared" si="18"/>
@@ -16869,7 +16869,7 @@
         <v>1</v>
       </c>
       <c r="D61" s="87" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="E61" s="89">
         <f t="shared" si="18"/>
@@ -18210,7 +18210,7 @@
         <v>1</v>
       </c>
       <c r="D70" s="87" t="s">
-        <v>933</v>
+        <v>921</v>
       </c>
       <c r="E70" s="89">
         <f t="shared" si="18"/>
@@ -26816,7 +26816,7 @@
         <v>1</v>
       </c>
       <c r="D140" s="87" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="E140" s="89">
         <f t="shared" si="55"/>
@@ -26975,7 +26975,7 @@
         <v>1</v>
       </c>
       <c r="D141" s="87" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="E141" s="89">
         <f t="shared" si="55"/>
@@ -28285,7 +28285,7 @@
         <v>10</v>
       </c>
       <c r="N152" s="91" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="O152" s="109">
         <v>12</v>
@@ -28375,7 +28375,7 @@
         <v>20</v>
       </c>
       <c r="N153" s="91" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="O153" s="109">
         <v>12</v>
@@ -28457,7 +28457,7 @@
         <v>10</v>
       </c>
       <c r="N154" s="91" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="O154" s="109">
         <v>12</v>
@@ -28537,7 +28537,7 @@
         <v>20</v>
       </c>
       <c r="N155" s="91" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="O155" s="109">
         <v>12</v>
@@ -28611,7 +28611,7 @@
         <v>10</v>
       </c>
       <c r="N156" s="91" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="O156" s="109">
         <v>12</v>
@@ -28685,7 +28685,7 @@
         <v>20</v>
       </c>
       <c r="N157" s="91" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="O157" s="109">
         <v>12</v>
@@ -28759,7 +28759,7 @@
         <v>10</v>
       </c>
       <c r="N158" s="91" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="O158" s="109">
         <v>12</v>
@@ -28833,7 +28833,7 @@
         <v>20</v>
       </c>
       <c r="N159" s="91" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="O159" s="109">
         <v>12</v>
@@ -30728,7 +30728,7 @@
         <v>1</v>
       </c>
       <c r="D177" s="87" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="E177" s="89">
         <f t="shared" si="70"/>
@@ -30898,7 +30898,7 @@
         <v>10</v>
       </c>
       <c r="N178" s="91" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="O178" s="109">
         <v>60</v>
@@ -53987,6 +53987,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="107e75b3-53cc-4838-92d2-ebc011bd4832">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="888ccf44-0d39-41a2-ab17-f7efb2bf6977" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004FD8CECCB51EC843BF514AFE68379818" ma:contentTypeVersion="18" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="eda339f53f012ceb64677667a741b441">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="107e75b3-53cc-4838-92d2-ebc011bd4832" xmlns:ns3="888ccf44-0d39-41a2-ab17-f7efb2bf6977" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04a86f3db711706e561c315688f1c464" ns2:_="" ns3:_="">
     <xsd:import namespace="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
@@ -54235,27 +54255,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="107e75b3-53cc-4838-92d2-ebc011bd4832">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="888ccf44-0d39-41a2-ab17-f7efb2bf6977" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2288FB7-E85A-4FE8-9E7A-FE572FF16064}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="888ccf44-0d39-41a2-ab17-f7efb2bf6977"/>
+    <ds:schemaRef ds:uri="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F91B7B9-75FF-4624-B506-952B5B54766C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -54272,29 +54297,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2288FB7-E85A-4FE8-9E7A-FE572FF16064}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="888ccf44-0d39-41a2-ab17-f7efb2bf6977"/>
-    <ds:schemaRef ds:uri="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update test cases in testcases.xlsx
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/prw_energinet_dk/Documents/Dokumenter/GitHub/MTB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7784DD6-5403-4993-9B56-0D0A90D642B8}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2822A63F-9E62-5889-8F7B-BDC091F69563}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14480" yWindow="-21710" windowWidth="51420" windowHeight="21100" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -3346,12 +3346,6 @@
     <t>RfG_Fault_2_20_WG</t>
   </si>
   <si>
-    <t>RfG_Fault_3_ROCOF_curveOF</t>
-  </si>
-  <si>
-    <t>RfG_Fault_3_ROCOF_curveUF</t>
-  </si>
-  <si>
     <t>RfG_Fault_3_SCR_freqStep1</t>
   </si>
   <si>
@@ -3490,9 +3484,6 @@
     <t>RfG_Qpf_Pref-change</t>
   </si>
   <si>
-    <t>RfG_Qpf_Qref-change</t>
-  </si>
-  <si>
     <t>RfG_proc_Freq_limit_down</t>
   </si>
   <si>
@@ -3515,6 +3506,15 @@
   </si>
   <si>
     <t>RfG_SystemProtect+fault</t>
+  </si>
+  <si>
+    <t>RfG_Fault_3_RoCoF_curveOF</t>
+  </si>
+  <si>
+    <t>RfG_Fault_3_RoCoF_curveUF</t>
+  </si>
+  <si>
+    <t>RfG_Qpf_PFref-change</t>
   </si>
 </sst>
 </file>
@@ -5772,7 +5772,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -6108,7 +6108,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="291" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="B19" s="283" t="b">
         <v>0</v>
@@ -6117,7 +6117,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="293" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -9414,8 +9414,8 @@
   <dimension ref="A1:CQ218"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J60" sqref="J60"/>
+      <pane ySplit="2" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -9619,7 +9619,7 @@
         <v>100</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>101</v>
@@ -13508,7 +13508,9 @@
       <c r="R34" s="96">
         <v>0.5</v>
       </c>
-      <c r="S34" s="96"/>
+      <c r="S34" s="96">
+        <v>0</v>
+      </c>
       <c r="T34" s="5"/>
       <c r="U34" s="85"/>
       <c r="V34" s="85"/>
@@ -13646,7 +13648,9 @@
       <c r="R35" s="97">
         <v>0</v>
       </c>
-      <c r="S35" s="97"/>
+      <c r="S35" s="97">
+        <v>0</v>
+      </c>
       <c r="U35" s="89"/>
       <c r="V35" s="89"/>
       <c r="W35" s="108"/>
@@ -13753,7 +13757,9 @@
       <c r="R36" s="96">
         <v>0.5</v>
       </c>
-      <c r="S36" s="96"/>
+      <c r="S36" s="96">
+        <v>0</v>
+      </c>
       <c r="T36" s="5"/>
       <c r="U36" s="85"/>
       <c r="V36" s="85"/>
@@ -13863,7 +13869,9 @@
       <c r="R37" s="97">
         <v>0</v>
       </c>
-      <c r="S37" s="97"/>
+      <c r="S37" s="97">
+        <v>0</v>
+      </c>
       <c r="U37" s="89"/>
       <c r="V37" s="89"/>
       <c r="W37" s="108"/>
@@ -13970,7 +13978,9 @@
       <c r="R38" s="96">
         <v>0.5</v>
       </c>
-      <c r="S38" s="96"/>
+      <c r="S38" s="96">
+        <v>0</v>
+      </c>
       <c r="T38" s="5"/>
       <c r="U38" s="85"/>
       <c r="V38" s="85"/>
@@ -14080,7 +14090,9 @@
       <c r="R39" s="97">
         <v>0</v>
       </c>
-      <c r="S39" s="97"/>
+      <c r="S39" s="97">
+        <v>0</v>
+      </c>
       <c r="U39" s="89"/>
       <c r="V39" s="89"/>
       <c r="W39" s="89"/>
@@ -16333,7 +16345,7 @@
         <v>1</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>925</v>
+        <v>933</v>
       </c>
       <c r="E57" s="5">
         <f t="shared" si="18"/>
@@ -16459,7 +16471,7 @@
         <v>1</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="E58" s="5">
         <f t="shared" si="18"/>
@@ -16587,7 +16599,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="87" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="E59" s="89">
         <f t="shared" si="18"/>
@@ -16722,7 +16734,7 @@
         <v>1</v>
       </c>
       <c r="D60" s="87" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="E60" s="89">
         <f t="shared" si="18"/>
@@ -16857,7 +16869,7 @@
         <v>1</v>
       </c>
       <c r="D61" s="87" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="E61" s="89">
         <f t="shared" si="18"/>
@@ -18035,7 +18047,7 @@
         <v>1</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="E69" s="5">
         <f t="shared" si="18"/>
@@ -18198,7 +18210,7 @@
         <v>1</v>
       </c>
       <c r="D70" s="87" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="E70" s="89">
         <f t="shared" si="18"/>
@@ -23316,7 +23328,7 @@
         <v>20</v>
       </c>
       <c r="P110" s="97" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="Q110" s="97">
         <v>1</v>
@@ -23326,7 +23338,7 @@
       </c>
       <c r="S110" s="97"/>
       <c r="T110" s="89" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="U110" s="89">
         <v>5</v>
@@ -23336,7 +23348,7 @@
       </c>
       <c r="W110" s="89"/>
       <c r="X110" s="97" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="Y110" s="97">
         <v>10</v>
@@ -23397,7 +23409,7 @@
         <v>1</v>
       </c>
       <c r="D111" s="87" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="E111" s="89">
         <f t="shared" si="35"/>
@@ -23449,7 +23461,7 @@
         <v>0</v>
       </c>
       <c r="T111" s="89" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="U111" s="89">
         <v>40</v>
@@ -26804,7 +26816,7 @@
         <v>1</v>
       </c>
       <c r="D140" s="87" t="s">
-        <v>877</v>
+        <v>931</v>
       </c>
       <c r="E140" s="89">
         <f t="shared" si="55"/>
@@ -26963,7 +26975,7 @@
         <v>1</v>
       </c>
       <c r="D141" s="87" t="s">
-        <v>878</v>
+        <v>932</v>
       </c>
       <c r="E141" s="89">
         <f t="shared" si="55"/>
@@ -27122,7 +27134,7 @@
         <v>1</v>
       </c>
       <c r="D142" s="87" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="E142" s="89">
         <f t="shared" si="55"/>
@@ -27255,7 +27267,7 @@
         <v>1</v>
       </c>
       <c r="D143" s="87" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="E143" s="89">
         <f t="shared" si="55"/>
@@ -27388,7 +27400,7 @@
         <v>1</v>
       </c>
       <c r="D144" s="87" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="E144" s="89">
         <f t="shared" ref="E144:E145" si="68">inp_Uc/inp_Un</f>
@@ -27508,7 +27520,7 @@
         <v>1</v>
       </c>
       <c r="D145" s="87" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="E145" s="89">
         <f t="shared" si="68"/>
@@ -27629,7 +27641,7 @@
         <v>1</v>
       </c>
       <c r="D146" s="87" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="E146" s="89">
         <f t="shared" ref="E146:E178" si="70">inp_Uc/inp_Un</f>
@@ -27730,7 +27742,7 @@
         <v>1</v>
       </c>
       <c r="D147" s="87" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="E147" s="89">
         <f t="shared" si="70"/>
@@ -27832,7 +27844,7 @@
         <v>1</v>
       </c>
       <c r="D148" s="87" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="E148" s="89">
         <f t="shared" si="70"/>
@@ -27933,7 +27945,7 @@
         <v>1</v>
       </c>
       <c r="D149" s="87" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="E149" s="89">
         <f t="shared" si="70"/>
@@ -28036,7 +28048,7 @@
         <v>1</v>
       </c>
       <c r="D150" s="87" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="E150" s="89">
         <f t="shared" si="70"/>
@@ -28137,7 +28149,7 @@
         <v>1</v>
       </c>
       <c r="D151" s="87" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="E151" s="89">
         <f t="shared" si="70"/>
@@ -28240,7 +28252,7 @@
         <v>1</v>
       </c>
       <c r="D152" s="87" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="E152" s="89">
         <f t="shared" si="70"/>
@@ -28273,7 +28285,7 @@
         <v>10</v>
       </c>
       <c r="N152" s="91" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="O152" s="109">
         <v>12</v>
@@ -28330,7 +28342,7 @@
         <v>1</v>
       </c>
       <c r="D153" s="87" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="E153" s="89">
         <f t="shared" si="70"/>
@@ -28363,7 +28375,7 @@
         <v>20</v>
       </c>
       <c r="N153" s="91" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="O153" s="109">
         <v>12</v>
@@ -28412,7 +28424,7 @@
         <v>1</v>
       </c>
       <c r="D154" s="87" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="E154" s="89">
         <f t="shared" si="70"/>
@@ -28445,7 +28457,7 @@
         <v>10</v>
       </c>
       <c r="N154" s="91" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="O154" s="109">
         <v>12</v>
@@ -28492,7 +28504,7 @@
         <v>1</v>
       </c>
       <c r="D155" s="87" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="E155" s="89">
         <f t="shared" si="70"/>
@@ -28525,7 +28537,7 @@
         <v>20</v>
       </c>
       <c r="N155" s="91" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="O155" s="109">
         <v>12</v>
@@ -28566,7 +28578,7 @@
         <v>1</v>
       </c>
       <c r="D156" s="87" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="E156" s="89">
         <f t="shared" si="70"/>
@@ -28599,7 +28611,7 @@
         <v>10</v>
       </c>
       <c r="N156" s="91" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="O156" s="109">
         <v>12</v>
@@ -28640,7 +28652,7 @@
         <v>1</v>
       </c>
       <c r="D157" s="87" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E157" s="89">
         <f t="shared" si="70"/>
@@ -28673,7 +28685,7 @@
         <v>20</v>
       </c>
       <c r="N157" s="91" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="O157" s="109">
         <v>12</v>
@@ -28714,7 +28726,7 @@
         <v>1</v>
       </c>
       <c r="D158" s="87" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E158" s="89">
         <f t="shared" si="70"/>
@@ -28747,7 +28759,7 @@
         <v>10</v>
       </c>
       <c r="N158" s="91" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="O158" s="109">
         <v>12</v>
@@ -28788,7 +28800,7 @@
         <v>1</v>
       </c>
       <c r="D159" s="87" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E159" s="89">
         <f t="shared" si="70"/>
@@ -28821,7 +28833,7 @@
         <v>20</v>
       </c>
       <c r="N159" s="91" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="O159" s="109">
         <v>12</v>
@@ -28862,7 +28874,7 @@
         <v>1</v>
       </c>
       <c r="D160" s="87" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="E160" s="89">
         <f t="shared" si="70"/>
@@ -28936,7 +28948,7 @@
         <v>1</v>
       </c>
       <c r="D161" s="87" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E161" s="89">
         <f t="shared" si="70"/>
@@ -29010,7 +29022,7 @@
         <v>1</v>
       </c>
       <c r="D162" s="87" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="E162" s="89">
         <f t="shared" si="70"/>
@@ -29084,7 +29096,7 @@
         <v>1</v>
       </c>
       <c r="D163" s="87" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="E163" s="89">
         <f t="shared" si="70"/>
@@ -29158,7 +29170,7 @@
         <v>1</v>
       </c>
       <c r="D164" s="87" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="E164" s="89">
         <f t="shared" si="70"/>
@@ -29265,7 +29277,7 @@
         <v>1</v>
       </c>
       <c r="D165" s="87" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="E165" s="89">
         <f t="shared" si="70"/>
@@ -29372,7 +29384,7 @@
         <v>1</v>
       </c>
       <c r="D166" s="87" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="E166" s="89">
         <f t="shared" si="70"/>
@@ -29478,7 +29490,7 @@
         <v>1</v>
       </c>
       <c r="D167" s="87" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="E167" s="89">
         <f t="shared" si="70"/>
@@ -29584,7 +29596,7 @@
         <v>1</v>
       </c>
       <c r="D168" s="87" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="E168" s="89">
         <f t="shared" si="70"/>
@@ -29762,7 +29774,7 @@
         <v>1</v>
       </c>
       <c r="D169" s="87" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="E169" s="89">
         <f t="shared" si="70"/>
@@ -29940,7 +29952,7 @@
         <v>1</v>
       </c>
       <c r="D170" s="87" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="E170" s="89">
         <f t="shared" si="70"/>
@@ -30047,7 +30059,7 @@
         <v>1</v>
       </c>
       <c r="D171" s="87" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="E171" s="89">
         <f t="shared" si="70"/>
@@ -30154,7 +30166,7 @@
         <v>1</v>
       </c>
       <c r="D172" s="87" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="E172" s="89">
         <f t="shared" si="70"/>
@@ -30261,7 +30273,7 @@
         <v>1</v>
       </c>
       <c r="D173" s="87" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="E173" s="89">
         <f t="shared" si="70"/>
@@ -30368,7 +30380,7 @@
         <v>1</v>
       </c>
       <c r="D174" s="87" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="E174" s="89">
         <f t="shared" si="70"/>
@@ -30473,7 +30485,7 @@
         <v>1</v>
       </c>
       <c r="D175" s="87" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="E175" s="89">
         <f t="shared" si="70"/>
@@ -30578,7 +30590,7 @@
         <v>1</v>
       </c>
       <c r="D176" s="87" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="E176" s="89">
         <f t="shared" si="70"/>
@@ -30716,7 +30728,7 @@
         <v>1</v>
       </c>
       <c r="D177" s="87" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="E177" s="89">
         <f t="shared" si="70"/>
@@ -30853,7 +30865,7 @@
         <v>1</v>
       </c>
       <c r="D178" s="87" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="E178" s="89">
         <f t="shared" si="70"/>
@@ -30886,7 +30898,7 @@
         <v>10</v>
       </c>
       <c r="N178" s="91" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="O178" s="109">
         <v>60</v>
@@ -31348,7 +31360,7 @@
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>datavalidation!$E$1:$E$2</xm:f>
@@ -50352,13 +50364,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="113" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="B3" s="113" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="C3" s="113" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D3" s="113" t="s">
         <v>140</v>
@@ -50392,13 +50404,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="113" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="B5" s="113" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C5" s="113" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="D5" s="113" t="s">
         <v>14</v>
@@ -53975,6 +53987,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="107e75b3-53cc-4838-92d2-ebc011bd4832">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="888ccf44-0d39-41a2-ab17-f7efb2bf6977" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004FD8CECCB51EC843BF514AFE68379818" ma:contentTypeVersion="18" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="eda339f53f012ceb64677667a741b441">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="107e75b3-53cc-4838-92d2-ebc011bd4832" xmlns:ns3="888ccf44-0d39-41a2-ab17-f7efb2bf6977" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04a86f3db711706e561c315688f1c464" ns2:_="" ns3:_="">
     <xsd:import namespace="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
@@ -54223,27 +54255,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="107e75b3-53cc-4838-92d2-ebc011bd4832">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="888ccf44-0d39-41a2-ab17-f7efb2bf6977" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2288FB7-E85A-4FE8-9E7A-FE572FF16064}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="888ccf44-0d39-41a2-ab17-f7efb2bf6977"/>
+    <ds:schemaRef ds:uri="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F91B7B9-75FF-4624-B506-952B5B54766C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -54260,29 +54297,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2288FB7-E85A-4FE8-9E7A-FE572FF16064}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="888ccf44-0d39-41a2-ab17-f7efb2bf6977"/>
-    <ds:schemaRef ds:uri="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>